<commit_message>
#28 resolved import errors but arelle is not validating
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C33A139-C6DA-1646-974A-71E2D7B9E120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CBA805-B69A-E84F-BACE-D277747A4E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="834" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26131,7 +26131,7 @@
   <dimension ref="A1:K106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
#30 edits to ACFR template
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60491F8-56B5-6745-B7DB-D5CC36320469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A484448C-2984-784A-9513-B25EF6972768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="834" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lookup Net Position" sheetId="8" state="hidden" r:id="rId1"/>
+    <sheet name="Lookup Net Position" sheetId="8" r:id="rId1"/>
     <sheet name="Lookup GovWide Stmt Activities" sheetId="20" state="hidden" r:id="rId2"/>
     <sheet name="Lookup PropFunds" sheetId="23" state="hidden" r:id="rId3"/>
     <sheet name="Lookup PropFunds CashFlows" sheetId="26" state="hidden" r:id="rId4"/>
@@ -19174,8 +19174,8 @@
   </sheetPr>
   <dimension ref="A1:G616"/>
   <sheetViews>
-    <sheetView topLeftCell="A578" workbookViewId="0">
-      <selection activeCell="B616" sqref="B616"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="C156" sqref="C156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -36194,8 +36194,8 @@
   </sheetPr>
   <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L57" sqref="L57"/>
+    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
#28 added placeholder function
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A484448C-2984-784A-9513-B25EF6972768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EB14E6-B5AD-304C-945E-21424B028E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="834" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Net Position" sheetId="8" r:id="rId1"/>
@@ -19174,7 +19174,7 @@
   </sheetPr>
   <dimension ref="A1:G616"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C156" sqref="C156"/>
     </sheetView>
   </sheetViews>
@@ -34792,8 +34792,8 @@
   </sheetPr>
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64:XFD64"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -56230,7 +56230,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
started a new text doc
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EB14E6-B5AD-304C-945E-21424B028E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D140FFCC-AFDC-3B4A-A42B-1B5CD5809106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="834" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Net Position" sheetId="8" r:id="rId1"/>
@@ -19174,8 +19174,8 @@
   </sheetPr>
   <dimension ref="A1:G616"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C156" sqref="C156"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -34792,7 +34792,7 @@
   </sheetPr>
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
editted filled Clayton sample
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarrahahmed/Desktop/CLOSUP/process-xbrl/app/static/input_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960699EA-5401-5B4D-86CB-16D8D15D30B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F82A9C-9FFF-7348-B6BC-6076A774A843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" tabRatio="834" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="834" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Net Position" sheetId="8" r:id="rId1"/>
@@ -12097,12 +12097,10 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12114,18 +12112,12 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12146,6 +12138,14 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12771,8 +12771,8 @@
   </sheetPr>
   <dimension ref="A1:C514"/>
   <sheetViews>
-    <sheetView topLeftCell="A300" zoomScale="56" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A256" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -26105,31 +26105,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:J65">
-    <cfRule type="expression" dxfId="13" priority="3" stopIfTrue="1">
-      <formula>D$7=""</formula>
+    <cfRule type="expression" dxfId="13" priority="7" stopIfTrue="1">
+      <formula>#REF!=""</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="12" priority="4" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="expression" dxfId="11" priority="3" stopIfTrue="1">
+      <formula>D$7=""</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="5" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="notEqual">
       <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="7" stopIfTrue="1">
-      <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D69:J69">
-    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
-      <formula>D$7=""</formula>
+    <cfRule type="cellIs" dxfId="8" priority="10" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="7" priority="9" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
+    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
+      <formula>D$7=""</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="5" priority="11" operator="notEqual">
       <formula>#REF!</formula>
@@ -26205,8 +26205,8 @@
   </sheetPr>
   <dimension ref="A1:C358"/>
   <sheetViews>
-    <sheetView topLeftCell="A141" zoomScale="56" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B201" sqref="B201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -46030,7 +46030,7 @@
   </sheetPr>
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
issue 62- completed custom tags for statement of net position. Need more info to do others
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/app/static/input_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarrahahmed/Desktop/CLOSUP/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F82A9C-9FFF-7348-B6BC-6076A774A843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F151A140-A923-2E4C-9F3B-1095D449F58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="834" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="28800" windowHeight="17280" tabRatio="834" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Net Position" sheetId="8" r:id="rId1"/>
@@ -12097,10 +12097,12 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="0"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12112,12 +12114,18 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12138,14 +12146,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12771,7 +12771,7 @@
   </sheetPr>
   <dimension ref="A1:C514"/>
   <sheetViews>
-    <sheetView topLeftCell="A256" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A90" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -26105,31 +26105,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:J65">
-    <cfRule type="expression" dxfId="13" priority="7" stopIfTrue="1">
-      <formula>#REF!=""</formula>
+    <cfRule type="expression" dxfId="13" priority="3" stopIfTrue="1">
+      <formula>D$7=""</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="12" priority="4" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="3" stopIfTrue="1">
-      <formula>D$7=""</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="notEqual">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="notEqual">
       <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="7" stopIfTrue="1">
+      <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D69:J69">
-    <cfRule type="cellIs" dxfId="8" priority="10" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
+    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
+      <formula>D$7=""</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="7" priority="9" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
-      <formula>D$7=""</formula>
+    <cfRule type="cellIs" dxfId="6" priority="10" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="5" priority="11" operator="notEqual">
       <formula>#REF!</formula>
@@ -26205,7 +26205,7 @@
   </sheetPr>
   <dimension ref="A1:C358"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A196" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B201" sqref="B201"/>
     </sheetView>
   </sheetViews>
@@ -46030,8 +46030,8 @@
   </sheetPr>
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="116" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -46138,7 +46138,7 @@
     </row>
     <row r="9" spans="1:6" ht="15">
       <c r="A9" s="6" t="str">
-        <f>IF(B9="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B9,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B9="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B9)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B9,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B9" s="15"/>
@@ -46152,7 +46152,7 @@
     </row>
     <row r="10" spans="1:6" ht="15">
       <c r="A10" s="6" t="str">
-        <f>IF(B10="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B10,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B10="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B10)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B10,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B10" s="15"/>
@@ -46166,7 +46166,7 @@
     </row>
     <row r="11" spans="1:6" ht="15">
       <c r="A11" s="6" t="str">
-        <f>IF(B11="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B11,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B11="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B11)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B11,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B11" s="15"/>
@@ -46180,7 +46180,7 @@
     </row>
     <row r="12" spans="1:6" ht="15">
       <c r="A12" s="6" t="str">
-        <f>IF(B12="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B12,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B12="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B12)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B12,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B12" s="15"/>
@@ -46194,7 +46194,7 @@
     </row>
     <row r="13" spans="1:6" ht="15">
       <c r="A13" s="6" t="str">
-        <f>IF(B13="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B13,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B13="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B13)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B13,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B13" s="15"/>
@@ -46205,7 +46205,7 @@
     </row>
     <row r="14" spans="1:6" ht="15">
       <c r="A14" s="6" t="str">
-        <f>IF(B14="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B14,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B14="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B14)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B14,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B14" s="15"/>
@@ -46216,7 +46216,7 @@
     </row>
     <row r="15" spans="1:6" ht="15">
       <c r="A15" s="6" t="str">
-        <f>IF(B15="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B15,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B15="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B15)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B15,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B15" s="15"/>
@@ -46227,7 +46227,7 @@
     </row>
     <row r="16" spans="1:6" ht="15">
       <c r="A16" s="6" t="str">
-        <f>IF(B16="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B16,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B16="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B16)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B16,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B16" s="15"/>
@@ -46241,7 +46241,7 @@
     </row>
     <row r="17" spans="1:6" ht="15">
       <c r="A17" s="6" t="str">
-        <f>IF(B17="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B17,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B17="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B17)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B17,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B17" s="15"/>
@@ -46255,7 +46255,7 @@
     </row>
     <row r="18" spans="1:6" ht="15" hidden="1">
       <c r="A18" s="6" t="str">
-        <f>IF(B18="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B18,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B18="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B18)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B18,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B18" s="15"/>
@@ -46269,7 +46269,7 @@
     </row>
     <row r="19" spans="1:6" ht="15" hidden="1">
       <c r="A19" s="6" t="str">
-        <f>IF(B19="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B19,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B19="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B19)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B19,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B19" s="15"/>
@@ -46283,7 +46283,7 @@
     </row>
     <row r="20" spans="1:6" ht="15" hidden="1">
       <c r="A20" s="6" t="str">
-        <f>IF(B20="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B20,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B20="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B20)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B20,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B20" s="15"/>
@@ -46297,7 +46297,7 @@
     </row>
     <row r="21" spans="1:6" ht="15" hidden="1">
       <c r="A21" s="6" t="str">
-        <f>IF(B21="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B21,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B21="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B21)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B21,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B21" s="15"/>
@@ -46311,7 +46311,7 @@
     </row>
     <row r="22" spans="1:6" ht="15">
       <c r="A22" s="6" t="str">
-        <f>IF(B22="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B22,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B22="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B22)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B22,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B22" s="15"/>
@@ -46358,7 +46358,7 @@
     </row>
     <row r="25" spans="1:6" ht="15">
       <c r="A25" s="6" t="str">
-        <f>IF(B25="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B25,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B25="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B25)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B25,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B25" s="15"/>
@@ -46372,7 +46372,7 @@
     </row>
     <row r="26" spans="1:6" ht="15">
       <c r="A26" s="6" t="str">
-        <f>IF(B26="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B26,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B26="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B26)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B26,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B26" s="15"/>
@@ -46383,7 +46383,7 @@
     </row>
     <row r="27" spans="1:6" ht="15">
       <c r="A27" s="6" t="str">
-        <f>IF(B27="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B27,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B27="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B27)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B27,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B27" s="16"/>
@@ -46394,7 +46394,7 @@
     </row>
     <row r="28" spans="1:6" ht="15">
       <c r="A28" s="6" t="str">
-        <f>IF(B28="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B28,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B28="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B28)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B28,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B28" s="16"/>
@@ -46405,7 +46405,7 @@
     </row>
     <row r="29" spans="1:6" ht="15">
       <c r="A29" s="6" t="str">
-        <f>IF(B29="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B29,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B29="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B29)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B29,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B29" s="16"/>
@@ -46416,7 +46416,7 @@
     </row>
     <row r="30" spans="1:6" ht="15">
       <c r="A30" s="6" t="str">
-        <f>IF(B30="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B30,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B30="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B30)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B30,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B30" s="15"/>
@@ -46427,7 +46427,7 @@
     </row>
     <row r="31" spans="1:6" ht="15">
       <c r="A31" s="6" t="str">
-        <f>IF(B31="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B31,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B31="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B31)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B31,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B31" s="15"/>
@@ -46576,7 +46576,7 @@
     </row>
     <row r="41" spans="1:6" ht="15">
       <c r="A41" s="6" t="str">
-        <f>IF(B41="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B41,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B41="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B41)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B41,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B41" s="15"/>
@@ -46590,7 +46590,7 @@
     </row>
     <row r="42" spans="1:6" ht="15">
       <c r="A42" s="6" t="str">
-        <f>IF(B42="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B42,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B42="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B42)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B42,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B42" s="15"/>
@@ -46604,7 +46604,7 @@
     </row>
     <row r="43" spans="1:6" ht="15">
       <c r="A43" s="6" t="str">
-        <f>IF(B43="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B43,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B43="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B43)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B43,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B43" s="15"/>
@@ -46618,7 +46618,7 @@
     </row>
     <row r="44" spans="1:6" ht="15">
       <c r="A44" s="6" t="str">
-        <f>IF(B44="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B44,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B44="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B44)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B44,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B44" s="15"/>
@@ -46632,7 +46632,7 @@
     </row>
     <row r="45" spans="1:6" ht="15">
       <c r="A45" s="6" t="str">
-        <f>IF(B45="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B45,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B45="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B45)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B45,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B45" s="15"/>
@@ -46753,7 +46753,7 @@
     </row>
     <row r="54" spans="1:6" ht="15">
       <c r="A54" s="6" t="str">
-        <f>IF(B54="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B54,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B54="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B54)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B54,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B54" s="15"/>
@@ -46767,7 +46767,7 @@
     </row>
     <row r="55" spans="1:6" ht="15">
       <c r="A55" s="6" t="str">
-        <f>IF(B55="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B55,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B55="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B55)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B55,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B55" s="15"/>
@@ -46781,7 +46781,7 @@
     </row>
     <row r="56" spans="1:6" ht="15">
       <c r="A56" s="6" t="str">
-        <f>IF(B56="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B56,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B56="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B56)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B56,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B56" s="15"/>
@@ -46795,7 +46795,7 @@
     </row>
     <row r="57" spans="1:6" ht="16" customHeight="1">
       <c r="A57" s="6" t="str">
-        <f>IF(B57="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B57,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B57="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B57)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B57,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B57" s="15"/>
@@ -46809,7 +46809,7 @@
     </row>
     <row r="58" spans="1:6" ht="16" customHeight="1">
       <c r="A58" s="6" t="str">
-        <f>IF(B58="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B58,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B58="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B58)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B58,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B58" s="15"/>
@@ -46823,7 +46823,7 @@
     </row>
     <row r="59" spans="1:6" ht="16" customHeight="1">
       <c r="A59" s="6" t="str">
-        <f>IF(B59="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B59,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B59="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B59)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B59,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B59" s="15"/>
@@ -46940,7 +46940,7 @@
     </row>
     <row r="67" spans="1:6" ht="15">
       <c r="A67" s="6" t="str">
-        <f>IF(B67="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B67,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B67="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B67)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B67,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B67" s="15"/>
@@ -46951,7 +46951,7 @@
     </row>
     <row r="68" spans="1:6" ht="15">
       <c r="A68" s="6" t="str">
-        <f>IF(B68="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B68,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B68="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B68)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B68,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B68" s="15"/>
@@ -46962,7 +46962,7 @@
     </row>
     <row r="69" spans="1:6" ht="15">
       <c r="A69" s="6" t="str">
-        <f>IF(B69="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B69,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B69="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B69)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B69,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B69" s="15"/>
@@ -46973,7 +46973,7 @@
     </row>
     <row r="70" spans="1:6" ht="15">
       <c r="A70" s="6" t="str">
-        <f>IF(B70="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B70,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B70="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B70)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B70,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B70" s="15"/>
@@ -47122,7 +47122,7 @@
     </row>
     <row r="80" spans="1:6" ht="15">
       <c r="A80" s="6" t="str">
-        <f>IF(B80="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B80,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B80="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B80)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B80,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B80" s="15"/>
@@ -47136,7 +47136,7 @@
     </row>
     <row r="81" spans="1:6" ht="15">
       <c r="A81" s="6" t="str">
-        <f>IF(B81="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B81,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B81="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B81)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B81,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B81" s="15"/>
@@ -47150,7 +47150,7 @@
     </row>
     <row r="82" spans="1:6" ht="15">
       <c r="A82" s="6" t="str">
-        <f>IF(B82="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B82,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B82="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B82)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B82,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B82" s="15"/>
@@ -47164,7 +47164,7 @@
     </row>
     <row r="83" spans="1:6" ht="15">
       <c r="A83" s="6" t="str">
-        <f>IF(B83="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B83,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B83="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B83)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B83,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B83" s="15"/>
@@ -47289,7 +47289,7 @@
     </row>
     <row r="92" spans="1:6" ht="15">
       <c r="A92" s="6" t="str">
-        <f>IF(B92="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B92,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B92="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B92)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B92,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B92" s="15"/>
@@ -47300,7 +47300,7 @@
     </row>
     <row r="93" spans="1:6" ht="15">
       <c r="A93" s="6" t="str">
-        <f>IF(B93="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B93,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B93="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B93)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B93,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B93" s="15"/>
@@ -47311,7 +47311,7 @@
     </row>
     <row r="94" spans="1:6" ht="15">
       <c r="A94" s="6" t="str">
-        <f>IF(B94="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B94,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B94="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B94)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B94,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B94" s="15"/>
@@ -47322,7 +47322,7 @@
     </row>
     <row r="95" spans="1:6" ht="15">
       <c r="A95" s="6" t="str">
-        <f>IF(B95="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B95,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B95="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B95)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B95,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B95" s="15"/>
@@ -47475,43 +47475,43 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{17CB63B2-6582-4D03-B5CB-EC836B51979D}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{17CB63B2-6582-4D03-B5CB-EC836B51979D}">
           <x14:formula1>
             <xm:f>'Lookup Net Position'!$B$2:$B$201</xm:f>
           </x14:formula1>
           <xm:sqref>B9:B22</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2DD168EE-A03C-8F4C-872A-75D1E96C9387}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{2DD168EE-A03C-8F4C-872A-75D1E96C9387}">
           <x14:formula1>
             <xm:f>'Lookup Net Position'!$B$376:$B$468</xm:f>
           </x14:formula1>
           <xm:sqref>B25:B31</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4FFB8072-34D5-0E4C-AD99-305AB4DE3537}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{4FFB8072-34D5-0E4C-AD99-305AB4DE3537}">
           <x14:formula1>
             <xm:f>'Lookup Net Position'!$B$338:$B$354</xm:f>
           </x14:formula1>
           <xm:sqref>B41:B45</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5E57702C-3DA0-0A46-8890-D2C20B8F1A6A}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{5E57702C-3DA0-0A46-8890-D2C20B8F1A6A}">
           <x14:formula1>
             <xm:f>'Lookup Net Position'!$B$202:$B$315</xm:f>
           </x14:formula1>
           <xm:sqref>B54:B59</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{89640B5B-A8EB-F245-8EA4-3FEF01E0F642}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{89640B5B-A8EB-F245-8EA4-3FEF01E0F642}">
           <x14:formula1>
             <xm:f>'Lookup Net Position'!$B$469:$B$514</xm:f>
           </x14:formula1>
           <xm:sqref>B67:B70</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AC956507-5236-0F49-901C-44C6F0615B5B}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{AC956507-5236-0F49-901C-44C6F0615B5B}">
           <x14:formula1>
             <xm:f>'Lookup Net Position'!$B$316:$B$337</xm:f>
           </x14:formula1>
           <xm:sqref>B80:B83</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{70A74EAE-D4A3-124D-8A1A-56BFB96B62AC}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{70A74EAE-D4A3-124D-8A1A-56BFB96B62AC}">
           <x14:formula1>
             <xm:f>'Lookup Net Position'!$B$355:$B$375</xm:f>
           </x14:formula1>
@@ -47530,8 +47530,8 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView topLeftCell="A5" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
Issue 62- completed custom tags for statement of activities
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarrahahmed/Desktop/CLOSUP/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F151A140-A923-2E4C-9F3B-1095D449F58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596403B2-A9BA-524B-A087-856E21D06BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="28800" windowHeight="17280" tabRatio="834" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="28800" windowHeight="17280" tabRatio="834" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Net Position" sheetId="8" r:id="rId1"/>
@@ -46030,8 +46030,8 @@
   </sheetPr>
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="116" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A3" zoomScale="116" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -47530,13 +47530,13 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="33" customWidth="1"/>
+    <col min="1" max="1" width="68.6640625" style="33" customWidth="1"/>
     <col min="2" max="2" width="41.5" style="33" customWidth="1"/>
     <col min="3" max="3" width="15" style="33" customWidth="1"/>
     <col min="4" max="4" width="17" style="33" customWidth="1"/>
@@ -47663,7 +47663,7 @@
     </row>
     <row r="9" spans="1:10" ht="17" customHeight="1">
       <c r="A9" s="50" t="str">
-        <f>IF(B9="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B9,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B9,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B9,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B9="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B9) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B9, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B9, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B9, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B9" s="15"/>
@@ -47682,9 +47682,9 @@
       </c>
       <c r="J9" s="244"/>
     </row>
-    <row r="10" spans="1:10" ht="15">
-      <c r="A10" s="6" t="str">
-        <f>IF(B10="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B10,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B10,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B10,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+    <row r="10" spans="1:10" ht="16">
+      <c r="A10" s="50" t="str">
+        <f>IF(B10="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B10) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B10, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B10, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B10, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B10" s="15"/>
@@ -47703,9 +47703,9 @@
       </c>
       <c r="J10" s="244"/>
     </row>
-    <row r="11" spans="1:10" ht="15">
-      <c r="A11" s="6" t="str">
-        <f>IF(B11="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B11,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B11,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B11,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+    <row r="11" spans="1:10" ht="16">
+      <c r="A11" s="50" t="str">
+        <f>IF(B11="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B11) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B11, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B11, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B11, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B11" s="15"/>
@@ -47724,9 +47724,9 @@
       </c>
       <c r="J11" s="244"/>
     </row>
-    <row r="12" spans="1:10" ht="15">
-      <c r="A12" s="6" t="str">
-        <f>IF(B12="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B12,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B12,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B12,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+    <row r="12" spans="1:10" ht="16">
+      <c r="A12" s="50" t="str">
+        <f>IF(B12="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B12) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B12, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B12, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B12, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B12" s="15"/>
@@ -47745,9 +47745,9 @@
       </c>
       <c r="J12" s="244"/>
     </row>
-    <row r="13" spans="1:10" ht="15">
-      <c r="A13" s="6" t="str">
-        <f>IF(B13="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B13,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B13,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B13,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+    <row r="13" spans="1:10" ht="16">
+      <c r="A13" s="50" t="str">
+        <f>IF(B13="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B13) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B13, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B13, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B13, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B13" s="15"/>
@@ -47766,9 +47766,9 @@
       </c>
       <c r="J13" s="244"/>
     </row>
-    <row r="14" spans="1:10" ht="15">
-      <c r="A14" s="6" t="str">
-        <f>IF(B14="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B14,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B14,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B14,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+    <row r="14" spans="1:10" ht="16">
+      <c r="A14" s="50" t="str">
+        <f>IF(B14="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B14) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B14, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B14, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B14, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B14" s="15"/>
@@ -47787,9 +47787,9 @@
       </c>
       <c r="J14" s="244"/>
     </row>
-    <row r="15" spans="1:10" ht="15">
-      <c r="A15" s="6" t="str">
-        <f>IF(B15="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B15,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B15,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B15,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+    <row r="15" spans="1:10" ht="16">
+      <c r="A15" s="50" t="str">
+        <f>IF(B15="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B15) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B15, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B15, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B15, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B15" s="15"/>
@@ -47808,9 +47808,9 @@
       </c>
       <c r="J15" s="244"/>
     </row>
-    <row r="16" spans="1:10" ht="15">
-      <c r="A16" s="6" t="str">
-        <f>IF(B16="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B16,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B16,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B16,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+    <row r="16" spans="1:10" ht="16">
+      <c r="A16" s="50" t="str">
+        <f>IF(B16="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B16) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B16, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B16, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B16, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B16" s="15"/>
@@ -47829,9 +47829,9 @@
       </c>
       <c r="J16" s="244"/>
     </row>
-    <row r="17" spans="1:10" ht="15">
-      <c r="A17" s="6" t="str">
-        <f>IF(B17="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B17,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B17,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B17,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+    <row r="17" spans="1:10" ht="16">
+      <c r="A17" s="50" t="str">
+        <f>IF(B17="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B17) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B17, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B17, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B17, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B17" s="15"/>
@@ -47850,9 +47850,9 @@
       </c>
       <c r="J17" s="244"/>
     </row>
-    <row r="18" spans="1:10" ht="15" hidden="1">
-      <c r="A18" s="6" t="str">
-        <f>IF(B18="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B18,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B18,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B18,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+    <row r="18" spans="1:10" ht="16" hidden="1">
+      <c r="A18" s="50" t="str">
+        <f>IF(B18="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B18) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B18, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B18, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B18, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B18" s="15"/>
@@ -47871,9 +47871,9 @@
       </c>
       <c r="J18" s="244"/>
     </row>
-    <row r="19" spans="1:10" ht="15" hidden="1">
-      <c r="A19" s="6" t="str">
-        <f>IF(B19="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B19,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B19,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B19,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+    <row r="19" spans="1:10" ht="16" hidden="1">
+      <c r="A19" s="50" t="str">
+        <f>IF(B19="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B19) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B19, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B19, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B19, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B19" s="15"/>
@@ -47892,9 +47892,9 @@
       </c>
       <c r="J19" s="244"/>
     </row>
-    <row r="20" spans="1:10" ht="15" hidden="1">
-      <c r="A20" s="6" t="str">
-        <f>IF(B20="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B20,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B20,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B20,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+    <row r="20" spans="1:10" ht="16" hidden="1">
+      <c r="A20" s="50" t="str">
+        <f>IF(B20="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B20) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B20, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B20, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B20, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B20" s="15"/>
@@ -47913,9 +47913,9 @@
       </c>
       <c r="J20" s="244"/>
     </row>
-    <row r="21" spans="1:10" ht="15" hidden="1">
-      <c r="A21" s="6" t="str">
-        <f>IF(B21="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B21,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B21,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B21,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+    <row r="21" spans="1:10" ht="16" hidden="1">
+      <c r="A21" s="50" t="str">
+        <f>IF(B21="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B21) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B21, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B21, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B21, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B21" s="15"/>
@@ -47934,9 +47934,9 @@
       </c>
       <c r="J21" s="244"/>
     </row>
-    <row r="22" spans="1:10" ht="15">
-      <c r="A22" s="6" t="str">
-        <f>IF(B22="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B22,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B22,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B22,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+    <row r="22" spans="1:10" ht="16">
+      <c r="A22" s="50" t="str">
+        <f>IF(B22="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B22) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B22, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B22, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B22, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B22" s="15"/>
@@ -48000,7 +48000,7 @@
     </row>
     <row r="25" spans="1:10" ht="15">
       <c r="A25" s="6" t="str">
-        <f>IF(B25="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B25,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B25,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B25,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B25="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B25) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B25, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B25, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B25, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B25" s="15"/>
@@ -48021,7 +48021,7 @@
     </row>
     <row r="26" spans="1:10" ht="15">
       <c r="A26" s="6" t="str">
-        <f>IF(B26="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B26,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B26,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B26,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B26="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B26) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B26, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B26, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B26, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B26" s="15"/>
@@ -48042,7 +48042,7 @@
     </row>
     <row r="27" spans="1:10" ht="15">
       <c r="A27" s="6" t="str">
-        <f>IF(B27="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B27,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B27,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B27,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B27="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B27) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B27, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B27, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B27, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B27" s="15"/>
@@ -48063,7 +48063,7 @@
     </row>
     <row r="28" spans="1:10" ht="15">
       <c r="A28" s="6" t="str">
-        <f>IF(B28="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B28,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B28,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B28,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B28="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B28) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B28, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B28, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B28, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B28" s="15"/>
@@ -48084,7 +48084,7 @@
     </row>
     <row r="29" spans="1:10" ht="15">
       <c r="A29" s="6" t="str">
-        <f>IF(B29="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B29,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B29,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B29,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B29="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B29) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B29, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B29, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B29, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B29" s="15"/>
@@ -48102,7 +48102,7 @@
     </row>
     <row r="30" spans="1:10" ht="15">
       <c r="A30" s="6" t="str">
-        <f>IF(B30="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B30,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B30,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B30,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B30="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B30) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B30, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B30, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B30, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B30" s="15"/>
@@ -48123,7 +48123,7 @@
     </row>
     <row r="31" spans="1:10" ht="15">
       <c r="A31" s="6" t="str">
-        <f>IF(B31="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B31,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B31,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B31,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B31="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B31) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B31, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B31, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B31, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B31" s="15"/>
@@ -48144,7 +48144,7 @@
     </row>
     <row r="32" spans="1:10" ht="15" hidden="1">
       <c r="A32" s="6" t="str">
-        <f>IF(B32="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B32,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B32,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B32,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B32="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B32) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B32, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B32, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B32, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B32" s="15"/>
@@ -48165,7 +48165,7 @@
     </row>
     <row r="33" spans="1:10" ht="15" hidden="1">
       <c r="A33" s="6" t="str">
-        <f>IF(B33="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B33,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B33,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B33,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B33="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B33) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B33, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B33, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B33, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B33" s="15"/>
@@ -48186,7 +48186,7 @@
     </row>
     <row r="34" spans="1:10" ht="15" hidden="1">
       <c r="A34" s="6" t="str">
-        <f>IF(B34="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B34,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B34,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B34,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B34="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B34) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B34, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B34, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B34, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B34" s="15"/>
@@ -48207,7 +48207,7 @@
     </row>
     <row r="35" spans="1:10" ht="15" hidden="1">
       <c r="A35" s="6" t="str">
-        <f>IF(B35="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B35,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B35,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B35,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B35="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B35) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B35, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B35, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B35, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B35" s="15"/>
@@ -48228,7 +48228,7 @@
     </row>
     <row r="36" spans="1:10" ht="15">
       <c r="A36" s="6" t="str">
-        <f>IF(B36="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B36,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B36,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B36,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B36="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B36) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B36, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B36, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B36, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B36" s="15"/>
@@ -48341,7 +48341,7 @@
     </row>
     <row r="41" spans="1:10" ht="15">
       <c r="A41" s="6" t="str">
-        <f>IF(B41="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B41,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B41,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B41,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B41="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B41) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B41, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B41, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B41, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B41" s="15"/>
@@ -48368,7 +48368,7 @@
     </row>
     <row r="42" spans="1:10" ht="15">
       <c r="A42" s="6" t="str">
-        <f>IF(B42="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B42,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B42,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B42,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B42="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B42) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B42, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B42, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B42, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B42" s="15"/>
@@ -48395,7 +48395,7 @@
     </row>
     <row r="43" spans="1:10" ht="15">
       <c r="A43" s="6" t="str">
-        <f>IF(B43="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B43,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B43,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B43,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B43="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B43) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B43, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B43, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B43, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B43" s="15"/>
@@ -48422,7 +48422,7 @@
     </row>
     <row r="44" spans="1:10" ht="15">
       <c r="A44" s="6" t="str">
-        <f>IF(B44="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B44,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B44,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B44,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B44="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B44) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B44, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B44, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B44, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B44" s="15"/>
@@ -48449,7 +48449,7 @@
     </row>
     <row r="45" spans="1:10" ht="15">
       <c r="A45" s="6" t="str">
-        <f>IF(B45="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B45,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B45,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B45,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B45="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B45) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B45, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B45, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B45, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B45" s="15"/>
@@ -48476,7 +48476,7 @@
     </row>
     <row r="46" spans="1:10" ht="15" hidden="1">
       <c r="A46" s="6" t="str">
-        <f>IF(B46="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B46,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B46,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B46,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B46="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B46) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B46, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B46, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B46, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B46" s="15"/>
@@ -48503,7 +48503,7 @@
     </row>
     <row r="47" spans="1:10" ht="15" hidden="1">
       <c r="A47" s="6" t="str">
-        <f>IF(B47="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B47,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B47,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B47,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B47="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B47) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B47, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B47, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B47, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B47" s="15"/>
@@ -48530,7 +48530,7 @@
     </row>
     <row r="48" spans="1:10" ht="15" hidden="1">
       <c r="A48" s="6" t="str">
-        <f>IF(B48="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B48,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B48,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B48,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B48="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B48) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B48, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B48, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B48, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B48" s="15"/>
@@ -48557,7 +48557,7 @@
     </row>
     <row r="49" spans="1:10" ht="15">
       <c r="A49" s="6" t="str">
-        <f>IF(B49="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B49,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D),",",_xlfn.XLOOKUP(B49,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$C:$C), ",",_xlfn.XLOOKUP(B49,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$E:$E)))</f>
+        <f>IF(B49="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B49) = 0, "acfr:ExpensesCustom, acfr:RevenueForOtherProgramsCustom, acfr:NetExpenseRevenueCustom", _xlfn.CONCAT(_xlfn.XLOOKUP(B49, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D), ",", _xlfn.XLOOKUP(B49, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$C:$C), ",", _xlfn.XLOOKUP(B49, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$E:$E))))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B49" s="15"/>
@@ -48654,7 +48654,7 @@
     </row>
     <row r="54" spans="1:10" ht="15">
       <c r="A54" s="6" t="str">
-        <f>IF(B54="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B54,'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D))</f>
+        <f>IF(B54="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B54) = 0, "acfr:GeneralRevenuesCustom", _xlfn.XLOOKUP(B54, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B54" s="15"/>
@@ -48672,7 +48672,7 @@
     </row>
     <row r="55" spans="1:10" ht="15">
       <c r="A55" s="6" t="str">
-        <f>IF(B55="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B55,'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D))</f>
+        <f>IF(B55="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B55) = 0, "acfr:GeneralRevenuesCustom", _xlfn.XLOOKUP(B55, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B55" s="15"/>
@@ -48690,7 +48690,7 @@
     </row>
     <row r="56" spans="1:10" ht="15">
       <c r="A56" s="6" t="str">
-        <f>IF(B56="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B56,'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D))</f>
+        <f>IF(B56="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B56) = 0, "acfr:GeneralRevenuesCustom", _xlfn.XLOOKUP(B56, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B56" s="15"/>
@@ -48708,7 +48708,7 @@
     </row>
     <row r="57" spans="1:10" ht="15">
       <c r="A57" s="6" t="str">
-        <f>IF(B57="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B57,'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D))</f>
+        <f>IF(B57="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B57) = 0, "acfr:GeneralRevenuesCustom", _xlfn.XLOOKUP(B57, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B57" s="15"/>
@@ -48726,7 +48726,7 @@
     </row>
     <row r="58" spans="1:10" ht="15">
       <c r="A58" s="6" t="str">
-        <f>IF(B58="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B58,'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D))</f>
+        <f>IF(B58="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B58) = 0, "acfr:GeneralRevenuesCustom", _xlfn.XLOOKUP(B58, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B58" s="15"/>
@@ -48744,7 +48744,7 @@
     </row>
     <row r="59" spans="1:10" ht="15">
       <c r="A59" s="6" t="str">
-        <f>IF(B59="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B59,'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D))</f>
+        <f>IF(B59="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B59) = 0, "acfr:GeneralRevenuesCustom", _xlfn.XLOOKUP(B59, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B59" s="15"/>
@@ -48762,7 +48762,7 @@
     </row>
     <row r="60" spans="1:10" ht="15">
       <c r="A60" s="6" t="str">
-        <f>IF(B60="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B60,'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D))</f>
+        <f>IF(B60="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B60) = 0, "acfr:GeneralRevenuesCustom", _xlfn.XLOOKUP(B60, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B60" s="15"/>
@@ -48780,7 +48780,7 @@
     </row>
     <row r="61" spans="1:10" ht="15">
       <c r="A61" s="6" t="str">
-        <f>IF(B61="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B61,'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D))</f>
+        <f>IF(B61="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B61) = 0, "acfr:GeneralRevenuesCustom", _xlfn.XLOOKUP(B61, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B61" s="15"/>
@@ -48798,7 +48798,7 @@
     </row>
     <row r="62" spans="1:10" ht="15">
       <c r="A62" s="6" t="str">
-        <f>IF(B62="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B62,'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D))</f>
+        <f>IF(B62="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B62) = 0, "acfr:GeneralRevenuesCustom", _xlfn.XLOOKUP(B62, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B62" s="15"/>
@@ -48816,7 +48816,7 @@
     </row>
     <row r="63" spans="1:10" ht="15">
       <c r="A63" s="6" t="str">
-        <f>IF(B63="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B63,'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D))</f>
+        <f>IF(B63="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B63) = 0, "acfr:GeneralRevenuesCustom", _xlfn.XLOOKUP(B63, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B63" s="15"/>
@@ -48871,7 +48871,7 @@
     </row>
     <row r="66" spans="1:10" ht="15">
       <c r="A66" s="6" t="str">
-        <f>IF(B66="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B66,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D))</f>
+        <f>IF(B66="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B66) = 0, "acfr:AdjustmentsForTransferOfRevenuesWithinActivitiesCustom", _xlfn.XLOOKUP(B66, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B66" s="15"/>
@@ -48889,7 +48889,7 @@
     </row>
     <row r="67" spans="1:10" ht="15">
       <c r="A67" s="6" t="str">
-        <f>IF(B67="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B67,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D))</f>
+        <f>IF(B67="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B67) = 0, "acfr:AdjustmentsForTransferOfRevenuesWithinActivitiesCustom", _xlfn.XLOOKUP(B67, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B67" s="15"/>
@@ -48907,7 +48907,7 @@
     </row>
     <row r="68" spans="1:10" ht="15">
       <c r="A68" s="6" t="str">
-        <f>IF(B68="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B68,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D))</f>
+        <f>IF(B68="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B68) = 0, "acfr:AdjustmentsForTransferOfRevenuesWithinActivitiesCustom", _xlfn.XLOOKUP(B68, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B68" s="15"/>
@@ -48925,7 +48925,7 @@
     </row>
     <row r="69" spans="1:10" ht="15">
       <c r="A69" s="6" t="str">
-        <f>IF(B69="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B69,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D))</f>
+        <f>IF(B69="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B69) = 0, "acfr:AdjustmentsForTransferOfRevenuesWithinActivitiesCustom", _xlfn.XLOOKUP(B69, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B69" s="15"/>
@@ -48943,7 +48943,7 @@
     </row>
     <row r="70" spans="1:10" ht="15">
       <c r="A70" s="6" t="str">
-        <f>IF(B70="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B70,'Lookup GovWide Stmt Activities'!$B:$B,'Lookup GovWide Stmt Activities'!$D:$D))</f>
+        <f>IF(B70="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovWide Stmt Activities'!$B:$B, B70) = 0, "acfr:AdjustmentsForTransferOfRevenuesWithinActivitiesCustom", _xlfn.XLOOKUP(B70, 'Lookup GovWide Stmt Activities'!$B:$B, 'Lookup GovWide Stmt Activities'!$D:$D)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B70" s="15"/>
@@ -49226,15 +49226,18 @@
       <formula>J$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B22 B25:B36 B41:B49" xr:uid="{F3C11D5E-2141-5546-AF1F-2279D6DA74D8}">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B41:B49" xr:uid="{F3C11D5E-2141-5546-AF1F-2279D6DA74D8}">
       <formula1>program_revenues</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B54:B63" xr:uid="{96AC2388-DB7C-8442-BE26-CB837586D707}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B54:B63" xr:uid="{96AC2388-DB7C-8442-BE26-CB837586D707}">
       <formula1>general_revenues</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B66:B70" xr:uid="{A7A9E828-3622-4441-839C-4C8E5DABEB87}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B66:B70" xr:uid="{A7A9E828-3622-4441-839C-4C8E5DABEB87}">
       <formula1>transfers</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B9:B22 B25:B36" xr:uid="{5B081783-9278-9542-AB7A-E156D9F5E750}">
+      <formula1>program_revenues</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
issue 62- finished adding custom tags
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarrahahmed/Desktop/CLOSUP/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596403B2-A9BA-524B-A087-856E21D06BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D70992D-F977-1A45-A28C-CD9D8F6EBF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="28800" windowHeight="17280" tabRatio="834" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="28800" windowHeight="17280" tabRatio="834" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Net Position" sheetId="8" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5346" uniqueCount="3615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5349" uniqueCount="3618">
   <si>
     <t>Statement of Net Position</t>
   </si>
@@ -10938,6 +10938,15 @@
   </si>
   <si>
     <t>Label (without Spaces)</t>
+  </si>
+  <si>
+    <t>acfr:FundBalanceAssignedCustom</t>
+  </si>
+  <si>
+    <t>acfr:FundBalanceCommittedCustom</t>
+  </si>
+  <si>
+    <t>acfr:FundBalanceRestrictedCustom</t>
   </si>
 </sst>
 </file>
@@ -11558,7 +11567,7 @@
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="249">
+  <cellXfs count="250">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -12041,6 +12050,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="27" fillId="18" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -12771,7 +12781,7 @@
   </sheetPr>
   <dimension ref="A1:C514"/>
   <sheetViews>
-    <sheetView topLeftCell="A90" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A202" zoomScale="75" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -18451,15 +18461,15 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="75" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView topLeftCell="A59" zoomScale="96" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" style="120" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" style="120" customWidth="1"/>
     <col min="2" max="2" width="29.5" style="171" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" style="120" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" style="120" customWidth="1"/>
@@ -18593,7 +18603,7 @@
     </row>
     <row r="9" spans="1:10" ht="15">
       <c r="A9" s="108" t="str">
-        <f>IF(B9="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B9,#REF!,#REF!))</f>
+        <f>IF(B9="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B9) = 0, "acfr:AssetsCustomModifiedAccrual", _xlfn.XLOOKUP(B9, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B9" s="166"/>
@@ -18611,7 +18621,7 @@
     </row>
     <row r="10" spans="1:10" ht="15">
       <c r="A10" s="108" t="str">
-        <f>IF(B10="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B10,#REF!,#REF!))</f>
+        <f>IF(B10="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B10) = 0, "acfr:AssetsCustomModifiedAccrual", _xlfn.XLOOKUP(B10, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B10" s="166"/>
@@ -18629,7 +18639,7 @@
     </row>
     <row r="11" spans="1:10" ht="15">
       <c r="A11" s="108" t="str">
-        <f>IF(B11="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B11,#REF!,#REF!))</f>
+        <f>IF(B11="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B11) = 0, "acfr:AssetsCustomModifiedAccrual", _xlfn.XLOOKUP(B11, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B11" s="166"/>
@@ -18647,7 +18657,7 @@
     </row>
     <row r="12" spans="1:10" ht="15">
       <c r="A12" s="108" t="str">
-        <f>IF(B12="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B12,#REF!,#REF!))</f>
+        <f>IF(B12="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B12) = 0, "acfr:AssetsCustomModifiedAccrual", _xlfn.XLOOKUP(B12, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B12" s="166"/>
@@ -18665,7 +18675,7 @@
     </row>
     <row r="13" spans="1:10" ht="15">
       <c r="A13" s="108" t="str">
-        <f>IF(B13="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B13,#REF!,#REF!))</f>
+        <f>IF(B13="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B13) = 0, "acfr:AssetsCustomModifiedAccrual", _xlfn.XLOOKUP(B13, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B13" s="166"/>
@@ -18683,7 +18693,7 @@
     </row>
     <row r="14" spans="1:10" ht="15">
       <c r="A14" s="108" t="str">
-        <f>IF(B14="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B14,#REF!,#REF!))</f>
+        <f>IF(B14="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B14) = 0, "acfr:AssetsCustomModifiedAccrual", _xlfn.XLOOKUP(B14, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B14" s="166"/>
@@ -18701,7 +18711,7 @@
     </row>
     <row r="15" spans="1:10" ht="15">
       <c r="A15" s="108" t="str">
-        <f>IF(B15="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B15,#REF!,#REF!))</f>
+        <f>IF(B15="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B15) = 0, "acfr:AssetsCustomModifiedAccrual", _xlfn.XLOOKUP(B15, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B15" s="166"/>
@@ -18719,7 +18729,7 @@
     </row>
     <row r="16" spans="1:10" ht="15">
       <c r="A16" s="108" t="str">
-        <f>IF(B16="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B16,#REF!,#REF!))</f>
+        <f>IF(B16="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B16) = 0, "acfr:AssetsCustomModifiedAccrual", _xlfn.XLOOKUP(B16, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B16" s="166"/>
@@ -18737,7 +18747,7 @@
     </row>
     <row r="17" spans="1:10" ht="15">
       <c r="A17" s="108" t="str">
-        <f>IF(B17="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B17,#REF!,#REF!))</f>
+        <f>IF(B17="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B17) = 0, "acfr:AssetsCustomModifiedAccrual", _xlfn.XLOOKUP(B17, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B17" s="166"/>
@@ -18755,7 +18765,7 @@
     </row>
     <row r="18" spans="1:10" ht="15">
       <c r="A18" s="108" t="str">
-        <f>IF(B18="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B18,#REF!,#REF!))</f>
+        <f>IF(B18="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B18) = 0, "acfr:AssetsCustomModifiedAccrual", _xlfn.XLOOKUP(B18, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B18" s="166"/>
@@ -18838,7 +18848,7 @@
     </row>
     <row r="22" spans="1:10" ht="15">
       <c r="A22" s="108" t="str">
-        <f>IF(B22="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B22,#REF!,#REF!))</f>
+        <f>IF(B22="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B22) = 0, "acfr:LiabilitiesCustomModifiedAccrual", _xlfn.XLOOKUP(B22, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B22" s="166"/>
@@ -18856,7 +18866,7 @@
     </row>
     <row r="23" spans="1:10" ht="15">
       <c r="A23" s="108" t="str">
-        <f>IF(B23="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B23,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B23="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B23) = 0, "acfr:LiabilitiesCustomModifiedAccrual", _xlfn.XLOOKUP(B23, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B23" s="166"/>
@@ -18874,7 +18884,7 @@
     </row>
     <row r="24" spans="1:10" ht="15">
       <c r="A24" s="108" t="str">
-        <f>IF(B24="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B24,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B24="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B24) = 0, "acfr:LiabilitiesCustomModifiedAccrual", _xlfn.XLOOKUP(B24, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B24" s="166"/>
@@ -18892,7 +18902,7 @@
     </row>
     <row r="25" spans="1:10" ht="15">
       <c r="A25" s="108" t="str">
-        <f>IF(B25="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B25,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B25="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B25) = 0, "acfr:LiabilitiesCustomModifiedAccrual", _xlfn.XLOOKUP(B25, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B25" s="166"/>
@@ -18910,7 +18920,7 @@
     </row>
     <row r="26" spans="1:10" ht="15">
       <c r="A26" s="108" t="str">
-        <f>IF(B26="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B26,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B26="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B26) = 0, "acfr:LiabilitiesCustomModifiedAccrual", _xlfn.XLOOKUP(B26, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B26" s="166"/>
@@ -18928,7 +18938,7 @@
     </row>
     <row r="27" spans="1:10" ht="15">
       <c r="A27" s="108" t="str">
-        <f>IF(B27="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B27,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B27="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B27) = 0, "acfr:LiabilitiesCustomModifiedAccrual", _xlfn.XLOOKUP(B27, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B27" s="166"/>
@@ -18946,7 +18956,7 @@
     </row>
     <row r="28" spans="1:10" ht="15">
       <c r="A28" s="108" t="str">
-        <f>IF(B28="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B28,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B28="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B28) = 0, "acfr:LiabilitiesCustomModifiedAccrual", _xlfn.XLOOKUP(B28, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B28" s="166"/>
@@ -18964,7 +18974,7 @@
     </row>
     <row r="29" spans="1:10" ht="15">
       <c r="A29" s="108" t="str">
-        <f>IF(B29="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B29,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B29="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B29) = 0, "acfr:LiabilitiesCustomModifiedAccrual", _xlfn.XLOOKUP(B29, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B29" s="166"/>
@@ -18982,7 +18992,7 @@
     </row>
     <row r="30" spans="1:10" ht="15">
       <c r="A30" s="108" t="str">
-        <f>IF(B30="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B30,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B30="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B30) = 0, "acfr:LiabilitiesCustomModifiedAccrual", _xlfn.XLOOKUP(B30, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B30" s="166"/>
@@ -19000,7 +19010,7 @@
     </row>
     <row r="31" spans="1:10" ht="15">
       <c r="A31" s="108" t="str">
-        <f>IF(B31="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B31,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B31="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B31) = 0, "acfr:LiabilitiesCustomModifiedAccrual", _xlfn.XLOOKUP(B31, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B31" s="166"/>
@@ -19083,7 +19093,7 @@
     </row>
     <row r="35" spans="1:10" ht="15">
       <c r="A35" s="108" t="str">
-        <f>IF(B35="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B35,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B35="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B35) = 0, "acfr:DeferredInflowsOfResourcesCustomModifiedAccrual", _xlfn.XLOOKUP(B35, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B35" s="166"/>
@@ -19101,7 +19111,7 @@
     </row>
     <row r="36" spans="1:10" ht="15">
       <c r="A36" s="108" t="str">
-        <f>IF(B36="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B36,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B36="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B36) = 0, "acfr:DeferredInflowsOfResourcesCustomModifiedAccrual", _xlfn.XLOOKUP(B36, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B36" s="166"/>
@@ -19119,7 +19129,7 @@
     </row>
     <row r="37" spans="1:10" ht="15">
       <c r="A37" s="108" t="str">
-        <f>IF(B37="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B37,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B37="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B37) = 0, "acfr:DeferredInflowsOfResourcesCustomModifiedAccrual", _xlfn.XLOOKUP(B37, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B37" s="166"/>
@@ -19137,7 +19147,7 @@
     </row>
     <row r="38" spans="1:10" ht="15">
       <c r="A38" s="108" t="str">
-        <f>IF(B38="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B38,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B38="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B38) = 0, "acfr:DeferredInflowsOfResourcesCustomModifiedAccrual", _xlfn.XLOOKUP(B38, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B38" s="166"/>
@@ -19155,7 +19165,7 @@
     </row>
     <row r="39" spans="1:10" ht="15">
       <c r="A39" s="108" t="str">
-        <f>IF(B39="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B39,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B39="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B39) = 0, "acfr:DeferredInflowsOfResourcesCustomModifiedAccrual", _xlfn.XLOOKUP(B39, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B39" s="166"/>
@@ -19173,7 +19183,7 @@
     </row>
     <row r="40" spans="1:10" ht="15">
       <c r="A40" s="108" t="str">
-        <f>IF(B40="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B40,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B40="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B40) = 0, "acfr:DeferredInflowsOfResourcesCustomModifiedAccrual", _xlfn.XLOOKUP(B40, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B40" s="166"/>
@@ -19191,7 +19201,7 @@
     </row>
     <row r="41" spans="1:10" ht="15">
       <c r="A41" s="108" t="str">
-        <f>IF(B41="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B41,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B41="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B41) = 0, "acfr:DeferredInflowsOfResourcesCustomModifiedAccrual", _xlfn.XLOOKUP(B41, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B41" s="166"/>
@@ -19209,7 +19219,7 @@
     </row>
     <row r="42" spans="1:10" ht="15">
       <c r="A42" s="108" t="str">
-        <f>IF(B42="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B42,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B42="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B42) = 0, "acfr:DeferredInflowsOfResourcesCustomModifiedAccrual", _xlfn.XLOOKUP(B42, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B42" s="166"/>
@@ -19227,7 +19237,7 @@
     </row>
     <row r="43" spans="1:10" ht="15">
       <c r="A43" s="108" t="str">
-        <f>IF(B43="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B43,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B43="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B43) = 0, "acfr:DeferredInflowsOfResourcesCustomModifiedAccrual", _xlfn.XLOOKUP(B43, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B43" s="166"/>
@@ -19245,7 +19255,7 @@
     </row>
     <row r="44" spans="1:10" ht="15">
       <c r="A44" s="108" t="str">
-        <f>IF(B44="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B44,'Lookup Net Position'!$B$2:$B$500,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B44="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Balance'!$B$2:$B$276, B44) = 0, "acfr:DeferredInflowsOfResourcesCustomModifiedAccrual", _xlfn.XLOOKUP(B44, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B44" s="166"/>
@@ -19328,7 +19338,7 @@
     </row>
     <row r="48" spans="1:10" ht="15">
       <c r="A48" s="108" t="str">
-        <f>IF(B48="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B48,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B48="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B48, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B48" s="166"/>
@@ -19346,7 +19356,7 @@
     </row>
     <row r="49" spans="1:10" ht="15">
       <c r="A49" s="108" t="str">
-        <f>IF(B49="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B49,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B49="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B49, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B49" s="166"/>
@@ -19364,7 +19374,7 @@
     </row>
     <row r="50" spans="1:10" ht="15">
       <c r="A50" s="108" t="str">
-        <f>IF(B50="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B50,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B50="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B50, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B50" s="166"/>
@@ -19382,7 +19392,7 @@
     </row>
     <row r="51" spans="1:10" ht="15">
       <c r="A51" s="108" t="str">
-        <f>IF(B51="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B51,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B51="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B51, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B51" s="166"/>
@@ -19400,7 +19410,7 @@
     </row>
     <row r="52" spans="1:10" ht="15">
       <c r="A52" s="108" t="str">
-        <f>IF(B52="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B52,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B52="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B52, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B52" s="166"/>
@@ -19418,7 +19428,7 @@
     </row>
     <row r="53" spans="1:10" ht="15">
       <c r="A53" s="108" t="str">
-        <f>IF(B53="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B53,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B53="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B53, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B53" s="166"/>
@@ -19436,7 +19446,7 @@
     </row>
     <row r="54" spans="1:10" ht="15">
       <c r="A54" s="108" t="str">
-        <f>IF(B54="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B54,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B54="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B54, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B54" s="166"/>
@@ -19454,7 +19464,7 @@
     </row>
     <row r="55" spans="1:10" ht="15">
       <c r="A55" s="108" t="str">
-        <f>IF(B55="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B55,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B55="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B55, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B55" s="166"/>
@@ -19472,7 +19482,7 @@
     </row>
     <row r="56" spans="1:10" ht="15">
       <c r="A56" s="108" t="str">
-        <f>IF(B56="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B56,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B56="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B56, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B56" s="166"/>
@@ -19490,7 +19500,7 @@
     </row>
     <row r="57" spans="1:10" ht="15">
       <c r="A57" s="108" t="str">
-        <f>IF(B57="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B57,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B57="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B57, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B57" s="166"/>
@@ -19508,7 +19518,7 @@
     </row>
     <row r="58" spans="1:10" ht="15">
       <c r="A58" s="108" t="str">
-        <f>IF(B58="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B58,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!#REF!))</f>
+        <f>IF(B58="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B58, 'Lookup GovFund Balance'!$B$2:$B$276, 'Lookup GovFund Balance'!$C$2:$C$276))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B58" s="166"/>
@@ -19524,85 +19534,127 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="16">
+    <row r="59" spans="1:10" ht="15">
       <c r="A59" s="108" t="s">
+        <v>3615</v>
+      </c>
+      <c r="B59" s="166"/>
+      <c r="C59" s="208"/>
+      <c r="D59" s="209"/>
+      <c r="E59" s="209"/>
+      <c r="F59" s="209"/>
+      <c r="G59" s="209"/>
+      <c r="H59" s="210"/>
+      <c r="I59" s="210"/>
+      <c r="J59" s="249"/>
+    </row>
+    <row r="60" spans="1:10" ht="15">
+      <c r="A60" s="108" t="s">
+        <v>3616</v>
+      </c>
+      <c r="B60" s="166"/>
+      <c r="C60" s="208"/>
+      <c r="D60" s="209"/>
+      <c r="E60" s="209"/>
+      <c r="F60" s="209"/>
+      <c r="G60" s="209"/>
+      <c r="H60" s="210"/>
+      <c r="I60" s="210"/>
+      <c r="J60" s="249"/>
+    </row>
+    <row r="61" spans="1:10" ht="16">
+      <c r="A61" s="131" t="s">
+        <v>3617</v>
+      </c>
+      <c r="B61" s="166"/>
+      <c r="C61" s="208"/>
+      <c r="D61" s="209"/>
+      <c r="E61" s="209"/>
+      <c r="F61" s="209"/>
+      <c r="G61" s="209"/>
+      <c r="H61" s="210"/>
+      <c r="I61" s="210"/>
+      <c r="J61" s="249"/>
+    </row>
+    <row r="62" spans="1:10" ht="16">
+      <c r="A62" s="108" t="s">
         <v>1084</v>
       </c>
-      <c r="B59" s="169" t="s">
+      <c r="B62" s="169" t="s">
         <v>2475</v>
       </c>
-      <c r="C59" s="217">
-        <f t="shared" ref="C59:H59" si="7">SUM(C48:C58)</f>
+      <c r="C62" s="217">
+        <f>SUM(C48:C58)</f>
         <v>0</v>
       </c>
-      <c r="D59" s="217">
-        <f t="shared" si="7"/>
+      <c r="D62" s="217">
+        <f>SUM(D48:D58)</f>
         <v>0</v>
       </c>
-      <c r="E59" s="217">
-        <f t="shared" si="7"/>
+      <c r="E62" s="217">
+        <f>SUM(E48:E58)</f>
         <v>0</v>
       </c>
-      <c r="F59" s="217">
-        <f t="shared" si="7"/>
+      <c r="F62" s="217">
+        <f>SUM(F48:F58)</f>
         <v>0</v>
       </c>
-      <c r="G59" s="217">
-        <f t="shared" si="7"/>
+      <c r="G62" s="217">
+        <f>SUM(G48:G58)</f>
         <v>0</v>
       </c>
-      <c r="H59" s="218">
-        <f t="shared" si="7"/>
+      <c r="H62" s="218">
+        <f>SUM(H48:H58)</f>
         <v>0</v>
       </c>
-      <c r="I59" s="218">
-        <f t="shared" ref="I59" si="8">SUM(I48:I58)</f>
+      <c r="I62" s="218">
+        <f>SUM(I48:I58)</f>
         <v>0</v>
       </c>
-      <c r="J59" s="218">
-        <f>SUM(C59:I59)</f>
+      <c r="J62" s="218">
+        <f>SUM(C62:I62)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="32">
-      <c r="A60" s="114" t="s">
+    <row r="63" spans="1:10" ht="32">
+      <c r="A63" s="114" t="s">
         <v>2476</v>
       </c>
-      <c r="B60" s="170" t="s">
+      <c r="B63" s="170" t="s">
         <v>2477</v>
       </c>
-      <c r="C60" s="219">
-        <f>SUM(C59, C45, C32)</f>
+      <c r="C63" s="219">
+        <f>SUM(C62, C45, C32)</f>
         <v>0</v>
       </c>
-      <c r="D60" s="219">
-        <f t="shared" ref="D60:J60" si="9">SUM(D59, D45, D32)</f>
+      <c r="D63" s="219">
+        <f>SUM(D62, D45, D32)</f>
         <v>0</v>
       </c>
-      <c r="E60" s="219">
-        <f t="shared" si="9"/>
+      <c r="E63" s="219">
+        <f>SUM(E62, E45, E32)</f>
         <v>0</v>
       </c>
-      <c r="F60" s="219"/>
-      <c r="G60" s="219">
-        <f t="shared" si="9"/>
+      <c r="F63" s="219"/>
+      <c r="G63" s="219">
+        <f>SUM(G62, G45, G32)</f>
         <v>0</v>
       </c>
-      <c r="H60" s="219">
-        <f t="shared" si="9"/>
+      <c r="H63" s="219">
+        <f>SUM(H62, H45, H32)</f>
         <v>0</v>
       </c>
-      <c r="I60" s="219">
-        <f t="shared" si="9"/>
+      <c r="I63" s="219">
+        <f>SUM(I62, I45, I32)</f>
         <v>0</v>
       </c>
-      <c r="J60" s="219">
-        <f t="shared" si="9"/>
+      <c r="J63" s="219">
+        <f>SUM(J62, J45, J32)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D8:G18 D21:G31 C32:I33 D35:G44 C45:I46 D48:G58 C59:G59">
+  <conditionalFormatting sqref="D8:G18 D21:G31 C32:I33 D35:G44 C45:I46 D48:G61 C62:G62">
     <cfRule type="expression" dxfId="34" priority="2" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
@@ -19624,25 +19676,35 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:J6" xr:uid="{0D7B8D02-DC8C-0B46-ABA0-A3421D2F5523}">
       <formula1>"Select fund type or delete column, General Fund, Special Revenue Fund, Capital Project, Debt Service, Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48:B58" xr:uid="{51E25186-1EB2-CD4B-B4A7-8C43F9322904}">
-      <formula1>fund_balance</formula1>
-    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="B59:B61" xr:uid="{0725135B-1ABA-044F-ABE3-FFE608A89DA3}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{24181F37-3456-9247-9E1E-6FECB2D9D2BE}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{51E25186-1EB2-CD4B-B4A7-8C43F9322904}">
+          <x14:formula1>
+            <xm:f>'Lookup GovFund Balance'!$B$176:$B$189</xm:f>
+          </x14:formula1>
+          <xm:sqref>B48:B58</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{24181F37-3456-9247-9E1E-6FECB2D9D2BE}">
           <x14:formula1>
             <xm:f>'Lookup GovFund Balance'!$B$190:$B$276</xm:f>
           </x14:formula1>
           <xm:sqref>B22:B31</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B2665086-3AD7-4E48-B875-3BE4D2879C8C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{B2665086-3AD7-4E48-B875-3BE4D2879C8C}">
           <x14:formula1>
-            <xm:f>'Lookup GovFund Balance'!$B$2:$B$163</xm:f>
+            <xm:f>'Lookup GovFund Balance'!$B$2:$B$164</xm:f>
           </x14:formula1>
           <xm:sqref>B9:B18</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{F4479D55-EB5C-EE45-B5CD-6F72ECE895E0}">
+          <x14:formula1>
+            <xm:f>'Lookup GovFund Balance'!$B$165:$B$173</xm:f>
+          </x14:formula1>
+          <xm:sqref>B35:B44</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -19837,13 +19899,13 @@
   </sheetPr>
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="81" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="81" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="33" customWidth="1"/>
+    <col min="1" max="1" width="28" style="33" customWidth="1"/>
     <col min="2" max="2" width="41.5" style="33" customWidth="1"/>
     <col min="3" max="3" width="15" style="33" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" style="33" customWidth="1"/>
@@ -19998,7 +20060,7 @@
     </row>
     <row r="9" spans="1:10" ht="15">
       <c r="A9" s="6" t="str">
-        <f>IF(B9="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B9,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B9="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B9) = 0, "acfr:RevenuesCustomModifiedAccrual", _xlfn.XLOOKUP(B9, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B9" s="15"/>
@@ -20016,7 +20078,7 @@
     </row>
     <row r="10" spans="1:10" ht="15">
       <c r="A10" s="6" t="str">
-        <f>IF(B10="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B10,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B10="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B10) = 0, "acfr:RevenuesCustomModifiedAccrual", _xlfn.XLOOKUP(B10, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B10" s="15"/>
@@ -20034,7 +20096,7 @@
     </row>
     <row r="11" spans="1:10" ht="15">
       <c r="A11" s="6" t="str">
-        <f>IF(B11="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B11,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B11="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B11) = 0, "acfr:RevenuesCustomModifiedAccrual", _xlfn.XLOOKUP(B11, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B11" s="15"/>
@@ -20052,7 +20114,7 @@
     </row>
     <row r="12" spans="1:10" ht="15">
       <c r="A12" s="6" t="str">
-        <f>IF(B12="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B12,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B12="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B12) = 0, "acfr:RevenuesCustomModifiedAccrual", _xlfn.XLOOKUP(B12, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B12" s="15"/>
@@ -20070,7 +20132,7 @@
     </row>
     <row r="13" spans="1:10" ht="15">
       <c r="A13" s="6" t="str">
-        <f>IF(B13="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B13,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B13="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B13) = 0, "acfr:RevenuesCustomModifiedAccrual", _xlfn.XLOOKUP(B13, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B13" s="15"/>
@@ -20088,7 +20150,7 @@
     </row>
     <row r="14" spans="1:10" ht="15">
       <c r="A14" s="6" t="str">
-        <f>IF(B14="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B14,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B14="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B14) = 0, "acfr:RevenuesCustomModifiedAccrual", _xlfn.XLOOKUP(B14, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B14" s="15"/>
@@ -20106,7 +20168,7 @@
     </row>
     <row r="15" spans="1:10" ht="15">
       <c r="A15" s="6" t="str">
-        <f>IF(B15="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B15,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B15="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B15) = 0, "acfr:RevenuesCustomModifiedAccrual", _xlfn.XLOOKUP(B15, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B15" s="15"/>
@@ -20124,7 +20186,7 @@
     </row>
     <row r="16" spans="1:10" ht="15">
       <c r="A16" s="6" t="str">
-        <f>IF(B16="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B16,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B16="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B16) = 0, "acfr:RevenuesCustomModifiedAccrual", _xlfn.XLOOKUP(B16, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B16" s="15"/>
@@ -20142,7 +20204,7 @@
     </row>
     <row r="17" spans="1:10" ht="15">
       <c r="A17" s="6" t="str">
-        <f>IF(B17="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B17,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B17="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B17) = 0, "acfr:RevenuesCustomModifiedAccrual", _xlfn.XLOOKUP(B17, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B17" s="15"/>
@@ -20160,7 +20222,7 @@
     </row>
     <row r="18" spans="1:10" ht="15" hidden="1">
       <c r="A18" s="6" t="str">
-        <f>IF(B18="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B18,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B18="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B18) = 0, "acfr:RevenuesCustomModifiedAccrual", _xlfn.XLOOKUP(B18, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B18" s="15"/>
@@ -20178,7 +20240,7 @@
     </row>
     <row r="19" spans="1:10" ht="15" hidden="1">
       <c r="A19" s="6" t="str">
-        <f>IF(B19="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B19,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B19="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B19) = 0, "acfr:RevenuesCustomModifiedAccrual", _xlfn.XLOOKUP(B19, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B19" s="15"/>
@@ -20196,7 +20258,7 @@
     </row>
     <row r="20" spans="1:10" ht="15" hidden="1">
       <c r="A20" s="6" t="str">
-        <f>IF(B20="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B20,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B20="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B20) = 0, "acfr:RevenuesCustomModifiedAccrual", _xlfn.XLOOKUP(B20, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B20" s="15"/>
@@ -20214,7 +20276,7 @@
     </row>
     <row r="21" spans="1:10" ht="15" hidden="1">
       <c r="A21" s="6" t="str">
-        <f>IF(B21="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B21,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B21="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B21) = 0, "acfr:RevenuesCustomModifiedAccrual", _xlfn.XLOOKUP(B21, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B21" s="15"/>
@@ -20232,7 +20294,7 @@
     </row>
     <row r="22" spans="1:10" ht="15">
       <c r="A22" s="6" t="str">
-        <f>IF(B22="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B22,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B22="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B22) = 0, "acfr:RevenuesCustomModifiedAccrual", _xlfn.XLOOKUP(B22, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B22" s="15"/>
@@ -20304,7 +20366,7 @@
     </row>
     <row r="26" spans="1:10" ht="15">
       <c r="A26" s="6" t="str">
-        <f>IF(B26="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B26,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B26="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B26) = 0, "acfr:ExpendituresCustomModifiedAccrual", _xlfn.XLOOKUP(B26, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B26" s="15"/>
@@ -20322,7 +20384,7 @@
     </row>
     <row r="27" spans="1:10" ht="15">
       <c r="A27" s="6" t="str">
-        <f>IF(B27="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B27,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B27="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B27) = 0, "acfr:ExpendituresCustomModifiedAccrual", _xlfn.XLOOKUP(B27, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B27" s="15"/>
@@ -20340,7 +20402,7 @@
     </row>
     <row r="28" spans="1:10" ht="15">
       <c r="A28" s="6" t="str">
-        <f>IF(B28="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B28,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B28="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B28) = 0, "acfr:ExpendituresCustomModifiedAccrual", _xlfn.XLOOKUP(B28, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B28" s="15"/>
@@ -20358,7 +20420,7 @@
     </row>
     <row r="29" spans="1:10" ht="15">
       <c r="A29" s="6" t="str">
-        <f>IF(B29="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B29,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B29="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B29) = 0, "acfr:ExpendituresCustomModifiedAccrual", _xlfn.XLOOKUP(B29, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B29" s="15"/>
@@ -20376,7 +20438,7 @@
     </row>
     <row r="30" spans="1:10" ht="15">
       <c r="A30" s="6" t="str">
-        <f>IF(B30="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B30,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B30="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B30) = 0, "acfr:ExpendituresCustomModifiedAccrual", _xlfn.XLOOKUP(B30, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B30" s="15"/>
@@ -20394,7 +20456,7 @@
     </row>
     <row r="31" spans="1:10" ht="15">
       <c r="A31" s="6" t="str">
-        <f>IF(B31="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B31,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B31="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B31) = 0, "acfr:ExpendituresCustomModifiedAccrual", _xlfn.XLOOKUP(B31, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B31" s="15"/>
@@ -20412,7 +20474,7 @@
     </row>
     <row r="32" spans="1:10" ht="15">
       <c r="A32" s="6" t="str">
-        <f>IF(B32="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B32,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B32="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B32) = 0, "acfr:ExpendituresCustomModifiedAccrual", _xlfn.XLOOKUP(B32, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B32" s="15"/>
@@ -20430,7 +20492,7 @@
     </row>
     <row r="33" spans="1:10" ht="15">
       <c r="A33" s="6" t="str">
-        <f>IF(B33="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B33,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B33="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B33) = 0, "acfr:ExpendituresCustomModifiedAccrual", _xlfn.XLOOKUP(B33, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B33" s="15"/>
@@ -20448,7 +20510,7 @@
     </row>
     <row r="34" spans="1:10" ht="15">
       <c r="A34" s="6" t="str">
-        <f>IF(B34="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B34,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B34="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B34) = 0, "acfr:ExpendituresCustomModifiedAccrual", _xlfn.XLOOKUP(B34, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B34" s="15"/>
@@ -20572,7 +20634,7 @@
     </row>
     <row r="39" spans="1:10" ht="15">
       <c r="A39" s="6" t="str">
-        <f>IF(B39="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B39,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B39="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B39) = 0, "acfr:OtherFinancingSourcesUsesCustom", _xlfn.XLOOKUP(B39, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B39" s="15"/>
@@ -20590,7 +20652,7 @@
     </row>
     <row r="40" spans="1:10" ht="15">
       <c r="A40" s="6" t="str">
-        <f>IF(B40="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B40,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B40="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B40) = 0, "acfr:OtherFinancingSourcesUsesCustom", _xlfn.XLOOKUP(B40, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B40" s="15"/>
@@ -20608,7 +20670,7 @@
     </row>
     <row r="41" spans="1:10" ht="15">
       <c r="A41" s="6" t="str">
-        <f>IF(B41="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B41,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B41="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B41) = 0, "acfr:OtherFinancingSourcesUsesCustom", _xlfn.XLOOKUP(B41, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B41" s="15"/>
@@ -20626,7 +20688,7 @@
     </row>
     <row r="42" spans="1:10" ht="16" customHeight="1">
       <c r="A42" s="6" t="str">
-        <f>IF(B42="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B42,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B42="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B42) = 0, "acfr:OtherFinancingSourcesUsesCustom", _xlfn.XLOOKUP(B42, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B42" s="15"/>
@@ -20644,7 +20706,7 @@
     </row>
     <row r="43" spans="1:10" ht="16" customHeight="1">
       <c r="A43" s="6" t="str">
-        <f>IF(B43="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B43,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B43="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B43) = 0, "acfr:OtherFinancingSourcesUsesCustom", _xlfn.XLOOKUP(B43, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B43" s="15"/>
@@ -20662,7 +20724,7 @@
     </row>
     <row r="44" spans="1:10" ht="16" customHeight="1">
       <c r="A44" s="6" t="str">
-        <f>IF(B44="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B44,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B44="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B44) = 0, "acfr:OtherFinancingSourcesUsesCustom", _xlfn.XLOOKUP(B44, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B44" s="15"/>
@@ -20680,7 +20742,7 @@
     </row>
     <row r="45" spans="1:10" ht="16" hidden="1" customHeight="1">
       <c r="A45" s="6" t="str">
-        <f>IF(B45="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B45,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B45="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B45) = 0, "acfr:OtherFinancingSourcesUsesCustom", _xlfn.XLOOKUP(B45, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B45" s="15"/>
@@ -20698,7 +20760,7 @@
     </row>
     <row r="46" spans="1:10" ht="16" hidden="1" customHeight="1">
       <c r="A46" s="6" t="str">
-        <f>IF(B46="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B46,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B46="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B46) = 0, "acfr:OtherFinancingSourcesUsesCustom", _xlfn.XLOOKUP(B46, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B46" s="15"/>
@@ -20716,7 +20778,7 @@
     </row>
     <row r="47" spans="1:10" ht="15" hidden="1">
       <c r="A47" s="6" t="str">
-        <f>IF(B47="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B47,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B47="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B47) = 0, "acfr:OtherFinancingSourcesUsesCustom", _xlfn.XLOOKUP(B47, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B47" s="15"/>
@@ -20734,7 +20796,7 @@
     </row>
     <row r="48" spans="1:10" ht="15" hidden="1">
       <c r="A48" s="6" t="str">
-        <f>IF(B48="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B48,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B48="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B48) = 0, "acfr:OtherFinancingSourcesUsesCustom", _xlfn.XLOOKUP(B48, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B48" s="15"/>
@@ -20752,7 +20814,7 @@
     </row>
     <row r="49" spans="1:10" ht="15" hidden="1">
       <c r="A49" s="6" t="str">
-        <f>IF(B49="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B49,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B49="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B49) = 0, "acfr:OtherFinancingSourcesUsesCustom", _xlfn.XLOOKUP(B49, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B49" s="15"/>
@@ -20770,7 +20832,7 @@
     </row>
     <row r="50" spans="1:10" ht="15">
       <c r="A50" s="6" t="str">
-        <f>IF(B50="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B50,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B50="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B50) = 0, "acfr:OtherFinancingSourcesUsesCustom", _xlfn.XLOOKUP(B50, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B50" s="15"/>
@@ -20788,7 +20850,7 @@
     </row>
     <row r="51" spans="1:10" ht="15">
       <c r="A51" s="6" t="str">
-        <f>IF(B51="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B51,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B51="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B51) = 0, "acfr:OtherFinancingSourcesUsesCustom", _xlfn.XLOOKUP(B51, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B51" s="15"/>
@@ -20806,7 +20868,7 @@
     </row>
     <row r="52" spans="1:10" ht="15">
       <c r="A52" s="6" t="str">
-        <f>IF(B52="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B52,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B52="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B52) = 0, "acfr:OtherFinancingSourcesUsesCustom", _xlfn.XLOOKUP(B52, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B52" s="15"/>
@@ -20824,7 +20886,7 @@
     </row>
     <row r="53" spans="1:10" ht="15">
       <c r="A53" s="6" t="str">
-        <f>IF(B53="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B53,'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392,'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392))</f>
+        <f>IF(B53="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, B53) = 0, "acfr:OtherFinancingSourcesUsesCustom", _xlfn.XLOOKUP(B53, 'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$392, 'Lookup GovFund Stmt Rev Exp Ch'!$C$2:$C$392)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B53" s="15"/>
@@ -21224,19 +21286,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C93DFAB6-EE30-6F40-B82C-3A9FB7CAB85D}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{C93DFAB6-EE30-6F40-B82C-3A9FB7CAB85D}">
           <x14:formula1>
             <xm:f>'Lookup GovFund Stmt Rev Exp Ch'!$B$160:$B$170</xm:f>
           </x14:formula1>
           <xm:sqref>B39:B53</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D4D1AB10-08C4-B544-9EDE-7CF75EB31E07}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{D4D1AB10-08C4-B544-9EDE-7CF75EB31E07}">
           <x14:formula1>
             <xm:f>'Lookup GovFund Stmt Rev Exp Ch'!$B$171:$B$352</xm:f>
           </x14:formula1>
           <xm:sqref>B26:B34</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{01544FF9-537B-8F47-BAD2-6BA555B7160B}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{01544FF9-537B-8F47-BAD2-6BA555B7160B}">
           <x14:formula1>
             <xm:f>'Lookup GovFund Stmt Rev Exp Ch'!$B$2:$B$159</xm:f>
           </x14:formula1>
@@ -21305,7 +21367,7 @@
         <v>2852</v>
       </c>
       <c r="B6" s="174">
-        <f>'GovFund Balance Sheet'!J59</f>
+        <f>'GovFund Balance Sheet'!J62</f>
         <v>0</v>
       </c>
     </row>
@@ -21407,10 +21469,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:K106"/>
+  <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A15" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -21577,7 +21639,7 @@
     </row>
     <row r="10" spans="1:11" ht="15">
       <c r="A10" s="108" t="str">
-        <f>IF(B10="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B10,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B10="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B10)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B10,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B10" s="15"/>
@@ -21595,7 +21657,7 @@
     </row>
     <row r="11" spans="1:11" ht="15">
       <c r="A11" s="108" t="str">
-        <f>IF(B11="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B11,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B11="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B11)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B11,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B11" s="15"/>
@@ -21613,7 +21675,7 @@
     </row>
     <row r="12" spans="1:11" ht="15">
       <c r="A12" s="108" t="str">
-        <f>IF(B12="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B12,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B12="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B12)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B12,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B12" s="15"/>
@@ -21631,7 +21693,7 @@
     </row>
     <row r="13" spans="1:11" ht="15">
       <c r="A13" s="108" t="str">
-        <f>IF(B13="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B13,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B13="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B13)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B13,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B13" s="15"/>
@@ -21649,7 +21711,7 @@
     </row>
     <row r="14" spans="1:11" ht="15">
       <c r="A14" s="108" t="str">
-        <f>IF(B14="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B14,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B14="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B14)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B14,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B14" s="15"/>
@@ -21667,7 +21729,7 @@
     </row>
     <row r="15" spans="1:11" ht="15">
       <c r="A15" s="108" t="str">
-        <f>IF(B15="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B15,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B15="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B15)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B15,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B15" s="15"/>
@@ -21685,7 +21747,7 @@
     </row>
     <row r="16" spans="1:11" ht="15">
       <c r="A16" s="108" t="str">
-        <f>IF(B16="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B16,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B16="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B16)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B16,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B16" s="15"/>
@@ -21703,7 +21765,7 @@
     </row>
     <row r="17" spans="1:10" ht="15">
       <c r="A17" s="108" t="str">
-        <f>IF(B17="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B17,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B17="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B17)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B17,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B17" s="15"/>
@@ -21721,7 +21783,7 @@
     </row>
     <row r="18" spans="1:10" ht="15">
       <c r="A18" s="108" t="str">
-        <f>IF(B18="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B18,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B18="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B18)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B18,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B18" s="15"/>
@@ -21739,7 +21801,7 @@
     </row>
     <row r="19" spans="1:10" ht="15" hidden="1">
       <c r="A19" s="108" t="str">
-        <f>IF(B19="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B19,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B19="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B19)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B19,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B19" s="15"/>
@@ -21757,7 +21819,7 @@
     </row>
     <row r="20" spans="1:10" ht="15" hidden="1">
       <c r="A20" s="108" t="str">
-        <f>IF(B20="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B20,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B20="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B20)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B20,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B20" s="15"/>
@@ -21775,7 +21837,7 @@
     </row>
     <row r="21" spans="1:10" ht="15" hidden="1">
       <c r="A21" s="108" t="str">
-        <f>IF(B21="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B21,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B21="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B21)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B21,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B21" s="15"/>
@@ -21793,7 +21855,7 @@
     </row>
     <row r="22" spans="1:10" ht="15" hidden="1">
       <c r="A22" s="108" t="str">
-        <f>IF(B22="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B22,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B22="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B22)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B22,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B22" s="15"/>
@@ -21811,7 +21873,7 @@
     </row>
     <row r="23" spans="1:10" ht="15">
       <c r="A23" s="108" t="str">
-        <f>IF(B23="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B23,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B23="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B23)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B23,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B23" s="15"/>
@@ -21883,7 +21945,7 @@
     </row>
     <row r="26" spans="1:10" ht="15">
       <c r="A26" s="108" t="str">
-        <f>IF(B26="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B26,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B26="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B26)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B26,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B26" s="109"/>
@@ -21901,7 +21963,7 @@
     </row>
     <row r="27" spans="1:10" ht="15">
       <c r="A27" s="108" t="str">
-        <f>IF(B27="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B27,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B27="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B27)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B27,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B27" s="109"/>
@@ -21919,7 +21981,7 @@
     </row>
     <row r="28" spans="1:10" ht="15">
       <c r="A28" s="108" t="str">
-        <f>IF(B28="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B28,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B28="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B28)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B28,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B28" s="110"/>
@@ -21937,7 +21999,7 @@
     </row>
     <row r="29" spans="1:10" ht="15">
       <c r="A29" s="108" t="str">
-        <f>IF(B29="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B29,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B29="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B29)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B29,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B29" s="110"/>
@@ -21955,7 +22017,7 @@
     </row>
     <row r="30" spans="1:10" ht="15">
       <c r="A30" s="108" t="str">
-        <f>IF(B30="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B30,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B30="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B30)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B30,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B30" s="110"/>
@@ -21973,7 +22035,7 @@
     </row>
     <row r="31" spans="1:10" ht="15" hidden="1">
       <c r="A31" s="108" t="str">
-        <f>IF(B31="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B31,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B31="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B31)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B31,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B31" s="109"/>
@@ -21991,7 +22053,7 @@
     </row>
     <row r="32" spans="1:10" ht="15" hidden="1">
       <c r="A32" s="108" t="str">
-        <f>IF(B32="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B32,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B32="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B32)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B32,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B32" s="109"/>
@@ -22009,7 +22071,7 @@
     </row>
     <row r="33" spans="1:10" ht="15" hidden="1">
       <c r="A33" s="108" t="str">
-        <f>IF(B33="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B33,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B33="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B33)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B33,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B33" s="109"/>
@@ -22027,7 +22089,7 @@
     </row>
     <row r="34" spans="1:10" ht="15" hidden="1">
       <c r="A34" s="108" t="str">
-        <f>IF(B34="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B34,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B34="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B34)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B34,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B34" s="109"/>
@@ -22045,7 +22107,7 @@
     </row>
     <row r="35" spans="1:10" ht="15" hidden="1">
       <c r="A35" s="108" t="str">
-        <f>IF(B35="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B35,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B35="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B35)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B35,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B35" s="109"/>
@@ -22063,7 +22125,7 @@
     </row>
     <row r="36" spans="1:10" ht="15" hidden="1">
       <c r="A36" s="108" t="str">
-        <f>IF(B36="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B36,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B36="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B36)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B36,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B36" s="109"/>
@@ -22081,7 +22143,7 @@
     </row>
     <row r="37" spans="1:10" ht="15">
       <c r="A37" s="108" t="str">
-        <f>IF(B37="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B37,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B37="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B37)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B37,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B37" s="109"/>
@@ -22219,7 +22281,7 @@
     </row>
     <row r="43" spans="1:10" ht="15">
       <c r="A43" s="108" t="str">
-        <f>IF(B43="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B43,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B43="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B43)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B43,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B43" s="109"/>
@@ -22237,7 +22299,7 @@
     </row>
     <row r="44" spans="1:10" ht="15">
       <c r="A44" s="108" t="str">
-        <f>IF(B44="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B44,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B44="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B44)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B44,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B44" s="109"/>
@@ -22255,7 +22317,7 @@
     </row>
     <row r="45" spans="1:10" ht="15">
       <c r="A45" s="108" t="str">
-        <f>IF(B45="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B45,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B45="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B45)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B45,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B45" s="109"/>
@@ -22273,7 +22335,7 @@
     </row>
     <row r="46" spans="1:10" ht="16" customHeight="1">
       <c r="A46" s="108" t="str">
-        <f>IF(B46="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B46,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B46="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B46)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B46,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B46" s="109"/>
@@ -22291,7 +22353,7 @@
     </row>
     <row r="47" spans="1:10" ht="16" customHeight="1">
       <c r="A47" s="108" t="str">
-        <f>IF(B47="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B47,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B47="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B47)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B47,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B47" s="109"/>
@@ -22309,7 +22371,7 @@
     </row>
     <row r="48" spans="1:10" ht="16" hidden="1" customHeight="1">
       <c r="A48" s="108" t="str">
-        <f>IF(B48="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B48,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B48="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B48)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B48,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B48" s="109"/>
@@ -22327,7 +22389,7 @@
     </row>
     <row r="49" spans="1:10" ht="16" hidden="1" customHeight="1">
       <c r="A49" s="108" t="str">
-        <f>IF(B49="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B49,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B49="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B49)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B49,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B49" s="109"/>
@@ -22345,7 +22407,7 @@
     </row>
     <row r="50" spans="1:10" ht="16" hidden="1" customHeight="1">
       <c r="A50" s="108" t="str">
-        <f>IF(B50="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B50,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B50="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B50)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B50,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B50" s="109"/>
@@ -22363,7 +22425,7 @@
     </row>
     <row r="51" spans="1:10" ht="15" hidden="1">
       <c r="A51" s="108" t="str">
-        <f>IF(B51="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B51,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B51="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B51)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B51,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B51" s="109"/>
@@ -22381,7 +22443,7 @@
     </row>
     <row r="52" spans="1:10" ht="15" hidden="1">
       <c r="A52" s="108" t="str">
-        <f>IF(B52="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B52,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B52="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B52)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B52,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B52" s="109"/>
@@ -22399,7 +22461,7 @@
     </row>
     <row r="53" spans="1:10" ht="15">
       <c r="A53" s="108" t="str">
-        <f>IF(B53="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B53,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B53="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B53)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B53,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B53" s="109"/>
@@ -22471,7 +22533,7 @@
     </row>
     <row r="56" spans="1:10" ht="15">
       <c r="A56" s="108" t="str">
-        <f>IF(B56="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B56,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B56="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B56)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B56,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B56" s="109"/>
@@ -22483,13 +22545,13 @@
       <c r="H56" s="208"/>
       <c r="I56" s="208"/>
       <c r="J56" s="231">
-        <f t="shared" ref="J56:J66" si="9">IF(J$7="","",SUM(D56:I56))</f>
+        <f t="shared" ref="J56:J69" si="9">IF(J$7="","",SUM(D56:I56))</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15">
       <c r="A57" s="108" t="str">
-        <f>IF(B57="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B57,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B57="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B57)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B57,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B57" s="109"/>
@@ -22507,7 +22569,7 @@
     </row>
     <row r="58" spans="1:10" ht="15">
       <c r="A58" s="108" t="str">
-        <f>IF(B58="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B58,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B58="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B58)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B58,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B58" s="109"/>
@@ -22525,7 +22587,7 @@
     </row>
     <row r="59" spans="1:10" ht="15" hidden="1">
       <c r="A59" s="108" t="str">
-        <f>IF(B59="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B59,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B59="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B59)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B59,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B59" s="109"/>
@@ -22543,7 +22605,7 @@
     </row>
     <row r="60" spans="1:10" ht="15" hidden="1">
       <c r="A60" s="108" t="str">
-        <f>IF(B60="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B60,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B60="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B60)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B60,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B60" s="109"/>
@@ -22561,7 +22623,7 @@
     </row>
     <row r="61" spans="1:10" ht="15" hidden="1">
       <c r="A61" s="108" t="str">
-        <f>IF(B61="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B61,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B61="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B61)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B61,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B61" s="109"/>
@@ -22579,7 +22641,7 @@
     </row>
     <row r="62" spans="1:10" ht="15" hidden="1">
       <c r="A62" s="108" t="str">
-        <f>IF(B62="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B62,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B62="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B62)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B62,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B62" s="109"/>
@@ -22597,7 +22659,7 @@
     </row>
     <row r="63" spans="1:10" ht="15" hidden="1">
       <c r="A63" s="108" t="str">
-        <f>IF(B63="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B63,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B63="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B63)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B63,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B63" s="109"/>
@@ -22615,7 +22677,7 @@
     </row>
     <row r="64" spans="1:10" ht="15">
       <c r="A64" s="108" t="str">
-        <f>IF(B64="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B64,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B64="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B64)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B64,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B64" s="109"/>
@@ -22632,168 +22694,159 @@
       </c>
     </row>
     <row r="65" spans="1:10" ht="15">
-      <c r="A65" s="108" t="s">
+      <c r="A65" s="108" t="str">
+        <f>IF(B65="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B65)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B65,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B65" s="109"/>
+      <c r="C65" s="208"/>
+      <c r="D65" s="208"/>
+      <c r="E65" s="208"/>
+      <c r="F65" s="208"/>
+      <c r="G65" s="208"/>
+      <c r="H65" s="208"/>
+      <c r="I65" s="208"/>
+      <c r="J65" s="231"/>
+    </row>
+    <row r="66" spans="1:10" ht="15">
+      <c r="A66" s="108" t="str">
+        <f>IF(B66="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B66)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B66,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B66" s="109"/>
+      <c r="C66" s="208"/>
+      <c r="D66" s="208"/>
+      <c r="E66" s="208"/>
+      <c r="F66" s="208"/>
+      <c r="G66" s="208"/>
+      <c r="H66" s="208"/>
+      <c r="I66" s="208"/>
+      <c r="J66" s="231"/>
+    </row>
+    <row r="67" spans="1:10" ht="15">
+      <c r="A67" s="108" t="str">
+        <f>IF(B67="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B67)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B67,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B67" s="109"/>
+      <c r="C67" s="208"/>
+      <c r="D67" s="208"/>
+      <c r="E67" s="208"/>
+      <c r="F67" s="208"/>
+      <c r="G67" s="208"/>
+      <c r="H67" s="208"/>
+      <c r="I67" s="208"/>
+      <c r="J67" s="231"/>
+    </row>
+    <row r="68" spans="1:10" ht="15">
+      <c r="A68" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="B65" s="108" t="s">
+      <c r="B68" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="C65" s="231">
+      <c r="C68" s="231">
         <f>SUM(C56:C64)</f>
         <v>0</v>
       </c>
-      <c r="D65" s="231" t="str">
-        <f t="shared" ref="D65:I65" si="11">IF(D$7="Type fund name","",SUM(D56:D64))</f>
+      <c r="D68" s="231" t="str">
+        <f t="shared" ref="D68:I68" si="11">IF(D$7="Type fund name","",SUM(D56:D64))</f>
         <v/>
       </c>
-      <c r="E65" s="231" t="str">
+      <c r="E68" s="231" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="F65" s="231" t="str">
+      <c r="F68" s="231" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="G65" s="231" t="str">
+      <c r="G68" s="231" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="H65" s="231" t="str">
+      <c r="H68" s="231" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="I65" s="231" t="str">
+      <c r="I68" s="231" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="J65" s="231">
+      <c r="J68" s="231">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="15">
-      <c r="A66" s="114" t="s">
+    <row r="69" spans="1:10" ht="15">
+      <c r="A69" s="114" t="s">
         <v>39</v>
       </c>
-      <c r="B66" s="111" t="s">
+      <c r="B69" s="111" t="s">
         <v>40</v>
       </c>
-      <c r="C66" s="219">
-        <f>C54+C65</f>
+      <c r="C69" s="219">
+        <f>C54+C68</f>
         <v>0</v>
       </c>
-      <c r="D66" s="219" t="str">
-        <f t="shared" ref="D66:I66" si="12">IF(D$7 = "Type fund name", "", D54+D65)</f>
+      <c r="D69" s="219" t="str">
+        <f t="shared" ref="D69:I69" si="12">IF(D$7 = "Type fund name", "", D54+D68)</f>
         <v/>
       </c>
-      <c r="E66" s="219" t="str">
+      <c r="E69" s="219" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="F66" s="219" t="str">
+      <c r="F69" s="219" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="G66" s="219" t="str">
+      <c r="G69" s="219" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="H66" s="219" t="str">
+      <c r="H69" s="219" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="I66" s="219" t="str">
+      <c r="I69" s="219" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="J66" s="233">
+      <c r="J69" s="233">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15">
-      <c r="A67" s="104"/>
-      <c r="B67" s="104"/>
-      <c r="C67" s="112"/>
-      <c r="D67" s="112"/>
-      <c r="E67" s="112"/>
-      <c r="F67" s="112"/>
-      <c r="G67" s="112"/>
-      <c r="H67" s="112"/>
-      <c r="I67" s="112"/>
-      <c r="J67" s="107"/>
-    </row>
-    <row r="68" spans="1:10" ht="15">
-      <c r="A68" s="104"/>
-      <c r="B68" s="105" t="s">
+    <row r="70" spans="1:10" ht="15">
+      <c r="A70" s="104"/>
+      <c r="B70" s="104"/>
+      <c r="C70" s="112"/>
+      <c r="D70" s="112"/>
+      <c r="E70" s="112"/>
+      <c r="F70" s="112"/>
+      <c r="G70" s="112"/>
+      <c r="H70" s="112"/>
+      <c r="I70" s="112"/>
+      <c r="J70" s="107"/>
+    </row>
+    <row r="71" spans="1:10" ht="15">
+      <c r="A71" s="104"/>
+      <c r="B71" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="C68" s="105"/>
-      <c r="D68" s="105"/>
-      <c r="E68" s="105"/>
-      <c r="F68" s="105"/>
-      <c r="G68" s="105"/>
-      <c r="H68" s="105"/>
-      <c r="I68" s="105"/>
-      <c r="J68" s="115"/>
-    </row>
-    <row r="69" spans="1:10" ht="15">
-      <c r="A69" s="108" t="str">
-        <f>IF(B69="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B69,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B69" s="109"/>
-      <c r="C69" s="208"/>
-      <c r="D69" s="208"/>
-      <c r="E69" s="208"/>
-      <c r="F69" s="208"/>
-      <c r="G69" s="208"/>
-      <c r="H69" s="208"/>
-      <c r="I69" s="208"/>
-      <c r="J69" s="231">
-        <f t="shared" ref="J69:J78" si="13">IF(J$7="","",SUM(D69:I69))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="15">
-      <c r="A70" s="108" t="str">
-        <f>IF(B70="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B70,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B70" s="109"/>
-      <c r="C70" s="208"/>
-      <c r="D70" s="208"/>
-      <c r="E70" s="208"/>
-      <c r="F70" s="208"/>
-      <c r="G70" s="208"/>
-      <c r="H70" s="208"/>
-      <c r="I70" s="208"/>
-      <c r="J70" s="231">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="15">
-      <c r="A71" s="108" t="str">
-        <f>IF(B71="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B71,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B71" s="109"/>
-      <c r="C71" s="208"/>
-      <c r="D71" s="208"/>
-      <c r="E71" s="208"/>
-      <c r="F71" s="208"/>
-      <c r="G71" s="208"/>
-      <c r="H71" s="208"/>
-      <c r="I71" s="208"/>
-      <c r="J71" s="231">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="15" hidden="1">
+      <c r="C71" s="105"/>
+      <c r="D71" s="105"/>
+      <c r="E71" s="105"/>
+      <c r="F71" s="105"/>
+      <c r="G71" s="105"/>
+      <c r="H71" s="105"/>
+      <c r="I71" s="105"/>
+      <c r="J71" s="115"/>
+    </row>
+    <row r="72" spans="1:10" ht="15">
       <c r="A72" s="108" t="str">
-        <f>IF(B72="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B72,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B72="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B72)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B72,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B72" s="109"/>
@@ -22805,13 +22858,13 @@
       <c r="H72" s="208"/>
       <c r="I72" s="208"/>
       <c r="J72" s="231">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="J72:J81" si="13">IF(J$7="","",SUM(D72:I72))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15" hidden="1">
+    <row r="73" spans="1:10" ht="15">
       <c r="A73" s="108" t="str">
-        <f>IF(B73="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B73,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B73="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B73)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B73,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B73" s="109"/>
@@ -22827,9 +22880,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15" hidden="1">
+    <row r="74" spans="1:10" ht="15">
       <c r="A74" s="108" t="str">
-        <f>IF(B74="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B74,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B74="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B74)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B74,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B74" s="109"/>
@@ -22847,7 +22900,7 @@
     </row>
     <row r="75" spans="1:10" ht="15" hidden="1">
       <c r="A75" s="108" t="str">
-        <f>IF(B75="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B75,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B75="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B75)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B75,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B75" s="109"/>
@@ -22865,7 +22918,7 @@
     </row>
     <row r="76" spans="1:10" ht="15" hidden="1">
       <c r="A76" s="108" t="str">
-        <f>IF(B76="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B76,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B76="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B76)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B76,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B76" s="109"/>
@@ -22881,9 +22934,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="15">
+    <row r="77" spans="1:10" ht="15" hidden="1">
       <c r="A77" s="108" t="str">
-        <f>IF(B77="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B77,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420))</f>
+        <f>IF(B77="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B77)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B77,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B77" s="109"/>
@@ -22899,105 +22952,150 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15">
-      <c r="A78" s="111" t="s">
+    <row r="78" spans="1:10" ht="15" hidden="1">
+      <c r="A78" s="108" t="str">
+        <f>IF(B78="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B78)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B78,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B78" s="109"/>
+      <c r="C78" s="208"/>
+      <c r="D78" s="208"/>
+      <c r="E78" s="208"/>
+      <c r="F78" s="208"/>
+      <c r="G78" s="208"/>
+      <c r="H78" s="208"/>
+      <c r="I78" s="208"/>
+      <c r="J78" s="231">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="15" hidden="1">
+      <c r="A79" s="108" t="str">
+        <f>IF(B79="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B79)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B79,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B79" s="109"/>
+      <c r="C79" s="208"/>
+      <c r="D79" s="208"/>
+      <c r="E79" s="208"/>
+      <c r="F79" s="208"/>
+      <c r="G79" s="208"/>
+      <c r="H79" s="208"/>
+      <c r="I79" s="208"/>
+      <c r="J79" s="231">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="15">
+      <c r="A80" s="108" t="str">
+        <f>IF(B80="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B80)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B80,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B80" s="109"/>
+      <c r="C80" s="208"/>
+      <c r="D80" s="208"/>
+      <c r="E80" s="208"/>
+      <c r="F80" s="208"/>
+      <c r="G80" s="208"/>
+      <c r="H80" s="208"/>
+      <c r="I80" s="208"/>
+      <c r="J80" s="231">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="15">
+      <c r="A81" s="111" t="s">
         <v>50</v>
       </c>
-      <c r="B78" s="111" t="s">
+      <c r="B81" s="111" t="s">
         <v>51</v>
       </c>
-      <c r="C78" s="219">
-        <f>IF(C7="","",SUM(C69:C77))</f>
+      <c r="C81" s="219">
+        <f>IF(C7="","",SUM(C72:C80))</f>
         <v>0</v>
       </c>
-      <c r="D78" s="219" t="str">
-        <f t="shared" ref="D78:I78" si="14">IF(D7="Type fund name","",SUM(D69:D77))</f>
+      <c r="D81" s="219" t="str">
+        <f t="shared" ref="D81:I81" si="14">IF(D7="Type fund name","",SUM(D72:D80))</f>
         <v/>
       </c>
-      <c r="E78" s="219" t="str">
+      <c r="E81" s="219" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="F78" s="219" t="str">
+      <c r="F81" s="219" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="G78" s="219" t="str">
+      <c r="G81" s="219" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="H78" s="219" t="str">
+      <c r="H81" s="219" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="I78" s="219" t="str">
+      <c r="I81" s="219" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="J78" s="232">
+      <c r="J81" s="232">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="16">
-      <c r="C79" s="116"/>
-      <c r="D79" s="116"/>
-      <c r="E79" s="116"/>
-      <c r="F79" s="116"/>
-      <c r="G79" s="116"/>
-      <c r="H79" s="116"/>
-      <c r="I79" s="116"/>
-      <c r="J79" s="112"/>
-    </row>
-    <row r="80" spans="1:10" ht="15">
-      <c r="J80" s="112"/>
-    </row>
-    <row r="81" spans="10:10" ht="15">
-      <c r="J81" s="112"/>
-    </row>
-    <row r="82" spans="10:10" ht="15">
+    <row r="82" spans="1:10" ht="16">
+      <c r="C82" s="116"/>
+      <c r="D82" s="116"/>
+      <c r="E82" s="116"/>
+      <c r="F82" s="116"/>
+      <c r="G82" s="116"/>
+      <c r="H82" s="116"/>
+      <c r="I82" s="116"/>
       <c r="J82" s="112"/>
     </row>
-    <row r="83" spans="10:10" ht="15">
+    <row r="83" spans="1:10" ht="15">
       <c r="J83" s="112"/>
     </row>
-    <row r="84" spans="10:10" ht="15">
+    <row r="84" spans="1:10" ht="15">
       <c r="J84" s="112"/>
     </row>
-    <row r="85" spans="10:10" ht="15">
+    <row r="85" spans="1:10" ht="15">
       <c r="J85" s="112"/>
     </row>
-    <row r="86" spans="10:10" ht="15">
+    <row r="86" spans="1:10" ht="15">
       <c r="J86" s="112"/>
     </row>
-    <row r="87" spans="10:10" ht="15">
+    <row r="87" spans="1:10" ht="15">
       <c r="J87" s="112"/>
     </row>
-    <row r="88" spans="10:10" ht="15">
+    <row r="88" spans="1:10" ht="15">
       <c r="J88" s="112"/>
     </row>
-    <row r="89" spans="10:10" ht="15">
+    <row r="89" spans="1:10" ht="15">
       <c r="J89" s="112"/>
     </row>
-    <row r="90" spans="10:10" ht="15">
+    <row r="90" spans="1:10" ht="15">
       <c r="J90" s="112"/>
     </row>
-    <row r="91" spans="10:10" ht="15">
+    <row r="91" spans="1:10" ht="15">
       <c r="J91" s="112"/>
     </row>
-    <row r="92" spans="10:10" ht="15">
+    <row r="92" spans="1:10" ht="15">
       <c r="J92" s="112"/>
     </row>
-    <row r="93" spans="10:10" ht="15">
+    <row r="93" spans="1:10" ht="15">
       <c r="J93" s="112"/>
     </row>
-    <row r="94" spans="10:10" ht="15">
+    <row r="94" spans="1:10" ht="15">
       <c r="J94" s="112"/>
     </row>
-    <row r="95" spans="10:10" ht="15">
+    <row r="95" spans="1:10" ht="15">
       <c r="J95" s="112"/>
     </row>
-    <row r="96" spans="10:10" ht="15">
+    <row r="96" spans="1:10" ht="15">
       <c r="J96" s="112"/>
     </row>
     <row r="97" spans="10:10" ht="15">
@@ -23030,14 +23128,23 @@
     <row r="106" spans="10:10" ht="15">
       <c r="J106" s="112"/>
     </row>
+    <row r="107" spans="10:10" ht="15">
+      <c r="J107" s="112"/>
+    </row>
+    <row r="108" spans="10:10" ht="15">
+      <c r="J108" s="112"/>
+    </row>
+    <row r="109" spans="10:10" ht="15">
+      <c r="J109" s="112"/>
+    </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
-  <conditionalFormatting sqref="C24 C38 C54:I54 C65:C66 C78:I78">
+  <conditionalFormatting sqref="C24 C38 C54:I54 C68:C69 C81:I81">
     <cfRule type="expression" dxfId="30" priority="6" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D65:I65">
+  <conditionalFormatting sqref="D68:I68">
     <cfRule type="expression" dxfId="29" priority="4" stopIfTrue="1">
       <formula>D$7=""</formula>
     </cfRule>
@@ -23047,25 +23154,44 @@
       <formula>K$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43:B53" xr:uid="{3020B3D5-A2C3-4F4B-8EFD-A19414110BEC}">
-      <formula1>current_liabilities</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56:B64" xr:uid="{0AF5B33B-114A-5D47-AC98-0EF208D28A50}">
-      <formula1>noncurrent_liabilities</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B69:B77" xr:uid="{62718926-C752-384A-817F-8A854F7BD996}">
-      <formula1>net_position</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B26:B37" xr:uid="{E796ED53-BB10-BA41-A5DA-36CA177F44A2}">
-      <formula1>noncurrent_assets</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:B23" xr:uid="{BEF100DB-73F2-E445-82C4-2C8C8EBF4AB4}">
-      <formula1>current_assets</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{3020B3D5-A2C3-4F4B-8EFD-A19414110BEC}">
+          <x14:formula1>
+            <xm:f>'Lookup Net Position'!$B$202:$B$315</xm:f>
+          </x14:formula1>
+          <xm:sqref>B43:B53</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{0AF5B33B-114A-5D47-AC98-0EF208D28A50}">
+          <x14:formula1>
+            <xm:f>'Lookup Net Position'!$B$469:$B$514</xm:f>
+          </x14:formula1>
+          <xm:sqref>B56:B67</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{62718926-C752-384A-817F-8A854F7BD996}">
+          <x14:formula1>
+            <xm:f>'Lookup Net Position'!$B$355:$B$375</xm:f>
+          </x14:formula1>
+          <xm:sqref>B72:B80</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{E796ED53-BB10-BA41-A5DA-36CA177F44A2}">
+          <x14:formula1>
+            <xm:f>'Lookup Net Position'!$B$376:$B$468</xm:f>
+          </x14:formula1>
+          <xm:sqref>B26:B37</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{BEF100DB-73F2-E445-82C4-2C8C8EBF4AB4}">
+          <x14:formula1>
+            <xm:f>'Lookup Net Position'!$B$2:$B$201</xm:f>
+          </x14:formula1>
+          <xm:sqref>B10:B23</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -23076,13 +23202,13 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="84" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="84" customWidth="1"/>
     <col min="2" max="2" width="41.5" style="84" customWidth="1"/>
     <col min="3" max="10" width="18.6640625" style="84" customWidth="1"/>
     <col min="11" max="16384" width="9" style="84"/>
@@ -23229,7 +23355,7 @@
     </row>
     <row r="9" spans="1:10" ht="15">
       <c r="A9" s="108" t="str">
-        <f>IF(B9="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B9,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B9="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B9) = 0, "acfr:OperatingRevenueCustom", _xlfn.XLOOKUP(B9, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B9" s="133"/>
@@ -23247,7 +23373,7 @@
     </row>
     <row r="10" spans="1:10" ht="15">
       <c r="A10" s="108" t="str">
-        <f>IF(B10="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B10,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B10="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B10) = 0, "acfr:OperatingRevenueCustom", _xlfn.XLOOKUP(B10, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B10" s="133"/>
@@ -23265,7 +23391,7 @@
     </row>
     <row r="11" spans="1:10" ht="15">
       <c r="A11" s="108" t="str">
-        <f>IF(B11="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B11,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B11="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B11) = 0, "acfr:OperatingRevenueCustom", _xlfn.XLOOKUP(B11, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B11" s="133"/>
@@ -23283,7 +23409,7 @@
     </row>
     <row r="12" spans="1:10" ht="15">
       <c r="A12" s="108" t="str">
-        <f>IF(B12="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B12,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B12="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B12) = 0, "acfr:OperatingRevenueCustom", _xlfn.XLOOKUP(B12, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B12" s="133"/>
@@ -23301,7 +23427,7 @@
     </row>
     <row r="13" spans="1:10" ht="15">
       <c r="A13" s="108" t="str">
-        <f>IF(B13="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B13,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B13="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B13) = 0, "acfr:OperatingRevenueCustom", _xlfn.XLOOKUP(B13, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B13" s="133"/>
@@ -23319,7 +23445,7 @@
     </row>
     <row r="14" spans="1:10" ht="15">
       <c r="A14" s="108" t="str">
-        <f>IF(B14="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B14,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B14="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B14) = 0, "acfr:OperatingRevenueCustom", _xlfn.XLOOKUP(B14, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B14" s="133"/>
@@ -23337,7 +23463,7 @@
     </row>
     <row r="15" spans="1:10" ht="15">
       <c r="A15" s="108" t="str">
-        <f>IF(B15="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B15,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B15="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B15) = 0, "acfr:OperatingRevenueCustom", _xlfn.XLOOKUP(B15, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B15" s="133"/>
@@ -23355,7 +23481,7 @@
     </row>
     <row r="16" spans="1:10" ht="15">
       <c r="A16" s="108" t="str">
-        <f>IF(B16="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B16,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B16="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B16) = 0, "acfr:OperatingRevenueCustom", _xlfn.XLOOKUP(B16, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B16" s="133"/>
@@ -23373,7 +23499,7 @@
     </row>
     <row r="17" spans="1:10" ht="15">
       <c r="A17" s="108" t="str">
-        <f>IF(B17="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B17,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B17="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B17) = 0, "acfr:OperatingRevenueCustom", _xlfn.XLOOKUP(B17, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B17" s="133"/>
@@ -23391,7 +23517,7 @@
     </row>
     <row r="18" spans="1:10" ht="15" hidden="1">
       <c r="A18" s="108" t="str">
-        <f>IF(B18="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B18,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B18="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B18) = 0, "acfr:OperatingRevenueCustom", _xlfn.XLOOKUP(B18, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B18" s="133"/>
@@ -23409,7 +23535,7 @@
     </row>
     <row r="19" spans="1:10" ht="15" hidden="1">
       <c r="A19" s="108" t="str">
-        <f>IF(B19="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B19,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B19="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B19) = 0, "acfr:OperatingRevenueCustom", _xlfn.XLOOKUP(B19, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B19" s="133"/>
@@ -23427,7 +23553,7 @@
     </row>
     <row r="20" spans="1:10" ht="15" hidden="1">
       <c r="A20" s="108" t="str">
-        <f>IF(B20="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B20,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B20="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B20) = 0, "acfr:OperatingRevenueCustom", _xlfn.XLOOKUP(B20, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B20" s="133"/>
@@ -23445,7 +23571,7 @@
     </row>
     <row r="21" spans="1:10" ht="15" hidden="1">
       <c r="A21" s="108" t="str">
-        <f>IF(B21="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B21,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B21="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B21) = 0, "acfr:OperatingRevenueCustom", _xlfn.XLOOKUP(B21, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B21" s="133"/>
@@ -23463,7 +23589,7 @@
     </row>
     <row r="22" spans="1:10" ht="15">
       <c r="A22" s="108" t="str">
-        <f>IF(B22="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B22,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B22="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B22) = 0, "acfr:OperatingRevenueCustom", _xlfn.XLOOKUP(B22, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B22" s="133"/>
@@ -23547,7 +23673,7 @@
     </row>
     <row r="26" spans="1:10" ht="15">
       <c r="A26" s="108" t="str">
-        <f>IF(B26="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B26,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B26="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B26) = 0, "acfr:OperatingExpensesCustom", _xlfn.XLOOKUP(B26, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B26" s="133"/>
@@ -23565,7 +23691,7 @@
     </row>
     <row r="27" spans="1:10" ht="15">
       <c r="A27" s="108" t="str">
-        <f>IF(B27="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B27,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B27="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B27) = 0, "acfr:OperatingExpensesCustom", _xlfn.XLOOKUP(B27, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B27" s="133"/>
@@ -23583,7 +23709,7 @@
     </row>
     <row r="28" spans="1:10" ht="15">
       <c r="A28" s="108" t="str">
-        <f>IF(B28="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B28,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B28="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B28) = 0, "acfr:OperatingExpensesCustom", _xlfn.XLOOKUP(B28, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B28" s="133"/>
@@ -23601,7 +23727,7 @@
     </row>
     <row r="29" spans="1:10" ht="15">
       <c r="A29" s="108" t="str">
-        <f>IF(B29="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B29,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B29="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B29) = 0, "acfr:OperatingExpensesCustom", _xlfn.XLOOKUP(B29, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B29" s="133"/>
@@ -23619,7 +23745,7 @@
     </row>
     <row r="30" spans="1:10" ht="15">
       <c r="A30" s="108" t="str">
-        <f>IF(B30="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B30,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B30="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B30) = 0, "acfr:OperatingExpensesCustom", _xlfn.XLOOKUP(B30, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B30" s="133"/>
@@ -23637,7 +23763,7 @@
     </row>
     <row r="31" spans="1:10" ht="15" hidden="1">
       <c r="A31" s="108" t="str">
-        <f>IF(B31="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B31,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B31="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B31) = 0, "acfr:OperatingExpensesCustom", _xlfn.XLOOKUP(B31, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B31" s="133"/>
@@ -23655,7 +23781,7 @@
     </row>
     <row r="32" spans="1:10" ht="15" hidden="1">
       <c r="A32" s="108" t="str">
-        <f>IF(B32="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B32,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B32="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B32) = 0, "acfr:OperatingExpensesCustom", _xlfn.XLOOKUP(B32, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B32" s="133"/>
@@ -23673,7 +23799,7 @@
     </row>
     <row r="33" spans="1:10" ht="15" hidden="1">
       <c r="A33" s="108" t="str">
-        <f>IF(B33="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B33,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B33="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B33) = 0, "acfr:OperatingExpensesCustom", _xlfn.XLOOKUP(B33, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B33" s="133"/>
@@ -23691,7 +23817,7 @@
     </row>
     <row r="34" spans="1:10" ht="15" hidden="1">
       <c r="A34" s="108" t="str">
-        <f>IF(B34="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B34,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B34="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B34) = 0, "acfr:OperatingExpensesCustom", _xlfn.XLOOKUP(B34, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B34" s="133"/>
@@ -23709,7 +23835,7 @@
     </row>
     <row r="35" spans="1:10" ht="15" hidden="1">
       <c r="A35" s="108" t="str">
-        <f>IF(B35="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B35,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B35="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B35) = 0, "acfr:OperatingExpensesCustom", _xlfn.XLOOKUP(B35, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B35" s="133"/>
@@ -23727,7 +23853,7 @@
     </row>
     <row r="36" spans="1:10" ht="15" hidden="1">
       <c r="A36" s="108" t="str">
-        <f>IF(B36="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B36,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B36="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B36) = 0, "acfr:OperatingExpensesCustom", _xlfn.XLOOKUP(B36, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B36" s="133"/>
@@ -23745,7 +23871,7 @@
     </row>
     <row r="37" spans="1:10" ht="15">
       <c r="A37" s="108" t="str">
-        <f>IF(B37="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B37,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B37="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B37) = 0, "acfr:OperatingExpensesCustom", _xlfn.XLOOKUP(B37, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B37" s="133"/>
@@ -23829,7 +23955,7 @@
     </row>
     <row r="41" spans="1:10" ht="15">
       <c r="A41" s="108" t="str">
-        <f>IF(B41="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B41,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B41="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B41) = 0, "acfr:NonoperatingRevenuesExpensesCustom", _xlfn.XLOOKUP(B41, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B41" s="109"/>
@@ -23844,7 +23970,7 @@
     </row>
     <row r="42" spans="1:10" ht="15">
       <c r="A42" s="108" t="str">
-        <f>IF(B42="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B42,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B42="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B42) = 0, "acfr:NonoperatingRevenuesExpensesCustom", _xlfn.XLOOKUP(B42, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B42" s="109"/>
@@ -23862,7 +23988,7 @@
     </row>
     <row r="43" spans="1:10" ht="15">
       <c r="A43" s="108" t="str">
-        <f>IF(B43="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B43,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B43="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B43) = 0, "acfr:NonoperatingRevenuesExpensesCustom", _xlfn.XLOOKUP(B43, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B43" s="109"/>
@@ -23880,7 +24006,7 @@
     </row>
     <row r="44" spans="1:10" ht="16" customHeight="1">
       <c r="A44" s="108" t="str">
-        <f>IF(B44="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B44,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B44="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B44) = 0, "acfr:NonoperatingRevenuesExpensesCustom", _xlfn.XLOOKUP(B44, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B44" s="109"/>
@@ -23898,7 +24024,7 @@
     </row>
     <row r="45" spans="1:10" ht="16" customHeight="1">
       <c r="A45" s="108" t="str">
-        <f>IF(B45="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B45,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B45="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B45) = 0, "acfr:NonoperatingRevenuesExpensesCustom", _xlfn.XLOOKUP(B45, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B45" s="109"/>
@@ -23916,7 +24042,7 @@
     </row>
     <row r="46" spans="1:10" ht="16" hidden="1" customHeight="1">
       <c r="A46" s="108" t="str">
-        <f>IF(B46="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B46,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B46="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B46) = 0, "acfr:NonoperatingRevenuesExpensesCustom", _xlfn.XLOOKUP(B46, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B46" s="109"/>
@@ -23934,7 +24060,7 @@
     </row>
     <row r="47" spans="1:10" ht="16" hidden="1" customHeight="1">
       <c r="A47" s="108" t="str">
-        <f>IF(B47="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B47,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B47="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B47) = 0, "acfr:NonoperatingRevenuesExpensesCustom", _xlfn.XLOOKUP(B47, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B47" s="109"/>
@@ -23952,7 +24078,7 @@
     </row>
     <row r="48" spans="1:10" ht="16" hidden="1" customHeight="1">
       <c r="A48" s="108" t="str">
-        <f>IF(B48="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B48,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B48="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B48) = 0, "acfr:NonoperatingRevenuesExpensesCustom", _xlfn.XLOOKUP(B48, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B48" s="109"/>
@@ -23970,7 +24096,7 @@
     </row>
     <row r="49" spans="1:10" ht="15" hidden="1">
       <c r="A49" s="108" t="str">
-        <f>IF(B49="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B49,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B49="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B49) = 0, "acfr:NonoperatingRevenuesExpensesCustom", _xlfn.XLOOKUP(B49, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B49" s="109"/>
@@ -23988,7 +24114,7 @@
     </row>
     <row r="50" spans="1:10" ht="15" hidden="1">
       <c r="A50" s="108" t="str">
-        <f>IF(B50="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B50,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B50="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B50) = 0, "acfr:NonoperatingRevenuesExpensesCustom", _xlfn.XLOOKUP(B50, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B50" s="109"/>
@@ -24006,7 +24132,7 @@
     </row>
     <row r="51" spans="1:10" ht="15">
       <c r="A51" s="108" t="str">
-        <f>IF(B51="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B51,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B51="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B51) = 0, "acfr:NonoperatingRevenuesExpensesCustom", _xlfn.XLOOKUP(B51, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B51" s="109"/>
@@ -24130,7 +24256,7 @@
     </row>
     <row r="56" spans="1:10" ht="15">
       <c r="A56" s="108" t="str">
-        <f>IF(B56="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B56,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B56="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B56) = 0, "acfr:ContributionsCustom", _xlfn.XLOOKUP(B56, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B56" s="109"/>
@@ -24148,7 +24274,7 @@
     </row>
     <row r="57" spans="1:10" ht="15">
       <c r="A57" s="108" t="str">
-        <f>IF(B57="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B57,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B57="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B57) = 0, "acfr:ContributionsCustom", _xlfn.XLOOKUP(B57, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B57" s="109"/>
@@ -24166,7 +24292,7 @@
     </row>
     <row r="58" spans="1:10" ht="15">
       <c r="A58" s="108" t="str">
-        <f>IF(B58="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B58,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B58="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B58) = 0, "acfr:ContributionsCustom", _xlfn.XLOOKUP(B58, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B58" s="109"/>
@@ -24184,7 +24310,7 @@
     </row>
     <row r="59" spans="1:10" ht="15">
       <c r="A59" s="108" t="str">
-        <f>IF(B59="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B59,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B59="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B59) = 0, "acfr:ContributionsCustom", _xlfn.XLOOKUP(B59, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B59" s="109"/>
@@ -24202,7 +24328,7 @@
     </row>
     <row r="60" spans="1:10" ht="15" hidden="1">
       <c r="A60" s="108" t="str">
-        <f>IF(B60="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B60,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B60="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B60) = 0, "acfr:ContributionsCustom", _xlfn.XLOOKUP(B60, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B60" s="109"/>
@@ -24220,7 +24346,7 @@
     </row>
     <row r="61" spans="1:10" ht="15" hidden="1">
       <c r="A61" s="108" t="str">
-        <f>IF(B61="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B61,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B61="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B61) = 0, "acfr:ContributionsCustom", _xlfn.XLOOKUP(B61, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B61" s="109"/>
@@ -24238,7 +24364,7 @@
     </row>
     <row r="62" spans="1:10" ht="15" hidden="1">
       <c r="A62" s="108" t="str">
-        <f>IF(B62="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B62,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B62="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B62) = 0, "acfr:ContributionsCustom", _xlfn.XLOOKUP(B62, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B62" s="109"/>
@@ -24256,7 +24382,7 @@
     </row>
     <row r="63" spans="1:10" ht="15" hidden="1">
       <c r="A63" s="108" t="str">
-        <f>IF(B63="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B63,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B63="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B63) = 0, "acfr:ContributionsCustom", _xlfn.XLOOKUP(B63, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B63" s="109"/>
@@ -24274,7 +24400,7 @@
     </row>
     <row r="64" spans="1:10" ht="15">
       <c r="A64" s="108" t="str">
-        <f>IF(B64="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B64,'Lookup PropFunds'!$A$2:$A$296,'Lookup PropFunds'!$C$2:$C$296))</f>
+        <f>IF(B64="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds'!$A$2:$A$296, B64) = 0, "acfr:ContributionsCustom", _xlfn.XLOOKUP(B64, 'Lookup PropFunds'!$A$2:$A$296, 'Lookup PropFunds'!$C$2:$C$296)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B64" s="109"/>
@@ -24589,25 +24715,25 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6FA5A616-5FB2-FA40-81D3-2AC8DD3447E2}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{6FA5A616-5FB2-FA40-81D3-2AC8DD3447E2}">
           <x14:formula1>
             <xm:f>'Lookup PropFunds'!$A$134:$A$246</xm:f>
           </x14:formula1>
           <xm:sqref>B41:B51</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{17875760-A80E-4E45-89DB-9E8399277505}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{17875760-A80E-4E45-89DB-9E8399277505}">
           <x14:formula1>
             <xm:f>'Lookup PropFunds'!$A$249:$A$262</xm:f>
           </x14:formula1>
           <xm:sqref>B56:B64</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EA644A82-E899-114D-AFE5-A9991B6DEBD7}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{EA644A82-E899-114D-AFE5-A9991B6DEBD7}">
           <x14:formula1>
             <xm:f>'Lookup PropFunds'!$A$59:$A$133</xm:f>
           </x14:formula1>
           <xm:sqref>B26:B37</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D627255-0A0A-CF49-9F1C-1F96236A1988}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{5D627255-0A0A-CF49-9F1C-1F96236A1988}">
           <x14:formula1>
             <xm:f>'Lookup PropFunds'!$A$2:$A$57</xm:f>
           </x14:formula1>
@@ -24626,13 +24752,13 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L87" sqref="L87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="84" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" style="84" customWidth="1"/>
     <col min="2" max="2" width="41.5" style="84" customWidth="1"/>
     <col min="3" max="10" width="18.6640625" style="84" customWidth="1"/>
     <col min="11" max="16384" width="9" style="84"/>
@@ -24768,7 +24894,7 @@
     </row>
     <row r="9" spans="1:10" ht="15">
       <c r="A9" s="108" t="str">
-        <f>IF(B9="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B9,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B9="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B9) = 0, "acfr:CashFlowsFromOperatingActivitiesCustom", _xlfn.XLOOKUP(B9, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B9" s="109"/>
@@ -24786,7 +24912,7 @@
     </row>
     <row r="10" spans="1:10" ht="15">
       <c r="A10" s="108" t="str">
-        <f>IF(B10="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B10,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B10="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B10) = 0, "acfr:CashFlowsFromOperatingActivitiesCustom", _xlfn.XLOOKUP(B10, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B10" s="109"/>
@@ -24804,7 +24930,7 @@
     </row>
     <row r="11" spans="1:10" ht="15">
       <c r="A11" s="108" t="str">
-        <f>IF(B11="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B11,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B11="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B11) = 0, "acfr:CashFlowsFromOperatingActivitiesCustom", _xlfn.XLOOKUP(B11, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B11" s="109"/>
@@ -24822,7 +24948,7 @@
     </row>
     <row r="12" spans="1:10" ht="15">
       <c r="A12" s="108" t="str">
-        <f>IF(B12="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B12,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B12="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B12) = 0, "acfr:CashFlowsFromOperatingActivitiesCustom", _xlfn.XLOOKUP(B12, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B12" s="109"/>
@@ -24840,7 +24966,7 @@
     </row>
     <row r="13" spans="1:10" ht="15">
       <c r="A13" s="108" t="str">
-        <f>IF(B13="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B13,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B13="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B13) = 0, "acfr:CashFlowsFromOperatingActivitiesCustom", _xlfn.XLOOKUP(B13, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B13" s="109"/>
@@ -24858,7 +24984,7 @@
     </row>
     <row r="14" spans="1:10" ht="15">
       <c r="A14" s="108" t="str">
-        <f>IF(B14="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B14,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B14="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B14) = 0, "acfr:CashFlowsFromOperatingActivitiesCustom", _xlfn.XLOOKUP(B14, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B14" s="109"/>
@@ -24876,7 +25002,7 @@
     </row>
     <row r="15" spans="1:10" ht="15">
       <c r="A15" s="108" t="str">
-        <f>IF(B15="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B15,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B15="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B15) = 0, "acfr:CashFlowsFromOperatingActivitiesCustom", _xlfn.XLOOKUP(B15, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B15" s="109"/>
@@ -24894,7 +25020,7 @@
     </row>
     <row r="16" spans="1:10" ht="15" hidden="1">
       <c r="A16" s="108" t="str">
-        <f>IF(B16="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B16,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B16="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B16) = 0, "acfr:CashFlowsFromOperatingActivitiesCustom", _xlfn.XLOOKUP(B16, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B16" s="109"/>
@@ -24912,7 +25038,7 @@
     </row>
     <row r="17" spans="1:10" ht="15" hidden="1">
       <c r="A17" s="108" t="str">
-        <f>IF(B17="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B17,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B17="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B17) = 0, "acfr:CashFlowsFromOperatingActivitiesCustom", _xlfn.XLOOKUP(B17, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B17" s="109"/>
@@ -24930,7 +25056,7 @@
     </row>
     <row r="18" spans="1:10" ht="15" hidden="1">
       <c r="A18" s="108" t="str">
-        <f>IF(B18="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B18,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B18="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B18) = 0, "acfr:CashFlowsFromOperatingActivitiesCustom", _xlfn.XLOOKUP(B18, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B18" s="109"/>
@@ -24948,7 +25074,7 @@
     </row>
     <row r="19" spans="1:10" ht="15" hidden="1">
       <c r="A19" s="108" t="str">
-        <f>IF(B19="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B19,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B19="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B19) = 0, "acfr:CashFlowsFromOperatingActivitiesCustom", _xlfn.XLOOKUP(B19, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B19" s="109"/>
@@ -24966,7 +25092,7 @@
     </row>
     <row r="20" spans="1:10" ht="15">
       <c r="A20" s="108" t="str">
-        <f>IF(B20="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B20,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B20="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B20) = 0, "acfr:CashFlowsFromOperatingActivitiesCustom", _xlfn.XLOOKUP(B20, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B20" s="109"/>
@@ -24984,7 +25110,7 @@
     </row>
     <row r="21" spans="1:10" ht="15">
       <c r="A21" s="108" t="str">
-        <f>IF(B21="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B21,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B21="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B21) = 0, "acfr:CashFlowsFromOperatingActivitiesCustom", _xlfn.XLOOKUP(B21, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B21" s="109"/>
@@ -25002,7 +25128,7 @@
     </row>
     <row r="22" spans="1:10" ht="15">
       <c r="A22" s="108" t="str">
-        <f>IF(B22="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B22,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B22="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B22) = 0, "acfr:CashFlowsFromOperatingActivitiesCustom", _xlfn.XLOOKUP(B22, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B22" s="109"/>
@@ -25086,7 +25212,8 @@
     </row>
     <row r="26" spans="1:10" ht="15">
       <c r="A26" s="108" t="str">
-        <f>IF(B26="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B26,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B26="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B26) = 0,
+"acfr:ProceedsFromPaymentsForOtherNonCapitalFinancingActivitiesCustom", _xlfn.XLOOKUP(B26, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B26" s="109"/>
@@ -25104,7 +25231,8 @@
     </row>
     <row r="27" spans="1:10" ht="15">
       <c r="A27" s="108" t="str">
-        <f>IF(B27="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B27,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B27="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B27) = 0,
+"acfr:ProceedsFromPaymentsForOtherNonCapitalFinancingActivitiesCustom", _xlfn.XLOOKUP(B27, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B27" s="109"/>
@@ -25122,7 +25250,8 @@
     </row>
     <row r="28" spans="1:10" ht="15">
       <c r="A28" s="108" t="str">
-        <f>IF(B28="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B28,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B28="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B28) = 0,
+"acfr:ProceedsFromPaymentsForOtherNonCapitalFinancingActivitiesCustom", _xlfn.XLOOKUP(B28, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B28" s="109"/>
@@ -25140,7 +25269,8 @@
     </row>
     <row r="29" spans="1:10" ht="15">
       <c r="A29" s="108" t="str">
-        <f>IF(B29="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B29,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B29="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B29) = 0,
+"acfr:ProceedsFromPaymentsForOtherNonCapitalFinancingActivitiesCustom", _xlfn.XLOOKUP(B29, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B29" s="109"/>
@@ -25158,7 +25288,8 @@
     </row>
     <row r="30" spans="1:10" ht="15">
       <c r="A30" s="108" t="str">
-        <f>IF(B30="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B30,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B30="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B30) = 0,
+"acfr:ProceedsFromPaymentsForOtherNonCapitalFinancingActivitiesCustom", _xlfn.XLOOKUP(B30, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B30" s="109"/>
@@ -25176,7 +25307,8 @@
     </row>
     <row r="31" spans="1:10" ht="15" hidden="1">
       <c r="A31" s="108" t="str">
-        <f>IF(B31="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B31,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B31="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B31) = 0,
+"acfr:ProceedsFromPaymentsForOtherNonCapitalFinancingActivitiesCustom", _xlfn.XLOOKUP(B31, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B31" s="109"/>
@@ -25194,7 +25326,8 @@
     </row>
     <row r="32" spans="1:10" ht="15" hidden="1">
       <c r="A32" s="108" t="str">
-        <f>IF(B32="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B32,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B32="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B32) = 0,
+"acfr:ProceedsFromPaymentsForOtherNonCapitalFinancingActivitiesCustom", _xlfn.XLOOKUP(B32, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B32" s="109"/>
@@ -25212,7 +25345,8 @@
     </row>
     <row r="33" spans="1:10" ht="15" hidden="1">
       <c r="A33" s="108" t="str">
-        <f>IF(B33="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B33,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B33="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B33) = 0,
+"acfr:ProceedsFromPaymentsForOtherNonCapitalFinancingActivitiesCustom", _xlfn.XLOOKUP(B33, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B33" s="109"/>
@@ -25230,7 +25364,8 @@
     </row>
     <row r="34" spans="1:10" ht="15" hidden="1">
       <c r="A34" s="108" t="str">
-        <f>IF(B34="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B34,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B34="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B34) = 0,
+"acfr:ProceedsFromPaymentsForOtherNonCapitalFinancingActivitiesCustom", _xlfn.XLOOKUP(B34, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B34" s="109"/>
@@ -25248,7 +25383,8 @@
     </row>
     <row r="35" spans="1:10" ht="15" hidden="1">
       <c r="A35" s="108" t="str">
-        <f>IF(B35="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B35,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B35="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B35) = 0,
+"acfr:ProceedsFromPaymentsForOtherNonCapitalFinancingActivitiesCustom", _xlfn.XLOOKUP(B35, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B35" s="109"/>
@@ -25266,7 +25402,8 @@
     </row>
     <row r="36" spans="1:10" s="97" customFormat="1" ht="15">
       <c r="A36" s="108" t="str">
-        <f>IF(B36="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B36,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B36="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B36) = 0,
+"acfr:ProceedsFromPaymentsForOtherNonCapitalFinancingActivitiesCustom", _xlfn.XLOOKUP(B36, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B36" s="109"/>
@@ -25284,7 +25421,8 @@
     </row>
     <row r="37" spans="1:10" ht="15">
       <c r="A37" s="108" t="str">
-        <f>IF(B37="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B37,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B37="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B37) = 0,
+"acfr:ProceedsFromPaymentsForOtherNonCapitalFinancingActivitiesCustom", _xlfn.XLOOKUP(B37, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B37" s="109"/>
@@ -25368,7 +25506,8 @@
     </row>
     <row r="41" spans="1:10" ht="15">
       <c r="A41" s="108" t="str">
-        <f>IF(B41="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B41,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B41="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B41) = 0,
+"acfr:ProceedsFromPaymentsForOtherCapitalAndFinancingRelatedActivitiesCustom", _xlfn.XLOOKUP(B41, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B41" s="109"/>
@@ -25386,7 +25525,8 @@
     </row>
     <row r="42" spans="1:10" ht="16" customHeight="1">
       <c r="A42" s="108" t="str">
-        <f>IF(B42="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B42,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B42="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B42) = 0,
+"acfr:ProceedsFromPaymentsForOtherCapitalAndFinancingRelatedActivitiesCustom", _xlfn.XLOOKUP(B42, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B42" s="109"/>
@@ -25404,7 +25544,8 @@
     </row>
     <row r="43" spans="1:10" ht="16" customHeight="1">
       <c r="A43" s="108" t="str">
-        <f>IF(B43="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B43,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B43="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B43) = 0,
+"acfr:ProceedsFromPaymentsForOtherCapitalAndFinancingRelatedActivitiesCustom", _xlfn.XLOOKUP(B43, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B43" s="109"/>
@@ -25422,7 +25563,8 @@
     </row>
     <row r="44" spans="1:10" ht="16" customHeight="1">
       <c r="A44" s="108" t="str">
-        <f>IF(B44="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B44,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B44="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B44) = 0,
+"acfr:ProceedsFromPaymentsForOtherCapitalAndFinancingRelatedActivitiesCustom", _xlfn.XLOOKUP(B44, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B44" s="109"/>
@@ -25440,7 +25582,8 @@
     </row>
     <row r="45" spans="1:10" ht="16" hidden="1" customHeight="1">
       <c r="A45" s="108" t="str">
-        <f>IF(B45="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B45,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B45="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B45) = 0,
+"acfr:ProceedsFromPaymentsForOtherCapitalAndFinancingRelatedActivitiesCustom", _xlfn.XLOOKUP(B45, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B45" s="109"/>
@@ -25458,7 +25601,8 @@
     </row>
     <row r="46" spans="1:10" ht="16" hidden="1" customHeight="1">
       <c r="A46" s="108" t="str">
-        <f>IF(B46="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B46,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B46="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B46) = 0,
+"acfr:ProceedsFromPaymentsForOtherCapitalAndFinancingRelatedActivitiesCustom", _xlfn.XLOOKUP(B46, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B46" s="109"/>
@@ -25476,7 +25620,8 @@
     </row>
     <row r="47" spans="1:10" ht="15" hidden="1">
       <c r="A47" s="108" t="str">
-        <f>IF(B47="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B47,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B47="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B47) = 0,
+"acfr:ProceedsFromPaymentsForOtherCapitalAndFinancingRelatedActivitiesCustom", _xlfn.XLOOKUP(B47, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B47" s="109"/>
@@ -25494,7 +25639,8 @@
     </row>
     <row r="48" spans="1:10" ht="15" hidden="1">
       <c r="A48" s="108" t="str">
-        <f>IF(B48="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B48,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B48="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B48) = 0,
+"acfr:ProceedsFromPaymentsForOtherCapitalAndFinancingRelatedActivitiesCustom", _xlfn.XLOOKUP(B48, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B48" s="109"/>
@@ -25512,7 +25658,8 @@
     </row>
     <row r="49" spans="1:10" ht="15" hidden="1">
       <c r="A49" s="108" t="str">
-        <f>IF(B49="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B49,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B49="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B49) = 0,
+"acfr:ProceedsFromPaymentsForOtherCapitalAndFinancingRelatedActivitiesCustom", _xlfn.XLOOKUP(B49, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B49" s="109"/>
@@ -25530,7 +25677,8 @@
     </row>
     <row r="50" spans="1:10" ht="15">
       <c r="A50" s="108" t="str">
-        <f>IF(B50="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B50,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B50="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B50) = 0,
+"acfr:ProceedsFromPaymentsForOtherCapitalAndFinancingRelatedActivitiesCustom", _xlfn.XLOOKUP(B50, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B50" s="109"/>
@@ -25548,7 +25696,8 @@
     </row>
     <row r="51" spans="1:10" ht="15">
       <c r="A51" s="108" t="str">
-        <f>IF(B51="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B51,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B51="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B51) = 0,
+"acfr:ProceedsFromPaymentsForOtherCapitalAndFinancingRelatedActivitiesCustom", _xlfn.XLOOKUP(B51, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B51" s="109"/>
@@ -25632,7 +25781,8 @@
     </row>
     <row r="55" spans="1:10" ht="15">
       <c r="A55" s="108" t="str">
-        <f>IF(B55="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B55,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B55="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B55) = 0,
+"acfr:ProceedsFromPaymentsForOtherInvestingActivitiesCustom", _xlfn.XLOOKUP(B55, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B55" s="109"/>
@@ -25650,7 +25800,8 @@
     </row>
     <row r="56" spans="1:10" ht="15">
       <c r="A56" s="108" t="str">
-        <f>IF(B56="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B56,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B56="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B56) = 0,
+"acfr:ProceedsFromPaymentsForOtherInvestingActivitiesCustom", _xlfn.XLOOKUP(B56, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B56" s="109"/>
@@ -25668,7 +25819,8 @@
     </row>
     <row r="57" spans="1:10" ht="15" hidden="1">
       <c r="A57" s="108" t="str">
-        <f>IF(B57="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B57,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B57="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B57) = 0,
+"acfr:ProceedsFromPaymentsForOtherInvestingActivitiesCustom", _xlfn.XLOOKUP(B57, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B57" s="109"/>
@@ -25686,7 +25838,8 @@
     </row>
     <row r="58" spans="1:10" ht="15" hidden="1">
       <c r="A58" s="108" t="str">
-        <f>IF(B58="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B58,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B58="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B58) = 0,
+"acfr:ProceedsFromPaymentsForOtherInvestingActivitiesCustom", _xlfn.XLOOKUP(B58, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B58" s="109"/>
@@ -25704,7 +25857,8 @@
     </row>
     <row r="59" spans="1:10" ht="15" hidden="1">
       <c r="A59" s="108" t="str">
-        <f>IF(B59="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B59,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B59="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B59) = 0,
+"acfr:ProceedsFromPaymentsForOtherInvestingActivitiesCustom", _xlfn.XLOOKUP(B59, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B59" s="109"/>
@@ -25722,7 +25876,8 @@
     </row>
     <row r="60" spans="1:10" ht="15" hidden="1">
       <c r="A60" s="108" t="str">
-        <f>IF(B60="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B60,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B60="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B60) = 0,
+"acfr:ProceedsFromPaymentsForOtherInvestingActivitiesCustom", _xlfn.XLOOKUP(B60, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B60" s="109"/>
@@ -25740,7 +25895,8 @@
     </row>
     <row r="61" spans="1:10" ht="15" hidden="1">
       <c r="A61" s="108" t="str">
-        <f>IF(B61="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B61,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B61="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B61) = 0,
+"acfr:ProceedsFromPaymentsForOtherInvestingActivitiesCustom", _xlfn.XLOOKUP(B61, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B61" s="109"/>
@@ -25758,7 +25914,8 @@
     </row>
     <row r="62" spans="1:10" ht="15">
       <c r="A62" s="108" t="str">
-        <f>IF(B62="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B62,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B62="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B62) = 0,
+"acfr:ProceedsFromPaymentsForOtherInvestingActivitiesCustom", _xlfn.XLOOKUP(B62, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B62" s="109"/>
@@ -25776,7 +25933,8 @@
     </row>
     <row r="63" spans="1:10" ht="15">
       <c r="A63" s="108" t="str">
-        <f>IF(B63="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B63,'Lookup PropFunds CashFlows'!$B$2:$B$74,'Lookup PropFunds CashFlows'!$C$2:$C$74))</f>
+        <f>IF(B63="", "Choose from drop-down --&gt;", IF(COUNTIF('Lookup PropFunds CashFlows'!$B$2:$B$74, B63) = 0,
+"acfr:ProceedsFromPaymentsForOtherInvestingActivitiesCustom", _xlfn.XLOOKUP(B63, 'Lookup PropFunds CashFlows'!$B$2:$B$74, 'Lookup PropFunds CashFlows'!$C$2:$C$74)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B63" s="109"/>
@@ -26168,25 +26326,25 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EF3CE8D3-824D-D342-8991-B399369E5D1F}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{EF3CE8D3-824D-D342-8991-B399369E5D1F}">
           <x14:formula1>
             <xm:f>'Lookup PropFunds CashFlows'!$B$40:$B$74</xm:f>
           </x14:formula1>
           <xm:sqref>B9:B22</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8C60F6D6-E0D1-B44C-A6F7-DED0D3730BFE}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{8C60F6D6-E0D1-B44C-A6F7-DED0D3730BFE}">
           <x14:formula1>
             <xm:f>'Lookup PropFunds CashFlows'!$B$21:$B$39</xm:f>
           </x14:formula1>
           <xm:sqref>B26:B37</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2E348E09-9902-2B41-B16D-37E2F8DE3135}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{2E348E09-9902-2B41-B16D-37E2F8DE3135}">
           <x14:formula1>
             <xm:f>'Lookup PropFunds CashFlows'!$B$2:$B$15</xm:f>
           </x14:formula1>
           <xm:sqref>B41:B51</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9F9EA262-D7F4-214A-AA87-6EFB9500F700}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{9F9EA262-D7F4-214A-AA87-6EFB9500F700}">
           <x14:formula1>
             <xm:f>'Lookup PropFunds CashFlows'!$B$16:$B$20</xm:f>
           </x14:formula1>
@@ -26205,8 +26363,8 @@
   </sheetPr>
   <dimension ref="A1:C358"/>
   <sheetViews>
-    <sheetView topLeftCell="A196" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B201" sqref="B201"/>
+    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D135" sqref="D135:D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -33186,8 +33344,8 @@
   </sheetPr>
   <dimension ref="A1:E311"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A273" workbookViewId="0">
+      <selection activeCell="D262" sqref="D262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -39539,7 +39697,7 @@
   </sheetPr>
   <dimension ref="A1:E442"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A146" zoomScale="125" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -46030,8 +46188,8 @@
   </sheetPr>
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="116" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="A28" zoomScale="81" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -46138,7 +46296,7 @@
     </row>
     <row r="9" spans="1:6" ht="15">
       <c r="A9" s="6" t="str">
-        <f>IF(B9="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B9)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B9,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B9="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B9)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B9,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B9" s="15"/>
@@ -46152,7 +46310,7 @@
     </row>
     <row r="10" spans="1:6" ht="15">
       <c r="A10" s="6" t="str">
-        <f>IF(B10="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B10)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B10,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B10="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B10)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B10,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B10" s="15"/>
@@ -46166,7 +46324,7 @@
     </row>
     <row r="11" spans="1:6" ht="15">
       <c r="A11" s="6" t="str">
-        <f>IF(B11="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B11)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B11,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B11="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B11)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B11,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B11" s="15"/>
@@ -46180,7 +46338,7 @@
     </row>
     <row r="12" spans="1:6" ht="15">
       <c r="A12" s="6" t="str">
-        <f>IF(B12="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B12)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B12,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B12="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B12)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B12,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B12" s="15"/>
@@ -46194,7 +46352,7 @@
     </row>
     <row r="13" spans="1:6" ht="15">
       <c r="A13" s="6" t="str">
-        <f>IF(B13="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B13)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B13,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B13="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B13)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B13,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B13" s="15"/>
@@ -46205,7 +46363,7 @@
     </row>
     <row r="14" spans="1:6" ht="15">
       <c r="A14" s="6" t="str">
-        <f>IF(B14="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B14)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B14,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B14="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B14)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B14,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B14" s="15"/>
@@ -46216,7 +46374,7 @@
     </row>
     <row r="15" spans="1:6" ht="15">
       <c r="A15" s="6" t="str">
-        <f>IF(B15="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B15)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B15,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B15="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B15)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B15,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B15" s="15"/>
@@ -46227,7 +46385,7 @@
     </row>
     <row r="16" spans="1:6" ht="15">
       <c r="A16" s="6" t="str">
-        <f>IF(B16="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B16)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B16,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B16="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B16)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B16,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B16" s="15"/>
@@ -46241,7 +46399,7 @@
     </row>
     <row r="17" spans="1:6" ht="15">
       <c r="A17" s="6" t="str">
-        <f>IF(B17="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B17)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B17,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B17="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B17)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B17,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B17" s="15"/>
@@ -46255,7 +46413,7 @@
     </row>
     <row r="18" spans="1:6" ht="15" hidden="1">
       <c r="A18" s="6" t="str">
-        <f>IF(B18="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B18)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B18,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B18="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B18)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B18,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B18" s="15"/>
@@ -46269,7 +46427,7 @@
     </row>
     <row r="19" spans="1:6" ht="15" hidden="1">
       <c r="A19" s="6" t="str">
-        <f>IF(B19="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B19)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B19,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B19="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B19)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B19,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B19" s="15"/>
@@ -46283,7 +46441,7 @@
     </row>
     <row r="20" spans="1:6" ht="15" hidden="1">
       <c r="A20" s="6" t="str">
-        <f>IF(B20="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B20)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B20,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B20="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B20)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B20,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B20" s="15"/>
@@ -46297,7 +46455,7 @@
     </row>
     <row r="21" spans="1:6" ht="15" hidden="1">
       <c r="A21" s="6" t="str">
-        <f>IF(B21="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B21)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B21,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B21="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B21)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B21,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B21" s="15"/>
@@ -46311,7 +46469,7 @@
     </row>
     <row r="22" spans="1:6" ht="15">
       <c r="A22" s="6" t="str">
-        <f>IF(B22="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B22)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B22,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B22="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B22)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B22,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B22" s="15"/>
@@ -46358,7 +46516,7 @@
     </row>
     <row r="25" spans="1:6" ht="15">
       <c r="A25" s="6" t="str">
-        <f>IF(B25="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B25)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B25,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B25="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B25)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B25,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B25" s="15"/>
@@ -46372,7 +46530,7 @@
     </row>
     <row r="26" spans="1:6" ht="15">
       <c r="A26" s="6" t="str">
-        <f>IF(B26="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B26)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B26,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B26="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B26)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B26,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B26" s="15"/>
@@ -46383,7 +46541,7 @@
     </row>
     <row r="27" spans="1:6" ht="15">
       <c r="A27" s="6" t="str">
-        <f>IF(B27="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B27)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B27,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B27="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B27)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B27,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B27" s="16"/>
@@ -46394,7 +46552,7 @@
     </row>
     <row r="28" spans="1:6" ht="15">
       <c r="A28" s="6" t="str">
-        <f>IF(B28="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B28)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B28,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B28="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B28)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B28,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B28" s="16"/>
@@ -46405,7 +46563,7 @@
     </row>
     <row r="29" spans="1:6" ht="15">
       <c r="A29" s="6" t="str">
-        <f>IF(B29="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B29)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B29,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B29="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B29)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B29,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B29" s="16"/>
@@ -46416,7 +46574,7 @@
     </row>
     <row r="30" spans="1:6" ht="15">
       <c r="A30" s="6" t="str">
-        <f>IF(B30="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B30)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B30,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B30="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B30)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B30,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B30" s="15"/>
@@ -46427,7 +46585,7 @@
     </row>
     <row r="31" spans="1:6" ht="15">
       <c r="A31" s="6" t="str">
-        <f>IF(B31="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B31)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B31,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B31="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B31)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B31,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B31" s="15"/>
@@ -46576,7 +46734,7 @@
     </row>
     <row r="41" spans="1:6" ht="15">
       <c r="A41" s="6" t="str">
-        <f>IF(B41="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B41)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B41,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B41="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B41)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B41,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B41" s="15"/>
@@ -46590,7 +46748,7 @@
     </row>
     <row r="42" spans="1:6" ht="15">
       <c r="A42" s="6" t="str">
-        <f>IF(B42="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B42)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B42,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B42="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B42)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B42,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B42" s="15"/>
@@ -46604,7 +46762,7 @@
     </row>
     <row r="43" spans="1:6" ht="15">
       <c r="A43" s="6" t="str">
-        <f>IF(B43="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B43)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B43,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B43="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B43)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B43,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B43" s="15"/>
@@ -46618,7 +46776,7 @@
     </row>
     <row r="44" spans="1:6" ht="15">
       <c r="A44" s="6" t="str">
-        <f>IF(B44="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B44)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B44,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B44="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B44)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B44,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B44" s="15"/>
@@ -46632,7 +46790,7 @@
     </row>
     <row r="45" spans="1:6" ht="15">
       <c r="A45" s="6" t="str">
-        <f>IF(B45="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B45)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B45,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B45="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B45)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B45,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B45" s="15"/>
@@ -46753,7 +46911,7 @@
     </row>
     <row r="54" spans="1:6" ht="15">
       <c r="A54" s="6" t="str">
-        <f>IF(B54="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B54)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B54,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B54="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B54)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B54,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B54" s="15"/>
@@ -46940,7 +47098,7 @@
     </row>
     <row r="67" spans="1:6" ht="15">
       <c r="A67" s="6" t="str">
-        <f>IF(B67="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B67)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B67,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B67="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B67)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B67,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B67" s="15"/>
@@ -46951,7 +47109,7 @@
     </row>
     <row r="68" spans="1:6" ht="15">
       <c r="A68" s="6" t="str">
-        <f>IF(B68="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B68)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B68,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B68="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B68)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B68,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B68" s="15"/>
@@ -46962,7 +47120,7 @@
     </row>
     <row r="69" spans="1:6" ht="15">
       <c r="A69" s="6" t="str">
-        <f>IF(B69="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B69)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B69,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B69="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B69)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B69,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B69" s="15"/>
@@ -46973,7 +47131,7 @@
     </row>
     <row r="70" spans="1:6" ht="15">
       <c r="A70" s="6" t="str">
-        <f>IF(B70="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B70)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B70,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B70="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B70)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B70,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B70" s="15"/>
@@ -47122,7 +47280,7 @@
     </row>
     <row r="80" spans="1:6" ht="15">
       <c r="A80" s="6" t="str">
-        <f>IF(B80="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B80)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B80,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B80="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B80)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B80,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B80" s="15"/>
@@ -47136,7 +47294,7 @@
     </row>
     <row r="81" spans="1:6" ht="15">
       <c r="A81" s="6" t="str">
-        <f>IF(B81="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B81)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B81,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B81="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B81)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B81,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B81" s="15"/>
@@ -47150,7 +47308,7 @@
     </row>
     <row r="82" spans="1:6" ht="15">
       <c r="A82" s="6" t="str">
-        <f>IF(B82="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B82)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B82,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B82="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B82)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B82,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B82" s="15"/>
@@ -47164,7 +47322,7 @@
     </row>
     <row r="83" spans="1:6" ht="15">
       <c r="A83" s="6" t="str">
-        <f>IF(B83="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B83)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B83,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B83="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B83)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B83,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B83" s="15"/>
@@ -47289,7 +47447,7 @@
     </row>
     <row r="92" spans="1:6" ht="15">
       <c r="A92" s="6" t="str">
-        <f>IF(B92="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B92)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B92,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B92="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B92)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B92,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B92" s="15"/>
@@ -47300,7 +47458,7 @@
     </row>
     <row r="93" spans="1:6" ht="15">
       <c r="A93" s="6" t="str">
-        <f>IF(B93="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B93)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B93,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B93="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B93)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B93,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B93" s="15"/>
@@ -47311,7 +47469,7 @@
     </row>
     <row r="94" spans="1:6" ht="15">
       <c r="A94" s="6" t="str">
-        <f>IF(B94="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B94)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B94,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B94="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B94)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B94,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B94" s="15"/>
@@ -47322,7 +47480,7 @@
     </row>
     <row r="95" spans="1:6" ht="15">
       <c r="A95" s="6" t="str">
-        <f>IF(B95="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$420,B95)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B95,'Lookup Net Position'!$B$2:$B$420,'Lookup Net Position'!$C$2:$C$420)))</f>
+        <f>IF(B95="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B95)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B95,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B95" s="15"/>
@@ -47530,8 +47688,8 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView topLeftCell="A23" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -49226,8 +49384,8 @@
       <formula>J$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B41:B49" xr:uid="{F3C11D5E-2141-5546-AF1F-2279D6DA74D8}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B41:B49 B9:B22 B25:B36" xr:uid="{F3C11D5E-2141-5546-AF1F-2279D6DA74D8}">
       <formula1>program_revenues</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B54:B63" xr:uid="{96AC2388-DB7C-8442-BE26-CB837586D707}">
@@ -49236,9 +49394,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B66:B70" xr:uid="{A7A9E828-3622-4441-839C-4C8E5DABEB87}">
       <formula1>transfers</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B9:B22 B25:B36" xr:uid="{5B081783-9278-9542-AB7A-E156D9F5E750}">
-      <formula1>program_revenues</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Issue 67- added readme
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarrahahmed/Desktop/CLOSUP/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB83A5A1-7C18-6946-999B-4A0C4DE4E06A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F55631-3268-B742-933A-242379D4950A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" tabRatio="834" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17280" tabRatio="834" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Net Position" sheetId="8" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5349" uniqueCount="3618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5367" uniqueCount="3636">
   <si>
     <t>Statement of Net Position</t>
   </si>
@@ -10947,6 +10947,60 @@
   </si>
   <si>
     <t>Custom Restricted Fund Balance</t>
+  </si>
+  <si>
+    <t>This template is designed to help you prepare your financial statements for submission and convert them into XBRL format.</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>1. Enter Financial Statements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Fill in the financial data in the corresponding cells. Ensure all required fields are completed.</t>
+  </si>
+  <si>
+    <t>2. Verify Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Double-check all entries for accuracy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Ensure that all calculations and formulas are correct.</t>
+  </si>
+  <si>
+    <t>3. Save the File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Once all data is entered and verified, save the Excel file with an appropriate name indicating its contents and date.</t>
+  </si>
+  <si>
+    <t>4. Upload for XBRL Conversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Navigate to the XBRL conversion tool provided by your organization.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Upload the saved Excel file to the converter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Follow the instructions provided by the conversion tool to complete the process.</t>
+  </si>
+  <si>
+    <t>5. Review XBRL Output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - After conversion, review the XBRL output to ensure it accurately reflects the entered financial statements.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Make any necessary adjustments in the original Excel file and repeat the upload process if needed.</t>
+  </si>
+  <si>
+    <t>READ ME:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Open the relevant sheets in this Excel file (e.g.,Net Position, PropFunds, Statement of Activities).</t>
   </si>
 </sst>
 </file>
@@ -11575,7 +11629,7 @@
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="255">
+  <cellXfs count="256">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -12059,6 +12113,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="27" fillId="18" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="27" fillId="18" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -12068,9 +12126,8 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="27" fillId="18" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -12080,11 +12137,314 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
   </cellStyles>
-  <dxfs count="151">
+  <dxfs count="91">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12124,9 +12484,10 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12152,9 +12513,34 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12180,107 +12566,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -12433,9 +12718,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -12445,109 +12727,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
+          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12570,115 +12750,19 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
+          <bgColor theme="1" tint="0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12750,9 +12834,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -12767,526 +12848,9 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -20349,18 +19913,18 @@
       </c>
     </row>
     <row r="59" spans="1:10" ht="15">
-      <c r="A59" s="250" t="s">
+      <c r="A59" s="252" t="s">
         <v>3615</v>
       </c>
-      <c r="B59" s="251"/>
-      <c r="C59" s="251"/>
-      <c r="D59" s="251"/>
-      <c r="E59" s="251"/>
-      <c r="F59" s="251"/>
-      <c r="G59" s="251"/>
-      <c r="H59" s="251"/>
-      <c r="I59" s="251"/>
-      <c r="J59" s="252"/>
+      <c r="B59" s="253"/>
+      <c r="C59" s="253"/>
+      <c r="D59" s="253"/>
+      <c r="E59" s="253"/>
+      <c r="F59" s="253"/>
+      <c r="G59" s="253"/>
+      <c r="H59" s="253"/>
+      <c r="I59" s="253"/>
+      <c r="J59" s="254"/>
     </row>
     <row r="60" spans="1:10" ht="15">
       <c r="A60" s="108" t="str">
@@ -20375,7 +19939,7 @@
       <c r="G60" s="209"/>
       <c r="H60" s="210"/>
       <c r="I60" s="210"/>
-      <c r="J60" s="253">
+      <c r="J60" s="250">
         <v>0</v>
       </c>
     </row>
@@ -20392,23 +19956,23 @@
       <c r="G61" s="209"/>
       <c r="H61" s="210"/>
       <c r="I61" s="210"/>
-      <c r="J61" s="253">
+      <c r="J61" s="250">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="15">
-      <c r="A62" s="250" t="s">
+      <c r="A62" s="252" t="s">
         <v>3616</v>
       </c>
-      <c r="B62" s="251"/>
-      <c r="C62" s="251"/>
-      <c r="D62" s="251"/>
-      <c r="E62" s="251"/>
-      <c r="F62" s="251"/>
-      <c r="G62" s="251"/>
-      <c r="H62" s="251"/>
-      <c r="I62" s="251"/>
-      <c r="J62" s="252"/>
+      <c r="B62" s="253"/>
+      <c r="C62" s="253"/>
+      <c r="D62" s="253"/>
+      <c r="E62" s="253"/>
+      <c r="F62" s="253"/>
+      <c r="G62" s="253"/>
+      <c r="H62" s="253"/>
+      <c r="I62" s="253"/>
+      <c r="J62" s="254"/>
     </row>
     <row r="63" spans="1:10" ht="15">
       <c r="A63" s="108" t="str">
@@ -20445,18 +20009,18 @@
       </c>
     </row>
     <row r="65" spans="1:10" ht="15">
-      <c r="A65" s="250" t="s">
+      <c r="A65" s="252" t="s">
         <v>3617</v>
       </c>
-      <c r="B65" s="251"/>
-      <c r="C65" s="251"/>
-      <c r="D65" s="251"/>
-      <c r="E65" s="251"/>
-      <c r="F65" s="251"/>
-      <c r="G65" s="251"/>
-      <c r="H65" s="251"/>
-      <c r="I65" s="251"/>
-      <c r="J65" s="252"/>
+      <c r="B65" s="253"/>
+      <c r="C65" s="253"/>
+      <c r="D65" s="253"/>
+      <c r="E65" s="253"/>
+      <c r="F65" s="253"/>
+      <c r="G65" s="253"/>
+      <c r="H65" s="253"/>
+      <c r="I65" s="253"/>
+      <c r="J65" s="254"/>
     </row>
     <row r="66" spans="1:10" ht="16">
       <c r="A66" s="131" t="str">
@@ -20500,31 +20064,31 @@
         <v>2475</v>
       </c>
       <c r="C68" s="217">
-        <f>SUM(C48:C58)</f>
+        <f t="shared" ref="C68:I68" si="7">SUM(C48:C58)</f>
         <v>0</v>
       </c>
       <c r="D68" s="217">
-        <f>SUM(D48:D58)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E68" s="217">
-        <f>SUM(E48:E58)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F68" s="217">
-        <f>SUM(F48:F58)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G68" s="217">
-        <f>SUM(G48:G58)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H68" s="218">
-        <f>SUM(H48:H58)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I68" s="218">
-        <f>SUM(I48:I58)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J68" s="218">
@@ -20575,59 +20139,59 @@
     <mergeCell ref="A62:J62"/>
     <mergeCell ref="A65:J65"/>
   </mergeCells>
-  <conditionalFormatting sqref="D8:G18 D21:G31 C32:I33 D35:G44 C45:I46 D48:G58 C68:G68 D67:G67 D60:G61 D63:G64">
-    <cfRule type="expression" dxfId="138" priority="10" stopIfTrue="1">
+  <conditionalFormatting sqref="A9:A18">
+    <cfRule type="containsText" dxfId="58" priority="7" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22:A31">
+    <cfRule type="containsText" dxfId="57" priority="6" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35:A44">
+    <cfRule type="containsText" dxfId="56" priority="5" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A48:A58">
+    <cfRule type="containsText" dxfId="55" priority="4" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:A61">
+    <cfRule type="containsText" dxfId="54" priority="3" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:A64">
+    <cfRule type="containsText" dxfId="53" priority="2" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66:A67">
+    <cfRule type="containsText" dxfId="52" priority="1" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A66)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:G18 D21:G31 C32:I33 D35:G44 C45:I46 D48:G58 D60:G61 D63:G64 C68:G68">
+    <cfRule type="expression" dxfId="51" priority="10" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D66:G67">
+    <cfRule type="expression" dxfId="50" priority="8" stopIfTrue="1">
+      <formula>D$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D7:I7">
-    <cfRule type="expression" dxfId="137" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="9" stopIfTrue="1">
       <formula>D$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J45:J46">
-    <cfRule type="expression" dxfId="136" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="11" stopIfTrue="1">
       <formula>I$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D66:G66">
-    <cfRule type="expression" dxfId="103" priority="8" stopIfTrue="1">
-      <formula>D$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A18">
-    <cfRule type="containsText" dxfId="22" priority="7" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22:A31">
-    <cfRule type="containsText" dxfId="21" priority="6" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35:A44">
-    <cfRule type="containsText" dxfId="20" priority="5" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A48:A58">
-    <cfRule type="containsText" dxfId="19" priority="4" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60:A61">
-    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A63:A64">
-    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A66:A67">
-    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -20867,7 +20431,7 @@
   <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="81" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -22229,24 +21793,24 @@
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
   <phoneticPr fontId="14" type="noConversion"/>
-  <conditionalFormatting sqref="D7:I7 D8:J23 C23 D25:J35 C35 C36:J36 D37:J63 C59:J60 J64 D65:J69 D71:J71">
-    <cfRule type="expression" dxfId="135" priority="20" stopIfTrue="1">
-      <formula>C$7=""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A9:A22">
-    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="47" priority="3" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:A34">
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:A53">
-    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="45" priority="1" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7:I7 D8:J23 C23 D25:J35 C35 C36:J36 D37:J63 C59:J60 J64 D65:J69 D71:J71">
+    <cfRule type="expression" dxfId="44" priority="20" stopIfTrue="1">
+      <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
@@ -22454,7 +22018,7 @@
   <dimension ref="A1:K109"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q45" sqref="Q45"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -24121,44 +23685,44 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A10:A23">
+    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:A37">
+    <cfRule type="containsText" dxfId="42" priority="4" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:A53">
+    <cfRule type="containsText" dxfId="41" priority="3" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:A67">
+    <cfRule type="containsText" dxfId="40" priority="2" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A72:A80">
+    <cfRule type="containsText" dxfId="39" priority="1" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A72)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C24 C38 C54:I54 C68:C69 C81:I81">
-    <cfRule type="expression" dxfId="134" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="11" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D68:I68">
-    <cfRule type="expression" dxfId="133" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="9" stopIfTrue="1">
       <formula>D$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="expression" dxfId="132" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="8" stopIfTrue="1">
       <formula>K$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10:A23">
-    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26:A37">
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A43:A53">
-    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56:A67">
-    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A72:A80">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A72)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24209,8 +23773,8 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -25681,60 +25245,60 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A9:A22">
+    <cfRule type="containsText" dxfId="35" priority="4" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:A37">
+    <cfRule type="containsText" dxfId="34" priority="3" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:A51">
+    <cfRule type="containsText" dxfId="33" priority="2" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:A64">
+    <cfRule type="containsText" dxfId="32" priority="1" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C23:C24 C38:C39 C70:J70">
-    <cfRule type="expression" dxfId="131" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="15" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="130" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="7" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:I54">
-    <cfRule type="expression" dxfId="129" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="6" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65:I66">
-    <cfRule type="expression" dxfId="128" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="5" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:J70">
-    <cfRule type="cellIs" dxfId="127" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="16" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="17" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="18" operator="notEqual">
+    <cfRule type="cellIs" dxfId="25" priority="18" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D70:I70">
-    <cfRule type="expression" dxfId="124" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="19" stopIfTrue="1">
       <formula>#REF!=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A22">
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26:A37">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41:A51">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56:A64">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -27259,108 +26823,108 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A9:A22">
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:A37">
+    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:A51">
+    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55:A63">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="123" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="22" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="122" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="21" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:I24 C53:I53">
-    <cfRule type="expression" dxfId="121" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="28" stopIfTrue="1">
       <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:I52">
-    <cfRule type="expression" dxfId="120" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:I64">
-    <cfRule type="expression" dxfId="119" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="17" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D69:I69">
-    <cfRule type="expression" dxfId="118" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
       <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:J65">
-    <cfRule type="expression" dxfId="117" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="7" stopIfTrue="1">
       <formula>D$7=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="10" operator="notEqual">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
       <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D69:J69">
-    <cfRule type="expression" dxfId="112" priority="12" stopIfTrue="1">
-      <formula>D$7=""</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="13" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="15" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="14" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="12" stopIfTrue="1">
+      <formula>D$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J4 J8:J22 J24:J64 J70:J1048574">
-    <cfRule type="expression" dxfId="108" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="23" stopIfTrue="1">
       <formula>COUNTA(D2:I2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:J22 J24:J64 J70:J78">
-    <cfRule type="expression" dxfId="107" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="84" stopIfTrue="1">
       <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J68">
-    <cfRule type="expression" dxfId="106" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
+      <formula>#REF!=""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>COUNTA(D69:I69)=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="105" priority="6" stopIfTrue="1">
-      <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1048575:J1048576">
-    <cfRule type="expression" dxfId="104" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="86" stopIfTrue="1">
       <formula>COUNTA(D1:I3)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A22">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26:A37">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A26)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41:A51">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55:A63">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -47162,10 +46726,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8474313-8EAC-0141-BA8E-861AF31ED060}">
-  <dimension ref="B1:E6"/>
+  <dimension ref="B1:E32"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -47217,6 +46781,96 @@
         <v>1092</v>
       </c>
       <c r="E6" s="2"/>
+    </row>
+    <row r="10" spans="2:5" ht="14">
+      <c r="B10" s="255" t="s">
+        <v>3634</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" t="s">
+        <v>3618</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="60" t="s">
+        <v>3619</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" t="s">
+        <v>3620</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="2" t="s">
+        <v>3635</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" t="s">
+        <v>3621</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>3622</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>3623</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
+        <v>3624</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>3625</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="s">
+        <v>3626</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>3627</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" t="s">
+        <v>3628</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" t="s">
+        <v>3629</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" t="s">
+        <v>3630</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
+        <v>3631</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" t="s">
+        <v>3632</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
+        <v>3633</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -47435,7 +47089,7 @@
         <f>IF(B16="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B16)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B16,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B16" s="254"/>
+      <c r="B16" s="251"/>
       <c r="C16" s="202"/>
       <c r="D16" s="203"/>
       <c r="E16" s="200" t="str">
@@ -48636,71 +48290,71 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A9:A22">
+    <cfRule type="expression" dxfId="90" priority="16">
+      <formula>A9="acfr:CurrentAssetsCustom"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25:A31">
+    <cfRule type="containsText" dxfId="89" priority="3" operator="containsText" text="acfr:NonCurrentAssetsCustom">
+      <formula>NOT(ISERROR(SEARCH("acfr:NonCurrentAssetsCustom",A25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:A45">
+    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="acfr:DeferredOutflowsOfResourcesCustom">
+      <formula>NOT(ISERROR(SEARCH("acfr:DeferredOutflowsOfResourcesCustom",A41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="87" priority="13" operator="containsText" text="acfr:DeferredOutflowsOfResourcesCustom">
+      <formula>NOT(ISERROR(SEARCH("acfr:DeferredOutflowsOfResourcesCustom",A41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:A59">
+    <cfRule type="containsText" dxfId="86" priority="1" operator="containsText" text="acfr:CurrentLiabilitiesCustom">
+      <formula>NOT(ISERROR(SEARCH("acfr:CurrentLiabilitiesCustom",A54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="85" priority="12" operator="containsText" text="acfr:CurrentLiabilitiesCustom">
+      <formula>NOT(ISERROR(SEARCH("acfr:CurrentLiabilitiesCustom",A54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67:A70">
+    <cfRule type="containsText" dxfId="84" priority="11" operator="containsText" text="acfr:NoncurrentLiabilitiesCustom">
+      <formula>NOT(ISERROR(SEARCH("acfr:NoncurrentLiabilitiesCustom",A67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A80:A83">
+    <cfRule type="containsText" dxfId="83" priority="10" operator="containsText" text="acfr:DeferredInflowsOfResourcesCustom">
+      <formula>NOT(ISERROR(SEARCH("acfr:DeferredInflowsOfResourcesCustom",A80)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A92:A95">
+    <cfRule type="containsText" dxfId="82" priority="9" operator="containsText" text="acfr:RestrictedComponentsOfNetPositionCustom">
+      <formula>NOT(ISERROR(SEARCH("acfr:RestrictedComponentsOfNetPositionCustom",A92)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15">
+    <cfRule type="containsText" dxfId="81" priority="15" operator="containsText" text="acfr:CurrentAssetsCustom">
+      <formula>NOT(ISERROR(SEARCH("acfr:CurrentAssetsCustom",B15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C101:F101">
-    <cfRule type="cellIs" dxfId="101" priority="34" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="34" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="35" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="35" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="36" operator="notEqual">
+    <cfRule type="cellIs" dxfId="78" priority="36" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:F37 C23:F23 C37:F37 D39:F101 C50 C65:F65 C76:C77 C89 C101">
-    <cfRule type="expression" dxfId="98" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="18" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A22">
-    <cfRule type="expression" dxfId="97" priority="16">
-      <formula>A9="acfr:CurrentAssetsCustom"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="96" priority="15" operator="containsText" text="acfr:CurrentAssetsCustom">
-      <formula>NOT(ISERROR(SEARCH("acfr:CurrentAssetsCustom",B15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41:A45">
-    <cfRule type="containsText" dxfId="76" priority="13" operator="containsText" text="acfr:DeferredOutflowsOfResourcesCustom">
-      <formula>NOT(ISERROR(SEARCH("acfr:DeferredOutflowsOfResourcesCustom",A41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="2" operator="containsText" text="acfr:DeferredOutflowsOfResourcesCustom">
-      <formula>NOT(ISERROR(SEARCH("acfr:DeferredOutflowsOfResourcesCustom",A41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:A59">
-    <cfRule type="containsText" dxfId="73" priority="12" operator="containsText" text="acfr:CurrentLiabilitiesCustom">
-      <formula>NOT(ISERROR(SEARCH("acfr:CurrentLiabilitiesCustom",A54)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="1" operator="containsText" text="acfr:CurrentLiabilitiesCustom">
-      <formula>NOT(ISERROR(SEARCH("acfr:CurrentLiabilitiesCustom",A54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67:A70">
-    <cfRule type="containsText" dxfId="95" priority="11" operator="containsText" text="acfr:NoncurrentLiabilitiesCustom">
-      <formula>NOT(ISERROR(SEARCH("acfr:NoncurrentLiabilitiesCustom",A67)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A80:A83">
-    <cfRule type="containsText" dxfId="94" priority="10" operator="containsText" text="acfr:DeferredInflowsOfResourcesCustom">
-      <formula>NOT(ISERROR(SEARCH("acfr:DeferredInflowsOfResourcesCustom",A80)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A92:A95">
-    <cfRule type="containsText" dxfId="93" priority="9" operator="containsText" text="acfr:RestrictedComponentsOfNetPositionCustom">
-      <formula>NOT(ISERROR(SEARCH("acfr:RestrictedComponentsOfNetPositionCustom",A92)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="M68">
-    <cfRule type="expression" dxfId="92" priority="8">
+    <cfRule type="expression" dxfId="76" priority="8">
       <formula>$A$9:$A$22="acfr:CurrentAssetsCustom"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25:A31">
-    <cfRule type="containsText" dxfId="77" priority="3" operator="containsText" text="acfr:NonCurrentAssetsCustom">
-      <formula>NOT(ISERROR(SEARCH("acfr:NonCurrentAssetsCustom",A25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
@@ -50422,94 +50076,89 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A9:A22">
+    <cfRule type="containsText" dxfId="75" priority="9" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25:A36">
+    <cfRule type="containsText" dxfId="74" priority="8" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:A63">
+    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66:A70">
+    <cfRule type="containsText" dxfId="72" priority="1" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A66)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:B49">
+    <cfRule type="containsText" dxfId="71" priority="3" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C23 C37 C50 D53:G63">
-    <cfRule type="expression" dxfId="150" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="58" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:J64">
-    <cfRule type="expression" dxfId="149" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="43" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:J72">
-    <cfRule type="expression" dxfId="148" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="19" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:F6 D52:F52">
-    <cfRule type="expression" dxfId="147" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="55" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39:G51">
-    <cfRule type="expression" dxfId="146" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="15" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:J70">
-    <cfRule type="expression" dxfId="145" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="11" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D74:J77 I78:I99">
-    <cfRule type="expression" dxfId="144" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="10" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39:H50">
-    <cfRule type="expression" dxfId="143" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="14" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38:I38">
-    <cfRule type="expression" dxfId="142" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="52" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:J6 D7:I37 I39:I51">
-    <cfRule type="expression" dxfId="141" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="48" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52:J63">
-    <cfRule type="expression" dxfId="140" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="12" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:J50">
-    <cfRule type="expression" dxfId="139" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="13" stopIfTrue="1">
       <formula>J$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A22">
-    <cfRule type="containsText" dxfId="70" priority="9" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25:A36">
-    <cfRule type="containsText" dxfId="69" priority="8" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A25)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B41:B49">
-    <cfRule type="containsText" dxfId="68" priority="7" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",B41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:A63">
-    <cfRule type="containsText" dxfId="67" priority="5" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41:A49">
-    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A66:A70">
-    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">

</xml_diff>

<commit_message>
issue 8- made sure there are no extraneous numbers on propfund stmt of rev exp and ch
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarrahahmed/Desktop/CLOSUP/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F55631-3268-B742-933A-242379D4950A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D5C3B0-7AEE-9B4D-92E4-8C882D27E900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17280" tabRatio="834" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17280" tabRatio="834" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Net Position" sheetId="8" r:id="rId1"/>
@@ -12117,6 +12117,9 @@
     <xf numFmtId="0" fontId="32" fillId="5" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -12125,9 +12128,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -12142,21 +12142,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12184,12 +12169,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12204,9 +12186,27 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -19913,18 +19913,18 @@
       </c>
     </row>
     <row r="59" spans="1:10" ht="15">
-      <c r="A59" s="252" t="s">
+      <c r="A59" s="253" t="s">
         <v>3615</v>
       </c>
-      <c r="B59" s="253"/>
-      <c r="C59" s="253"/>
-      <c r="D59" s="253"/>
-      <c r="E59" s="253"/>
-      <c r="F59" s="253"/>
-      <c r="G59" s="253"/>
-      <c r="H59" s="253"/>
-      <c r="I59" s="253"/>
-      <c r="J59" s="254"/>
+      <c r="B59" s="254"/>
+      <c r="C59" s="254"/>
+      <c r="D59" s="254"/>
+      <c r="E59" s="254"/>
+      <c r="F59" s="254"/>
+      <c r="G59" s="254"/>
+      <c r="H59" s="254"/>
+      <c r="I59" s="254"/>
+      <c r="J59" s="255"/>
     </row>
     <row r="60" spans="1:10" ht="15">
       <c r="A60" s="108" t="str">
@@ -19961,18 +19961,18 @@
       </c>
     </row>
     <row r="62" spans="1:10" ht="15">
-      <c r="A62" s="252" t="s">
+      <c r="A62" s="253" t="s">
         <v>3616</v>
       </c>
-      <c r="B62" s="253"/>
-      <c r="C62" s="253"/>
-      <c r="D62" s="253"/>
-      <c r="E62" s="253"/>
-      <c r="F62" s="253"/>
-      <c r="G62" s="253"/>
-      <c r="H62" s="253"/>
-      <c r="I62" s="253"/>
-      <c r="J62" s="254"/>
+      <c r="B62" s="254"/>
+      <c r="C62" s="254"/>
+      <c r="D62" s="254"/>
+      <c r="E62" s="254"/>
+      <c r="F62" s="254"/>
+      <c r="G62" s="254"/>
+      <c r="H62" s="254"/>
+      <c r="I62" s="254"/>
+      <c r="J62" s="255"/>
     </row>
     <row r="63" spans="1:10" ht="15">
       <c r="A63" s="108" t="str">
@@ -20009,18 +20009,18 @@
       </c>
     </row>
     <row r="65" spans="1:10" ht="15">
-      <c r="A65" s="252" t="s">
+      <c r="A65" s="253" t="s">
         <v>3617</v>
       </c>
-      <c r="B65" s="253"/>
-      <c r="C65" s="253"/>
-      <c r="D65" s="253"/>
-      <c r="E65" s="253"/>
-      <c r="F65" s="253"/>
-      <c r="G65" s="253"/>
-      <c r="H65" s="253"/>
-      <c r="I65" s="253"/>
-      <c r="J65" s="254"/>
+      <c r="B65" s="254"/>
+      <c r="C65" s="254"/>
+      <c r="D65" s="254"/>
+      <c r="E65" s="254"/>
+      <c r="F65" s="254"/>
+      <c r="G65" s="254"/>
+      <c r="H65" s="254"/>
+      <c r="I65" s="254"/>
+      <c r="J65" s="255"/>
     </row>
     <row r="66" spans="1:10" ht="16">
       <c r="A66" s="131" t="str">
@@ -20430,8 +20430,8 @@
   </sheetPr>
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="81" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A4" zoomScale="81" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -23773,8 +23773,8 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -26891,17 +26891,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D69:J69">
-    <cfRule type="cellIs" dxfId="8" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="expression" dxfId="8" priority="12" stopIfTrue="1">
+      <formula>D$7=""</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="13" stopIfTrue="1" operator="equal">
       <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="15" operator="notEqual">
-      <formula>#REF!</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="14" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="12" stopIfTrue="1">
-      <formula>D$7=""</formula>
+    <cfRule type="cellIs" dxfId="5" priority="15" operator="notEqual">
+      <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J4 J8:J22 J24:J64 J70:J1048574">
@@ -26915,11 +26915,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J68">
-    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
+      <formula>COUNTA(D69:I69)=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="6" stopIfTrue="1">
       <formula>#REF!=""</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
-      <formula>COUNTA(D69:I69)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1048575:J1048576">
@@ -46728,7 +46728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8474313-8EAC-0141-BA8E-861AF31ED060}">
   <dimension ref="B1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="92" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -46783,7 +46783,7 @@
       <c r="E6" s="2"/>
     </row>
     <row r="10" spans="2:5" ht="14">
-      <c r="B10" s="255" t="s">
+      <c r="B10" s="252" t="s">
         <v>3634</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added footnotes issue 69 ( could not switch issues)
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarrahahmed/Desktop/CLOSUP/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D5C3B0-7AEE-9B4D-92E4-8C882D27E900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934C8AF1-DD68-4144-8232-20177E39C8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17280" tabRatio="834" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" tabRatio="834" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Net Position" sheetId="8" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5367" uniqueCount="3636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5376" uniqueCount="3637">
   <si>
     <t>Statement of Net Position</t>
   </si>
@@ -11001,6 +11001,9 @@
   </si>
   <si>
     <t xml:space="preserve">   - Open the relevant sheets in this Excel file (e.g.,Net Position, PropFunds, Statement of Activities).</t>
+  </si>
+  <si>
+    <t>Note:</t>
   </si>
 </sst>
 </file>
@@ -11326,7 +11329,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -11621,6 +11624,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -11629,7 +11654,7 @@
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="256">
+  <cellXfs count="260">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -12128,6 +12153,18 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -18839,10 +18876,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="119" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="119" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72:B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -20133,11 +20170,22 @@
         <v>0</v>
       </c>
     </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="256" t="s">
+        <v>3636</v>
+      </c>
+      <c r="B72" s="257"/>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="258"/>
+      <c r="B73" s="259"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A59:J59"/>
     <mergeCell ref="A62:J62"/>
     <mergeCell ref="A65:J65"/>
+    <mergeCell ref="A72:B73"/>
   </mergeCells>
   <conditionalFormatting sqref="A9:A18">
     <cfRule type="containsText" dxfId="58" priority="7" operator="containsText" text="custom">
@@ -20248,10 +20296,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A3" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -20418,7 +20466,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="256" t="s">
+        <v>3636</v>
+      </c>
+      <c r="B35" s="257"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="258"/>
+      <c r="B36" s="259"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A35:B36"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -20428,10 +20489,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="81" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView topLeftCell="A17" zoomScale="81" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72:B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -21790,8 +21851,21 @@
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
     </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="256" t="s">
+        <v>3636</v>
+      </c>
+      <c r="B72" s="257"/>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="258"/>
+      <c r="B73" s="259"/>
+    </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="A72:B73"/>
+  </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="A9:A22">
     <cfRule type="containsText" dxfId="47" priority="3" operator="containsText" text="custom">
@@ -21861,10 +21935,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="A29" sqref="A29:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -22005,7 +22079,20 @@
       </c>
       <c r="B26" s="175"/>
     </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="256" t="s">
+        <v>3636</v>
+      </c>
+      <c r="B29" s="257"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="258"/>
+      <c r="B30" s="259"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A29:B30"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -22017,8 +22104,8 @@
   </sheetPr>
   <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A9" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84:B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -23606,9 +23693,15 @@
       <c r="J83" s="112"/>
     </row>
     <row r="84" spans="1:10" ht="15">
+      <c r="A84" s="256" t="s">
+        <v>3636</v>
+      </c>
+      <c r="B84" s="257"/>
       <c r="J84" s="112"/>
     </row>
     <row r="85" spans="1:10" ht="15">
+      <c r="A85" s="258"/>
+      <c r="B85" s="259"/>
       <c r="J85" s="112"/>
     </row>
     <row r="86" spans="1:10" ht="15">
@@ -23685,6 +23778,9 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="A84:B85"/>
+  </mergeCells>
   <conditionalFormatting sqref="A10:A23">
     <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A10)))</formula>
@@ -23773,8 +23869,8 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView topLeftCell="A6" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73:B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -25163,9 +25259,15 @@
       <c r="J72" s="112"/>
     </row>
     <row r="73" spans="1:10" ht="15">
+      <c r="A73" s="256" t="s">
+        <v>3636</v>
+      </c>
+      <c r="B73" s="257"/>
       <c r="J73" s="112"/>
     </row>
     <row r="74" spans="1:10" ht="15">
+      <c r="A74" s="258"/>
+      <c r="B74" s="259"/>
       <c r="J74" s="112"/>
     </row>
     <row r="75" spans="1:10" ht="15">
@@ -25245,6 +25347,9 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="A73:B74"/>
+  </mergeCells>
   <conditionalFormatting sqref="A9:A22">
     <cfRule type="containsText" dxfId="35" priority="4" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
@@ -25343,8 +25448,8 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView topLeftCell="A23" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -26788,8 +26893,10 @@
       <c r="J76" s="138"/>
     </row>
     <row r="77" spans="1:10" ht="15">
-      <c r="A77" s="104"/>
-      <c r="B77" s="154"/>
+      <c r="A77" s="256" t="s">
+        <v>3636</v>
+      </c>
+      <c r="B77" s="257"/>
       <c r="C77" s="155"/>
       <c r="D77" s="155"/>
       <c r="E77" s="155"/>
@@ -26800,8 +26907,8 @@
       <c r="J77" s="138"/>
     </row>
     <row r="78" spans="1:10" ht="15">
-      <c r="A78" s="104"/>
-      <c r="B78" s="154"/>
+      <c r="A78" s="258"/>
+      <c r="B78" s="259"/>
       <c r="C78" s="155"/>
       <c r="D78" s="155"/>
       <c r="E78" s="155"/>
@@ -26823,6 +26930,9 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="A77:B78"/>
+  </mergeCells>
   <conditionalFormatting sqref="A9:A22">
     <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
@@ -26928,7 +27038,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74:B78" xr:uid="{98ECD2C2-C0B9-E74C-B5D0-14A316D496F4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74:B76" xr:uid="{98ECD2C2-C0B9-E74C-B5D0-14A316D496F4}">
       <formula1>net_position</formula1>
     </dataValidation>
   </dataValidations>
@@ -46887,10 +46997,10 @@
   <sheetPr codeName="Sheet8">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="81" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView topLeftCell="A68" zoomScale="81" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104:B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -48288,8 +48398,21 @@
       <c r="C102" s="36"/>
       <c r="D102" s="37"/>
     </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="256" t="s">
+        <v>3636</v>
+      </c>
+      <c r="B104" s="257"/>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="258"/>
+      <c r="B105" s="259"/>
+    </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="A104:B105"/>
+  </mergeCells>
   <conditionalFormatting sqref="A9:A22">
     <cfRule type="expression" dxfId="90" priority="16">
       <formula>A9="acfr:CurrentAssetsCustom"</formula>
@@ -48440,8 +48563,8 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="84" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView topLeftCell="A39" zoomScale="84" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -50015,54 +50138,60 @@
       <c r="I79" s="54"/>
     </row>
     <row r="80" spans="1:10" ht="15">
+      <c r="A80" s="256" t="s">
+        <v>3636</v>
+      </c>
+      <c r="B80" s="257"/>
       <c r="I80" s="54"/>
     </row>
-    <row r="81" spans="9:9" ht="15">
+    <row r="81" spans="1:9" ht="15">
+      <c r="A81" s="258"/>
+      <c r="B81" s="259"/>
       <c r="I81" s="54"/>
     </row>
-    <row r="82" spans="9:9" ht="15">
+    <row r="82" spans="1:9" ht="15">
       <c r="I82" s="54"/>
     </row>
-    <row r="83" spans="9:9" ht="15">
+    <row r="83" spans="1:9" ht="15">
       <c r="I83" s="54"/>
     </row>
-    <row r="84" spans="9:9" ht="15">
+    <row r="84" spans="1:9" ht="15">
       <c r="I84" s="54"/>
     </row>
-    <row r="85" spans="9:9" ht="15">
+    <row r="85" spans="1:9" ht="15">
       <c r="I85" s="54"/>
     </row>
-    <row r="86" spans="9:9" ht="15">
+    <row r="86" spans="1:9" ht="15">
       <c r="I86" s="54"/>
     </row>
-    <row r="87" spans="9:9" ht="15">
+    <row r="87" spans="1:9" ht="15">
       <c r="I87" s="54"/>
     </row>
-    <row r="88" spans="9:9" ht="15">
+    <row r="88" spans="1:9" ht="15">
       <c r="I88" s="54"/>
     </row>
-    <row r="89" spans="9:9" ht="14">
+    <row r="89" spans="1:9" ht="14">
       <c r="I89" s="20"/>
     </row>
-    <row r="90" spans="9:9" ht="15">
+    <row r="90" spans="1:9" ht="15">
       <c r="I90" s="53"/>
     </row>
-    <row r="91" spans="9:9" ht="15">
+    <row r="91" spans="1:9" ht="15">
       <c r="I91" s="54"/>
     </row>
-    <row r="92" spans="9:9" ht="15">
+    <row r="92" spans="1:9" ht="15">
       <c r="I92" s="54"/>
     </row>
-    <row r="93" spans="9:9" ht="15">
+    <row r="93" spans="1:9" ht="15">
       <c r="I93" s="54"/>
     </row>
-    <row r="94" spans="9:9" ht="15">
+    <row r="94" spans="1:9" ht="15">
       <c r="I94" s="54"/>
     </row>
-    <row r="95" spans="9:9" ht="15">
+    <row r="95" spans="1:9" ht="15">
       <c r="I95" s="54"/>
     </row>
-    <row r="96" spans="9:9" ht="15">
+    <row r="96" spans="1:9" ht="15">
       <c r="I96" s="54"/>
     </row>
     <row r="97" spans="9:9" ht="15">
@@ -50076,6 +50205,9 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="A80:B81"/>
+  </mergeCells>
   <conditionalFormatting sqref="A9:A22">
     <cfRule type="containsText" dxfId="75" priority="9" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>

</xml_diff>

<commit_message>
replaced file with Sarrah upload
refer to https://github.com/closup/process-xbrl/pull/95/commits/ab16b5a33a772042b5aa55fea57e1f8913126bb7
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarrahahmed/Desktop/CLOSUP/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D5C3B0-7AEE-9B4D-92E4-8C882D27E900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F63CED0-37A6-DE43-B209-0B12063A4F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17280" tabRatio="834" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17260" tabRatio="834" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Net Position" sheetId="8" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5367" uniqueCount="3636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5378" uniqueCount="3638">
   <si>
     <t>Statement of Net Position</t>
   </si>
@@ -11001,6 +11001,12 @@
   </si>
   <si>
     <t xml:space="preserve">   - Open the relevant sheets in this Excel file (e.g.,Net Position, PropFunds, Statement of Activities).</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -Select "Choose file(s))" on the Inline XBRL Conversion Tool Website. You will select the excel sheet, and can also upload 0-5 word documents which may include content such as auditors letters, notes, or other text. Once you have selected files, you can adjust their ordering. Then, simply select "combine and convert files". Please be patient, the conversion may take up to one minute or possibly more, depending on the number of files being uploaded. </t>
   </si>
 </sst>
 </file>
@@ -11012,7 +11018,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="34">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -11215,6 +11221,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="19">
     <fill>
@@ -11326,7 +11338,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -11621,6 +11633,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -11629,7 +11676,7 @@
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="256">
+  <cellXfs count="273">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -12120,6 +12167,41 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -12128,6 +12210,18 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -12142,6 +12236,21 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12169,9 +12278,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12186,27 +12298,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -18839,10 +18933,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="119" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView topLeftCell="A47" zoomScale="119" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -19913,18 +20007,18 @@
       </c>
     </row>
     <row r="59" spans="1:10" ht="15">
-      <c r="A59" s="253" t="s">
+      <c r="A59" s="266" t="s">
         <v>3615</v>
       </c>
-      <c r="B59" s="254"/>
-      <c r="C59" s="254"/>
-      <c r="D59" s="254"/>
-      <c r="E59" s="254"/>
-      <c r="F59" s="254"/>
-      <c r="G59" s="254"/>
-      <c r="H59" s="254"/>
-      <c r="I59" s="254"/>
-      <c r="J59" s="255"/>
+      <c r="B59" s="267"/>
+      <c r="C59" s="267"/>
+      <c r="D59" s="267"/>
+      <c r="E59" s="267"/>
+      <c r="F59" s="267"/>
+      <c r="G59" s="267"/>
+      <c r="H59" s="267"/>
+      <c r="I59" s="267"/>
+      <c r="J59" s="268"/>
     </row>
     <row r="60" spans="1:10" ht="15">
       <c r="A60" s="108" t="str">
@@ -19961,18 +20055,18 @@
       </c>
     </row>
     <row r="62" spans="1:10" ht="15">
-      <c r="A62" s="253" t="s">
+      <c r="A62" s="266" t="s">
         <v>3616</v>
       </c>
-      <c r="B62" s="254"/>
-      <c r="C62" s="254"/>
-      <c r="D62" s="254"/>
-      <c r="E62" s="254"/>
-      <c r="F62" s="254"/>
-      <c r="G62" s="254"/>
-      <c r="H62" s="254"/>
-      <c r="I62" s="254"/>
-      <c r="J62" s="255"/>
+      <c r="B62" s="267"/>
+      <c r="C62" s="267"/>
+      <c r="D62" s="267"/>
+      <c r="E62" s="267"/>
+      <c r="F62" s="267"/>
+      <c r="G62" s="267"/>
+      <c r="H62" s="267"/>
+      <c r="I62" s="267"/>
+      <c r="J62" s="268"/>
     </row>
     <row r="63" spans="1:10" ht="15">
       <c r="A63" s="108" t="str">
@@ -20009,18 +20103,18 @@
       </c>
     </row>
     <row r="65" spans="1:10" ht="15">
-      <c r="A65" s="253" t="s">
+      <c r="A65" s="266" t="s">
         <v>3617</v>
       </c>
-      <c r="B65" s="254"/>
-      <c r="C65" s="254"/>
-      <c r="D65" s="254"/>
-      <c r="E65" s="254"/>
-      <c r="F65" s="254"/>
-      <c r="G65" s="254"/>
-      <c r="H65" s="254"/>
-      <c r="I65" s="254"/>
-      <c r="J65" s="255"/>
+      <c r="B65" s="267"/>
+      <c r="C65" s="267"/>
+      <c r="D65" s="267"/>
+      <c r="E65" s="267"/>
+      <c r="F65" s="267"/>
+      <c r="G65" s="267"/>
+      <c r="H65" s="267"/>
+      <c r="I65" s="267"/>
+      <c r="J65" s="268"/>
     </row>
     <row r="66" spans="1:10" ht="16">
       <c r="A66" s="131" t="str">
@@ -20133,11 +20227,22 @@
         <v>0</v>
       </c>
     </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="258"/>
+      <c r="B72" s="264" t="s">
+        <v>3636</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="258"/>
+      <c r="B73" s="265"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A59:J59"/>
     <mergeCell ref="A62:J62"/>
     <mergeCell ref="A65:J65"/>
+    <mergeCell ref="B72:B73"/>
   </mergeCells>
   <conditionalFormatting sqref="A9:A18">
     <cfRule type="containsText" dxfId="58" priority="7" operator="containsText" text="custom">
@@ -20248,10 +20353,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A3" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -20418,7 +20523,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="269" t="s">
+        <v>3636</v>
+      </c>
+      <c r="B35" s="264"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="270"/>
+      <c r="B36" s="265"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A35:B36"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -20428,10 +20546,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="81" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView topLeftCell="A23" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -21789,6 +21907,16 @@
       <c r="H71" s="20"/>
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="255"/>
+      <c r="B72" s="253" t="s">
+        <v>3636</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="255"/>
+      <c r="B73" s="254"/>
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
@@ -21861,10 +21989,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -22005,7 +22133,20 @@
       </c>
       <c r="B26" s="175"/>
     </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="269" t="s">
+        <v>3636</v>
+      </c>
+      <c r="B29" s="264"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="270"/>
+      <c r="B30" s="265"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A29:B30"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -22017,8 +22158,8 @@
   </sheetPr>
   <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A83" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M65" sqref="M65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -22864,9 +23005,11 @@
     <row r="45" spans="1:10" ht="15">
       <c r="A45" s="108" t="str">
         <f>IF(B45="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B45)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B45,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B45" s="109"/>
+        <v>acfr:DueToComponentUnit</v>
+      </c>
+      <c r="B45" s="109" t="s">
+        <v>281</v>
+      </c>
       <c r="C45" s="208"/>
       <c r="D45" s="208"/>
       <c r="E45" s="208"/>
@@ -23606,9 +23749,15 @@
       <c r="J83" s="112"/>
     </row>
     <row r="84" spans="1:10" ht="15">
+      <c r="A84" s="257"/>
+      <c r="B84" s="262" t="s">
+        <v>3636</v>
+      </c>
       <c r="J84" s="112"/>
     </row>
     <row r="85" spans="1:10" ht="15">
+      <c r="A85" s="257"/>
+      <c r="B85" s="263"/>
       <c r="J85" s="112"/>
     </row>
     <row r="86" spans="1:10" ht="15">
@@ -23685,6 +23834,9 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="B84:B85"/>
+  </mergeCells>
   <conditionalFormatting sqref="A10:A23">
     <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A10)))</formula>
@@ -23773,8 +23925,8 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView topLeftCell="A14" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -25163,9 +25315,15 @@
       <c r="J72" s="112"/>
     </row>
     <row r="73" spans="1:10" ht="15">
+      <c r="A73" s="259"/>
+      <c r="B73" s="271" t="s">
+        <v>3636</v>
+      </c>
       <c r="J73" s="112"/>
     </row>
     <row r="74" spans="1:10" ht="15">
+      <c r="A74" s="259"/>
+      <c r="B74" s="272"/>
       <c r="J74" s="112"/>
     </row>
     <row r="75" spans="1:10" ht="15">
@@ -25245,6 +25403,9 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="B73:B74"/>
+  </mergeCells>
   <conditionalFormatting sqref="A9:A22">
     <cfRule type="containsText" dxfId="35" priority="4" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
@@ -25343,8 +25504,8 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -26788,8 +26949,10 @@
       <c r="J76" s="138"/>
     </row>
     <row r="77" spans="1:10" ht="15">
-      <c r="A77" s="104"/>
-      <c r="B77" s="154"/>
+      <c r="A77" s="257"/>
+      <c r="B77" s="262" t="s">
+        <v>3636</v>
+      </c>
       <c r="C77" s="155"/>
       <c r="D77" s="155"/>
       <c r="E77" s="155"/>
@@ -26800,8 +26963,8 @@
       <c r="J77" s="138"/>
     </row>
     <row r="78" spans="1:10" ht="15">
-      <c r="A78" s="104"/>
-      <c r="B78" s="154"/>
+      <c r="A78" s="257"/>
+      <c r="B78" s="263"/>
       <c r="C78" s="155"/>
       <c r="D78" s="155"/>
       <c r="E78" s="155"/>
@@ -26823,6 +26986,9 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="B77:B78"/>
+  </mergeCells>
   <conditionalFormatting sqref="A9:A22">
     <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
@@ -26891,17 +27057,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D69:J69">
-    <cfRule type="expression" dxfId="8" priority="12" stopIfTrue="1">
-      <formula>D$7=""</formula>
+    <cfRule type="cellIs" dxfId="8" priority="13" stopIfTrue="1" operator="equal">
+      <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="13" stopIfTrue="1" operator="equal">
-      <formula>0</formula>
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="notEqual">
+      <formula>#REF!</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="14" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="15" operator="notEqual">
-      <formula>#REF!</formula>
+    <cfRule type="expression" dxfId="5" priority="12" stopIfTrue="1">
+      <formula>D$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J4 J8:J22 J24:J64 J70:J1048574">
@@ -26915,11 +27081,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J68">
-    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
+      <formula>#REF!=""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>COUNTA(D69:I69)=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="6" stopIfTrue="1">
-      <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1048575:J1048576">
@@ -26928,7 +27094,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74:B78" xr:uid="{98ECD2C2-C0B9-E74C-B5D0-14A316D496F4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74:B76" xr:uid="{98ECD2C2-C0B9-E74C-B5D0-14A316D496F4}">
       <formula1>net_position</formula1>
     </dataValidation>
   </dataValidations>
@@ -46726,10 +46892,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8474313-8EAC-0141-BA8E-861AF31ED060}">
-  <dimension ref="B1:E32"/>
+  <dimension ref="B1:E40"/>
   <sheetViews>
     <sheetView zoomScale="92" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -46857,20 +47023,28 @@
         <v>3630</v>
       </c>
     </row>
-    <row r="30" spans="2:2">
-      <c r="B30" t="s">
-        <v>3631</v>
+    <row r="29" spans="2:2">
+      <c r="B29" s="261" t="s">
+        <v>3637</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" t="s">
-        <v>3632</v>
+        <v>3631</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" t="s">
+        <v>3632</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
         <v>3633</v>
       </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="260"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -46887,10 +47061,10 @@
   <sheetPr codeName="Sheet8">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="81" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView topLeftCell="A59" zoomScale="81" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -48288,8 +48462,24 @@
       <c r="C102" s="36"/>
       <c r="D102" s="37"/>
     </row>
+    <row r="103" spans="1:6">
+      <c r="B103" s="256"/>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="257"/>
+      <c r="B104" s="262" t="s">
+        <v>3636</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="257"/>
+      <c r="B105" s="263"/>
+    </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="B104:B105"/>
+  </mergeCells>
   <conditionalFormatting sqref="A9:A22">
     <cfRule type="expression" dxfId="90" priority="16">
       <formula>A9="acfr:CurrentAssetsCustom"</formula>
@@ -48440,8 +48630,8 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="84" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView topLeftCell="A44" zoomScale="84" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -50015,54 +50205,60 @@
       <c r="I79" s="54"/>
     </row>
     <row r="80" spans="1:10" ht="15">
+      <c r="A80" s="257"/>
+      <c r="B80" s="264" t="s">
+        <v>3636</v>
+      </c>
       <c r="I80" s="54"/>
     </row>
-    <row r="81" spans="9:9" ht="15">
+    <row r="81" spans="1:9" ht="15">
+      <c r="A81" s="257"/>
+      <c r="B81" s="265"/>
       <c r="I81" s="54"/>
     </row>
-    <row r="82" spans="9:9" ht="15">
+    <row r="82" spans="1:9" ht="15">
       <c r="I82" s="54"/>
     </row>
-    <row r="83" spans="9:9" ht="15">
+    <row r="83" spans="1:9" ht="15">
       <c r="I83" s="54"/>
     </row>
-    <row r="84" spans="9:9" ht="15">
+    <row r="84" spans="1:9" ht="15">
       <c r="I84" s="54"/>
     </row>
-    <row r="85" spans="9:9" ht="15">
+    <row r="85" spans="1:9" ht="15">
       <c r="I85" s="54"/>
     </row>
-    <row r="86" spans="9:9" ht="15">
+    <row r="86" spans="1:9" ht="15">
       <c r="I86" s="54"/>
     </row>
-    <row r="87" spans="9:9" ht="15">
+    <row r="87" spans="1:9" ht="15">
       <c r="I87" s="54"/>
     </row>
-    <row r="88" spans="9:9" ht="15">
+    <row r="88" spans="1:9" ht="15">
       <c r="I88" s="54"/>
     </row>
-    <row r="89" spans="9:9" ht="14">
+    <row r="89" spans="1:9" ht="14">
       <c r="I89" s="20"/>
     </row>
-    <row r="90" spans="9:9" ht="15">
+    <row r="90" spans="1:9" ht="15">
       <c r="I90" s="53"/>
     </row>
-    <row r="91" spans="9:9" ht="15">
+    <row r="91" spans="1:9" ht="15">
       <c r="I91" s="54"/>
     </row>
-    <row r="92" spans="9:9" ht="15">
+    <row r="92" spans="1:9" ht="15">
       <c r="I92" s="54"/>
     </row>
-    <row r="93" spans="9:9" ht="15">
+    <row r="93" spans="1:9" ht="15">
       <c r="I93" s="54"/>
     </row>
-    <row r="94" spans="9:9" ht="15">
+    <row r="94" spans="1:9" ht="15">
       <c r="I94" s="54"/>
     </row>
-    <row r="95" spans="9:9" ht="15">
+    <row r="95" spans="1:9" ht="15">
       <c r="I95" s="54"/>
     </row>
-    <row r="96" spans="9:9" ht="15">
+    <row r="96" spans="1:9" ht="15">
       <c r="I96" s="54"/>
     </row>
     <row r="97" spans="9:9" ht="15">
@@ -50076,6 +50272,9 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="B80:B81"/>
+  </mergeCells>
   <conditionalFormatting sqref="A9:A22">
     <cfRule type="containsText" dxfId="75" priority="9" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>

</xml_diff>

<commit_message>
Addressed Propfunds Net Position issues
I added deferred outflows and inflows, modeling it after our statement of net position.
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarrahahmed/Desktop/CLOSUP/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D5C3B0-7AEE-9B4D-92E4-8C882D27E900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4EB1D5-2CFE-5745-8763-EB70F93AE294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17280" tabRatio="834" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17260" tabRatio="834" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Net Position" sheetId="8" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5367" uniqueCount="3636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5383" uniqueCount="3638">
   <si>
     <t>Statement of Net Position</t>
   </si>
@@ -11001,6 +11001,12 @@
   </si>
   <si>
     <t xml:space="preserve">   - Open the relevant sheets in this Excel file (e.g.,Net Position, PropFunds, Statement of Activities).</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -Select "Choose file(s))" on the Inline XBRL Conversion Tool Website. You will select the excel sheet, and can also upload 0-5 word documents which may include content such as auditors letters, notes, or other text. Once you have selected files, you can adjust their ordering. Then, simply select "combine and convert files". Please be patient, the conversion may take up to one minute or possibly more, depending on the number of files being uploaded. </t>
   </si>
 </sst>
 </file>
@@ -11012,7 +11018,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="34">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -11215,6 +11221,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="19">
     <fill>
@@ -11326,7 +11338,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -11621,6 +11633,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -11629,7 +11676,7 @@
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="256">
+  <cellXfs count="273">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -12120,6 +12167,41 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -12129,6 +12211,18 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -12137,7 +12231,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
   </cellStyles>
-  <dxfs count="91">
+  <dxfs count="95">
     <dxf>
       <fill>
         <patternFill>
@@ -12414,6 +12508,36 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -13159,8 +13283,8 @@
   </sheetPr>
   <dimension ref="A1:C514"/>
   <sheetViews>
-    <sheetView topLeftCell="A202" zoomScale="75" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A295" zoomScale="75" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A316" sqref="A316:C354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -18839,10 +18963,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="119" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView topLeftCell="A47" zoomScale="119" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -19913,18 +20037,18 @@
       </c>
     </row>
     <row r="59" spans="1:10" ht="15">
-      <c r="A59" s="253" t="s">
+      <c r="A59" s="266" t="s">
         <v>3615</v>
       </c>
-      <c r="B59" s="254"/>
-      <c r="C59" s="254"/>
-      <c r="D59" s="254"/>
-      <c r="E59" s="254"/>
-      <c r="F59" s="254"/>
-      <c r="G59" s="254"/>
-      <c r="H59" s="254"/>
-      <c r="I59" s="254"/>
-      <c r="J59" s="255"/>
+      <c r="B59" s="267"/>
+      <c r="C59" s="267"/>
+      <c r="D59" s="267"/>
+      <c r="E59" s="267"/>
+      <c r="F59" s="267"/>
+      <c r="G59" s="267"/>
+      <c r="H59" s="267"/>
+      <c r="I59" s="267"/>
+      <c r="J59" s="268"/>
     </row>
     <row r="60" spans="1:10" ht="15">
       <c r="A60" s="108" t="str">
@@ -19961,18 +20085,18 @@
       </c>
     </row>
     <row r="62" spans="1:10" ht="15">
-      <c r="A62" s="253" t="s">
+      <c r="A62" s="266" t="s">
         <v>3616</v>
       </c>
-      <c r="B62" s="254"/>
-      <c r="C62" s="254"/>
-      <c r="D62" s="254"/>
-      <c r="E62" s="254"/>
-      <c r="F62" s="254"/>
-      <c r="G62" s="254"/>
-      <c r="H62" s="254"/>
-      <c r="I62" s="254"/>
-      <c r="J62" s="255"/>
+      <c r="B62" s="267"/>
+      <c r="C62" s="267"/>
+      <c r="D62" s="267"/>
+      <c r="E62" s="267"/>
+      <c r="F62" s="267"/>
+      <c r="G62" s="267"/>
+      <c r="H62" s="267"/>
+      <c r="I62" s="267"/>
+      <c r="J62" s="268"/>
     </row>
     <row r="63" spans="1:10" ht="15">
       <c r="A63" s="108" t="str">
@@ -20009,18 +20133,18 @@
       </c>
     </row>
     <row r="65" spans="1:10" ht="15">
-      <c r="A65" s="253" t="s">
+      <c r="A65" s="266" t="s">
         <v>3617</v>
       </c>
-      <c r="B65" s="254"/>
-      <c r="C65" s="254"/>
-      <c r="D65" s="254"/>
-      <c r="E65" s="254"/>
-      <c r="F65" s="254"/>
-      <c r="G65" s="254"/>
-      <c r="H65" s="254"/>
-      <c r="I65" s="254"/>
-      <c r="J65" s="255"/>
+      <c r="B65" s="267"/>
+      <c r="C65" s="267"/>
+      <c r="D65" s="267"/>
+      <c r="E65" s="267"/>
+      <c r="F65" s="267"/>
+      <c r="G65" s="267"/>
+      <c r="H65" s="267"/>
+      <c r="I65" s="267"/>
+      <c r="J65" s="268"/>
     </row>
     <row r="66" spans="1:10" ht="16">
       <c r="A66" s="131" t="str">
@@ -20133,64 +20257,75 @@
         <v>0</v>
       </c>
     </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="258"/>
+      <c r="B72" s="264" t="s">
+        <v>3636</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="258"/>
+      <c r="B73" s="265"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A59:J59"/>
     <mergeCell ref="A62:J62"/>
     <mergeCell ref="A65:J65"/>
+    <mergeCell ref="B72:B73"/>
   </mergeCells>
   <conditionalFormatting sqref="A9:A18">
-    <cfRule type="containsText" dxfId="58" priority="7" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="62" priority="7" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:A31">
-    <cfRule type="containsText" dxfId="57" priority="6" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="61" priority="6" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:A44">
-    <cfRule type="containsText" dxfId="56" priority="5" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="60" priority="5" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:A58">
-    <cfRule type="containsText" dxfId="55" priority="4" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="59" priority="4" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:A61">
-    <cfRule type="containsText" dxfId="54" priority="3" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="58" priority="3" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:A64">
-    <cfRule type="containsText" dxfId="53" priority="2" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="57" priority="2" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66:A67">
-    <cfRule type="containsText" dxfId="52" priority="1" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="56" priority="1" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:G18 D21:G31 C32:I33 D35:G44 C45:I46 D48:G58 D60:G61 D63:G64 C68:G68">
-    <cfRule type="expression" dxfId="51" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="10" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D66:G67">
-    <cfRule type="expression" dxfId="50" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="8" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:I7">
-    <cfRule type="expression" dxfId="49" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="9" stopIfTrue="1">
       <formula>D$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J45:J46">
-    <cfRule type="expression" dxfId="48" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="11" stopIfTrue="1">
       <formula>I$6=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20248,10 +20383,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A3" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -20418,7 +20553,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="269" t="s">
+        <v>3636</v>
+      </c>
+      <c r="B35" s="264"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="270"/>
+      <c r="B36" s="265"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A35:B36"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -20428,10 +20576,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="81" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView topLeftCell="A23" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -21790,26 +21938,36 @@
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
     </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="255"/>
+      <c r="B72" s="253" t="s">
+        <v>3636</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="255"/>
+      <c r="B73" s="254"/>
+    </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="A9:A22">
-    <cfRule type="containsText" dxfId="47" priority="3" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:A34">
-    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="50" priority="2" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:A53">
-    <cfRule type="containsText" dxfId="45" priority="1" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="49" priority="1" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:I7 D8:J23 C23 D25:J35 C35 C36:J36 D37:J63 C59:J60 J64 D65:J69 D71:J71">
-    <cfRule type="expression" dxfId="44" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="20" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21861,10 +22019,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -22005,7 +22163,20 @@
       </c>
       <c r="B26" s="175"/>
     </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="269" t="s">
+        <v>3636</v>
+      </c>
+      <c r="B29" s="264"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="270"/>
+      <c r="B30" s="265"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A29:B30"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -22015,15 +22186,15 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:K109"/>
+  <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="84" customWidth="1"/>
+    <col min="1" max="1" width="33.83203125" style="84" customWidth="1"/>
     <col min="2" max="2" width="41.5" style="84" customWidth="1"/>
     <col min="3" max="10" width="18.6640625" style="84" customWidth="1"/>
     <col min="11" max="16384" width="9" style="84"/>
@@ -22399,7 +22570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15" hidden="1">
+    <row r="22" spans="1:10" ht="16" hidden="1">
       <c r="A22" s="108" t="str">
         <f>IF(B22="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B22)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B22,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
@@ -22669,7 +22840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15" hidden="1">
+    <row r="36" spans="1:10" ht="36" hidden="1">
       <c r="A36" s="108" t="str">
         <f>IF(B36="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B36)=0,"acfr:NoncurrentAssetsCustom",_xlfn.XLOOKUP(B36,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
@@ -22757,27 +22928,27 @@
         <v>0</v>
       </c>
       <c r="D39" s="232" t="str">
-        <f t="shared" ref="D39:I39" si="5">IF(D$7="Type fund name","",D24+D38)</f>
+        <f>IF(D$7="Type fund name","",D24+D38)</f>
         <v/>
       </c>
       <c r="E39" s="232" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(E$7="Type fund name","",E24+E38)</f>
         <v/>
       </c>
       <c r="F39" s="232" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(F$7="Type fund name","",F24+F38)</f>
         <v/>
       </c>
       <c r="G39" s="232" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(G$7="Type fund name","",G24+G38)</f>
         <v/>
       </c>
       <c r="H39" s="232" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(H$7="Type fund name","",H24+H38)</f>
         <v/>
       </c>
       <c r="I39" s="232" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(I$7="Type fund name","",I24+I38)</f>
         <v/>
       </c>
       <c r="J39" s="219">
@@ -22799,8 +22970,8 @@
     </row>
     <row r="41" spans="1:10" ht="15">
       <c r="A41" s="104"/>
-      <c r="B41" s="105" t="s">
-        <v>25</v>
+      <c r="B41" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="C41" s="105"/>
       <c r="D41" s="105"/>
@@ -22812,58 +22983,62 @@
       <c r="J41" s="105"/>
     </row>
     <row r="42" spans="1:10" ht="15">
-      <c r="A42" s="104"/>
-      <c r="B42" s="107" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C42" s="96"/>
-      <c r="D42" s="96"/>
-      <c r="E42" s="96"/>
-      <c r="F42" s="96"/>
-      <c r="G42" s="96"/>
-      <c r="H42" s="96"/>
-      <c r="I42" s="96"/>
-      <c r="J42" s="113"/>
+      <c r="A42" s="108" t="str">
+        <f>IF(B42="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B42)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B42,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B42" s="109"/>
+      <c r="C42" s="208"/>
+      <c r="D42" s="208"/>
+      <c r="E42" s="208"/>
+      <c r="F42" s="208"/>
+      <c r="G42" s="208"/>
+      <c r="H42" s="208"/>
+      <c r="I42" s="208"/>
+      <c r="J42" s="231">
+        <f t="shared" ref="J42:J53" si="5">IF(J$7="","",SUM(D42:I42))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:10" ht="15">
       <c r="A43" s="108" t="str">
-        <f>IF(B43="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B43)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B43,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B43="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B43)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B43,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B43" s="109"/>
-      <c r="C43" s="208"/>
-      <c r="D43" s="208"/>
-      <c r="E43" s="208"/>
-      <c r="F43" s="208"/>
-      <c r="G43" s="208"/>
-      <c r="H43" s="208"/>
-      <c r="I43" s="208"/>
+      <c r="C43" s="209"/>
+      <c r="D43" s="209"/>
+      <c r="E43" s="209"/>
+      <c r="F43" s="209"/>
+      <c r="G43" s="209"/>
+      <c r="H43" s="209"/>
+      <c r="I43" s="209"/>
       <c r="J43" s="231">
-        <f t="shared" ref="J43:J54" si="6">IF(J$7="","",SUM(D43:I43))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15">
       <c r="A44" s="108" t="str">
-        <f>IF(B44="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B44)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B44,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B44="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B44)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B44,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B44" s="109"/>
-      <c r="C44" s="209"/>
-      <c r="D44" s="209"/>
-      <c r="E44" s="209"/>
-      <c r="F44" s="209"/>
-      <c r="G44" s="209"/>
-      <c r="H44" s="209"/>
-      <c r="I44" s="209"/>
+      <c r="C44" s="208"/>
+      <c r="D44" s="208"/>
+      <c r="E44" s="208"/>
+      <c r="F44" s="208"/>
+      <c r="G44" s="208"/>
+      <c r="H44" s="208"/>
+      <c r="I44" s="208"/>
       <c r="J44" s="231">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15">
       <c r="A45" s="108" t="str">
-        <f>IF(B45="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B45)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B45,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B45="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B45)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B45,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B45" s="109"/>
@@ -22875,13 +23050,13 @@
       <c r="H45" s="208"/>
       <c r="I45" s="208"/>
       <c r="J45" s="231">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="16" customHeight="1">
       <c r="A46" s="108" t="str">
-        <f>IF(B46="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B46)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B46,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B46="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B46)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B46,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B46" s="109"/>
@@ -22893,13 +23068,13 @@
       <c r="H46" s="208"/>
       <c r="I46" s="208"/>
       <c r="J46" s="231">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="16" customHeight="1">
       <c r="A47" s="108" t="str">
-        <f>IF(B47="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B47)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B47,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B47="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B47)=0,"acfr:DeferredOutflowsOfResourcesCustom",_xlfn.XLOOKUP(B47,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B47" s="109"/>
@@ -22911,7 +23086,7 @@
       <c r="H47" s="208"/>
       <c r="I47" s="208"/>
       <c r="J47" s="231">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -22929,7 +23104,7 @@
       <c r="H48" s="208"/>
       <c r="I48" s="208"/>
       <c r="J48" s="231">
-        <f t="shared" ref="J48:J53" si="7">IF(J$7="","",SUM(D48:I48))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -22947,7 +23122,7 @@
       <c r="H49" s="208"/>
       <c r="I49" s="208"/>
       <c r="J49" s="231">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -22965,7 +23140,7 @@
       <c r="H50" s="208"/>
       <c r="I50" s="208"/>
       <c r="J50" s="231">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -22983,7 +23158,7 @@
       <c r="H51" s="208"/>
       <c r="I51" s="208"/>
       <c r="J51" s="231">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -23001,103 +23176,93 @@
       <c r="H52" s="208"/>
       <c r="I52" s="208"/>
       <c r="J52" s="231">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="15">
-      <c r="A53" s="108" t="str">
-        <f>IF(B53="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B53)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B53,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B53" s="109"/>
-      <c r="C53" s="208"/>
-      <c r="D53" s="208"/>
-      <c r="E53" s="208"/>
-      <c r="F53" s="208"/>
-      <c r="G53" s="208"/>
-      <c r="H53" s="208"/>
-      <c r="I53" s="208"/>
+      <c r="A53" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" s="231">
+        <f>IF(C$7="","",SUM(C42:C52))</f>
+        <v>0</v>
+      </c>
+      <c r="D53" s="231" t="str">
+        <f t="shared" ref="D53:I53" si="6">IF(D$7="Type fund name","",SUM(D42:D52))</f>
+        <v/>
+      </c>
+      <c r="E53" s="231" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="F53" s="231" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="G53" s="231" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H53" s="231" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I53" s="231" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
       <c r="J53" s="231">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15">
-      <c r="A54" s="108" t="s">
-        <v>32</v>
-      </c>
-      <c r="B54" s="108" t="s">
-        <v>33</v>
-      </c>
-      <c r="C54" s="231">
-        <f>IF(C$7="","",SUM(C43:C53))</f>
-        <v>0</v>
-      </c>
-      <c r="D54" s="231" t="str">
-        <f t="shared" ref="D54:I54" si="8">IF(D$7="Type fund name","",SUM(D43:D53))</f>
-        <v/>
-      </c>
-      <c r="E54" s="231" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="F54" s="231" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="G54" s="231" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="H54" s="231" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="I54" s="231" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="J54" s="231">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
+      <c r="A54" s="104"/>
+      <c r="B54" s="104"/>
+      <c r="C54" s="112"/>
+      <c r="D54" s="112"/>
+      <c r="E54" s="112"/>
+      <c r="F54" s="112"/>
+      <c r="G54" s="112"/>
+      <c r="H54" s="112"/>
+      <c r="I54" s="112"/>
+      <c r="J54" s="112"/>
     </row>
     <row r="55" spans="1:10" ht="15">
       <c r="A55" s="104"/>
-      <c r="B55" s="107" t="s">
-        <v>1065</v>
-      </c>
-      <c r="C55" s="107"/>
-      <c r="D55" s="107"/>
-      <c r="E55" s="107"/>
-      <c r="F55" s="107"/>
-      <c r="G55" s="107"/>
-      <c r="H55" s="107"/>
-      <c r="I55" s="107"/>
-      <c r="J55" s="96"/>
+      <c r="B55" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55" s="105"/>
+      <c r="D55" s="105"/>
+      <c r="E55" s="105"/>
+      <c r="F55" s="105"/>
+      <c r="G55" s="105"/>
+      <c r="H55" s="105"/>
+      <c r="I55" s="105"/>
+      <c r="J55" s="105"/>
     </row>
     <row r="56" spans="1:10" ht="15">
-      <c r="A56" s="108" t="str">
-        <f>IF(B56="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B56)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B56,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B56" s="109"/>
-      <c r="C56" s="208"/>
-      <c r="D56" s="208"/>
-      <c r="E56" s="208"/>
-      <c r="F56" s="208"/>
-      <c r="G56" s="208"/>
-      <c r="H56" s="208"/>
-      <c r="I56" s="208"/>
-      <c r="J56" s="231">
-        <f t="shared" ref="J56:J69" si="9">IF(J$7="","",SUM(D56:I56))</f>
-        <v>0</v>
-      </c>
+      <c r="A56" s="104"/>
+      <c r="B56" s="107" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C56" s="96"/>
+      <c r="D56" s="96"/>
+      <c r="E56" s="96"/>
+      <c r="F56" s="96"/>
+      <c r="G56" s="96"/>
+      <c r="H56" s="96"/>
+      <c r="I56" s="96"/>
+      <c r="J56" s="113"/>
     </row>
     <row r="57" spans="1:10" ht="15">
       <c r="A57" s="108" t="str">
-        <f>IF(B57="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B57)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B57,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B57="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B57)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B57,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B57" s="109"/>
@@ -23109,31 +23274,31 @@
       <c r="H57" s="208"/>
       <c r="I57" s="208"/>
       <c r="J57" s="231">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="J57:J68" si="7">IF(J$7="","",SUM(D57:I57))</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="15">
       <c r="A58" s="108" t="str">
-        <f>IF(B58="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B58)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B58,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B58="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B58)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B58,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B58" s="109"/>
-      <c r="C58" s="208"/>
-      <c r="D58" s="208"/>
-      <c r="E58" s="208"/>
-      <c r="F58" s="208"/>
-      <c r="G58" s="208"/>
-      <c r="H58" s="208"/>
-      <c r="I58" s="208"/>
+      <c r="C58" s="209"/>
+      <c r="D58" s="209"/>
+      <c r="E58" s="209"/>
+      <c r="F58" s="209"/>
+      <c r="G58" s="209"/>
+      <c r="H58" s="209"/>
+      <c r="I58" s="209"/>
       <c r="J58" s="231">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="15" hidden="1">
       <c r="A59" s="108" t="str">
-        <f>IF(B59="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B59)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B59,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B59="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B59)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B59,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B59" s="109"/>
@@ -23145,13 +23310,13 @@
       <c r="H59" s="208"/>
       <c r="I59" s="208"/>
       <c r="J59" s="231">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="15" hidden="1">
       <c r="A60" s="108" t="str">
-        <f>IF(B60="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B60)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B60,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B60="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B60)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B60,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B60" s="109"/>
@@ -23163,13 +23328,13 @@
       <c r="H60" s="208"/>
       <c r="I60" s="208"/>
       <c r="J60" s="231">
-        <f t="shared" ref="J60:J64" si="10">IF(J$7="","",SUM(D60:I60))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="15" hidden="1">
       <c r="A61" s="108" t="str">
-        <f>IF(B61="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B61)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B61,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B61="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B61)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B61,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B61" s="109"/>
@@ -23181,13 +23346,13 @@
       <c r="H61" s="208"/>
       <c r="I61" s="208"/>
       <c r="J61" s="231">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="15" hidden="1">
       <c r="A62" s="108" t="str">
-        <f>IF(B62="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B62)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B62,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B62="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B62)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B62,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B62" s="109"/>
@@ -23199,13 +23364,13 @@
       <c r="H62" s="208"/>
       <c r="I62" s="208"/>
       <c r="J62" s="231">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="J62:J67" si="8">IF(J$7="","",SUM(D62:I62))</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="15" hidden="1">
       <c r="A63" s="108" t="str">
-        <f>IF(B63="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B63)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B63,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B63="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B63)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B63,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B63" s="109"/>
@@ -23217,13 +23382,13 @@
       <c r="H63" s="208"/>
       <c r="I63" s="208"/>
       <c r="J63" s="231">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="15">
       <c r="A64" s="108" t="str">
-        <f>IF(B64="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B64)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B64,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B64="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B64)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B64,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B64" s="109"/>
@@ -23235,13 +23400,13 @@
       <c r="H64" s="208"/>
       <c r="I64" s="208"/>
       <c r="J64" s="231">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="15">
       <c r="A65" s="108" t="str">
-        <f>IF(B65="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B65)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B65,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B65="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B65)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B65,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B65" s="109"/>
@@ -23252,11 +23417,14 @@
       <c r="G65" s="208"/>
       <c r="H65" s="208"/>
       <c r="I65" s="208"/>
-      <c r="J65" s="231"/>
+      <c r="J65" s="231">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="66" spans="1:10" ht="15">
       <c r="A66" s="108" t="str">
-        <f>IF(B66="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B66)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B66,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B66="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B66)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B66,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B66" s="109"/>
@@ -23267,11 +23435,14 @@
       <c r="G66" s="208"/>
       <c r="H66" s="208"/>
       <c r="I66" s="208"/>
-      <c r="J66" s="231"/>
+      <c r="J66" s="231">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="67" spans="1:10" ht="15">
       <c r="A67" s="108" t="str">
-        <f>IF(B67="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B67)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B67,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B67="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B67)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B67,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B67" s="109"/>
@@ -23282,117 +23453,104 @@
       <c r="G67" s="208"/>
       <c r="H67" s="208"/>
       <c r="I67" s="208"/>
-      <c r="J67" s="231"/>
+      <c r="J67" s="231">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="68" spans="1:10" ht="15">
       <c r="A68" s="108" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B68" s="108" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C68" s="231">
-        <f>SUM(C56:C64)</f>
+        <f>IF(C$7="","",SUM(C57:C67))</f>
         <v>0</v>
       </c>
       <c r="D68" s="231" t="str">
-        <f t="shared" ref="D68:I68" si="11">IF(D$7="Type fund name","",SUM(D56:D64))</f>
+        <f t="shared" ref="D68:I68" si="9">IF(D$7="Type fund name","",SUM(D57:D67))</f>
         <v/>
       </c>
       <c r="E68" s="231" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F68" s="231" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G68" s="231" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="H68" s="231" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I68" s="231" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="J68" s="231">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="15">
-      <c r="A69" s="114" t="s">
-        <v>39</v>
-      </c>
-      <c r="B69" s="111" t="s">
-        <v>40</v>
-      </c>
-      <c r="C69" s="219">
-        <f>C54+C68</f>
-        <v>0</v>
-      </c>
-      <c r="D69" s="219" t="str">
-        <f t="shared" ref="D69:I69" si="12">IF(D$7 = "Type fund name", "", D54+D68)</f>
-        <v/>
-      </c>
-      <c r="E69" s="219" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="F69" s="219" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="G69" s="219" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="H69" s="219" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="I69" s="219" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="J69" s="233">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
+      <c r="A69" s="104"/>
+      <c r="B69" s="107" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C69" s="107"/>
+      <c r="D69" s="107"/>
+      <c r="E69" s="107"/>
+      <c r="F69" s="107"/>
+      <c r="G69" s="107"/>
+      <c r="H69" s="107"/>
+      <c r="I69" s="107"/>
+      <c r="J69" s="96"/>
     </row>
     <row r="70" spans="1:10" ht="15">
-      <c r="A70" s="104"/>
-      <c r="B70" s="104"/>
-      <c r="C70" s="112"/>
-      <c r="D70" s="112"/>
-      <c r="E70" s="112"/>
-      <c r="F70" s="112"/>
-      <c r="G70" s="112"/>
-      <c r="H70" s="112"/>
-      <c r="I70" s="112"/>
-      <c r="J70" s="107"/>
+      <c r="A70" s="108" t="str">
+        <f>IF(B70="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B70)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B70,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B70" s="109"/>
+      <c r="C70" s="208"/>
+      <c r="D70" s="208"/>
+      <c r="E70" s="208"/>
+      <c r="F70" s="208"/>
+      <c r="G70" s="208"/>
+      <c r="H70" s="208"/>
+      <c r="I70" s="208"/>
+      <c r="J70" s="231">
+        <f t="shared" ref="J70:J83" si="10">IF(J$7="","",SUM(D70:I70))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="71" spans="1:10" ht="15">
-      <c r="A71" s="104"/>
-      <c r="B71" s="105" t="s">
-        <v>46</v>
-      </c>
-      <c r="C71" s="105"/>
-      <c r="D71" s="105"/>
-      <c r="E71" s="105"/>
-      <c r="F71" s="105"/>
-      <c r="G71" s="105"/>
-      <c r="H71" s="105"/>
-      <c r="I71" s="105"/>
-      <c r="J71" s="115"/>
+      <c r="A71" s="108" t="str">
+        <f>IF(B71="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B71)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B71,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B71" s="109"/>
+      <c r="C71" s="208"/>
+      <c r="D71" s="208"/>
+      <c r="E71" s="208"/>
+      <c r="F71" s="208"/>
+      <c r="G71" s="208"/>
+      <c r="H71" s="208"/>
+      <c r="I71" s="208"/>
+      <c r="J71" s="231">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="72" spans="1:10" ht="15">
       <c r="A72" s="108" t="str">
-        <f>IF(B72="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B72)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B72,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B72="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B72)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B72,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B72" s="109"/>
@@ -23404,13 +23562,13 @@
       <c r="H72" s="208"/>
       <c r="I72" s="208"/>
       <c r="J72" s="231">
-        <f t="shared" ref="J72:J81" si="13">IF(J$7="","",SUM(D72:I72))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="15">
       <c r="A73" s="108" t="str">
-        <f>IF(B73="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B73)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B73,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B73="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B73)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B73,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B73" s="109"/>
@@ -23422,13 +23580,13 @@
       <c r="H73" s="208"/>
       <c r="I73" s="208"/>
       <c r="J73" s="231">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="15">
       <c r="A74" s="108" t="str">
-        <f>IF(B74="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B74)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B74,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B74="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B74)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B74,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B74" s="109"/>
@@ -23440,13 +23598,13 @@
       <c r="H74" s="208"/>
       <c r="I74" s="208"/>
       <c r="J74" s="231">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="J74:J78" si="11">IF(J$7="","",SUM(D74:I74))</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="15" hidden="1">
       <c r="A75" s="108" t="str">
-        <f>IF(B75="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B75)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B75,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B75="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B75)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B75,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B75" s="109"/>
@@ -23458,13 +23616,13 @@
       <c r="H75" s="208"/>
       <c r="I75" s="208"/>
       <c r="J75" s="231">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="15" hidden="1">
       <c r="A76" s="108" t="str">
-        <f>IF(B76="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B76)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B76,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B76="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B76)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B76,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B76" s="109"/>
@@ -23476,13 +23634,13 @@
       <c r="H76" s="208"/>
       <c r="I76" s="208"/>
       <c r="J76" s="231">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="15" hidden="1">
       <c r="A77" s="108" t="str">
-        <f>IF(B77="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B77)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B77,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B77="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B77)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B77,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B77" s="109"/>
@@ -23494,13 +23652,13 @@
       <c r="H77" s="208"/>
       <c r="I77" s="208"/>
       <c r="J77" s="231">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="15" hidden="1">
       <c r="A78" s="108" t="str">
-        <f>IF(B78="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B78)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B78,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B78="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B78)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B78,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B78" s="109"/>
@@ -23512,13 +23670,13 @@
       <c r="H78" s="208"/>
       <c r="I78" s="208"/>
       <c r="J78" s="231">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="15" hidden="1">
       <c r="A79" s="108" t="str">
-        <f>IF(B79="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B79)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B79,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B79="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B79)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B79,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B79" s="109"/>
@@ -23529,14 +23687,11 @@
       <c r="G79" s="208"/>
       <c r="H79" s="208"/>
       <c r="I79" s="208"/>
-      <c r="J79" s="231">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
+      <c r="J79" s="231"/>
     </row>
     <row r="80" spans="1:10" ht="15">
       <c r="A80" s="108" t="str">
-        <f>IF(B80="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B80)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B80,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <f>IF(B80="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B80)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B80,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B80" s="109"/>
@@ -23547,206 +23702,756 @@
       <c r="G80" s="208"/>
       <c r="H80" s="208"/>
       <c r="I80" s="208"/>
-      <c r="J80" s="231">
+      <c r="J80" s="231"/>
+    </row>
+    <row r="81" spans="1:10" ht="15">
+      <c r="A81" s="108" t="str">
+        <f>IF(B81="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B81)=0,"acfr:NoncurrentLiabilitiesCustom",_xlfn.XLOOKUP(B81,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B81" s="109"/>
+      <c r="C81" s="208"/>
+      <c r="D81" s="208"/>
+      <c r="E81" s="208"/>
+      <c r="F81" s="208"/>
+      <c r="G81" s="208"/>
+      <c r="H81" s="208"/>
+      <c r="I81" s="208"/>
+      <c r="J81" s="231"/>
+    </row>
+    <row r="82" spans="1:10" ht="15">
+      <c r="A82" s="108" t="s">
+        <v>37</v>
+      </c>
+      <c r="B82" s="108" t="s">
+        <v>38</v>
+      </c>
+      <c r="C82" s="231">
+        <f>SUM(C70:C78)</f>
+        <v>0</v>
+      </c>
+      <c r="D82" s="231" t="str">
+        <f t="shared" ref="D82:I82" si="12">IF(D$7="Type fund name","",SUM(D70:D78))</f>
+        <v/>
+      </c>
+      <c r="E82" s="231" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="F82" s="231" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="G82" s="231" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="H82" s="231" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="I82" s="231" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J82" s="231">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="15">
+      <c r="A83" s="114" t="s">
+        <v>39</v>
+      </c>
+      <c r="B83" s="111" t="s">
+        <v>40</v>
+      </c>
+      <c r="C83" s="219">
+        <f>C68+C82</f>
+        <v>0</v>
+      </c>
+      <c r="D83" s="219" t="str">
+        <f t="shared" ref="D83:I83" si="13">IF(D$7 = "Type fund name", "", D68+D82)</f>
+        <v/>
+      </c>
+      <c r="E83" s="219" t="str">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="15">
-      <c r="A81" s="111" t="s">
+        <v/>
+      </c>
+      <c r="F83" s="219" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="G83" s="219" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="H83" s="219" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="I83" s="219" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="J83" s="233">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="15">
+      <c r="A84" s="104"/>
+      <c r="B84" s="104"/>
+      <c r="C84" s="112"/>
+      <c r="D84" s="112"/>
+      <c r="E84" s="112"/>
+      <c r="F84" s="112"/>
+      <c r="G84" s="112"/>
+      <c r="H84" s="112"/>
+      <c r="I84" s="112"/>
+      <c r="J84" s="107"/>
+    </row>
+    <row r="85" spans="1:10" ht="15">
+      <c r="A85" s="104"/>
+      <c r="B85" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C85" s="105"/>
+      <c r="D85" s="105"/>
+      <c r="E85" s="105"/>
+      <c r="F85" s="105"/>
+      <c r="G85" s="105"/>
+      <c r="H85" s="105"/>
+      <c r="I85" s="105"/>
+      <c r="J85" s="105"/>
+    </row>
+    <row r="86" spans="1:10" ht="15">
+      <c r="A86" s="108" t="str">
+        <f>IF(B86="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B86)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B86,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B86" s="109"/>
+      <c r="C86" s="208"/>
+      <c r="D86" s="208"/>
+      <c r="E86" s="208"/>
+      <c r="F86" s="208"/>
+      <c r="G86" s="208"/>
+      <c r="H86" s="208"/>
+      <c r="I86" s="208"/>
+      <c r="J86" s="231">
+        <f t="shared" ref="J86:J97" si="14">IF(J$7="","",SUM(D86:I86))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="15">
+      <c r="A87" s="108" t="str">
+        <f>IF(B87="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B87)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B87,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B87" s="109"/>
+      <c r="C87" s="209"/>
+      <c r="D87" s="209"/>
+      <c r="E87" s="209"/>
+      <c r="F87" s="209"/>
+      <c r="G87" s="209"/>
+      <c r="H87" s="209"/>
+      <c r="I87" s="209"/>
+      <c r="J87" s="231">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="15">
+      <c r="A88" s="108" t="str">
+        <f>IF(B88="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B88)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B88,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B88" s="109"/>
+      <c r="C88" s="208"/>
+      <c r="D88" s="208"/>
+      <c r="E88" s="208"/>
+      <c r="F88" s="208"/>
+      <c r="G88" s="208"/>
+      <c r="H88" s="208"/>
+      <c r="I88" s="208"/>
+      <c r="J88" s="231">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="15">
+      <c r="A89" s="108" t="str">
+        <f>IF(B89="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B89)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B89,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B89" s="109"/>
+      <c r="C89" s="208"/>
+      <c r="D89" s="208"/>
+      <c r="E89" s="208"/>
+      <c r="F89" s="208"/>
+      <c r="G89" s="208"/>
+      <c r="H89" s="208"/>
+      <c r="I89" s="208"/>
+      <c r="J89" s="231">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="16" customHeight="1">
+      <c r="A90" s="108" t="str">
+        <f>IF(B90="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B90)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B90,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B90" s="109"/>
+      <c r="C90" s="208"/>
+      <c r="D90" s="208"/>
+      <c r="E90" s="208"/>
+      <c r="F90" s="208"/>
+      <c r="G90" s="208"/>
+      <c r="H90" s="208"/>
+      <c r="I90" s="208"/>
+      <c r="J90" s="231">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="16" customHeight="1">
+      <c r="A91" s="108" t="str">
+        <f>IF(B91="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B91)=0,"acfr:DeferredInflowsOfResourcesCustom",_xlfn.XLOOKUP(B91,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B91" s="109"/>
+      <c r="C91" s="208"/>
+      <c r="D91" s="208"/>
+      <c r="E91" s="208"/>
+      <c r="F91" s="208"/>
+      <c r="G91" s="208"/>
+      <c r="H91" s="208"/>
+      <c r="I91" s="208"/>
+      <c r="J91" s="231">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="16" hidden="1" customHeight="1">
+      <c r="A92" s="108" t="str">
+        <f>IF(B92="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B92)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B92,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B92" s="109"/>
+      <c r="C92" s="208"/>
+      <c r="D92" s="208"/>
+      <c r="E92" s="208"/>
+      <c r="F92" s="208"/>
+      <c r="G92" s="208"/>
+      <c r="H92" s="208"/>
+      <c r="I92" s="208"/>
+      <c r="J92" s="231">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="16" hidden="1" customHeight="1">
+      <c r="A93" s="108" t="str">
+        <f>IF(B93="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B93)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B93,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B93" s="109"/>
+      <c r="C93" s="208"/>
+      <c r="D93" s="208"/>
+      <c r="E93" s="208"/>
+      <c r="F93" s="208"/>
+      <c r="G93" s="208"/>
+      <c r="H93" s="208"/>
+      <c r="I93" s="208"/>
+      <c r="J93" s="231">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="16" hidden="1" customHeight="1">
+      <c r="A94" s="108" t="str">
+        <f>IF(B94="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B94)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B94,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B94" s="109"/>
+      <c r="C94" s="208"/>
+      <c r="D94" s="208"/>
+      <c r="E94" s="208"/>
+      <c r="F94" s="208"/>
+      <c r="G94" s="208"/>
+      <c r="H94" s="208"/>
+      <c r="I94" s="208"/>
+      <c r="J94" s="231">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="15" hidden="1">
+      <c r="A95" s="108" t="str">
+        <f>IF(B95="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B95)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B95,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B95" s="109"/>
+      <c r="C95" s="208"/>
+      <c r="D95" s="208"/>
+      <c r="E95" s="208"/>
+      <c r="F95" s="208"/>
+      <c r="G95" s="208"/>
+      <c r="H95" s="208"/>
+      <c r="I95" s="208"/>
+      <c r="J95" s="231">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="15" hidden="1">
+      <c r="A96" s="108" t="str">
+        <f>IF(B96="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B96)=0,"acfr:CurrentLiabilitiesCustom",_xlfn.XLOOKUP(B96,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B96" s="109"/>
+      <c r="C96" s="208"/>
+      <c r="D96" s="208"/>
+      <c r="E96" s="208"/>
+      <c r="F96" s="208"/>
+      <c r="G96" s="208"/>
+      <c r="H96" s="208"/>
+      <c r="I96" s="208"/>
+      <c r="J96" s="231">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="15">
+      <c r="A97" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C97" s="231">
+        <f>IF(C$7="","",SUM(C86:C96))</f>
+        <v>0</v>
+      </c>
+      <c r="D97" s="231" t="str">
+        <f t="shared" ref="D97:I97" si="15">IF(D$7="Type fund name","",SUM(D86:D96))</f>
+        <v/>
+      </c>
+      <c r="E97" s="231" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="F97" s="231" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="G97" s="231" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="H97" s="231" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="I97" s="231" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="J97" s="231">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="15">
+      <c r="A98" s="104"/>
+      <c r="B98" s="104"/>
+      <c r="C98" s="112"/>
+      <c r="D98" s="112"/>
+      <c r="E98" s="112"/>
+      <c r="F98" s="112"/>
+      <c r="G98" s="112"/>
+      <c r="H98" s="112"/>
+      <c r="I98" s="112"/>
+      <c r="J98" s="107"/>
+    </row>
+    <row r="99" spans="1:10" ht="15">
+      <c r="A99" s="104"/>
+      <c r="B99" s="105" t="s">
+        <v>46</v>
+      </c>
+      <c r="C99" s="105"/>
+      <c r="D99" s="105"/>
+      <c r="E99" s="105"/>
+      <c r="F99" s="105"/>
+      <c r="G99" s="105"/>
+      <c r="H99" s="105"/>
+      <c r="I99" s="105"/>
+      <c r="J99" s="115"/>
+    </row>
+    <row r="100" spans="1:10" ht="15">
+      <c r="A100" s="108" t="str">
+        <f>IF(B100="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B100)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B100,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B100" s="109"/>
+      <c r="C100" s="208"/>
+      <c r="D100" s="208"/>
+      <c r="E100" s="208"/>
+      <c r="F100" s="208"/>
+      <c r="G100" s="208"/>
+      <c r="H100" s="208"/>
+      <c r="I100" s="208"/>
+      <c r="J100" s="231">
+        <f t="shared" ref="J100:J109" si="16">IF(J$7="","",SUM(D100:I100))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="15">
+      <c r="A101" s="108" t="str">
+        <f>IF(B101="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B101)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B101,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B101" s="109"/>
+      <c r="C101" s="208"/>
+      <c r="D101" s="208"/>
+      <c r="E101" s="208"/>
+      <c r="F101" s="208"/>
+      <c r="G101" s="208"/>
+      <c r="H101" s="208"/>
+      <c r="I101" s="208"/>
+      <c r="J101" s="231">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="15">
+      <c r="A102" s="108" t="str">
+        <f>IF(B102="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B102)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B102,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B102" s="109"/>
+      <c r="C102" s="208"/>
+      <c r="D102" s="208"/>
+      <c r="E102" s="208"/>
+      <c r="F102" s="208"/>
+      <c r="G102" s="208"/>
+      <c r="H102" s="208"/>
+      <c r="I102" s="208"/>
+      <c r="J102" s="231">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="15">
+      <c r="A103" s="108" t="str">
+        <f>IF(B103="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B103)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B103,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B103" s="109"/>
+      <c r="C103" s="208"/>
+      <c r="D103" s="208"/>
+      <c r="E103" s="208"/>
+      <c r="F103" s="208"/>
+      <c r="G103" s="208"/>
+      <c r="H103" s="208"/>
+      <c r="I103" s="208"/>
+      <c r="J103" s="231">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A104" s="108" t="str">
+        <f>IF(B104="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B104)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B104,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B104" s="109"/>
+      <c r="C104" s="208"/>
+      <c r="D104" s="208"/>
+      <c r="E104" s="208"/>
+      <c r="F104" s="208"/>
+      <c r="G104" s="208"/>
+      <c r="H104" s="208"/>
+      <c r="I104" s="208"/>
+      <c r="J104" s="231">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A105" s="108" t="str">
+        <f>IF(B105="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B105)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B105,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B105" s="109"/>
+      <c r="C105" s="208"/>
+      <c r="D105" s="208"/>
+      <c r="E105" s="208"/>
+      <c r="F105" s="208"/>
+      <c r="G105" s="208"/>
+      <c r="H105" s="208"/>
+      <c r="I105" s="208"/>
+      <c r="J105" s="231">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A106" s="108" t="str">
+        <f>IF(B106="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B106)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B106,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B106" s="109"/>
+      <c r="C106" s="208"/>
+      <c r="D106" s="208"/>
+      <c r="E106" s="208"/>
+      <c r="F106" s="208"/>
+      <c r="G106" s="208"/>
+      <c r="H106" s="208"/>
+      <c r="I106" s="208"/>
+      <c r="J106" s="231">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A107" s="108" t="str">
+        <f>IF(B107="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B107)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B107,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B107" s="109"/>
+      <c r="C107" s="208"/>
+      <c r="D107" s="208"/>
+      <c r="E107" s="208"/>
+      <c r="F107" s="208"/>
+      <c r="G107" s="208"/>
+      <c r="H107" s="208"/>
+      <c r="I107" s="208"/>
+      <c r="J107" s="231">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A108" s="108" t="str">
+        <f>IF(B108="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B108)=0,"acfr:RestrictedComponentsOfNetPositionCustom",_xlfn.XLOOKUP(B108,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B108" s="109"/>
+      <c r="C108" s="208"/>
+      <c r="D108" s="208"/>
+      <c r="E108" s="208"/>
+      <c r="F108" s="208"/>
+      <c r="G108" s="208"/>
+      <c r="H108" s="208"/>
+      <c r="I108" s="208"/>
+      <c r="J108" s="231">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A109" s="111" t="s">
         <v>50</v>
       </c>
-      <c r="B81" s="111" t="s">
+      <c r="B109" s="111" t="s">
         <v>51</v>
       </c>
-      <c r="C81" s="219">
-        <f>IF(C7="","",SUM(C72:C80))</f>
-        <v>0</v>
-      </c>
-      <c r="D81" s="219" t="str">
-        <f t="shared" ref="D81:I81" si="14">IF(D7="Type fund name","",SUM(D72:D80))</f>
+      <c r="C109" s="219">
+        <f>IF(C7="","",SUM(C100:C108))</f>
+        <v>0</v>
+      </c>
+      <c r="D109" s="219" t="str">
+        <f>IF(D7="Type fund name","",SUM(D100:D108))</f>
         <v/>
       </c>
-      <c r="E81" s="219" t="str">
-        <f t="shared" si="14"/>
+      <c r="E109" s="219" t="str">
+        <f>IF(E7="Type fund name","",SUM(E100:E108))</f>
         <v/>
       </c>
-      <c r="F81" s="219" t="str">
-        <f t="shared" si="14"/>
+      <c r="F109" s="219" t="str">
+        <f>IF(F7="Type fund name","",SUM(F100:F108))</f>
         <v/>
       </c>
-      <c r="G81" s="219" t="str">
-        <f t="shared" si="14"/>
+      <c r="G109" s="219" t="str">
+        <f>IF(G7="Type fund name","",SUM(G100:G108))</f>
         <v/>
       </c>
-      <c r="H81" s="219" t="str">
-        <f t="shared" si="14"/>
+      <c r="H109" s="219" t="str">
+        <f>IF(H7="Type fund name","",SUM(H100:H108))</f>
         <v/>
       </c>
-      <c r="I81" s="219" t="str">
-        <f t="shared" si="14"/>
+      <c r="I109" s="219" t="str">
+        <f>IF(I7="Type fund name","",SUM(I100:I108))</f>
         <v/>
       </c>
-      <c r="J81" s="232">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="16">
-      <c r="C82" s="116"/>
-      <c r="D82" s="116"/>
-      <c r="E82" s="116"/>
-      <c r="F82" s="116"/>
-      <c r="G82" s="116"/>
-      <c r="H82" s="116"/>
-      <c r="I82" s="116"/>
-      <c r="J82" s="112"/>
-    </row>
-    <row r="83" spans="1:10" ht="15">
-      <c r="J83" s="112"/>
-    </row>
-    <row r="84" spans="1:10" ht="15">
-      <c r="J84" s="112"/>
-    </row>
-    <row r="85" spans="1:10" ht="15">
-      <c r="J85" s="112"/>
-    </row>
-    <row r="86" spans="1:10" ht="15">
-      <c r="J86" s="112"/>
-    </row>
-    <row r="87" spans="1:10" ht="15">
-      <c r="J87" s="112"/>
-    </row>
-    <row r="88" spans="1:10" ht="15">
-      <c r="J88" s="112"/>
-    </row>
-    <row r="89" spans="1:10" ht="15">
-      <c r="J89" s="112"/>
-    </row>
-    <row r="90" spans="1:10" ht="15">
-      <c r="J90" s="112"/>
-    </row>
-    <row r="91" spans="1:10" ht="15">
-      <c r="J91" s="112"/>
-    </row>
-    <row r="92" spans="1:10" ht="15">
-      <c r="J92" s="112"/>
-    </row>
-    <row r="93" spans="1:10" ht="15">
-      <c r="J93" s="112"/>
-    </row>
-    <row r="94" spans="1:10" ht="15">
-      <c r="J94" s="112"/>
-    </row>
-    <row r="95" spans="1:10" ht="15">
-      <c r="J95" s="112"/>
-    </row>
-    <row r="96" spans="1:10" ht="15">
-      <c r="J96" s="112"/>
-    </row>
-    <row r="97" spans="10:10" ht="15">
-      <c r="J97" s="112"/>
-    </row>
-    <row r="98" spans="10:10" ht="15">
-      <c r="J98" s="112"/>
-    </row>
-    <row r="99" spans="10:10" ht="15">
-      <c r="J99" s="112"/>
-    </row>
-    <row r="100" spans="10:10" ht="15">
-      <c r="J100" s="112"/>
-    </row>
-    <row r="101" spans="10:10" ht="15">
-      <c r="J101" s="112"/>
-    </row>
-    <row r="102" spans="10:10" ht="15">
-      <c r="J102" s="112"/>
-    </row>
-    <row r="103" spans="10:10" ht="15">
-      <c r="J103" s="112"/>
-    </row>
-    <row r="104" spans="10:10" ht="15">
-      <c r="J104" s="112"/>
-    </row>
-    <row r="105" spans="10:10" ht="15">
-      <c r="J105" s="112"/>
-    </row>
-    <row r="106" spans="10:10" ht="15">
-      <c r="J106" s="112"/>
-    </row>
-    <row r="107" spans="10:10" ht="15">
-      <c r="J107" s="112"/>
-    </row>
-    <row r="108" spans="10:10" ht="15">
-      <c r="J108" s="112"/>
-    </row>
-    <row r="109" spans="10:10" ht="15">
-      <c r="J109" s="112"/>
+      <c r="J109" s="232">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" s="33" customFormat="1" ht="16" hidden="1">
+      <c r="A110" s="84"/>
+      <c r="B110" s="84"/>
+      <c r="C110" s="116"/>
+      <c r="D110" s="116"/>
+      <c r="E110" s="116"/>
+      <c r="F110" s="116"/>
+      <c r="G110" s="116"/>
+      <c r="H110" s="116"/>
+      <c r="I110" s="116"/>
+      <c r="J110" s="112"/>
+    </row>
+    <row r="111" spans="1:10" s="33" customFormat="1" ht="15" hidden="1">
+      <c r="A111" s="84"/>
+      <c r="B111" s="84"/>
+      <c r="C111" s="84"/>
+      <c r="D111" s="84"/>
+      <c r="E111" s="84"/>
+      <c r="F111" s="84"/>
+      <c r="G111" s="84"/>
+      <c r="H111" s="84"/>
+      <c r="I111" s="84"/>
+      <c r="J111" s="112"/>
+    </row>
+    <row r="112" spans="1:10" s="33" customFormat="1" ht="15" hidden="1">
+      <c r="A112" s="257"/>
+      <c r="B112" s="262" t="s">
+        <v>3636</v>
+      </c>
+      <c r="C112" s="84"/>
+      <c r="D112" s="84"/>
+      <c r="E112" s="84"/>
+      <c r="F112" s="84"/>
+      <c r="G112" s="84"/>
+      <c r="H112" s="84"/>
+      <c r="I112" s="84"/>
+      <c r="J112" s="112"/>
+    </row>
+    <row r="113" spans="1:10" s="33" customFormat="1" ht="15" hidden="1">
+      <c r="A113" s="257"/>
+      <c r="B113" s="263"/>
+      <c r="C113" s="84"/>
+      <c r="D113" s="84"/>
+      <c r="E113" s="84"/>
+      <c r="F113" s="84"/>
+      <c r="G113" s="84"/>
+      <c r="H113" s="84"/>
+      <c r="I113" s="84"/>
+      <c r="J113" s="112"/>
+    </row>
+    <row r="114" spans="1:10" s="33" customFormat="1" ht="15">
+      <c r="A114" s="84"/>
+      <c r="B114" s="84"/>
+      <c r="C114" s="84"/>
+      <c r="D114" s="84"/>
+      <c r="E114" s="84"/>
+      <c r="F114" s="84"/>
+      <c r="G114" s="84"/>
+      <c r="H114" s="84"/>
+      <c r="I114" s="84"/>
+      <c r="J114" s="112"/>
+    </row>
+    <row r="115" spans="1:10" ht="15">
+      <c r="J115" s="112"/>
+    </row>
+    <row r="116" spans="1:10" ht="15">
+      <c r="J116" s="112"/>
+    </row>
+    <row r="117" spans="1:10" ht="15">
+      <c r="J117" s="112"/>
+    </row>
+    <row r="118" spans="1:10" ht="15">
+      <c r="J118" s="112"/>
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="B112:B113"/>
+  </mergeCells>
   <conditionalFormatting sqref="A10:A23">
-    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="47" priority="14" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:A37">
-    <cfRule type="containsText" dxfId="42" priority="4" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="46" priority="13" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A26)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A43:A53">
-    <cfRule type="containsText" dxfId="41" priority="3" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A43)))</formula>
+  <conditionalFormatting sqref="A57:A67">
+    <cfRule type="containsText" dxfId="45" priority="12" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A57)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A56:A67">
-    <cfRule type="containsText" dxfId="40" priority="2" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A56)))</formula>
+  <conditionalFormatting sqref="A70:A81">
+    <cfRule type="containsText" dxfId="44" priority="11" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A70)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A72:A80">
-    <cfRule type="containsText" dxfId="39" priority="1" operator="containsText" text="custom">
-      <formula>NOT(ISERROR(SEARCH("custom",A72)))</formula>
+  <conditionalFormatting sqref="A100:A108">
+    <cfRule type="containsText" dxfId="43" priority="10" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A100)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24 C38 C54:I54 C68:C69 C81:I81">
-    <cfRule type="expression" dxfId="38" priority="11" stopIfTrue="1">
+  <conditionalFormatting sqref="C24 C38 C68:I68 C82:C83 C109:I109">
+    <cfRule type="expression" dxfId="42" priority="20" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D68:I68">
-    <cfRule type="expression" dxfId="37" priority="9" stopIfTrue="1">
+  <conditionalFormatting sqref="D82:I82">
+    <cfRule type="expression" dxfId="41" priority="18" stopIfTrue="1">
       <formula>D$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="expression" dxfId="36" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="17" stopIfTrue="1">
       <formula>K$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42:A52">
+    <cfRule type="containsText" dxfId="39" priority="5" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53:I53">
+    <cfRule type="expression" dxfId="38" priority="6" stopIfTrue="1">
+      <formula>C$7=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A86:A96">
+    <cfRule type="containsText" dxfId="37" priority="1" operator="containsText" text="custom">
+      <formula>NOT(ISERROR(SEARCH("custom",A86)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C97:I97">
+    <cfRule type="expression" dxfId="36" priority="2" stopIfTrue="1">
+      <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{3020B3D5-A2C3-4F4B-8EFD-A19414110BEC}">
           <x14:formula1>
             <xm:f>'Lookup Net Position'!$B$202:$B$315</xm:f>
           </x14:formula1>
-          <xm:sqref>B43:B53</xm:sqref>
+          <xm:sqref>B57:B67 B48:B52 B92:B96</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{0AF5B33B-114A-5D47-AC98-0EF208D28A50}">
           <x14:formula1>
             <xm:f>'Lookup Net Position'!$B$469:$B$514</xm:f>
           </x14:formula1>
-          <xm:sqref>B56:B67</xm:sqref>
+          <xm:sqref>B70:B81</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{62718926-C752-384A-817F-8A854F7BD996}">
           <x14:formula1>
             <xm:f>'Lookup Net Position'!$B$355:$B$375</xm:f>
           </x14:formula1>
-          <xm:sqref>B72:B80</xm:sqref>
+          <xm:sqref>B100:B108</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{E796ED53-BB10-BA41-A5DA-36CA177F44A2}">
           <x14:formula1>
@@ -23759,6 +24464,18 @@
             <xm:f>'Lookup Net Position'!$B$2:$B$201</xm:f>
           </x14:formula1>
           <xm:sqref>B10:B23</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{1A045BB2-96D6-734E-95FE-7E3BC4BE9B80}">
+          <x14:formula1>
+            <xm:f>'Lookup Net Position'!$B$338:$B$354</xm:f>
+          </x14:formula1>
+          <xm:sqref>B42:B47</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{9515C0BB-B0C1-8646-8A2B-B3448D36D576}">
+          <x14:formula1>
+            <xm:f>'Lookup Net Position'!$B$316:$B$337</xm:f>
+          </x14:formula1>
+          <xm:sqref>B86:B91</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -23773,8 +24490,8 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView topLeftCell="A5" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -25163,9 +25880,15 @@
       <c r="J72" s="112"/>
     </row>
     <row r="73" spans="1:10" ht="15">
+      <c r="A73" s="259"/>
+      <c r="B73" s="271" t="s">
+        <v>3636</v>
+      </c>
       <c r="J73" s="112"/>
     </row>
     <row r="74" spans="1:10" ht="15">
+      <c r="A74" s="259"/>
+      <c r="B74" s="272"/>
       <c r="J74" s="112"/>
     </row>
     <row r="75" spans="1:10" ht="15">
@@ -25245,6 +25968,9 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="B73:B74"/>
+  </mergeCells>
   <conditionalFormatting sqref="A9:A22">
     <cfRule type="containsText" dxfId="35" priority="4" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
@@ -25343,8 +26069,8 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView topLeftCell="A2" zoomScale="74" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -26788,8 +27514,10 @@
       <c r="J76" s="138"/>
     </row>
     <row r="77" spans="1:10" ht="15">
-      <c r="A77" s="104"/>
-      <c r="B77" s="154"/>
+      <c r="A77" s="257"/>
+      <c r="B77" s="262" t="s">
+        <v>3636</v>
+      </c>
       <c r="C77" s="155"/>
       <c r="D77" s="155"/>
       <c r="E77" s="155"/>
@@ -26800,8 +27528,8 @@
       <c r="J77" s="138"/>
     </row>
     <row r="78" spans="1:10" ht="15">
-      <c r="A78" s="104"/>
-      <c r="B78" s="154"/>
+      <c r="A78" s="257"/>
+      <c r="B78" s="263"/>
       <c r="C78" s="155"/>
       <c r="D78" s="155"/>
       <c r="E78" s="155"/>
@@ -26823,6 +27551,9 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="B77:B78"/>
+  </mergeCells>
   <conditionalFormatting sqref="A9:A22">
     <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
@@ -26928,7 +27659,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74:B78" xr:uid="{98ECD2C2-C0B9-E74C-B5D0-14A316D496F4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74:B76" xr:uid="{98ECD2C2-C0B9-E74C-B5D0-14A316D496F4}">
       <formula1>net_position</formula1>
     </dataValidation>
   </dataValidations>
@@ -33953,10 +34684,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:E311"/>
+  <dimension ref="A1:E310"/>
   <sheetViews>
-    <sheetView topLeftCell="A273" workbookViewId="0">
-      <selection activeCell="D262" sqref="D262"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A313" sqref="A313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -38194,7 +38925,7 @@
         <v>acfr:Bond or Insurance Recoveries</v>
       </c>
       <c r="D249" s="120" t="str">
-        <f t="shared" ref="D249:D262" si="13">IF(RIGHT(B249, 8)="Abstract", "Abstract", "Capital Contributions")</f>
+        <f t="shared" ref="D249:D261" si="13">IF(RIGHT(B249, 8)="Abstract", "Abstract", "Capital Contributions")</f>
         <v>Capital Contributions</v>
       </c>
       <c r="E249" s="119"/>
@@ -38415,7 +39146,7 @@
         <v>acfr:Transfers of Capital Assets Out</v>
       </c>
       <c r="D262" s="120" t="str">
-        <f t="shared" si="13"/>
+        <f>IF(RIGHT(B262, 8)="Abstract", "Abstract", "Capital Contributions")</f>
         <v>Capital Contributions</v>
       </c>
       <c r="E262" s="119"/>
@@ -38998,6 +39729,9 @@
       </c>
       <c r="E296" s="119"/>
     </row>
+    <row r="306" spans="3:3" ht="15">
+      <c r="C306" s="104"/>
+    </row>
     <row r="307" spans="3:3" ht="15">
       <c r="C307" s="104"/>
     </row>
@@ -39005,13 +39739,10 @@
       <c r="C308" s="104"/>
     </row>
     <row r="309" spans="3:3" ht="15">
-      <c r="C309" s="104"/>
+      <c r="C309" s="132"/>
     </row>
     <row r="310" spans="3:3" ht="15">
-      <c r="C310" s="132"/>
-    </row>
-    <row r="311" spans="3:3" ht="15">
-      <c r="C311" s="129"/>
+      <c r="C310" s="129"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D296">
@@ -46726,10 +47457,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8474313-8EAC-0141-BA8E-861AF31ED060}">
-  <dimension ref="B1:E32"/>
+  <dimension ref="B1:E40"/>
   <sheetViews>
     <sheetView zoomScale="92" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -46857,20 +47588,28 @@
         <v>3630</v>
       </c>
     </row>
-    <row r="30" spans="2:2">
-      <c r="B30" t="s">
-        <v>3631</v>
+    <row r="29" spans="2:2">
+      <c r="B29" s="261" t="s">
+        <v>3637</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" t="s">
-        <v>3632</v>
+        <v>3631</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" t="s">
+        <v>3632</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
         <v>3633</v>
       </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="260"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -46887,15 +47626,15 @@
   <sheetPr codeName="Sheet8">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="81" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView topLeftCell="A41" zoomScale="88" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="33" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" style="33" customWidth="1"/>
     <col min="2" max="2" width="41.5" style="33" customWidth="1"/>
     <col min="3" max="5" width="18.6640625" style="33" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" style="33" customWidth="1"/>
@@ -48288,72 +49027,88 @@
       <c r="C102" s="36"/>
       <c r="D102" s="37"/>
     </row>
+    <row r="103" spans="1:6">
+      <c r="B103" s="256"/>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="257"/>
+      <c r="B104" s="262" t="s">
+        <v>3636</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="257"/>
+      <c r="B105" s="263"/>
+    </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="B104:B105"/>
+  </mergeCells>
   <conditionalFormatting sqref="A9:A22">
-    <cfRule type="expression" dxfId="90" priority="16">
+    <cfRule type="expression" dxfId="94" priority="16">
       <formula>A9="acfr:CurrentAssetsCustom"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:A31">
-    <cfRule type="containsText" dxfId="89" priority="3" operator="containsText" text="acfr:NonCurrentAssetsCustom">
+    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="acfr:NonCurrentAssetsCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:NonCurrentAssetsCustom",A25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:A45">
-    <cfRule type="containsText" dxfId="88" priority="2" operator="containsText" text="acfr:DeferredOutflowsOfResourcesCustom">
+    <cfRule type="containsText" dxfId="92" priority="2" operator="containsText" text="acfr:DeferredOutflowsOfResourcesCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:DeferredOutflowsOfResourcesCustom",A41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="13" operator="containsText" text="acfr:DeferredOutflowsOfResourcesCustom">
+    <cfRule type="containsText" dxfId="91" priority="13" operator="containsText" text="acfr:DeferredOutflowsOfResourcesCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:DeferredOutflowsOfResourcesCustom",A41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:A59">
-    <cfRule type="containsText" dxfId="86" priority="1" operator="containsText" text="acfr:CurrentLiabilitiesCustom">
+    <cfRule type="containsText" dxfId="90" priority="1" operator="containsText" text="acfr:CurrentLiabilitiesCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:CurrentLiabilitiesCustom",A54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="12" operator="containsText" text="acfr:CurrentLiabilitiesCustom">
+    <cfRule type="containsText" dxfId="89" priority="12" operator="containsText" text="acfr:CurrentLiabilitiesCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:CurrentLiabilitiesCustom",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67:A70">
-    <cfRule type="containsText" dxfId="84" priority="11" operator="containsText" text="acfr:NoncurrentLiabilitiesCustom">
+    <cfRule type="containsText" dxfId="88" priority="11" operator="containsText" text="acfr:NoncurrentLiabilitiesCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:NoncurrentLiabilitiesCustom",A67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A80:A83">
-    <cfRule type="containsText" dxfId="83" priority="10" operator="containsText" text="acfr:DeferredInflowsOfResourcesCustom">
+    <cfRule type="containsText" dxfId="87" priority="10" operator="containsText" text="acfr:DeferredInflowsOfResourcesCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:DeferredInflowsOfResourcesCustom",A80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92:A95">
-    <cfRule type="containsText" dxfId="82" priority="9" operator="containsText" text="acfr:RestrictedComponentsOfNetPositionCustom">
+    <cfRule type="containsText" dxfId="86" priority="9" operator="containsText" text="acfr:RestrictedComponentsOfNetPositionCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:RestrictedComponentsOfNetPositionCustom",A92)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="81" priority="15" operator="containsText" text="acfr:CurrentAssetsCustom">
+    <cfRule type="containsText" dxfId="85" priority="15" operator="containsText" text="acfr:CurrentAssetsCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:CurrentAssetsCustom",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101:F101">
-    <cfRule type="cellIs" dxfId="80" priority="34" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="34" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="35" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="35" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="36" operator="notEqual">
+    <cfRule type="cellIs" dxfId="82" priority="36" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:F37 C23:F23 C37:F37 D39:F101 C50 C65:F65 C76:C77 C89 C101">
-    <cfRule type="expression" dxfId="77" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="18" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M68">
-    <cfRule type="expression" dxfId="76" priority="8">
+    <cfRule type="expression" dxfId="80" priority="8">
       <formula>$A$9:$A$22="acfr:CurrentAssetsCustom"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -48440,8 +49195,8 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="84" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView topLeftCell="A44" zoomScale="84" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -50015,54 +50770,60 @@
       <c r="I79" s="54"/>
     </row>
     <row r="80" spans="1:10" ht="15">
+      <c r="A80" s="257"/>
+      <c r="B80" s="264" t="s">
+        <v>3636</v>
+      </c>
       <c r="I80" s="54"/>
     </row>
-    <row r="81" spans="9:9" ht="15">
+    <row r="81" spans="1:9" ht="15">
+      <c r="A81" s="257"/>
+      <c r="B81" s="265"/>
       <c r="I81" s="54"/>
     </row>
-    <row r="82" spans="9:9" ht="15">
+    <row r="82" spans="1:9" ht="15">
       <c r="I82" s="54"/>
     </row>
-    <row r="83" spans="9:9" ht="15">
+    <row r="83" spans="1:9" ht="15">
       <c r="I83" s="54"/>
     </row>
-    <row r="84" spans="9:9" ht="15">
+    <row r="84" spans="1:9" ht="15">
       <c r="I84" s="54"/>
     </row>
-    <row r="85" spans="9:9" ht="15">
+    <row r="85" spans="1:9" ht="15">
       <c r="I85" s="54"/>
     </row>
-    <row r="86" spans="9:9" ht="15">
+    <row r="86" spans="1:9" ht="15">
       <c r="I86" s="54"/>
     </row>
-    <row r="87" spans="9:9" ht="15">
+    <row r="87" spans="1:9" ht="15">
       <c r="I87" s="54"/>
     </row>
-    <row r="88" spans="9:9" ht="15">
+    <row r="88" spans="1:9" ht="15">
       <c r="I88" s="54"/>
     </row>
-    <row r="89" spans="9:9" ht="14">
+    <row r="89" spans="1:9" ht="14">
       <c r="I89" s="20"/>
     </row>
-    <row r="90" spans="9:9" ht="15">
+    <row r="90" spans="1:9" ht="15">
       <c r="I90" s="53"/>
     </row>
-    <row r="91" spans="9:9" ht="15">
+    <row r="91" spans="1:9" ht="15">
       <c r="I91" s="54"/>
     </row>
-    <row r="92" spans="9:9" ht="15">
+    <row r="92" spans="1:9" ht="15">
       <c r="I92" s="54"/>
     </row>
-    <row r="93" spans="9:9" ht="15">
+    <row r="93" spans="1:9" ht="15">
       <c r="I93" s="54"/>
     </row>
-    <row r="94" spans="9:9" ht="15">
+    <row r="94" spans="1:9" ht="15">
       <c r="I94" s="54"/>
     </row>
-    <row r="95" spans="9:9" ht="15">
+    <row r="95" spans="1:9" ht="15">
       <c r="I95" s="54"/>
     </row>
-    <row r="96" spans="9:9" ht="15">
+    <row r="96" spans="1:9" ht="15">
       <c r="I96" s="54"/>
     </row>
     <row r="97" spans="9:9" ht="15">
@@ -50076,88 +50837,91 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="B80:B81"/>
+  </mergeCells>
   <conditionalFormatting sqref="A9:A22">
-    <cfRule type="containsText" dxfId="75" priority="9" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="79" priority="9" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:A36">
-    <cfRule type="containsText" dxfId="74" priority="8" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="78" priority="8" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:A63">
-    <cfRule type="containsText" dxfId="73" priority="5" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="77" priority="5" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66:A70">
-    <cfRule type="containsText" dxfId="72" priority="1" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="76" priority="1" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:B49">
-    <cfRule type="containsText" dxfId="71" priority="3" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23 C37 C50 D53:G63">
-    <cfRule type="expression" dxfId="70" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="58" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:J64">
-    <cfRule type="expression" dxfId="69" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="43" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:J72">
-    <cfRule type="expression" dxfId="68" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="19" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:F6 D52:F52">
-    <cfRule type="expression" dxfId="67" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="55" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39:G51">
-    <cfRule type="expression" dxfId="66" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="15" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:J70">
-    <cfRule type="expression" dxfId="65" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="11" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D74:J77 I78:I99">
-    <cfRule type="expression" dxfId="64" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="10" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39:H50">
-    <cfRule type="expression" dxfId="63" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="14" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38:I38">
-    <cfRule type="expression" dxfId="62" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="52" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:J6 D7:I37 I39:I51">
-    <cfRule type="expression" dxfId="61" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="48" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52:J63">
-    <cfRule type="expression" dxfId="60" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="12" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:J50">
-    <cfRule type="expression" dxfId="59" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="13" stopIfTrue="1">
       <formula>J$6=""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
#122 uploading emailed template
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarrahahmed/Desktop/CLOSUP/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7005A4-4327-964A-AA98-262F64B11467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB18F61C-1862-5741-AEA4-14EC3334C849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" tabRatio="834" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17260" tabRatio="834" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Net Position" sheetId="8" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5390" uniqueCount="3645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5391" uniqueCount="3646">
   <si>
     <t>Statement of Net Position</t>
   </si>
@@ -10955,42 +10955,21 @@
     <t>Steps</t>
   </si>
   <si>
-    <t>1. Enter Financial Statements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   - Fill in the financial data in the corresponding cells. Ensure all required fields are completed.</t>
-  </si>
-  <si>
-    <t>2. Verify Data</t>
-  </si>
-  <si>
     <t xml:space="preserve">   - Double-check all entries for accuracy.</t>
   </si>
   <si>
     <t xml:space="preserve">   - Ensure that all calculations and formulas are correct.</t>
   </si>
   <si>
-    <t>3. Save the File</t>
-  </si>
-  <si>
     <t xml:space="preserve">   - Once all data is entered and verified, save the Excel file with an appropriate name indicating its contents and date.</t>
   </si>
   <si>
-    <t>4. Upload for XBRL Conversion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   - Navigate to the XBRL conversion tool provided by your organization.</t>
-  </si>
-  <si>
     <t xml:space="preserve">   - Upload the saved Excel file to the converter.</t>
   </si>
   <si>
     <t xml:space="preserve">   - Follow the instructions provided by the conversion tool to complete the process.</t>
   </si>
   <si>
-    <t>5. Review XBRL Output</t>
-  </si>
-  <si>
     <t xml:space="preserve">   - After conversion, review the XBRL output to ensure it accurately reflects the entered financial statements.</t>
   </si>
   <si>
@@ -11028,6 +11007,30 @@
   </si>
   <si>
     <t>Total Allocation of Internal Service Fund Activity</t>
+  </si>
+  <si>
+    <t>1. Begin by specifying the details of your municipality at the top of this sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Fill in the financial data in the corresponding cells. Ensure all relevant fields are completed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Navigate to the XBRL conversion tool on your browser.</t>
+  </si>
+  <si>
+    <t>2. Enter financial statements</t>
+  </si>
+  <si>
+    <t>2. Verify data</t>
+  </si>
+  <si>
+    <t>3. Save the file</t>
+  </si>
+  <si>
+    <t>4. Upload for XBRL conversion</t>
+  </si>
+  <si>
+    <t>5. Review XBRL output</t>
   </si>
 </sst>
 </file>
@@ -11697,7 +11700,7 @@
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="275">
+  <cellXfs count="270">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -12154,21 +12157,9 @@
     <xf numFmtId="165" fontId="23" fillId="13" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="27" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="10" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="10" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="1" fillId="10" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
@@ -12211,6 +12202,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="23" fillId="13" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="23" fillId="13" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -12244,14 +12243,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="44" fontId="23" fillId="13" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="23" fillId="13" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -12260,7 +12251,344 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
   </cellStyles>
-  <dxfs count="95">
+  <dxfs count="120">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -12288,13 +12616,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12338,6 +12659,13 @@
       <fill>
         <patternFill>
           <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12461,6 +12789,14 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -12484,14 +12820,6 @@
       <fill>
         <patternFill>
           <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12544,14 +12872,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12850,136 +13170,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -18994,8 +19184,8 @@
   </sheetPr>
   <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="119" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView zoomScale="65" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -20066,18 +20256,18 @@
       </c>
     </row>
     <row r="59" spans="1:10" ht="15">
-      <c r="A59" s="266" t="s">
+      <c r="A59" s="263" t="s">
         <v>3615</v>
       </c>
-      <c r="B59" s="267"/>
-      <c r="C59" s="267"/>
-      <c r="D59" s="267"/>
-      <c r="E59" s="267"/>
-      <c r="F59" s="267"/>
-      <c r="G59" s="267"/>
-      <c r="H59" s="267"/>
-      <c r="I59" s="267"/>
-      <c r="J59" s="268"/>
+      <c r="B59" s="264"/>
+      <c r="C59" s="264"/>
+      <c r="D59" s="264"/>
+      <c r="E59" s="264"/>
+      <c r="F59" s="264"/>
+      <c r="G59" s="264"/>
+      <c r="H59" s="264"/>
+      <c r="I59" s="264"/>
+      <c r="J59" s="265"/>
     </row>
     <row r="60" spans="1:10" ht="15">
       <c r="A60" s="108" t="str">
@@ -20092,7 +20282,7 @@
       <c r="G60" s="209"/>
       <c r="H60" s="210"/>
       <c r="I60" s="210"/>
-      <c r="J60" s="250">
+      <c r="J60" s="245">
         <v>0</v>
       </c>
     </row>
@@ -20109,23 +20299,23 @@
       <c r="G61" s="209"/>
       <c r="H61" s="210"/>
       <c r="I61" s="210"/>
-      <c r="J61" s="250">
+      <c r="J61" s="245">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="15">
-      <c r="A62" s="266" t="s">
+      <c r="A62" s="263" t="s">
         <v>3616</v>
       </c>
-      <c r="B62" s="267"/>
-      <c r="C62" s="267"/>
-      <c r="D62" s="267"/>
-      <c r="E62" s="267"/>
-      <c r="F62" s="267"/>
-      <c r="G62" s="267"/>
-      <c r="H62" s="267"/>
-      <c r="I62" s="267"/>
-      <c r="J62" s="268"/>
+      <c r="B62" s="264"/>
+      <c r="C62" s="264"/>
+      <c r="D62" s="264"/>
+      <c r="E62" s="264"/>
+      <c r="F62" s="264"/>
+      <c r="G62" s="264"/>
+      <c r="H62" s="264"/>
+      <c r="I62" s="264"/>
+      <c r="J62" s="265"/>
     </row>
     <row r="63" spans="1:10" ht="15">
       <c r="A63" s="108" t="str">
@@ -20140,7 +20330,7 @@
       <c r="G63" s="209"/>
       <c r="H63" s="210"/>
       <c r="I63" s="210"/>
-      <c r="J63" s="249">
+      <c r="J63" s="244">
         <v>0</v>
       </c>
     </row>
@@ -20157,23 +20347,23 @@
       <c r="G64" s="209"/>
       <c r="H64" s="210"/>
       <c r="I64" s="210"/>
-      <c r="J64" s="249">
+      <c r="J64" s="244">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="15">
-      <c r="A65" s="266" t="s">
+      <c r="A65" s="263" t="s">
         <v>3617</v>
       </c>
-      <c r="B65" s="267"/>
-      <c r="C65" s="267"/>
-      <c r="D65" s="267"/>
-      <c r="E65" s="267"/>
-      <c r="F65" s="267"/>
-      <c r="G65" s="267"/>
-      <c r="H65" s="267"/>
-      <c r="I65" s="267"/>
-      <c r="J65" s="268"/>
+      <c r="B65" s="264"/>
+      <c r="C65" s="264"/>
+      <c r="D65" s="264"/>
+      <c r="E65" s="264"/>
+      <c r="F65" s="264"/>
+      <c r="G65" s="264"/>
+      <c r="H65" s="264"/>
+      <c r="I65" s="264"/>
+      <c r="J65" s="265"/>
     </row>
     <row r="66" spans="1:10" ht="16">
       <c r="A66" s="131" t="str">
@@ -20188,7 +20378,7 @@
       <c r="G66" s="209"/>
       <c r="H66" s="210"/>
       <c r="I66" s="210"/>
-      <c r="J66" s="249">
+      <c r="J66" s="244">
         <v>0</v>
       </c>
     </row>
@@ -20205,7 +20395,7 @@
       <c r="G67" s="209"/>
       <c r="H67" s="210"/>
       <c r="I67" s="210"/>
-      <c r="J67" s="249">
+      <c r="J67" s="244">
         <v>0</v>
       </c>
     </row>
@@ -20257,44 +20447,47 @@
         <v>2477</v>
       </c>
       <c r="C69" s="219">
-        <f>SUM(C68, C45, C32)</f>
+        <f t="shared" ref="C69:J69" si="8">SUM(C68, C45, C32)</f>
         <v>0</v>
       </c>
       <c r="D69" s="219">
-        <f>SUM(D68, D45, D32)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E69" s="219">
-        <f>SUM(E68, E45, E32)</f>
-        <v>0</v>
-      </c>
-      <c r="F69" s="219"/>
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F69" s="219">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="G69" s="219">
-        <f>SUM(G68, G45, G32)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H69" s="219">
-        <f>SUM(H68, H45, H32)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I69" s="219">
-        <f>SUM(I68, I45, I32)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J69" s="219">
-        <f>SUM(J68, J45, J32)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="258"/>
-      <c r="B72" s="264" t="s">
-        <v>3636</v>
+      <c r="A72" s="253"/>
+      <c r="B72" s="261" t="s">
+        <v>3629</v>
       </c>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" s="258"/>
-      <c r="B73" s="265"/>
+      <c r="A73" s="253"/>
+      <c r="B73" s="262"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -20304,57 +20497,57 @@
     <mergeCell ref="B72:B73"/>
   </mergeCells>
   <conditionalFormatting sqref="A9:A18">
-    <cfRule type="containsText" dxfId="62" priority="7" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="102" priority="7" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:A31">
-    <cfRule type="containsText" dxfId="61" priority="6" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="101" priority="6" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:A44">
-    <cfRule type="containsText" dxfId="60" priority="5" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="100" priority="5" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:A58">
-    <cfRule type="containsText" dxfId="59" priority="4" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="99" priority="4" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:A61">
-    <cfRule type="containsText" dxfId="58" priority="3" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="98" priority="3" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:A64">
-    <cfRule type="containsText" dxfId="57" priority="2" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="97" priority="2" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66:A67">
-    <cfRule type="containsText" dxfId="56" priority="1" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="96" priority="1" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:G18 D21:G31 C32:I33 D35:G44 C45:I46 D48:G58 D60:G61 D63:G64 C68:G68">
-    <cfRule type="expression" dxfId="55" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="10" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D66:G67">
-    <cfRule type="expression" dxfId="54" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="8" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:I7">
-    <cfRule type="expression" dxfId="53" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="9" stopIfTrue="1">
       <formula>D$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J45:J46">
-    <cfRule type="expression" dxfId="52" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="11" stopIfTrue="1">
       <formula>I$6=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20414,7 +20607,7 @@
   </sheetPr>
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -20459,7 +20652,7 @@
         <v>44742</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="32">
+    <row r="6" spans="1:2" ht="16">
       <c r="A6" s="173" t="s">
         <v>2465</v>
       </c>
@@ -20496,8 +20689,8 @@
       <c r="B13" s="210"/>
     </row>
     <row r="14" spans="1:2" ht="15">
-      <c r="A14" s="273" t="s">
-        <v>3638</v>
+      <c r="A14" s="257" t="s">
+        <v>3631</v>
       </c>
       <c r="B14" s="210">
         <f>SUM(B9:B13)</f>
@@ -20527,8 +20720,8 @@
       <c r="B19" s="210"/>
     </row>
     <row r="20" spans="1:2" ht="15">
-      <c r="A20" s="273" t="s">
-        <v>3639</v>
+      <c r="A20" s="257" t="s">
+        <v>3632</v>
       </c>
       <c r="B20" s="210">
         <f>SUM(B16:B19)</f>
@@ -20558,8 +20751,8 @@
       <c r="B25" s="210"/>
     </row>
     <row r="26" spans="1:2" ht="15">
-      <c r="A26" s="274" t="s">
-        <v>3640</v>
+      <c r="A26" s="258" t="s">
+        <v>3633</v>
       </c>
       <c r="B26" s="210">
         <f>SUM(B22:B25)</f>
@@ -20589,8 +20782,8 @@
       <c r="B31" s="210"/>
     </row>
     <row r="32" spans="1:2" ht="15">
-      <c r="A32" s="273" t="s">
-        <v>3641</v>
+      <c r="A32" s="257" t="s">
+        <v>3634</v>
       </c>
       <c r="B32" s="224">
         <f>SUM(B28:B31)</f>
@@ -20607,14 +20800,14 @@
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="269" t="s">
-        <v>3636</v>
-      </c>
-      <c r="B36" s="264"/>
+      <c r="A36" s="266" t="s">
+        <v>3629</v>
+      </c>
+      <c r="B36" s="261"/>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="270"/>
-      <c r="B37" s="265"/>
+      <c r="A37" s="267"/>
+      <c r="B37" s="262"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -20631,8 +20824,8 @@
   </sheetPr>
   <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView topLeftCell="A5" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -21992,35 +22185,35 @@
       <c r="J71" s="20"/>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="255"/>
-      <c r="B72" s="253" t="s">
-        <v>3636</v>
+      <c r="A72" s="250"/>
+      <c r="B72" s="248" t="s">
+        <v>3629</v>
       </c>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" s="255"/>
-      <c r="B73" s="254"/>
+      <c r="A73" s="250"/>
+      <c r="B73" s="249"/>
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="A9:A22">
-    <cfRule type="containsText" dxfId="51" priority="3" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="91" priority="3" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:A34">
-    <cfRule type="containsText" dxfId="50" priority="2" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="90" priority="2" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:A53">
-    <cfRule type="containsText" dxfId="49" priority="1" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="89" priority="1" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:I7 D8:J23 C23 D25:J35 C35 C36:J36 D37:J63 C59:J60 J64 D65:J69 D71:J71">
-    <cfRule type="expression" dxfId="48" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="20" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22075,7 +22268,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -22124,7 +22317,7 @@
         <v>2852</v>
       </c>
       <c r="B6" s="174">
-        <f>'GovFund Balance Sheet'!J68</f>
+        <f>'GovFund Balance Sheet'!J60</f>
         <v>0</v>
       </c>
     </row>
@@ -22155,8 +22348,8 @@
       <c r="B12" s="210"/>
     </row>
     <row r="13" spans="1:2" ht="15">
-      <c r="A13" s="273" t="s">
-        <v>3642</v>
+      <c r="A13" s="257" t="s">
+        <v>3635</v>
       </c>
       <c r="B13" s="210">
         <f>SUM(B9:B12)</f>
@@ -22186,8 +22379,8 @@
       <c r="B18" s="210"/>
     </row>
     <row r="19" spans="1:2" ht="15">
-      <c r="A19" s="273" t="s">
-        <v>3643</v>
+      <c r="A19" s="257" t="s">
+        <v>3636</v>
       </c>
       <c r="B19" s="210">
         <f>SUM(B15:B18)</f>
@@ -22217,8 +22410,8 @@
       <c r="B24" s="210"/>
     </row>
     <row r="25" spans="1:2" ht="15">
-      <c r="A25" s="273" t="s">
-        <v>3644</v>
+      <c r="A25" s="257" t="s">
+        <v>3637</v>
       </c>
       <c r="B25" s="210">
         <f>SUM(B21:B24)</f>
@@ -22229,17 +22422,20 @@
       <c r="A26" s="176" t="s">
         <v>2850</v>
       </c>
-      <c r="B26" s="175"/>
+      <c r="B26" s="175">
+        <f>B6+B13+B19+B25</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="269" t="s">
-        <v>3636</v>
-      </c>
-      <c r="B29" s="264"/>
+      <c r="A29" s="266" t="s">
+        <v>3629</v>
+      </c>
+      <c r="B29" s="261"/>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="270"/>
-      <c r="B30" s="265"/>
+      <c r="A30" s="267"/>
+      <c r="B30" s="262"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -22256,8 +22452,8 @@
   </sheetPr>
   <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P101" sqref="P101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -22685,29 +22881,29 @@
         <f>SUM(C10:C23)</f>
         <v>0</v>
       </c>
-      <c r="D24" s="231" t="str">
-        <f t="shared" ref="D24:I24" si="1">IF(D$7="Type fund name","",SUM(D10:D23))</f>
-        <v/>
-      </c>
-      <c r="E24" s="231" t="str">
+      <c r="D24" s="231">
+        <f t="shared" ref="D24:I24" si="1">SUM(D10:D23)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="231">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F24" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="F24" s="231">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G24" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="G24" s="231">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H24" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="H24" s="231">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I24" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="I24" s="231">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J24" s="231">
         <f>IF(J7="","",SUM(J10:J23))</f>
@@ -22955,29 +23151,29 @@
         <f>SUM(C26:C32)</f>
         <v>0</v>
       </c>
-      <c r="D38" s="231" t="str">
-        <f t="shared" ref="D38:I38" si="4">IF(D$7="Type fund name","",SUM(D26:D32))</f>
-        <v/>
-      </c>
-      <c r="E38" s="231" t="str">
+      <c r="D38" s="231">
+        <f t="shared" ref="D38:I38" si="4">SUM(D26:D32)</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="231">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F38" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="F38" s="231">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="G38" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="G38" s="231">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H38" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="H38" s="231">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="I38" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="I38" s="231">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J38" s="231">
         <f>IF(J7="","",SUM(J26:J37))</f>
@@ -22995,29 +23191,29 @@
         <f>C24+C38</f>
         <v>0</v>
       </c>
-      <c r="D39" s="232" t="str">
-        <f t="shared" ref="D39:I39" si="5">IF(D$7="Type fund name","",D24+D38)</f>
-        <v/>
-      </c>
-      <c r="E39" s="232" t="str">
+      <c r="D39" s="219">
+        <f t="shared" ref="D39:I39" si="5">D24+D38</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="219">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F39" s="232" t="str">
+        <v>0</v>
+      </c>
+      <c r="F39" s="219">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="G39" s="232" t="str">
+        <v>0</v>
+      </c>
+      <c r="G39" s="219">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="H39" s="232" t="str">
+        <v>0</v>
+      </c>
+      <c r="H39" s="219">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I39" s="232" t="str">
+        <v>0</v>
+      </c>
+      <c r="I39" s="219">
         <f t="shared" si="5"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J39" s="219">
         <f>IF(J7="","",J24+J38)</f>
@@ -23259,29 +23455,29 @@
         <f>IF(C$7="","",SUM(C42:C52))</f>
         <v>0</v>
       </c>
-      <c r="D53" s="231" t="str">
-        <f t="shared" ref="D53:I53" si="7">IF(D$7="Type fund name","",SUM(D42:D52))</f>
-        <v/>
-      </c>
-      <c r="E53" s="231" t="str">
+      <c r="D53" s="231">
+        <f t="shared" ref="D53:I53" si="7">IF(D$7="","",SUM(D42:D52))</f>
+        <v>0</v>
+      </c>
+      <c r="E53" s="231">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="F53" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="F53" s="231">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G53" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="G53" s="231">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="H53" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="H53" s="231">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="I53" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="I53" s="231">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J53" s="231">
         <f t="shared" si="6"/>
@@ -23537,29 +23733,29 @@
         <f>IF(C$7="","",SUM(C57:C67))</f>
         <v>0</v>
       </c>
-      <c r="D68" s="231" t="str">
-        <f t="shared" ref="D68:I68" si="10">IF(D$7="Type fund name","",SUM(D57:D67))</f>
-        <v/>
-      </c>
-      <c r="E68" s="231" t="str">
+      <c r="D68" s="231">
+        <f t="shared" ref="D68:I68" si="10">IF(D$7="","",SUM(D57:D67))</f>
+        <v>0</v>
+      </c>
+      <c r="E68" s="231">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="F68" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="F68" s="231">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G68" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="G68" s="231">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H68" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="H68" s="231">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="I68" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="I68" s="231">
         <f t="shared" si="10"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J68" s="231">
         <f t="shared" si="8"/>
@@ -23798,29 +23994,29 @@
         <f>SUM(C70:C78)</f>
         <v>0</v>
       </c>
-      <c r="D82" s="231" t="str">
-        <f t="shared" ref="D82:I82" si="13">IF(D$7="Type fund name","",SUM(D70:D78))</f>
-        <v/>
-      </c>
-      <c r="E82" s="231" t="str">
+      <c r="D82" s="231">
+        <f t="shared" ref="D82:I82" si="13">SUM(D70:D78)</f>
+        <v>0</v>
+      </c>
+      <c r="E82" s="231">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="F82" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="F82" s="231">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="G82" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="G82" s="231">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="H82" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="H82" s="231">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I82" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="I82" s="231">
         <f t="shared" si="13"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J82" s="231">
         <f t="shared" si="11"/>
@@ -23838,29 +24034,29 @@
         <f>C68+C82</f>
         <v>0</v>
       </c>
-      <c r="D83" s="219" t="str">
-        <f t="shared" ref="D83:I83" si="14">IF(D$7 = "Type fund name", "", D68+D82)</f>
-        <v/>
-      </c>
-      <c r="E83" s="219" t="str">
+      <c r="D83" s="219">
+        <f t="shared" ref="D83:I83" si="14">D68+D82</f>
+        <v>0</v>
+      </c>
+      <c r="E83" s="219">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="F83" s="219" t="str">
+        <v>0</v>
+      </c>
+      <c r="F83" s="219">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="G83" s="219" t="str">
+        <v>0</v>
+      </c>
+      <c r="G83" s="219">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="H83" s="219" t="str">
+        <v>0</v>
+      </c>
+      <c r="H83" s="219">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="I83" s="219" t="str">
+        <v>0</v>
+      </c>
+      <c r="I83" s="219">
         <f t="shared" si="14"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J83" s="233">
         <f t="shared" si="11"/>
@@ -24102,29 +24298,29 @@
         <f>IF(C$7="","",SUM(C86:C96))</f>
         <v>0</v>
       </c>
-      <c r="D97" s="231" t="str">
-        <f t="shared" ref="D97:I97" si="16">IF(D$7="Type fund name","",SUM(D86:D96))</f>
-        <v/>
-      </c>
-      <c r="E97" s="231" t="str">
+      <c r="D97" s="231">
+        <f t="shared" ref="D97:I97" si="16">IF(D$7="","",SUM(D86:D96))</f>
+        <v>0</v>
+      </c>
+      <c r="E97" s="231">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="F97" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="F97" s="231">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="G97" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="G97" s="231">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="H97" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="H97" s="231">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="I97" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="I97" s="231">
         <f t="shared" si="16"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J97" s="231">
         <f t="shared" si="15"/>
@@ -24330,29 +24526,29 @@
         <f>IF(C7="","",SUM(C100:C108))</f>
         <v>0</v>
       </c>
-      <c r="D109" s="219" t="str">
-        <f t="shared" ref="D109:I109" si="18">IF(D7="Type fund name","",SUM(D100:D108))</f>
-        <v/>
-      </c>
-      <c r="E109" s="219" t="str">
+      <c r="D109" s="219">
+        <f t="shared" ref="D109:I109" si="18">IF(D7="","",SUM(D100:D108))</f>
+        <v>0</v>
+      </c>
+      <c r="E109" s="219">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="F109" s="219" t="str">
+        <v>0</v>
+      </c>
+      <c r="F109" s="219">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="G109" s="219" t="str">
+        <v>0</v>
+      </c>
+      <c r="G109" s="219">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="H109" s="219" t="str">
+        <v>0</v>
+      </c>
+      <c r="H109" s="219">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="I109" s="219" t="str">
+        <v>0</v>
+      </c>
+      <c r="I109" s="219">
         <f t="shared" si="18"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J109" s="232">
         <f t="shared" si="17"/>
@@ -24384,9 +24580,9 @@
       <c r="J111" s="112"/>
     </row>
     <row r="112" spans="1:10" s="33" customFormat="1" ht="15" hidden="1">
-      <c r="A112" s="257"/>
-      <c r="B112" s="262" t="s">
-        <v>3636</v>
+      <c r="A112" s="252"/>
+      <c r="B112" s="259" t="s">
+        <v>3629</v>
       </c>
       <c r="C112" s="84"/>
       <c r="D112" s="84"/>
@@ -24398,8 +24594,8 @@
       <c r="J112" s="112"/>
     </row>
     <row r="113" spans="1:10" s="33" customFormat="1" ht="15" hidden="1">
-      <c r="A113" s="257"/>
-      <c r="B113" s="263"/>
+      <c r="A113" s="252"/>
+      <c r="B113" s="260"/>
       <c r="C113" s="84"/>
       <c r="D113" s="84"/>
       <c r="E113" s="84"/>
@@ -24439,62 +24635,57 @@
     <mergeCell ref="B112:B113"/>
   </mergeCells>
   <conditionalFormatting sqref="A10:A23">
-    <cfRule type="containsText" dxfId="47" priority="14" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="87" priority="14" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:A37">
-    <cfRule type="containsText" dxfId="46" priority="13" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="86" priority="13" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:A52">
-    <cfRule type="containsText" dxfId="45" priority="5" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="85" priority="5" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:A67">
-    <cfRule type="containsText" dxfId="44" priority="12" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="84" priority="12" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:A81">
-    <cfRule type="containsText" dxfId="43" priority="11" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="83" priority="11" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86:A96">
-    <cfRule type="containsText" dxfId="42" priority="1" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="82" priority="1" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100:A108">
-    <cfRule type="containsText" dxfId="41" priority="10" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="81" priority="10" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A100)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24 C38 C68:I68 C82:C83 C109:I109">
-    <cfRule type="expression" dxfId="40" priority="20" stopIfTrue="1">
+  <conditionalFormatting sqref="C24:I24 C38:I38 C68:I68 C82:I83 C109:I109">
+    <cfRule type="expression" dxfId="80" priority="20" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53:I53">
-    <cfRule type="expression" dxfId="39" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="6" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C97:I97">
-    <cfRule type="expression" dxfId="38" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="2" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D82:I82">
-    <cfRule type="expression" dxfId="37" priority="18" stopIfTrue="1">
-      <formula>D$7=""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="expression" dxfId="36" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="17" stopIfTrue="1">
       <formula>K$6=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24558,8 +24749,8 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView topLeftCell="A28" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -24972,29 +25163,29 @@
         <f>IF(C$7="","",SUM(C9:C22))</f>
         <v>0</v>
       </c>
-      <c r="D23" s="231" t="str">
-        <f t="shared" ref="D23:I23" si="1">IF(D$7="Type fund name","",SUM(D9:D22))</f>
-        <v/>
-      </c>
-      <c r="E23" s="231" t="str">
+      <c r="D23" s="231">
+        <f t="shared" ref="D23:I23" si="1">IF(D$7="","",SUM(D9:D22))</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="231">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F23" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="F23" s="231">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G23" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="G23" s="231">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H23" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="H23" s="231">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I23" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="I23" s="231">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J23" s="231">
         <f>IF(J7="","",SUM(J9:J22))</f>
@@ -25254,29 +25445,29 @@
         <f>IF(C7="","",SUM(C26:C32))</f>
         <v>0</v>
       </c>
-      <c r="D38" s="231" t="str">
-        <f t="shared" ref="D38:I38" si="3">IF(D$7="Type fund name","",SUM(D26:D32))</f>
-        <v/>
-      </c>
-      <c r="E38" s="231" t="str">
+      <c r="D38" s="231">
+        <f t="shared" ref="D38:I38" si="3">IF(D7="","",SUM(D26:D32))</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="231">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="F38" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="F38" s="231">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G38" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="G38" s="231">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H38" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="H38" s="231">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I38" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="I38" s="231">
         <f t="shared" si="3"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J38" s="231">
         <f>IF(J7="","",SUM(J26:J37))</f>
@@ -25515,29 +25706,29 @@
         <f>IF(C7="","",SUM(C41:C51))</f>
         <v>0</v>
       </c>
-      <c r="D52" s="231" t="str">
-        <f t="shared" ref="D52:I52" si="6">IF(D$7="Type fund name","",SUM(D41:D51))</f>
-        <v/>
-      </c>
-      <c r="E52" s="231" t="str">
+      <c r="D52" s="231">
+        <f t="shared" ref="D52:I52" si="6">IF(D7="","",SUM(D41:D51))</f>
+        <v>0</v>
+      </c>
+      <c r="E52" s="231">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F52" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="F52" s="231">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="G52" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="G52" s="231">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H52" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="H52" s="231">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I52" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="I52" s="231">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J52" s="231">
         <f t="shared" si="4"/>
@@ -25556,11 +25747,11 @@
         <v>0</v>
       </c>
       <c r="D53" s="232" t="str">
-        <f t="shared" ref="D53:I53" si="7">IF(D$7="Type fund name","",D23-D38+D52)</f>
+        <f>IF(D$7="Type fund name","",D23-D38+D52)</f>
         <v/>
       </c>
       <c r="E53" s="232" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="E53:I53" si="7">IF(E$7="Type fund name","",E23-E38+E52)</f>
         <v/>
       </c>
       <c r="F53" s="232" t="str">
@@ -25783,29 +25974,29 @@
         <f>IF(C7="","",SUM(C56:C64))</f>
         <v>0</v>
       </c>
-      <c r="D65" s="231" t="str">
-        <f t="shared" ref="D65:I65" si="10">IF(D$7="Type fund name","",SUM(D56:D64))</f>
-        <v/>
-      </c>
-      <c r="E65" s="231" t="str">
+      <c r="D65" s="231">
+        <f t="shared" ref="D65:I65" si="10">IF(D7="","",SUM(D56:D64))</f>
+        <v>0</v>
+      </c>
+      <c r="E65" s="231">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="F65" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="F65" s="231">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G65" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="G65" s="231">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H65" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="H65" s="231">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="I65" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="I65" s="231">
         <f t="shared" si="10"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J65" s="231">
         <f t="shared" si="8"/>
@@ -25824,10 +26015,13 @@
         <v>0</v>
       </c>
       <c r="D66" s="233" t="str">
-        <f t="shared" ref="D66:I66" si="11">IF(D$7="Type fund name","",D53+D65)</f>
+        <f>IF(D$7="Type fund name","",D53+D65)</f>
         <v/>
       </c>
-      <c r="E66" s="233"/>
+      <c r="E66" s="233" t="str">
+        <f t="shared" ref="E66:I66" si="11">IF(E$7="Type fund name","",E53+E65)</f>
+        <v/>
+      </c>
       <c r="F66" s="233" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -25948,15 +26142,15 @@
       <c r="J72" s="112"/>
     </row>
     <row r="73" spans="1:10" ht="15">
-      <c r="A73" s="259"/>
-      <c r="B73" s="271" t="s">
-        <v>3636</v>
+      <c r="A73" s="254"/>
+      <c r="B73" s="268" t="s">
+        <v>3629</v>
       </c>
       <c r="J73" s="112"/>
     </row>
     <row r="74" spans="1:10" ht="15">
-      <c r="A74" s="259"/>
-      <c r="B74" s="272"/>
+      <c r="A74" s="254"/>
+      <c r="B74" s="269"/>
       <c r="J74" s="112"/>
     </row>
     <row r="75" spans="1:10" ht="15">
@@ -26040,58 +26234,58 @@
     <mergeCell ref="B73:B74"/>
   </mergeCells>
   <conditionalFormatting sqref="A9:A22">
-    <cfRule type="containsText" dxfId="35" priority="4" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="76" priority="4" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:A37">
-    <cfRule type="containsText" dxfId="34" priority="3" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:A51">
-    <cfRule type="containsText" dxfId="33" priority="2" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="74" priority="2" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:A64">
-    <cfRule type="containsText" dxfId="32" priority="1" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="73" priority="1" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A56)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23:C24 C38:C39 C70:J70">
-    <cfRule type="expression" dxfId="31" priority="15" stopIfTrue="1">
-      <formula>C$7=""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="30" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="7" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:I54">
-    <cfRule type="expression" dxfId="29" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="6" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65:I66">
-    <cfRule type="expression" dxfId="28" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="5" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:J70">
-    <cfRule type="cellIs" dxfId="27" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="16" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="17" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="18" operator="notEqual">
+    <cfRule type="cellIs" dxfId="67" priority="18" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D23:I23 C23:C24 D38:I38 C38:C39 C70:J70">
+    <cfRule type="expression" dxfId="66" priority="15" stopIfTrue="1">
+      <formula>C$7=""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D70:I70">
-    <cfRule type="expression" dxfId="24" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="19" stopIfTrue="1">
       <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26137,8 +26331,8 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="74" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView zoomScale="74" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -26540,32 +26734,32 @@
         <f>IF(C$7="","",SUM(C9:C22))</f>
         <v>0</v>
       </c>
-      <c r="D23" s="231" t="str">
-        <f t="shared" ref="D23:J23" si="1">IF(D$7="Type fund name","",SUM(D9:D22))</f>
-        <v/>
-      </c>
-      <c r="E23" s="231" t="str">
+      <c r="D23" s="231">
+        <f t="shared" ref="D23:I23" si="1">IF(D$7="","",SUM(D9:D22))</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="231">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="F23" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="F23" s="231">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G23" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="G23" s="231">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H23" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="H23" s="231">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I23" s="231" t="str">
+        <v>0</v>
+      </c>
+      <c r="I23" s="231">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J23" s="231">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J23" si="2">IF(J$7="Type fund name","",SUM(J9:J22))</f>
         <v>0</v>
       </c>
     </row>
@@ -26629,7 +26823,7 @@
       <c r="H27" s="208"/>
       <c r="I27" s="208"/>
       <c r="J27" s="235">
-        <f t="shared" ref="J27:J38" si="2">SUM(D27:I27)</f>
+        <f t="shared" ref="J27:J38" si="3">SUM(D27:I27)</f>
         <v>0</v>
       </c>
     </row>
@@ -26648,7 +26842,7 @@
       <c r="H28" s="208"/>
       <c r="I28" s="208"/>
       <c r="J28" s="235">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26667,7 +26861,7 @@
       <c r="H29" s="208"/>
       <c r="I29" s="208"/>
       <c r="J29" s="235">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26686,7 +26880,7 @@
       <c r="H30" s="208"/>
       <c r="I30" s="208"/>
       <c r="J30" s="235">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26705,7 +26899,7 @@
       <c r="H31" s="208"/>
       <c r="I31" s="208"/>
       <c r="J31" s="235">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26724,7 +26918,7 @@
       <c r="H32" s="208"/>
       <c r="I32" s="208"/>
       <c r="J32" s="235">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26743,7 +26937,7 @@
       <c r="H33" s="208"/>
       <c r="I33" s="208"/>
       <c r="J33" s="235">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26762,7 +26956,7 @@
       <c r="H34" s="208"/>
       <c r="I34" s="208"/>
       <c r="J34" s="235">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26781,7 +26975,7 @@
       <c r="H35" s="208"/>
       <c r="I35" s="208"/>
       <c r="J35" s="235">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26800,7 +26994,7 @@
       <c r="H36" s="208"/>
       <c r="I36" s="208"/>
       <c r="J36" s="235">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26819,7 +27013,7 @@
       <c r="H37" s="208"/>
       <c r="I37" s="208"/>
       <c r="J37" s="235">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -26834,32 +27028,32 @@
         <f>IF(C7="","",SUM(C26:C37))</f>
         <v>0</v>
       </c>
-      <c r="D38" s="231" t="str">
-        <f t="shared" ref="D38:I38" si="3">IF(D$7="Type fund name","",SUM(D26:D32))</f>
-        <v/>
-      </c>
-      <c r="E38" s="231" t="str">
+      <c r="D38" s="200">
+        <f t="shared" ref="D38:I38" si="4">IF(D7="","",SUM(D26:D37))</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="200">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="200">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G38" s="200">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H38" s="200">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I38" s="200">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="235">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="F38" s="231" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G38" s="231" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H38" s="231" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I38" s="231" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="J38" s="235">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -26923,7 +27117,7 @@
       <c r="H42" s="209"/>
       <c r="I42" s="209"/>
       <c r="J42" s="235">
-        <f t="shared" ref="J42:J64" si="4">SUM(D42:I42)</f>
+        <f t="shared" ref="J42:J64" si="5">SUM(D42:I42)</f>
         <v>0</v>
       </c>
     </row>
@@ -26942,7 +27136,7 @@
       <c r="H43" s="208"/>
       <c r="I43" s="208"/>
       <c r="J43" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -26961,7 +27155,7 @@
       <c r="H44" s="208"/>
       <c r="I44" s="208"/>
       <c r="J44" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -26980,7 +27174,7 @@
       <c r="H45" s="208"/>
       <c r="I45" s="208"/>
       <c r="J45" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -26999,7 +27193,7 @@
       <c r="H46" s="208"/>
       <c r="I46" s="208"/>
       <c r="J46" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -27018,7 +27212,7 @@
       <c r="H47" s="208"/>
       <c r="I47" s="208"/>
       <c r="J47" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -27037,7 +27231,7 @@
       <c r="H48" s="208"/>
       <c r="I48" s="208"/>
       <c r="J48" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -27056,7 +27250,7 @@
       <c r="H49" s="208"/>
       <c r="I49" s="208"/>
       <c r="J49" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -27075,7 +27269,7 @@
       <c r="H50" s="208"/>
       <c r="I50" s="208"/>
       <c r="J50" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -27094,7 +27288,7 @@
       <c r="H51" s="208"/>
       <c r="I51" s="208"/>
       <c r="J51" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -27109,32 +27303,32 @@
         <f>IF(C7="","",SUM(C41:C51))</f>
         <v>0</v>
       </c>
-      <c r="D52" s="231" t="str">
-        <f t="shared" ref="D52:I52" si="5">IF(D$7="Type fund name","",SUM(D41:D51))</f>
-        <v/>
-      </c>
-      <c r="E52" s="231" t="str">
+      <c r="D52" s="200">
+        <f t="shared" ref="D52:I52" si="6">IF(D7="","",SUM(D41:D51))</f>
+        <v>0</v>
+      </c>
+      <c r="E52" s="200">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="200">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G52" s="200">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H52" s="200">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I52" s="200">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J52" s="235">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F52" s="231" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="G52" s="231" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="H52" s="231" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I52" s="231" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="J52" s="235">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -27179,7 +27373,7 @@
       <c r="H55" s="208"/>
       <c r="I55" s="208"/>
       <c r="J55" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -27198,7 +27392,7 @@
       <c r="H56" s="208"/>
       <c r="I56" s="208"/>
       <c r="J56" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -27217,7 +27411,7 @@
       <c r="H57" s="208"/>
       <c r="I57" s="208"/>
       <c r="J57" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -27236,7 +27430,7 @@
       <c r="H58" s="208"/>
       <c r="I58" s="208"/>
       <c r="J58" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -27255,7 +27449,7 @@
       <c r="H59" s="208"/>
       <c r="I59" s="208"/>
       <c r="J59" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -27274,7 +27468,7 @@
       <c r="H60" s="208"/>
       <c r="I60" s="208"/>
       <c r="J60" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -27293,7 +27487,7 @@
       <c r="H61" s="208"/>
       <c r="I61" s="208"/>
       <c r="J61" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -27312,7 +27506,7 @@
       <c r="H62" s="208"/>
       <c r="I62" s="208"/>
       <c r="J62" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -27331,7 +27525,7 @@
       <c r="H63" s="208"/>
       <c r="I63" s="208"/>
       <c r="J63" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -27346,32 +27540,32 @@
         <f>IF(C7="","",SUM(C55:C63))</f>
         <v>0</v>
       </c>
-      <c r="D64" s="231" t="str">
-        <f t="shared" ref="D64:I64" si="6">IF(D$7="Type fund name","",SUM(D55:D63))</f>
-        <v/>
-      </c>
-      <c r="E64" s="231" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F64" s="231" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="G64" s="231" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H64" s="231" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I64" s="231" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+      <c r="D64" s="231">
+        <f t="shared" ref="D64:H64" si="7">IF(D7="","",SUM(D55:D63))</f>
+        <v>0</v>
+      </c>
+      <c r="E64" s="231">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F64" s="231">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G64" s="231">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H64" s="231">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I64" s="231">
+        <f>IF(I7="","",SUM(I55:I63))</f>
+        <v>0</v>
       </c>
       <c r="J64" s="235">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -27386,32 +27580,32 @@
         <f>C23+C38+C52+C64</f>
         <v>0</v>
       </c>
-      <c r="D65" s="219" t="str">
-        <f t="shared" ref="D65:J65" si="7">IF(D7="Type fund name","",D23+D38+D52+D64)</f>
-        <v/>
-      </c>
-      <c r="E65" s="219" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="F65" s="219" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G65" s="219" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="H65" s="219" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="I65" s="219" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+      <c r="D65" s="236">
+        <f t="shared" ref="D65:I65" si="8">D23+D38+D52+D64</f>
+        <v>0</v>
+      </c>
+      <c r="E65" s="236">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F65" s="236">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G65" s="236">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H65" s="236">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I65" s="236">
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="J65" s="219">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="J65" si="9">IF(J7="Type fund name","",J23+J38+J52+J64)</f>
         <v>0</v>
       </c>
     </row>
@@ -27456,7 +27650,7 @@
       <c r="H68" s="237"/>
       <c r="I68" s="237"/>
       <c r="J68" s="235">
-        <f t="shared" ref="J68" si="8">SUM(D68:I68)</f>
+        <f t="shared" ref="J68" si="10">SUM(D68:I68)</f>
         <v>0</v>
       </c>
     </row>
@@ -27467,29 +27661,32 @@
       <c r="B69" s="152" t="s">
         <v>2463</v>
       </c>
-      <c r="C69" s="238"/>
+      <c r="C69" s="219">
+        <f>IF(C7="Type fund name","",C65+C68)</f>
+        <v>0</v>
+      </c>
       <c r="D69" s="219" t="str">
-        <f t="shared" ref="D69:I69" si="9">IF(D7="Type fund name","",D65+D68)</f>
+        <f>IF(D7="Type fund name","",D65+D68)</f>
         <v/>
       </c>
       <c r="E69" s="219" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="E69:I69" si="11">IF(E7="Type fund name","",E65+E68)</f>
         <v/>
       </c>
       <c r="F69" s="219" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="G69" s="219" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H69" s="219" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="I69" s="219" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="J69" s="219">
@@ -27582,9 +27779,9 @@
       <c r="J76" s="138"/>
     </row>
     <row r="77" spans="1:10" ht="15">
-      <c r="A77" s="257"/>
-      <c r="B77" s="262" t="s">
-        <v>3636</v>
+      <c r="A77" s="252"/>
+      <c r="B77" s="259" t="s">
+        <v>3629</v>
       </c>
       <c r="C77" s="155"/>
       <c r="D77" s="155"/>
@@ -27596,8 +27793,8 @@
       <c r="J77" s="138"/>
     </row>
     <row r="78" spans="1:10" ht="15">
-      <c r="A78" s="257"/>
-      <c r="B78" s="263"/>
+      <c r="A78" s="252"/>
+      <c r="B78" s="260"/>
       <c r="C78" s="155"/>
       <c r="D78" s="155"/>
       <c r="E78" s="155"/>
@@ -27623,106 +27820,106 @@
     <mergeCell ref="B77:B78"/>
   </mergeCells>
   <conditionalFormatting sqref="A9:A22">
-    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="64" priority="4" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:A37">
-    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:A51">
-    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="62" priority="2" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55:A63">
-    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="61" priority="1" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A55)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="19" priority="22" stopIfTrue="1">
-      <formula>C$7=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="18" priority="21" stopIfTrue="1">
+  <conditionalFormatting sqref="C23:I23">
+    <cfRule type="expression" dxfId="60" priority="22" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:I24 C53:I53">
-    <cfRule type="expression" dxfId="17" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="28" stopIfTrue="1">
       <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C38:I38">
+    <cfRule type="expression" dxfId="58" priority="21" stopIfTrue="1">
+      <formula>C$7=""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C52:I52">
-    <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="19" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:I64">
-    <cfRule type="expression" dxfId="15" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="17" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D69:I69">
-    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
+  <conditionalFormatting sqref="C69:I69">
+    <cfRule type="expression" dxfId="55" priority="16" stopIfTrue="1">
       <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D65:J65">
-    <cfRule type="expression" dxfId="13" priority="7" stopIfTrue="1">
-      <formula>D$7=""</formula>
+  <conditionalFormatting sqref="C69:J69">
+    <cfRule type="expression" dxfId="54" priority="12" stopIfTrue="1">
+      <formula>C$7=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="13" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="14" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="notEqual">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
-      <formula>#REF!=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D69:J69">
-    <cfRule type="expression" dxfId="8" priority="12" stopIfTrue="1">
-      <formula>D$7=""</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="13" stopIfTrue="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="14" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="15" operator="notEqual">
+    <cfRule type="cellIs" dxfId="51" priority="15" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J4 J8:J22 J24:J64 J70:J1048574">
-    <cfRule type="expression" dxfId="4" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="23" stopIfTrue="1">
       <formula>COUNTA(D2:I2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:J22 J24:J64 J70:J78">
-    <cfRule type="expression" dxfId="3" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="84" stopIfTrue="1">
+      <formula>#REF!=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J65">
+    <cfRule type="expression" dxfId="48" priority="7" stopIfTrue="1">
+      <formula>J$7=""</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="8" stopIfTrue="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="9" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="10" operator="notEqual">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="11" stopIfTrue="1">
       <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J68">
-    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="5" stopIfTrue="1">
       <formula>COUNTA(D69:I69)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="6" stopIfTrue="1">
       <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1048575:J1048576">
-    <cfRule type="expression" dxfId="0" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="86" stopIfTrue="1">
       <formula>COUNTA(D1:I3)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30984,7 +31181,7 @@
       <c r="C340" s="184"/>
     </row>
     <row r="341" spans="3:3" ht="15">
-      <c r="C341" s="241"/>
+      <c r="C341" s="240"/>
     </row>
     <row r="342" spans="3:3" ht="15">
       <c r="C342" s="184"/>
@@ -41077,19 +41274,19 @@
       <c r="C121" s="184"/>
     </row>
     <row r="122" spans="3:3" ht="15">
-      <c r="C122" s="239"/>
+      <c r="C122" s="238"/>
     </row>
     <row r="123" spans="3:3" ht="15">
-      <c r="C123" s="239"/>
+      <c r="C123" s="238"/>
     </row>
     <row r="124" spans="3:3" ht="15">
-      <c r="C124" s="239"/>
+      <c r="C124" s="238"/>
     </row>
     <row r="125" spans="3:3" ht="15">
-      <c r="C125" s="239"/>
+      <c r="C125" s="238"/>
     </row>
     <row r="126" spans="3:3" ht="15">
-      <c r="C126" s="240"/>
+      <c r="C126" s="239"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D126">
@@ -47428,7 +47625,7 @@
       <c r="C413" s="21"/>
     </row>
     <row r="414" spans="3:3" ht="15">
-      <c r="C414" s="248"/>
+      <c r="C414" s="243"/>
     </row>
     <row r="415" spans="3:3" ht="15">
       <c r="C415" s="21"/>
@@ -47525,10 +47722,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8474313-8EAC-0141-BA8E-861AF31ED060}">
-  <dimension ref="B1:E40"/>
+  <dimension ref="B1:E42"/>
   <sheetViews>
-    <sheetView zoomScale="92" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -47581,9 +47778,12 @@
       </c>
       <c r="E6" s="2"/>
     </row>
+    <row r="7" spans="2:5">
+      <c r="E7" s="2"/>
+    </row>
     <row r="10" spans="2:5" ht="14">
-      <c r="B10" s="252" t="s">
-        <v>3634</v>
+      <c r="B10" s="247" t="s">
+        <v>3627</v>
       </c>
     </row>
     <row r="11" spans="2:5">
@@ -47597,87 +47797,95 @@
       </c>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" t="s">
+      <c r="B14" s="60" t="s">
+        <v>3638</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="60" t="s">
+        <v>3641</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="2" t="s">
+        <v>3628</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="2" t="s">
+        <v>3639</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="60" t="s">
+        <v>3642</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
         <v>3620</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="B15" s="2" t="s">
-        <v>3635</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="B16" t="s">
-        <v>3621</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" t="s">
-        <v>3622</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" t="s">
-        <v>3623</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" t="s">
-        <v>3624</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>3625</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" t="s">
-        <v>3626</v>
+        <v>3621</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="60" t="s">
+        <v>3643</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>3627</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" t="s">
-        <v>3628</v>
+        <v>3622</v>
       </c>
     </row>
     <row r="27" spans="2:2">
-      <c r="B27" t="s">
-        <v>3629</v>
+      <c r="B27" s="60" t="s">
+        <v>3644</v>
       </c>
     </row>
     <row r="28" spans="2:2">
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
+        <v>3640</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>3623</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
+        <v>3624</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" s="256" t="s">
         <v>3630</v>
       </c>
     </row>
-    <row r="29" spans="2:2">
-      <c r="B29" s="261" t="s">
-        <v>3637</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2">
-      <c r="B31" t="s">
-        <v>3631</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2">
-      <c r="B32" t="s">
-        <v>3632</v>
-      </c>
-    </row>
     <row r="33" spans="2:2">
-      <c r="B33" t="s">
-        <v>3633</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" s="260"/>
+      <c r="B33" s="60" t="s">
+        <v>3645</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>3625</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" t="s">
+        <v>3626</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="255"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -47696,8 +47904,8 @@
   </sheetPr>
   <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="88" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView topLeftCell="A24" zoomScale="88" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -47896,7 +48104,7 @@
         <f>IF(B16="","Choose from drop-down --&gt;",IF(COUNTIF('Lookup Net Position'!$B$2:$B$514,B16)=0,"acfr:CurrentAssetsCustom",_xlfn.XLOOKUP(B16,'Lookup Net Position'!$B$2:$B$514,'Lookup Net Position'!$C$2:$C$514)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B16" s="251"/>
+      <c r="B16" s="246"/>
       <c r="C16" s="202"/>
       <c r="D16" s="203"/>
       <c r="E16" s="200" t="str">
@@ -49096,17 +49304,17 @@
       <c r="D102" s="37"/>
     </row>
     <row r="103" spans="1:6">
-      <c r="B103" s="256"/>
+      <c r="B103" s="251"/>
     </row>
     <row r="104" spans="1:6">
-      <c r="A104" s="257"/>
-      <c r="B104" s="262" t="s">
-        <v>3636</v>
+      <c r="A104" s="252"/>
+      <c r="B104" s="259" t="s">
+        <v>3629</v>
       </c>
     </row>
     <row r="105" spans="1:6">
-      <c r="A105" s="257"/>
-      <c r="B105" s="263"/>
+      <c r="A105" s="252"/>
+      <c r="B105" s="260"/>
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
@@ -49114,69 +49322,69 @@
     <mergeCell ref="B104:B105"/>
   </mergeCells>
   <conditionalFormatting sqref="A9:A22">
-    <cfRule type="expression" dxfId="94" priority="16">
+    <cfRule type="expression" dxfId="39" priority="21">
       <formula>A9="acfr:CurrentAssetsCustom"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:A31">
-    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="acfr:NonCurrentAssetsCustom">
+    <cfRule type="containsText" dxfId="38" priority="8" operator="containsText" text="acfr:NonCurrentAssetsCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:NonCurrentAssetsCustom",A25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:A45">
-    <cfRule type="containsText" dxfId="92" priority="2" operator="containsText" text="acfr:DeferredOutflowsOfResourcesCustom">
+    <cfRule type="containsText" dxfId="37" priority="7" operator="containsText" text="acfr:DeferredOutflowsOfResourcesCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:DeferredOutflowsOfResourcesCustom",A41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="13" operator="containsText" text="acfr:DeferredOutflowsOfResourcesCustom">
+    <cfRule type="containsText" dxfId="36" priority="18" operator="containsText" text="acfr:DeferredOutflowsOfResourcesCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:DeferredOutflowsOfResourcesCustom",A41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:A59">
-    <cfRule type="containsText" dxfId="90" priority="1" operator="containsText" text="acfr:CurrentLiabilitiesCustom">
+    <cfRule type="containsText" dxfId="35" priority="6" operator="containsText" text="acfr:CurrentLiabilitiesCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:CurrentLiabilitiesCustom",A54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="12" operator="containsText" text="acfr:CurrentLiabilitiesCustom">
+    <cfRule type="containsText" dxfId="34" priority="17" operator="containsText" text="acfr:CurrentLiabilitiesCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:CurrentLiabilitiesCustom",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67:A70">
-    <cfRule type="containsText" dxfId="88" priority="11" operator="containsText" text="acfr:NoncurrentLiabilitiesCustom">
+    <cfRule type="containsText" dxfId="33" priority="16" operator="containsText" text="acfr:NoncurrentLiabilitiesCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:NoncurrentLiabilitiesCustom",A67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A80:A83">
-    <cfRule type="containsText" dxfId="87" priority="10" operator="containsText" text="acfr:DeferredInflowsOfResourcesCustom">
+    <cfRule type="containsText" dxfId="32" priority="15" operator="containsText" text="acfr:DeferredInflowsOfResourcesCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:DeferredInflowsOfResourcesCustom",A80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92:A95">
-    <cfRule type="containsText" dxfId="86" priority="9" operator="containsText" text="acfr:RestrictedComponentsOfNetPositionCustom">
+    <cfRule type="containsText" dxfId="31" priority="14" operator="containsText" text="acfr:RestrictedComponentsOfNetPositionCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:RestrictedComponentsOfNetPositionCustom",A92)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="85" priority="15" operator="containsText" text="acfr:CurrentAssetsCustom">
+    <cfRule type="containsText" dxfId="30" priority="20" operator="containsText" text="acfr:CurrentAssetsCustom">
       <formula>NOT(ISERROR(SEARCH("acfr:CurrentAssetsCustom",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101:F101">
-    <cfRule type="cellIs" dxfId="84" priority="34" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="39" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="35" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="40" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="36" operator="notEqual">
+    <cfRule type="cellIs" dxfId="27" priority="41" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:F37 C23:F23 C37:F37 D39:F101 C50 C65:F65 C76:C77 C89 C101">
-    <cfRule type="expression" dxfId="81" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="23" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M68">
-    <cfRule type="expression" dxfId="80" priority="8">
+    <cfRule type="expression" dxfId="25" priority="13">
       <formula>$A$9:$A$22="acfr:CurrentAssetsCustom"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -49206,6 +49414,72 @@
     <ignoredError sqref="E76" formula="1"/>
   </ignoredErrors>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="5" id="{F4230BA6-F328-4544-8648-B7D94C2E1B2A}">
+            <xm:f>'Master Info'!C5="N"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E8:F101</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="4" id="{AE130514-D2ED-854F-BBE4-3D5DA701565D}">
+            <xm:f>'Master Info'!C5="N"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E38:F38</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="3" id="{571FA1C0-847E-F648-A086-3F79FEE9EA5B}">
+            <xm:f>'Master Info'!C5="N"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="2" id="{F0E706EC-B5FD-434C-B52F-F67351DA57EF}">
+            <xm:f>'Master Info'!C6="N"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F38</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{AC3F68F1-5F2B-BC46-8027-79F6F176A53E}">
+            <xm:f>AND('Master Info'!C5="N", 'Master Info'!C6="N")</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D38</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{17CB63B2-6582-4D03-B5CB-EC836B51979D}">
@@ -49263,8 +49537,8 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="84" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView zoomScale="84" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -49400,20 +49674,20 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B9" s="15"/>
-      <c r="C9" s="242"/>
-      <c r="D9" s="243"/>
-      <c r="E9" s="243"/>
-      <c r="F9" s="243"/>
-      <c r="G9" s="244" t="str">
+      <c r="C9" s="202"/>
+      <c r="D9" s="203"/>
+      <c r="E9" s="203"/>
+      <c r="F9" s="203"/>
+      <c r="G9" s="226" t="str">
         <f>IF(OR(G$6="", B9=""),"",SUM(D9:F9) - C9)</f>
         <v/>
       </c>
-      <c r="H9" s="244"/>
-      <c r="I9" s="245" t="str">
+      <c r="H9" s="226"/>
+      <c r="I9" s="200" t="str">
         <f>IF(OR(I$6="", B9=""),"",SUM(G9:H9))</f>
         <v/>
       </c>
-      <c r="J9" s="244"/>
+      <c r="J9" s="226"/>
     </row>
     <row r="10" spans="1:10" ht="16">
       <c r="A10" s="50" t="str">
@@ -49421,20 +49695,17 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B10" s="15"/>
-      <c r="C10" s="242"/>
-      <c r="D10" s="243"/>
-      <c r="E10" s="243"/>
-      <c r="F10" s="243"/>
-      <c r="G10" s="244" t="str">
-        <f t="shared" ref="G10:G22" si="0">IF(OR(G$6="", B10=""),"",SUM(D10:F10) - C10)</f>
+      <c r="C10" s="202"/>
+      <c r="D10" s="203"/>
+      <c r="E10" s="203"/>
+      <c r="F10" s="203"/>
+      <c r="G10" s="226"/>
+      <c r="H10" s="226"/>
+      <c r="I10" s="200" t="str">
+        <f t="shared" ref="I10:I22" si="0">IF(OR(I$6="", B10=""),"",SUM(G10:H10))</f>
         <v/>
       </c>
-      <c r="H10" s="244"/>
-      <c r="I10" s="245" t="str">
-        <f t="shared" ref="I10:I22" si="1">IF(OR(I$6="", B10=""),"",SUM(G10:H10))</f>
-        <v/>
-      </c>
-      <c r="J10" s="244"/>
+      <c r="J10" s="226"/>
     </row>
     <row r="11" spans="1:10" ht="16">
       <c r="A11" s="50" t="str">
@@ -49442,20 +49713,20 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B11" s="15"/>
-      <c r="C11" s="242"/>
-      <c r="D11" s="243"/>
-      <c r="E11" s="243"/>
-      <c r="F11" s="243"/>
-      <c r="G11" s="244" t="str">
+      <c r="C11" s="202"/>
+      <c r="D11" s="203"/>
+      <c r="E11" s="203"/>
+      <c r="F11" s="203"/>
+      <c r="G11" s="226" t="str">
+        <f t="shared" ref="G11:G22" si="1">IF(OR(G$6="", B11=""),"",SUM(D11:F11) - C11)</f>
+        <v/>
+      </c>
+      <c r="H11" s="226"/>
+      <c r="I11" s="200" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H11" s="244"/>
-      <c r="I11" s="245" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J11" s="244"/>
+      <c r="J11" s="226"/>
     </row>
     <row r="12" spans="1:10" ht="16">
       <c r="A12" s="50" t="str">
@@ -49463,20 +49734,20 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B12" s="15"/>
-      <c r="C12" s="242"/>
-      <c r="D12" s="243"/>
-      <c r="E12" s="243"/>
-      <c r="F12" s="243"/>
-      <c r="G12" s="244" t="str">
+      <c r="C12" s="202"/>
+      <c r="D12" s="203"/>
+      <c r="E12" s="203"/>
+      <c r="F12" s="203"/>
+      <c r="G12" s="226" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H12" s="226"/>
+      <c r="I12" s="200" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H12" s="244"/>
-      <c r="I12" s="245" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J12" s="244"/>
+      <c r="J12" s="226"/>
     </row>
     <row r="13" spans="1:10" ht="16">
       <c r="A13" s="50" t="str">
@@ -49484,20 +49755,17 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B13" s="15"/>
-      <c r="C13" s="242"/>
-      <c r="D13" s="243"/>
-      <c r="E13" s="243"/>
-      <c r="F13" s="243"/>
-      <c r="G13" s="244" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H13" s="244"/>
-      <c r="I13" s="245" t="str">
+      <c r="C13" s="202"/>
+      <c r="D13" s="203"/>
+      <c r="E13" s="203"/>
+      <c r="F13" s="203"/>
+      <c r="G13" s="226" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J13" s="244"/>
+      <c r="H13" s="226"/>
+      <c r="I13" s="200"/>
+      <c r="J13" s="226"/>
     </row>
     <row r="14" spans="1:10" ht="16">
       <c r="A14" s="50" t="str">
@@ -49505,20 +49773,20 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B14" s="15"/>
-      <c r="C14" s="242"/>
-      <c r="D14" s="243"/>
-      <c r="E14" s="243"/>
-      <c r="F14" s="243"/>
-      <c r="G14" s="244" t="str">
+      <c r="C14" s="202"/>
+      <c r="D14" s="203"/>
+      <c r="E14" s="203"/>
+      <c r="F14" s="203"/>
+      <c r="G14" s="226" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H14" s="226"/>
+      <c r="I14" s="200" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H14" s="244"/>
-      <c r="I14" s="245" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J14" s="244"/>
+      <c r="J14" s="226"/>
     </row>
     <row r="15" spans="1:10" ht="16">
       <c r="A15" s="50" t="str">
@@ -49526,20 +49794,20 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B15" s="15"/>
-      <c r="C15" s="242"/>
-      <c r="D15" s="243"/>
-      <c r="E15" s="243"/>
-      <c r="F15" s="243"/>
-      <c r="G15" s="244" t="str">
+      <c r="C15" s="202"/>
+      <c r="D15" s="203"/>
+      <c r="E15" s="203"/>
+      <c r="F15" s="203"/>
+      <c r="G15" s="226" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H15" s="226"/>
+      <c r="I15" s="200" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H15" s="244"/>
-      <c r="I15" s="245" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J15" s="244"/>
+      <c r="J15" s="226"/>
     </row>
     <row r="16" spans="1:10" ht="16">
       <c r="A16" s="50" t="str">
@@ -49547,20 +49815,20 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B16" s="15"/>
-      <c r="C16" s="242"/>
-      <c r="D16" s="243"/>
-      <c r="E16" s="243"/>
-      <c r="F16" s="243"/>
-      <c r="G16" s="244" t="str">
+      <c r="C16" s="202"/>
+      <c r="D16" s="203"/>
+      <c r="E16" s="203"/>
+      <c r="F16" s="203"/>
+      <c r="G16" s="226" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H16" s="226"/>
+      <c r="I16" s="200" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H16" s="244"/>
-      <c r="I16" s="245" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J16" s="244"/>
+      <c r="J16" s="226"/>
     </row>
     <row r="17" spans="1:10" ht="16">
       <c r="A17" s="50" t="str">
@@ -49568,20 +49836,20 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B17" s="15"/>
-      <c r="C17" s="242"/>
-      <c r="D17" s="243"/>
-      <c r="E17" s="243"/>
-      <c r="F17" s="243"/>
-      <c r="G17" s="244" t="str">
+      <c r="C17" s="202"/>
+      <c r="D17" s="203"/>
+      <c r="E17" s="203"/>
+      <c r="F17" s="203"/>
+      <c r="G17" s="226" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H17" s="226"/>
+      <c r="I17" s="200" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H17" s="244"/>
-      <c r="I17" s="245" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J17" s="244"/>
+      <c r="J17" s="226"/>
     </row>
     <row r="18" spans="1:10" ht="16" hidden="1">
       <c r="A18" s="50" t="str">
@@ -49589,20 +49857,20 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B18" s="15"/>
-      <c r="C18" s="242"/>
-      <c r="D18" s="243"/>
-      <c r="E18" s="243"/>
-      <c r="F18" s="243"/>
-      <c r="G18" s="244" t="str">
+      <c r="C18" s="202"/>
+      <c r="D18" s="203"/>
+      <c r="E18" s="203"/>
+      <c r="F18" s="203"/>
+      <c r="G18" s="226" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H18" s="226"/>
+      <c r="I18" s="200" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H18" s="244"/>
-      <c r="I18" s="245" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J18" s="244"/>
+      <c r="J18" s="226"/>
     </row>
     <row r="19" spans="1:10" ht="16" hidden="1">
       <c r="A19" s="50" t="str">
@@ -49610,20 +49878,20 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B19" s="15"/>
-      <c r="C19" s="242"/>
-      <c r="D19" s="243"/>
-      <c r="E19" s="243"/>
-      <c r="F19" s="243"/>
-      <c r="G19" s="244" t="str">
+      <c r="C19" s="202"/>
+      <c r="D19" s="203"/>
+      <c r="E19" s="203"/>
+      <c r="F19" s="203"/>
+      <c r="G19" s="226" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H19" s="226"/>
+      <c r="I19" s="200" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H19" s="244"/>
-      <c r="I19" s="245" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J19" s="244"/>
+      <c r="J19" s="226"/>
     </row>
     <row r="20" spans="1:10" ht="16" hidden="1">
       <c r="A20" s="50" t="str">
@@ -49631,20 +49899,20 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B20" s="15"/>
-      <c r="C20" s="242"/>
-      <c r="D20" s="243"/>
-      <c r="E20" s="243"/>
-      <c r="F20" s="243"/>
-      <c r="G20" s="244" t="str">
+      <c r="C20" s="202"/>
+      <c r="D20" s="203"/>
+      <c r="E20" s="203"/>
+      <c r="F20" s="203"/>
+      <c r="G20" s="226" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H20" s="226"/>
+      <c r="I20" s="200" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H20" s="244"/>
-      <c r="I20" s="245" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J20" s="244"/>
+      <c r="J20" s="226"/>
     </row>
     <row r="21" spans="1:10" ht="16" hidden="1">
       <c r="A21" s="50" t="str">
@@ -49652,20 +49920,20 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B21" s="15"/>
-      <c r="C21" s="242"/>
-      <c r="D21" s="243"/>
-      <c r="E21" s="243"/>
-      <c r="F21" s="243"/>
-      <c r="G21" s="244" t="str">
+      <c r="C21" s="202"/>
+      <c r="D21" s="203"/>
+      <c r="E21" s="203"/>
+      <c r="F21" s="203"/>
+      <c r="G21" s="226" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H21" s="226"/>
+      <c r="I21" s="200" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H21" s="244"/>
-      <c r="I21" s="245" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J21" s="244"/>
+      <c r="J21" s="226"/>
     </row>
     <row r="22" spans="1:10" ht="16">
       <c r="A22" s="50" t="str">
@@ -49673,20 +49941,20 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B22" s="15"/>
-      <c r="C22" s="242"/>
-      <c r="D22" s="243"/>
-      <c r="E22" s="243"/>
-      <c r="F22" s="243"/>
-      <c r="G22" s="244" t="str">
+      <c r="C22" s="202"/>
+      <c r="D22" s="203"/>
+      <c r="E22" s="203"/>
+      <c r="F22" s="203"/>
+      <c r="G22" s="226" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H22" s="226"/>
+      <c r="I22" s="200" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H22" s="244"/>
-      <c r="I22" s="245" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J22" s="244"/>
+      <c r="J22" s="226"/>
     </row>
     <row r="23" spans="1:10" ht="15">
       <c r="A23" s="6" t="s">
@@ -49695,32 +49963,35 @@
       <c r="B23" s="6" t="s">
         <v>1100</v>
       </c>
-      <c r="C23" s="245">
-        <f t="shared" ref="C23:I23" si="2">IF(C6="","",SUM(C9:C22))</f>
-        <v>0</v>
-      </c>
-      <c r="D23" s="245">
+      <c r="C23" s="200"/>
+      <c r="D23" s="200">
+        <f t="shared" ref="D23:J23" si="2">IF(D6="","",SUM(D9:D22))</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="200">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E23" s="245">
+      <c r="F23" s="200">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F23" s="245">
+      <c r="G23" s="200">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G23" s="245">
+      <c r="H23" s="200">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H23" s="245"/>
-      <c r="I23" s="245">
+      <c r="I23" s="200">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J23" s="245"/>
+      <c r="J23" s="200">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:10" ht="15">
       <c r="A24" s="5"/>
@@ -49805,10 +50076,7 @@
       <c r="E28" s="203"/>
       <c r="F28" s="203"/>
       <c r="G28" s="226"/>
-      <c r="H28" s="226" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H28" s="226"/>
       <c r="I28" s="200" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -50012,7 +50280,10 @@
         <f>IF(I$6="","",SUM(I25:I36))</f>
         <v>0</v>
       </c>
-      <c r="J37" s="200"/>
+      <c r="J37" s="200">
+        <f>IF(J$6="","",SUM(J25:J36))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:10" ht="15">
       <c r="A38" s="6" t="s">
@@ -50042,14 +50313,17 @@
         <v>0</v>
       </c>
       <c r="H38" s="204">
-        <f t="shared" ref="H38:I38" si="9">IF(H$6="","",H23+H37)</f>
+        <f t="shared" ref="H38:J38" si="9">IF(H$6="","",H23+H37)</f>
         <v>0</v>
       </c>
       <c r="I38" s="204">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J38" s="204"/>
+      <c r="J38" s="204">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:10" ht="15">
       <c r="A39" s="5"/>
@@ -50109,12 +50383,9 @@
       <c r="D42" s="203"/>
       <c r="E42" s="203"/>
       <c r="F42" s="203"/>
-      <c r="G42" s="226" t="str">
-        <f t="shared" ref="G42:H49" si="11">IF(OR(G$6="", B42=""),"",0)</f>
-        <v/>
-      </c>
+      <c r="G42" s="226"/>
       <c r="H42" s="226" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="G42:H49" si="11">IF(OR(H$6="", C42=""),"",0)</f>
         <v/>
       </c>
       <c r="I42" s="200" t="str">
@@ -50136,10 +50407,7 @@
       <c r="D43" s="203"/>
       <c r="E43" s="203"/>
       <c r="F43" s="203"/>
-      <c r="G43" s="226" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
+      <c r="G43" s="226"/>
       <c r="H43" s="226" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -50163,10 +50431,7 @@
       <c r="D44" s="203"/>
       <c r="E44" s="203"/>
       <c r="F44" s="203"/>
-      <c r="G44" s="226" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
+      <c r="G44" s="226"/>
       <c r="H44" s="226" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -50190,10 +50455,7 @@
       <c r="D45" s="203"/>
       <c r="E45" s="203"/>
       <c r="F45" s="203"/>
-      <c r="G45" s="226" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
+      <c r="G45" s="226"/>
       <c r="H45" s="226" t="str">
         <f t="shared" si="11"/>
         <v/>
@@ -50707,7 +50969,10 @@
         <f>IF($C$6="","",SUM(G64:G70))</f>
         <v>0</v>
       </c>
-      <c r="H71" s="200"/>
+      <c r="H71" s="200">
+        <f>IF($H$6="","",SUM(H64:H70))</f>
+        <v>0</v>
+      </c>
       <c r="I71" s="200">
         <f>IF(I$6="","",SUM(I64:I70))</f>
         <v>0</v>
@@ -50733,15 +50998,15 @@
         <v>0</v>
       </c>
       <c r="H72" s="204">
-        <f t="shared" ref="H72:J72" si="19">SUM(H65:H71)</f>
+        <f>IF($H$6="","",SUM(H65:H71))</f>
         <v>0</v>
       </c>
       <c r="I72" s="204">
-        <f t="shared" si="19"/>
+        <f>IF(I$6="", "", SUM(I65:I71))</f>
         <v>0</v>
       </c>
       <c r="J72" s="204">
-        <f t="shared" si="19"/>
+        <f>IF(J$6="", "", SUM(J65:J71))</f>
         <v>0</v>
       </c>
     </row>
@@ -50770,17 +51035,20 @@
       <c r="D75" s="74"/>
       <c r="E75" s="74"/>
       <c r="F75" s="74"/>
-      <c r="G75" s="246">
+      <c r="G75" s="241">
         <f>G72+G23</f>
         <v>0</v>
       </c>
-      <c r="H75" s="246"/>
+      <c r="H75" s="241">
+        <f>IF($H$6="","",SUM(H72+H23))</f>
+        <v>0</v>
+      </c>
       <c r="I75" s="200">
         <f>IF(I$6="","",SUM(G75:H75))</f>
         <v>0</v>
       </c>
-      <c r="J75" s="246">
-        <f>J72+J50</f>
+      <c r="J75" s="241">
+        <f>IF(J$6="", "", SUM(J72+J50))</f>
         <v>0</v>
       </c>
     </row>
@@ -50798,7 +51066,7 @@
       <c r="G76" s="203"/>
       <c r="H76" s="203"/>
       <c r="I76" s="200">
-        <f t="shared" ref="I76" si="20">IF(I$6="","",SUM(G76:H76))</f>
+        <f t="shared" ref="I76" si="19">IF(I$6="","",SUM(G76:H76))</f>
         <v>0</v>
       </c>
       <c r="J76" s="203"/>
@@ -50814,20 +51082,20 @@
       <c r="D77" s="74"/>
       <c r="E77" s="74"/>
       <c r="F77" s="74"/>
-      <c r="G77" s="247">
+      <c r="G77" s="242">
         <f>G75+G76</f>
         <v>0</v>
       </c>
-      <c r="H77" s="247">
-        <f t="shared" ref="H77:J77" si="21">H75+H76</f>
-        <v>0</v>
-      </c>
-      <c r="I77" s="247">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="J77" s="247">
-        <f t="shared" si="21"/>
+      <c r="H77" s="242">
+        <f>IF($H$6="","",SUM(H75+H76))</f>
+        <v>0</v>
+      </c>
+      <c r="I77" s="242">
+        <f>IF(I$6="", "", SUM(I75+I76))</f>
+        <v>0</v>
+      </c>
+      <c r="J77" s="242">
+        <f>IF(J$6="", "", SUM(J75+J76))</f>
         <v>0</v>
       </c>
     </row>
@@ -50838,15 +51106,15 @@
       <c r="I79" s="54"/>
     </row>
     <row r="80" spans="1:10" ht="15">
-      <c r="A80" s="257"/>
-      <c r="B80" s="264" t="s">
-        <v>3636</v>
+      <c r="A80" s="252"/>
+      <c r="B80" s="261" t="s">
+        <v>3629</v>
       </c>
       <c r="I80" s="54"/>
     </row>
     <row r="81" spans="1:9" ht="15">
-      <c r="A81" s="257"/>
-      <c r="B81" s="265"/>
+      <c r="A81" s="252"/>
+      <c r="B81" s="262"/>
       <c r="I81" s="54"/>
     </row>
     <row r="82" spans="1:9" ht="15">
@@ -50909,88 +51177,88 @@
     <mergeCell ref="B80:B81"/>
   </mergeCells>
   <conditionalFormatting sqref="A9:A22">
-    <cfRule type="containsText" dxfId="79" priority="9" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="119" priority="9" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:A36">
-    <cfRule type="containsText" dxfId="78" priority="8" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="118" priority="8" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:A63">
-    <cfRule type="containsText" dxfId="77" priority="5" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="117" priority="5" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66:A70">
-    <cfRule type="containsText" dxfId="76" priority="1" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="116" priority="1" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:B49">
-    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="115" priority="3" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23 C37 C50 D53:G63">
-    <cfRule type="expression" dxfId="74" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="58" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:J64">
-    <cfRule type="expression" dxfId="73" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="43" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:J72">
-    <cfRule type="expression" dxfId="72" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="19" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:F6 D52:F52">
-    <cfRule type="expression" dxfId="71" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="55" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39:G51">
-    <cfRule type="expression" dxfId="70" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="15" stopIfTrue="1">
+      <formula>D$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7:J37 J39:J50">
+    <cfRule type="expression" dxfId="109" priority="13" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:J70">
-    <cfRule type="expression" dxfId="69" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="11" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D74:J77 I78:I99">
-    <cfRule type="expression" dxfId="68" priority="10" stopIfTrue="1">
+  <conditionalFormatting sqref="I78:I99 D74:J77">
+    <cfRule type="expression" dxfId="107" priority="10" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39:H50">
-    <cfRule type="expression" dxfId="67" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="14" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H38:I38">
-    <cfRule type="expression" dxfId="66" priority="52" stopIfTrue="1">
+  <conditionalFormatting sqref="H5:J6 I39:I51">
+    <cfRule type="expression" dxfId="105" priority="48" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:J6 D7:I37 I39:I51">
-    <cfRule type="expression" dxfId="65" priority="48" stopIfTrue="1">
-      <formula>D$6=""</formula>
+  <conditionalFormatting sqref="H38:J38">
+    <cfRule type="expression" dxfId="104" priority="52" stopIfTrue="1">
+      <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52:J63">
-    <cfRule type="expression" dxfId="64" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="12" stopIfTrue="1">
       <formula>H$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7:J50">
-    <cfRule type="expression" dxfId="63" priority="13" stopIfTrue="1">
-      <formula>J$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">

</xml_diff>

<commit_message>
pull in corrected template to allow merge #177
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarrahahmed/Desktop/CLOSUP/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A54DE2-7738-3A42-8FBC-69789D13A085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CD3C2B-D8DB-CF45-9F95-E643346CE5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17240" tabRatio="834" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-8280" windowWidth="38400" windowHeight="21600" tabRatio="834" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Net Position" sheetId="8" state="hidden" r:id="rId1"/>
@@ -13587,7 +13587,7 @@
   <dimension ref="A1:C514"/>
   <sheetViews>
     <sheetView topLeftCell="A295" zoomScale="75" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A316" sqref="A316:C354"/>
+      <selection activeCell="E319" sqref="E319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -19269,7 +19269,7 @@
   <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView zoomScale="119" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -20959,8 +20959,8 @@
   </sheetPr>
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -22652,7 +22652,7 @@
   <dimension ref="A1:K118"/>
   <sheetViews>
     <sheetView zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L80" sqref="L80"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -24992,8 +24992,8 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="75" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J82" sqref="J82"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -26606,7 +26606,7 @@
   <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="74" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N92" sqref="N92"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -28274,7 +28274,7 @@
   </sheetPr>
   <dimension ref="A1:C358"/>
   <sheetViews>
-    <sheetView topLeftCell="A149" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D135" sqref="D135:D136"/>
     </sheetView>
   </sheetViews>
@@ -31554,7 +31554,7 @@
   </sheetPr>
   <dimension ref="A1:E217"/>
   <sheetViews>
-    <sheetView topLeftCell="A175" zoomScale="75" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -35255,8 +35255,8 @@
   </sheetPr>
   <dimension ref="A1:E310"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A313" sqref="A313"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -35291,11 +35291,11 @@
         <v>1837</v>
       </c>
       <c r="C2" s="135" t="str">
-        <f t="shared" ref="C2:C65" si="0">"acfr:"&amp;A2</f>
-        <v>acfr:Charges to Other Funds</v>
+        <f>"acfr:"&amp;B2</f>
+        <v>acfr:ChargesToOtherFunds</v>
       </c>
       <c r="D2" s="120" t="str">
-        <f t="shared" ref="D2:D33" si="1">IF(RIGHT(B2, 8)="Abstract", "Abstract", "Operating Revenues")</f>
+        <f t="shared" ref="D2:D33" si="0">IF(RIGHT(B2, 8)="Abstract", "Abstract", "Operating Revenues")</f>
         <v>Operating Revenues</v>
       </c>
       <c r="E2" s="119"/>
@@ -35308,11 +35308,11 @@
         <v>1839</v>
       </c>
       <c r="C3" s="135" t="str">
+        <f t="shared" ref="C3:C66" si="1">"acfr:"&amp;B3</f>
+        <v>acfr:RevenueFares</v>
+      </c>
+      <c r="D3" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Fare Revenue</v>
-      </c>
-      <c r="D3" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E3" s="119"/>
@@ -35325,11 +35325,11 @@
         <v>1829</v>
       </c>
       <c r="C4" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:InterestAndPenaltiesForTaxFund</v>
+      </c>
+      <c r="D4" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Interest and Penalties for Tax Fund</v>
-      </c>
-      <c r="D4" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E4" s="119"/>
@@ -35342,11 +35342,11 @@
         <v>1870</v>
       </c>
       <c r="C5" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:OperatingContributionsAndPremiums</v>
+      </c>
+      <c r="D5" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Operating Contributions and Premiums</v>
-      </c>
-      <c r="D5" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E5" s="119"/>
@@ -35359,11 +35359,11 @@
         <v>1872</v>
       </c>
       <c r="C6" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:OperatingGrants</v>
+      </c>
+      <c r="D6" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Operating Grants</v>
-      </c>
-      <c r="D6" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E6" s="119"/>
@@ -35376,11 +35376,11 @@
         <v>1876</v>
       </c>
       <c r="C7" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:RevenueOperating</v>
+      </c>
+      <c r="D7" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Operating Revenue</v>
-      </c>
-      <c r="D7" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E7" s="119"/>
@@ -35393,11 +35393,11 @@
         <v>1874</v>
       </c>
       <c r="C8" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:OtherOperatingRevenue</v>
+      </c>
+      <c r="D8" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Other Operating Revenue</v>
-      </c>
-      <c r="D8" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E8" s="119"/>
@@ -35410,11 +35410,11 @@
         <v>1841</v>
       </c>
       <c r="C9" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:RegulatedOperatingRevenueWasteWater</v>
+      </c>
+      <c r="D9" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Regulated Operating Revenue, Waste Water</v>
-      </c>
-      <c r="D9" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E9" s="119"/>
@@ -35427,11 +35427,11 @@
         <v>1843</v>
       </c>
       <c r="C10" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:RegulatedOperatingRevenueWater</v>
+      </c>
+      <c r="D10" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Regulated Operating Revenue, Water</v>
-      </c>
-      <c r="D10" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E10" s="119"/>
@@ -35444,11 +35444,11 @@
         <v>1800</v>
       </c>
       <c r="C11" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesAmbulanceTransportFees</v>
+      </c>
+      <c r="D11" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Ambulance Transport Fees</v>
-      </c>
-      <c r="D11" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E11" s="119"/>
@@ -35461,11 +35461,11 @@
         <v>1782</v>
       </c>
       <c r="C12" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesAttorneyFeeReimbursement</v>
+      </c>
+      <c r="D12" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Attorney Fee Reimbursement</v>
-      </c>
-      <c r="D12" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E12" s="119"/>
@@ -35478,11 +35478,11 @@
         <v>1817</v>
       </c>
       <c r="C13" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesBondForfeituresAndBondCosts</v>
+      </c>
+      <c r="D13" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Bond Forfeitures and Bond Costs</v>
-      </c>
-      <c r="D13" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E13" s="119"/>
@@ -35495,11 +35495,11 @@
         <v>1798</v>
       </c>
       <c r="C14" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesBuildingInspectionFees</v>
+      </c>
+      <c r="D14" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Building Inspection Fees</v>
-      </c>
-      <c r="D14" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E14" s="119"/>
@@ -35512,11 +35512,11 @@
         <v>1821</v>
       </c>
       <c r="C15" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesBusinessLicensesAndPermits</v>
+      </c>
+      <c r="D15" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Business Licenses and Permits</v>
-      </c>
-      <c r="D15" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E15" s="119"/>
@@ -35529,11 +35529,11 @@
         <v>1822</v>
       </c>
       <c r="C16" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesCableTVFranchiseFees</v>
+      </c>
+      <c r="D16" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Cable TV Franchise Fees</v>
-      </c>
-      <c r="D16" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E16" s="119"/>
@@ -35546,11 +35546,11 @@
         <v>1812</v>
       </c>
       <c r="C17" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServices</v>
+      </c>
+      <c r="D17" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Charges for Services</v>
-      </c>
-      <c r="D17" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E17" s="119"/>
@@ -35563,11 +35563,11 @@
         <v>1776</v>
       </c>
       <c r="C18" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesCourtFilingFees</v>
+      </c>
+      <c r="D18" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Court Filing Fees</v>
-      </c>
-      <c r="D18" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E18" s="119"/>
@@ -35580,11 +35580,11 @@
         <v>1772</v>
       </c>
       <c r="C19" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesCourtRelatedCharges</v>
+      </c>
+      <c r="D19" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Court Related Charges</v>
-      </c>
-      <c r="D19" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E19" s="119"/>
@@ -35597,11 +35597,11 @@
         <v>1788</v>
       </c>
       <c r="C20" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesEstateInventoryFee</v>
+      </c>
+      <c r="D20" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Estate Inventory Fee</v>
-      </c>
-      <c r="D20" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E20" s="119"/>
@@ -35614,11 +35614,11 @@
         <v>1774</v>
       </c>
       <c r="C21" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesFees</v>
+      </c>
+      <c r="D21" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Fees</v>
-      </c>
-      <c r="D21" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E21" s="119"/>
@@ -35631,11 +35631,11 @@
         <v>1792</v>
       </c>
       <c r="C22" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesFriendOfTheCourtServiceFee</v>
+      </c>
+      <c r="D22" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Friend of the Court Service Fee</v>
-      </c>
-      <c r="D22" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E22" s="119"/>
@@ -35648,11 +35648,11 @@
         <v>1790</v>
       </c>
       <c r="C23" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesFriendOfTheCourtStatutoryHandlingFee</v>
+      </c>
+      <c r="D23" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Friend of the Court Statutory Handling Fee</v>
-      </c>
-      <c r="D23" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E23" s="119"/>
@@ -35665,11 +35665,11 @@
         <v>1784</v>
       </c>
       <c r="C24" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesGuardianAdLitemReimbursement</v>
+      </c>
+      <c r="D24" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Guardian Ad Litem Reimbursement</v>
-      </c>
-      <c r="D24" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E24" s="119"/>
@@ -35682,11 +35682,11 @@
         <v>1778</v>
       </c>
       <c r="C25" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesJuryDemandFees</v>
+      </c>
+      <c r="D25" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Jury Demand Fees</v>
-      </c>
-      <c r="D25" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E25" s="119"/>
@@ -35699,11 +35699,11 @@
         <v>1824</v>
       </c>
       <c r="C26" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesLicensesAndPermitsAndFranchiseFees</v>
+      </c>
+      <c r="D26" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Licenses and Permits and Franchise Fees</v>
-      </c>
-      <c r="D26" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E26" s="119"/>
@@ -35716,11 +35716,11 @@
         <v>1794</v>
       </c>
       <c r="C27" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesMiscellaneousCourtCostsAndFees</v>
+      </c>
+      <c r="D27" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Miscellaneous Court Costs and Fees</v>
-      </c>
-      <c r="D27" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E27" s="119"/>
@@ -35733,11 +35733,11 @@
         <v>1823</v>
       </c>
       <c r="C28" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesNonBusinessLicensesAndPermits</v>
+      </c>
+      <c r="D28" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Non Business Licenses and Permits</v>
-      </c>
-      <c r="D28" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E28" s="119"/>
@@ -35750,11 +35750,11 @@
         <v>1815</v>
       </c>
       <c r="C29" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesOrdinanceFinesAndCosts</v>
+      </c>
+      <c r="D29" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Ordinance Fines and Costs</v>
-      </c>
-      <c r="D29" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E29" s="119"/>
@@ -35767,11 +35767,11 @@
         <v>1810</v>
       </c>
       <c r="C30" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesRevenueFromParkingFacilities</v>
+      </c>
+      <c r="D30" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Parking Fees</v>
-      </c>
-      <c r="D30" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E30" s="119"/>
@@ -35784,11 +35784,11 @@
         <v>1804</v>
       </c>
       <c r="C31" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesPreForfeitureMailingNoticeCost</v>
+      </c>
+      <c r="D31" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Pre Forfeiture Mailing Notice Cost</v>
-      </c>
-      <c r="D31" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E31" s="119"/>
@@ -35801,11 +35801,11 @@
         <v>1786</v>
       </c>
       <c r="C32" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesProbationOversightFee</v>
+      </c>
+      <c r="D32" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Probation Oversight Fee</v>
-      </c>
-      <c r="D32" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E32" s="119"/>
@@ -35818,11 +35818,11 @@
         <v>1806</v>
       </c>
       <c r="C33" s="135" t="str">
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesSales</v>
+      </c>
+      <c r="D33" s="120" t="str">
         <f t="shared" si="0"/>
-        <v>acfr:Revenue for Sales</v>
-      </c>
-      <c r="D33" s="120" t="str">
-        <f t="shared" si="1"/>
         <v>Operating Revenues</v>
       </c>
       <c r="E33" s="119"/>
@@ -35835,8 +35835,8 @@
         <v>1796</v>
       </c>
       <c r="C34" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenue for Services Rendered</v>
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesServicesRendered</v>
       </c>
       <c r="D34" s="120" t="str">
         <f t="shared" ref="D34:D58" si="2">IF(RIGHT(B34, 8)="Abstract", "Abstract", "Operating Revenues")</f>
@@ -35852,8 +35852,8 @@
         <v>1816</v>
       </c>
       <c r="C35" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenue for Statute Costs</v>
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesStatuteCosts</v>
       </c>
       <c r="D35" s="120" t="str">
         <f t="shared" si="2"/>
@@ -35869,8 +35869,8 @@
         <v>1802</v>
       </c>
       <c r="C36" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenue for Title Search Fee</v>
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesTitleSearchFee</v>
       </c>
       <c r="D36" s="120" t="str">
         <f t="shared" si="2"/>
@@ -35886,8 +35886,8 @@
         <v>1814</v>
       </c>
       <c r="C37" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenue for Traffic Violations</v>
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesTrafficViolations</v>
       </c>
       <c r="D37" s="120" t="str">
         <f t="shared" si="2"/>
@@ -35903,8 +35903,8 @@
         <v>1808</v>
       </c>
       <c r="C38" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenue for Use and Admission Fees</v>
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesUseAndAdmissionFees</v>
       </c>
       <c r="D38" s="120" t="str">
         <f t="shared" si="2"/>
@@ -35920,8 +35920,8 @@
         <v>1780</v>
       </c>
       <c r="C39" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenue for Writ of Garnishment, Restitution, Attachment or Execution</v>
+        <f t="shared" si="1"/>
+        <v>acfr:ChargesForServicesWritOfGarnishmentRestitutionAttachmentOrExecution</v>
       </c>
       <c r="D39" s="120" t="str">
         <f t="shared" si="2"/>
@@ -35937,8 +35937,8 @@
         <v>1845</v>
       </c>
       <c r="C40" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenues from Auxiliary Enterprises</v>
+        <f t="shared" si="1"/>
+        <v>acfr:RevenuefromAuxiliaryEnterprises</v>
       </c>
       <c r="D40" s="120" t="str">
         <f t="shared" si="2"/>
@@ -35954,8 +35954,8 @@
         <v>1853</v>
       </c>
       <c r="C41" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenues from Charges for Utilities</v>
+        <f t="shared" si="1"/>
+        <v>acfr:RevenueFromChargesForUtilities</v>
       </c>
       <c r="D41" s="120" t="str">
         <f t="shared" si="2"/>
@@ -35971,8 +35971,8 @@
         <v>1847</v>
       </c>
       <c r="C42" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenues from Connection Fees</v>
+        <f t="shared" si="1"/>
+        <v>acfr:RevenueFromConnectionFees</v>
       </c>
       <c r="D42" s="120" t="str">
         <f t="shared" si="2"/>
@@ -35988,8 +35988,8 @@
         <v>1818</v>
       </c>
       <c r="C43" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenues from Fines and Forfeitures and Penalties</v>
+        <f t="shared" si="1"/>
+        <v>acfr:RevenueFromFinesAndForfeituresAndPenalties</v>
       </c>
       <c r="D43" s="120" t="str">
         <f t="shared" si="2"/>
@@ -36005,8 +36005,8 @@
         <v>1851</v>
       </c>
       <c r="C44" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenues from Installation Fees</v>
+        <f t="shared" si="1"/>
+        <v>acfr:RevenueFromInstallationFees</v>
       </c>
       <c r="D44" s="120" t="str">
         <f t="shared" si="2"/>
@@ -36022,8 +36022,8 @@
         <v>1865</v>
       </c>
       <c r="C45" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenues from Lottery License Application Fees</v>
+        <f t="shared" si="1"/>
+        <v>acfr:RevenueFromLotteryLicenseApplicationFees</v>
       </c>
       <c r="D45" s="120" t="str">
         <f t="shared" si="2"/>
@@ -36039,8 +36039,8 @@
         <v>1869</v>
       </c>
       <c r="C46" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenues from Lottery License Application Fees</v>
+        <f t="shared" si="1"/>
+        <v>acfr:ExpensesForLotteryLicenseApplicationFees</v>
       </c>
       <c r="D46" s="120" t="str">
         <f t="shared" si="2"/>
@@ -36056,8 +36056,8 @@
         <v>1867</v>
       </c>
       <c r="C47" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenues from Lottery Security Proceeds</v>
+        <f t="shared" si="1"/>
+        <v>acfr:RevenueFromLotterySecurityProceeds</v>
       </c>
       <c r="D47" s="120" t="str">
         <f t="shared" si="2"/>
@@ -36073,8 +36073,8 @@
         <v>1863</v>
       </c>
       <c r="C48" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenues from Lottery Ticket Sales</v>
+        <f t="shared" si="1"/>
+        <v>acfr:RevenueFromLotteryTicketSales</v>
       </c>
       <c r="D48" s="120" t="str">
         <f t="shared" si="2"/>
@@ -36090,8 +36090,8 @@
         <v>1857</v>
       </c>
       <c r="C49" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenues from Refunds and Rebates</v>
+        <f t="shared" si="1"/>
+        <v>acfr:RevenueFromRefundsAndRebates</v>
       </c>
       <c r="D49" s="120" t="str">
         <f t="shared" si="2"/>
@@ -36107,8 +36107,8 @@
         <v>1859</v>
       </c>
       <c r="C50" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenues from Reimbursements</v>
+        <f t="shared" si="1"/>
+        <v>acfr:RevenueFromReimbursements</v>
       </c>
       <c r="D50" s="120" t="str">
         <f t="shared" si="2"/>
@@ -36124,8 +36124,8 @@
         <v>1849</v>
       </c>
       <c r="C51" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenues from Rents</v>
+        <f t="shared" si="1"/>
+        <v>acfr:RevenueFromRents</v>
       </c>
       <c r="D51" s="120" t="str">
         <f t="shared" si="2"/>
@@ -36141,8 +36141,8 @@
         <v>1855</v>
       </c>
       <c r="C52" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenues from Sale of Fuel</v>
+        <f t="shared" si="1"/>
+        <v>acfr:RevenueFromSaleOfFuel</v>
       </c>
       <c r="D52" s="120" t="str">
         <f t="shared" si="2"/>
@@ -36158,8 +36158,8 @@
         <v>1825</v>
       </c>
       <c r="C53" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenues from Tuition and Fees</v>
+        <f t="shared" si="1"/>
+        <v>acfr:RevenueFromTuitionAndFees</v>
       </c>
       <c r="D53" s="120" t="str">
         <f t="shared" si="2"/>
@@ -36175,8 +36175,8 @@
         <v>1831</v>
       </c>
       <c r="C54" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Revenues from Tuition and Fees (Net of Allowances)</v>
+        <f t="shared" si="1"/>
+        <v>acfr:RevenueFromTuitionAndFeesNetOfAllowances</v>
       </c>
       <c r="D54" s="120" t="str">
         <f t="shared" si="2"/>
@@ -36192,8 +36192,8 @@
         <v>1833</v>
       </c>
       <c r="C55" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Scholarship Allowances</v>
+        <f t="shared" si="1"/>
+        <v>acfr:ScholarshipAllowances</v>
       </c>
       <c r="D55" s="120" t="str">
         <f t="shared" si="2"/>
@@ -36209,8 +36209,8 @@
         <v>1827</v>
       </c>
       <c r="C56" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Tax Collection Fees for Tax Fund</v>
+        <f t="shared" si="1"/>
+        <v>acfr:TaxCollectionFeesForTaxFund</v>
       </c>
       <c r="D56" s="120" t="str">
         <f t="shared" si="2"/>
@@ -36226,8 +36226,8 @@
         <v>1835</v>
       </c>
       <c r="C57" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Tuition and Fees, Allowance</v>
+        <f t="shared" si="1"/>
+        <v>acfr:TuitionAndFeesAllowances</v>
       </c>
       <c r="D57" s="120" t="str">
         <f t="shared" si="2"/>
@@ -36243,8 +36243,8 @@
         <v>1726</v>
       </c>
       <c r="C58" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Type of Activities Proprietary Funds [Axis]</v>
+        <f t="shared" si="1"/>
+        <v>acfr:TypeOfActivitiesProprietaryFundsAxis</v>
       </c>
       <c r="D58" s="120" t="str">
         <f t="shared" si="2"/>
@@ -36260,8 +36260,8 @@
         <v>1981</v>
       </c>
       <c r="C59" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Amortization Expense</v>
+        <f t="shared" si="1"/>
+        <v>acfr:AmortizationExpense</v>
       </c>
       <c r="D59" s="120" t="str">
         <f t="shared" ref="D59:D90" si="3">IF(RIGHT(B59, 8)="Abstract", "Abstract", "Operating Expenses")</f>
@@ -36277,8 +36277,8 @@
         <v>1985</v>
       </c>
       <c r="C60" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Bad Debt Expense</v>
+        <f t="shared" si="1"/>
+        <v>acfr:BadDebtExpense</v>
       </c>
       <c r="D60" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36294,8 +36294,8 @@
         <v>1944</v>
       </c>
       <c r="C61" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Benefits Expense</v>
+        <f t="shared" si="1"/>
+        <v>acfr:BenefitsExpense</v>
       </c>
       <c r="D61" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36311,8 +36311,8 @@
         <v>1942</v>
       </c>
       <c r="C62" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Benefits Expense, Pension and OPEB</v>
+        <f t="shared" si="1"/>
+        <v>acfr:BenefitsExpensePensionAndOPEB</v>
       </c>
       <c r="D62" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36328,8 +36328,8 @@
         <v>1948</v>
       </c>
       <c r="C63" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Communication Expense</v>
+        <f t="shared" si="1"/>
+        <v>acfr:CommunicationExpense</v>
       </c>
       <c r="D63" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36345,8 +36345,8 @@
         <v>1950</v>
       </c>
       <c r="C64" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Community Promotion Expense</v>
+        <f t="shared" si="1"/>
+        <v>acfr:CommunityPromotionExpense</v>
       </c>
       <c r="D64" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36362,8 +36362,8 @@
         <v>1978</v>
       </c>
       <c r="C65" s="135" t="str">
-        <f t="shared" si="0"/>
-        <v>acfr:Cost of Materials and Services Rendered</v>
+        <f t="shared" si="1"/>
+        <v>acfr:CostOfMaterialsAndServicesRendered</v>
       </c>
       <c r="D65" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36379,8 +36379,8 @@
         <v>1983</v>
       </c>
       <c r="C66" s="135" t="str">
-        <f t="shared" ref="C66:C129" si="4">"acfr:"&amp;A66</f>
-        <v>acfr:Depletion, Depreciation and Amortization Expense</v>
+        <f t="shared" si="1"/>
+        <v>acfr:DepletionDepreciationAndAmortizationExpense</v>
       </c>
       <c r="D66" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36396,8 +36396,8 @@
         <v>1980</v>
       </c>
       <c r="C67" s="135" t="str">
-        <f t="shared" si="4"/>
-        <v>acfr:Depreciation Expense</v>
+        <f t="shared" ref="C67:C130" si="4">"acfr:"&amp;B67</f>
+        <v>acfr:DepreciationExpense</v>
       </c>
       <c r="D67" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36414,7 +36414,7 @@
       </c>
       <c r="C68" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Academic Support</v>
+        <v>acfr:ExpensesForAcademicSupport</v>
       </c>
       <c r="D68" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36431,7 +36431,7 @@
       </c>
       <c r="C69" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Airport Services</v>
+        <v>acfr:ExpensesForAirportsServices</v>
       </c>
       <c r="D69" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36448,7 +36448,7 @@
       </c>
       <c r="C70" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Ambulance</v>
+        <v>acfr:ExpensesForAmbulance</v>
       </c>
       <c r="D70" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36465,7 +36465,7 @@
       </c>
       <c r="C71" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Auditorium, Civic Center</v>
+        <v>acfr:ExpensesForAuditoriumCivicCenter</v>
       </c>
       <c r="D71" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36482,7 +36482,7 @@
       </c>
       <c r="C72" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Auxiliary Enterprises</v>
+        <v>acfr:ExpensesForAuxiliaryEnterprises</v>
       </c>
       <c r="D72" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36499,7 +36499,7 @@
       </c>
       <c r="C73" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Claims and Judgments</v>
+        <v>acfr:ExpensesForClaimsAndJudgments</v>
       </c>
       <c r="D73" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36516,7 +36516,7 @@
       </c>
       <c r="C74" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Department of Public Works (DPW)</v>
+        <v>acfr:ExpensesForDepartmentOfPublicWorksDPW</v>
       </c>
       <c r="D74" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36533,7 +36533,7 @@
       </c>
       <c r="C75" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Engineers, Engineering</v>
+        <v>acfr:ExpensesForEngineersEngineering</v>
       </c>
       <c r="D75" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36550,7 +36550,7 @@
       </c>
       <c r="C76" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Equipment and Equipment Rental</v>
+        <v>acfr:ExpensesForEquipmentAndEquipmentRental</v>
       </c>
       <c r="D76" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36567,7 +36567,7 @@
       </c>
       <c r="C77" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for General Government Services</v>
+        <v>acfr:ExpensesForGeneralGovernmentServices</v>
       </c>
       <c r="D77" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36584,7 +36584,7 @@
       </c>
       <c r="C78" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Harbor Services</v>
+        <v>acfr:ExpensesForHarborServices</v>
       </c>
       <c r="D78" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36601,7 +36601,7 @@
       </c>
       <c r="C79" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Hospital Operations</v>
+        <v>acfr:ExpensesForHospitalOperations</v>
       </c>
       <c r="D79" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36618,7 +36618,7 @@
       </c>
       <c r="C80" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Hospitalization</v>
+        <v>acfr:ExpensesForHospitalization</v>
       </c>
       <c r="D80" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36635,7 +36635,7 @@
       </c>
       <c r="C81" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Information Technology</v>
+        <v>acfr:ExpensesForFinancialAndTaxAdministrationInformationTechnology</v>
       </c>
       <c r="D81" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36652,7 +36652,7 @@
       </c>
       <c r="C82" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Institutional Support</v>
+        <v>acfr:ExpensesForInstitutionalSupport</v>
       </c>
       <c r="D82" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36669,7 +36669,7 @@
       </c>
       <c r="C83" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Instruction</v>
+        <v>acfr:ExpensesForInstruction</v>
       </c>
       <c r="D83" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36686,7 +36686,7 @@
       </c>
       <c r="C84" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Lottery Game Costs</v>
+        <v>acfr:ExpensesForLotteryGameCosts</v>
       </c>
       <c r="D84" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36703,7 +36703,7 @@
       </c>
       <c r="C85" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Lottery Operator Fees</v>
+        <v>acfr:ExpensesForLotteryOperatorFees</v>
       </c>
       <c r="D85" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36720,7 +36720,7 @@
       </c>
       <c r="C86" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Lottery Prize Awards</v>
+        <v>acfr:ExpensesForLotteryPrizeAwards</v>
       </c>
       <c r="D86" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36737,7 +36737,7 @@
       </c>
       <c r="C87" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Lottery Promotion, Public Relations, and Point of Sale</v>
+        <v>acfr:ExpensesForLotteryPromotionPublicRelationsAndPointOfSale</v>
       </c>
       <c r="D87" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36754,7 +36754,7 @@
       </c>
       <c r="C88" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Lottery Retailer Bonuses</v>
+        <v>acfr:ExpensesForLotteryRetailerBonuses</v>
       </c>
       <c r="D88" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36771,7 +36771,7 @@
       </c>
       <c r="C89" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Lottery Retailer Commissions</v>
+        <v>acfr:ExpensesForLotteryRetailerCommissions</v>
       </c>
       <c r="D89" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36788,7 +36788,7 @@
       </c>
       <c r="C90" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Other Public Services</v>
+        <v>acfr:ExpensesForOtherPublicServices</v>
       </c>
       <c r="D90" s="120" t="str">
         <f t="shared" si="3"/>
@@ -36805,7 +36805,7 @@
       </c>
       <c r="C91" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Parks Administration</v>
+        <v>acfr:ExpensesForParksAdministration</v>
       </c>
       <c r="D91" s="120" t="str">
         <f t="shared" ref="D91:D122" si="5">IF(RIGHT(B91, 8)="Abstract", "Abstract", "Operating Expenses")</f>
@@ -36822,7 +36822,7 @@
       </c>
       <c r="C92" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Parks and Recreation</v>
+        <v>acfr:ExpensesForParksAndRecreation</v>
       </c>
       <c r="D92" s="120" t="str">
         <f t="shared" si="5"/>
@@ -36839,7 +36839,7 @@
       </c>
       <c r="C93" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Parks and Recreation Department</v>
+        <v>acfr:ExpensesForParksAndRecreationDepartment</v>
       </c>
       <c r="D93" s="120" t="str">
         <f t="shared" si="5"/>
@@ -36856,7 +36856,7 @@
       </c>
       <c r="C94" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Parks Facilities</v>
+        <v>acfr:ExpensesForParksFacilities</v>
       </c>
       <c r="D94" s="120" t="str">
         <f t="shared" si="5"/>
@@ -36873,7 +36873,7 @@
       </c>
       <c r="C95" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Parks Lighting</v>
+        <v>acfr:ExpensesForParksLighting</v>
       </c>
       <c r="D95" s="120" t="str">
         <f t="shared" si="5"/>
@@ -36890,7 +36890,7 @@
       </c>
       <c r="C96" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Parks Maintenance</v>
+        <v>acfr:ExpensesForParksMaintenance</v>
       </c>
       <c r="D96" s="120" t="str">
         <f t="shared" si="5"/>
@@ -36907,7 +36907,7 @@
       </c>
       <c r="C97" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Parks Policing</v>
+        <v>acfr:ExpensesForParksPolicing</v>
       </c>
       <c r="D97" s="120" t="str">
         <f t="shared" si="5"/>
@@ -36924,7 +36924,7 @@
       </c>
       <c r="C98" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Parks Supervision</v>
+        <v>acfr:ExpensesForParksSupervision</v>
       </c>
       <c r="D98" s="120" t="str">
         <f t="shared" si="5"/>
@@ -36941,7 +36941,7 @@
       </c>
       <c r="C99" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Professional and Contractual Services</v>
+        <v>acfr:ExpensesForProfessionalServices</v>
       </c>
       <c r="D99" s="120" t="str">
         <f t="shared" si="5"/>
@@ -36958,7 +36958,7 @@
       </c>
       <c r="C100" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Refunds and Rebates</v>
+        <v>acfr:ExpensesForRefundsAndRebates</v>
       </c>
       <c r="D100" s="120" t="str">
         <f t="shared" si="5"/>
@@ -36975,7 +36975,7 @@
       </c>
       <c r="C101" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Rubbish Collection</v>
+        <v>acfr:ExpensesForRubbishCollection</v>
       </c>
       <c r="D101" s="120" t="str">
         <f t="shared" si="5"/>
@@ -36992,7 +36992,7 @@
       </c>
       <c r="C102" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Salaries and Benefits</v>
+        <v>acfr:ExpensesForSalariesAndBenefits</v>
       </c>
       <c r="D102" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37009,7 +37009,7 @@
       </c>
       <c r="C103" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Sanitary Landfill</v>
+        <v>acfr:ExpensesForSanitaryLandfill</v>
       </c>
       <c r="D103" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37026,7 +37026,7 @@
       </c>
       <c r="C104" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Sanitation Department</v>
+        <v>acfr:ExpensesForSanitationDepartment</v>
       </c>
       <c r="D104" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37043,7 +37043,7 @@
       </c>
       <c r="C105" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Services and Supplies</v>
+        <v>acfr:ExpensesForServicesAndSupplies</v>
       </c>
       <c r="D105" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37060,7 +37060,7 @@
       </c>
       <c r="C106" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Sewage Disposal</v>
+        <v>acfr:ExpensesForSewageDisposal</v>
       </c>
       <c r="D106" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37077,7 +37077,7 @@
       </c>
       <c r="C107" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Special Assessments</v>
+        <v>acfr:ExpensesForSpecialAssessments</v>
       </c>
       <c r="D107" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37094,7 +37094,7 @@
       </c>
       <c r="C108" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for State Institutions</v>
+        <v>acfr:ExpensesForStateInstitutions</v>
       </c>
       <c r="D108" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37111,7 +37111,7 @@
       </c>
       <c r="C109" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Student Grants and Scholarships</v>
+        <v>acfr:ExpensesForStudentGrantsAndScholarships</v>
       </c>
       <c r="D109" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37128,7 +37128,7 @@
       </c>
       <c r="C110" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Student Services</v>
+        <v>acfr:ExpensesForStudentService</v>
       </c>
       <c r="D110" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37145,7 +37145,7 @@
       </c>
       <c r="C111" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Transportation Services</v>
+        <v>acfr:ExpensesForTransportationServices</v>
       </c>
       <c r="D111" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37162,7 +37162,7 @@
       </c>
       <c r="C112" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Expenses for Water and Sewer Systems</v>
+        <v>acfr:ExpensesForWaterAndSewerSystems</v>
       </c>
       <c r="D112" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37179,7 +37179,7 @@
       </c>
       <c r="C113" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Financial Aid Expense</v>
+        <v>acfr:FinancialAidExpense</v>
       </c>
       <c r="D113" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37196,7 +37196,7 @@
       </c>
       <c r="C114" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Health Services Expense</v>
+        <v>acfr:HealthServicesExpense</v>
       </c>
       <c r="D114" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37213,7 +37213,7 @@
       </c>
       <c r="C115" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Housing Assistance Payments</v>
+        <v>acfr:HousingAssistancePaymentsExpense</v>
       </c>
       <c r="D115" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37230,7 +37230,7 @@
       </c>
       <c r="C116" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Insurance Expense</v>
+        <v>acfr:InsuranceExpense</v>
       </c>
       <c r="D116" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37247,7 +37247,7 @@
       </c>
       <c r="C117" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Interest Expense</v>
+        <v>acfr:InterestExpense</v>
       </c>
       <c r="D117" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37264,7 +37264,7 @@
       </c>
       <c r="C118" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Interest Expense Imputed on Annuitized Prize Liability</v>
+        <v>acfr:InterestExpenseImputedOnAnnuitizedPrizeLiability</v>
       </c>
       <c r="D118" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37281,7 +37281,7 @@
       </c>
       <c r="C119" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Materials and Supplies Expense</v>
+        <v>acfr:MaterialsAndSuppliesExpense</v>
       </c>
       <c r="D119" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37298,7 +37298,7 @@
       </c>
       <c r="C120" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:OPEB Expense</v>
+        <v>acfr:OPEBExpense</v>
       </c>
       <c r="D120" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37315,7 +37315,7 @@
       </c>
       <c r="C121" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Operating Expense</v>
+        <v>acfr:OperatingExpense</v>
       </c>
       <c r="D121" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37332,7 +37332,7 @@
       </c>
       <c r="C122" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Operating Income (Loss)</v>
+        <v>acfr:OperatingIncomeLoss</v>
       </c>
       <c r="D122" s="120" t="str">
         <f t="shared" si="5"/>
@@ -37349,7 +37349,7 @@
       </c>
       <c r="C123" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Other Lottery Costs</v>
+        <v>acfr:OtherLotteryCosts</v>
       </c>
       <c r="D123" s="120" t="str">
         <f t="shared" ref="D123:D133" si="6">IF(RIGHT(B123, 8)="Abstract", "Abstract", "Operating Expenses")</f>
@@ -37366,7 +37366,7 @@
       </c>
       <c r="C124" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Other Operating Expenses</v>
+        <v>acfr:OtherOperatingExpenses</v>
       </c>
       <c r="D124" s="120" t="str">
         <f t="shared" si="6"/>
@@ -37383,7 +37383,7 @@
       </c>
       <c r="C125" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Pension Expense</v>
+        <v>acfr:PensionExpense</v>
       </c>
       <c r="D125" s="120" t="str">
         <f t="shared" si="6"/>
@@ -37400,7 +37400,7 @@
       </c>
       <c r="C126" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Printing and Publishing Expense</v>
+        <v>acfr:PrintingAndPublishingExpense</v>
       </c>
       <c r="D126" s="120" t="str">
         <f t="shared" si="6"/>
@@ -37417,7 +37417,7 @@
       </c>
       <c r="C127" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Protective Services</v>
+        <v>acfr:ExpensesForProtectiveServices</v>
       </c>
       <c r="D127" s="120" t="str">
         <f t="shared" si="6"/>
@@ -37434,7 +37434,7 @@
       </c>
       <c r="C128" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Rent Expense</v>
+        <v>acfr:RentExpense</v>
       </c>
       <c r="D128" s="120" t="str">
         <f t="shared" si="6"/>
@@ -37451,7 +37451,7 @@
       </c>
       <c r="C129" s="135" t="str">
         <f t="shared" si="4"/>
-        <v>acfr:Repair and Maintenance</v>
+        <v>acfr:RepairAndMaintenance</v>
       </c>
       <c r="D129" s="120" t="str">
         <f t="shared" si="6"/>
@@ -37467,8 +37467,8 @@
         <v>2001</v>
       </c>
       <c r="C130" s="135" t="str">
-        <f t="shared" ref="C130:C193" si="7">"acfr:"&amp;A130</f>
-        <v>acfr:Sewage Treatment Expense</v>
+        <f t="shared" si="4"/>
+        <v>acfr:SewageTreatmentExpense</v>
       </c>
       <c r="D130" s="120" t="str">
         <f t="shared" si="6"/>
@@ -37484,8 +37484,8 @@
         <v>1995</v>
       </c>
       <c r="C131" s="135" t="str">
-        <f t="shared" si="7"/>
-        <v>acfr:State Trunkline Overhead Expense</v>
+        <f t="shared" ref="C131:C194" si="7">"acfr:"&amp;B131</f>
+        <v>acfr:StateTrunklineOverheadExpense</v>
       </c>
       <c r="D131" s="120" t="str">
         <f t="shared" si="6"/>
@@ -37502,7 +37502,7 @@
       </c>
       <c r="C132" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Tenant Services Expense</v>
+        <v>acfr:TenantServicesExpenses</v>
       </c>
       <c r="D132" s="120" t="str">
         <f t="shared" si="6"/>
@@ -37519,7 +37519,7 @@
       </c>
       <c r="C133" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Utilities Expense</v>
+        <v>acfr:ExpensesForUtilities</v>
       </c>
       <c r="D133" s="120" t="str">
         <f t="shared" si="6"/>
@@ -37536,7 +37536,7 @@
       </c>
       <c r="C134" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Allowance for Chargebacks</v>
+        <v>acfr:AllowanceForChargebacks</v>
       </c>
       <c r="D134" s="120" t="str">
         <f t="shared" ref="D134:D165" si="8">IF(RIGHT(B134, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -37553,7 +37553,7 @@
       </c>
       <c r="C135" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Allowance for Refunds</v>
+        <v>acfr:AllowanceForRefunds</v>
       </c>
       <c r="D135" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37570,7 +37570,7 @@
       </c>
       <c r="C136" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Cash Over or Short</v>
+        <v>acfr:CashOverOrShort</v>
       </c>
       <c r="D136" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37587,7 +37587,7 @@
       </c>
       <c r="C137" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Contributions to Other Governments</v>
+        <v>acfr:ContributionsToOtherGovernments</v>
       </c>
       <c r="D137" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37604,7 +37604,7 @@
       </c>
       <c r="C138" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Debt Service, Interest and Fiscal Charges</v>
+        <v>acfr:DebtServiceInterestAndFiscalCharges</v>
       </c>
       <c r="D138" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37621,7 +37621,7 @@
       </c>
       <c r="C139" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Expenses for Other Welfare Services</v>
+        <v>acfr:ExpensesForOtherWelfareServices</v>
       </c>
       <c r="D139" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37638,7 +37638,7 @@
       </c>
       <c r="C140" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Federal Capital Grants</v>
+        <v>acfr:FederalCapitalGrants</v>
       </c>
       <c r="D140" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37655,7 +37655,7 @@
       </c>
       <c r="C141" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Federal Grants, Community Development Block Grants</v>
+        <v>acfr:FederalGrantsCommunityDevelopmentBlockGrants</v>
       </c>
       <c r="D141" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37672,7 +37672,7 @@
       </c>
       <c r="C142" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Federal Grants, Culture and Recreation</v>
+        <v>acfr:FederalGrantsCultureAndRecreation</v>
       </c>
       <c r="D142" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37689,7 +37689,7 @@
       </c>
       <c r="C143" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Federal Grants, General Government</v>
+        <v>acfr:FederalGrantsGeneralGovernment</v>
       </c>
       <c r="D143" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37706,7 +37706,7 @@
       </c>
       <c r="C144" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Federal Grants, Health and Hospital</v>
+        <v>acfr:FederalGrantsHealthAndHospital</v>
       </c>
       <c r="D144" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37723,7 +37723,7 @@
       </c>
       <c r="C145" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Federal Grants, Public Safety</v>
+        <v>acfr:FederalGrantsPublicSafety</v>
       </c>
       <c r="D145" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37740,7 +37740,7 @@
       </c>
       <c r="C146" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Federal Grants, Sanitation</v>
+        <v>acfr:FederalGrantsSanitation</v>
       </c>
       <c r="D146" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37757,7 +37757,7 @@
       </c>
       <c r="C147" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Federal Grants, Welfare</v>
+        <v>acfr:FederalGrantsWelfare</v>
       </c>
       <c r="D147" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37774,7 +37774,7 @@
       </c>
       <c r="C148" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Gain (Loss) on Sale of Capital Assets</v>
+        <v>acfr:GainLossOnSaleOfCapitalAssets</v>
       </c>
       <c r="D148" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37808,7 +37808,7 @@
       </c>
       <c r="C150" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Grant Related Expenses</v>
+        <v>acfr:GrantRelatedExpenses</v>
       </c>
       <c r="D150" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37825,7 +37825,7 @@
       </c>
       <c r="C151" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Grants, Contributions and Donations from Federal Governmental Entities</v>
+        <v>acfr:GrantsContributionsAndDonationsFromFederalGovernmentalEntities</v>
       </c>
       <c r="D151" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37842,7 +37842,7 @@
       </c>
       <c r="C152" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Grants, Contributions and Donations from Local Units</v>
+        <v>acfr:GrantsContributionsAndDonationsFromLocalUnits</v>
       </c>
       <c r="D152" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37859,7 +37859,7 @@
       </c>
       <c r="C153" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Grants, Contributions and Donations from Others</v>
+        <v>acfr:GrantsContributionsAndDonationsFromOthers</v>
       </c>
       <c r="D153" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37876,7 +37876,7 @@
       </c>
       <c r="C154" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Grants, Contributions and Donations from State Governmental Entities</v>
+        <v>acfr:GrantsContributionsAndDonationsFromStateGovernmentalEntities</v>
       </c>
       <c r="D154" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37893,7 +37893,7 @@
       </c>
       <c r="C155" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Investment Gains (Losses)</v>
+        <v>acfr:InvestmentGainsLosses</v>
       </c>
       <c r="D155" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37910,7 +37910,7 @@
       </c>
       <c r="C156" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Investment Income</v>
+        <v>acfr:InvestmentIncome</v>
       </c>
       <c r="D156" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37927,7 +37927,7 @@
       </c>
       <c r="C157" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Investment Income and Rentals</v>
+        <v>acfr:InvestmentIncomeAndRentals</v>
       </c>
       <c r="D157" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37944,7 +37944,7 @@
       </c>
       <c r="C158" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Issuance Cost and Amortization of Bond Discount</v>
+        <v>acfr:IssuanceCostAndAmortizationOfBondDiscount</v>
       </c>
       <c r="D158" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37961,7 +37961,7 @@
       </c>
       <c r="C159" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Lease Investment Income</v>
+        <v>acfr:LeaseInvestmentIncome</v>
       </c>
       <c r="D159" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37978,7 +37978,7 @@
       </c>
       <c r="C160" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Miscellaneous Other Revenue</v>
+        <v>acfr:MiscellaneousOtherRevenue</v>
       </c>
       <c r="D160" s="120" t="str">
         <f t="shared" si="8"/>
@@ -37995,7 +37995,7 @@
       </c>
       <c r="C161" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Nonoperating Expenses</v>
+        <v>acfr:NonoperatingExpenses</v>
       </c>
       <c r="D161" s="120" t="str">
         <f t="shared" si="8"/>
@@ -38012,7 +38012,7 @@
       </c>
       <c r="C162" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Nonoperating Revenues</v>
+        <v>acfr:NonoperatingRevenues</v>
       </c>
       <c r="D162" s="120" t="str">
         <f t="shared" si="8"/>
@@ -38029,7 +38029,7 @@
       </c>
       <c r="C163" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Nonoperating Revenues and (Expenses)</v>
+        <v>acfr:NonoperatingRevenuesAndExpenses</v>
       </c>
       <c r="D163" s="120" t="str">
         <f t="shared" si="8"/>
@@ -38046,7 +38046,7 @@
       </c>
       <c r="C164" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Other Nonoperating Revenues (Expenses)</v>
+        <v>acfr:OtherNonoperatingRevenuesExpenses</v>
       </c>
       <c r="D164" s="120" t="str">
         <f t="shared" si="8"/>
@@ -38063,7 +38063,7 @@
       </c>
       <c r="C165" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Payment in Lieu of Taxes</v>
+        <v>acfr:PaymentInLieuOfTaxes</v>
       </c>
       <c r="D165" s="120" t="str">
         <f t="shared" si="8"/>
@@ -38080,7 +38080,7 @@
       </c>
       <c r="C166" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Private Contributions and Donations</v>
+        <v>acfr:PrivateContributionsAndDonations</v>
       </c>
       <c r="D166" s="120" t="str">
         <f t="shared" ref="D166:D197" si="9">IF(RIGHT(B166, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -38097,7 +38097,7 @@
       </c>
       <c r="C167" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Project Costs</v>
+        <v>acfr:ProjectCosts</v>
       </c>
       <c r="D167" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38114,7 +38114,7 @@
       </c>
       <c r="C168" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Public and Private Contributions</v>
+        <v>acfr:PublicAndPrivateContributions</v>
       </c>
       <c r="D168" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38131,7 +38131,7 @@
       </c>
       <c r="C169" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Redemptions and Reconveyance</v>
+        <v>acfr:RedemptionsAndReconveyance</v>
       </c>
       <c r="D169" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38148,7 +38148,7 @@
       </c>
       <c r="C170" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Accommodations Tax (PA 263 of 1974)</v>
+        <v>acfr:RevenueFromAccomodationsTax</v>
       </c>
       <c r="D170" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38165,7 +38165,7 @@
       </c>
       <c r="C171" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Business License Tax</v>
+        <v>acfr:RevenueFromBusinessLicenseTax</v>
       </c>
       <c r="D171" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38182,7 +38182,7 @@
       </c>
       <c r="C172" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from City Utility Users Tax</v>
+        <v>acfr:RevenueFromCityUtilityUsersTax</v>
       </c>
       <c r="D172" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38199,7 +38199,7 @@
       </c>
       <c r="C173" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Collection Fees</v>
+        <v>acfr:RevenueFromCollectionFees</v>
       </c>
       <c r="D173" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38216,7 +38216,7 @@
       </c>
       <c r="C174" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Commercial Facilities Tax</v>
+        <v>acfr:RevenueFromCommercialFacilitiesTax</v>
       </c>
       <c r="D174" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38233,7 +38233,7 @@
       </c>
       <c r="C175" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Commercial Forest Reserve</v>
+        <v>acfr:RevenueFromCommercialForestReserve</v>
       </c>
       <c r="D175" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38250,7 +38250,7 @@
       </c>
       <c r="C176" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Community Wide Special Assessments</v>
+        <v>acfr:RevenueFromCommunityWideSpecialAssessments</v>
       </c>
       <c r="D176" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38267,7 +38267,7 @@
       </c>
       <c r="C177" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Connection Fees, Nonoperating</v>
+        <v>acfr:RevenuesFromConnectionFeesNonoperating</v>
       </c>
       <c r="D177" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38284,7 +38284,7 @@
       </c>
       <c r="C178" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Convention Tax</v>
+        <v>acfr:RevenueFromConventionTax</v>
       </c>
       <c r="D178" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38301,7 +38301,7 @@
       </c>
       <c r="C179" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Corporate Tax</v>
+        <v>acfr:RevenueFromCorporateTax</v>
       </c>
       <c r="D179" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38318,7 +38318,7 @@
       </c>
       <c r="C180" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from County Expense of Sale</v>
+        <v>acfr:RevenueFromCountyExpenseOfSale</v>
       </c>
       <c r="D180" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38335,7 +38335,7 @@
       </c>
       <c r="C181" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Current Personal Property Tax</v>
+        <v>acfr:RevenueFromCurrentPersonalPropertyTax</v>
       </c>
       <c r="D181" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38352,7 +38352,7 @@
       </c>
       <c r="C182" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Current Property Taxes, Extra or Special Voted</v>
+        <v>acfr:RevenueFromCurrentPropertyTaxesExtraOrSpecialVoted</v>
       </c>
       <c r="D182" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38369,7 +38369,7 @@
       </c>
       <c r="C183" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Current Real Property Tax</v>
+        <v>acfr:RevenuesFromCurrentRealPropertyTax</v>
       </c>
       <c r="D183" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38386,7 +38386,7 @@
       </c>
       <c r="C184" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Delinquent Personal Property Tax</v>
+        <v>acfr:RevenueFromDelinquentPersonalPropertyTax</v>
       </c>
       <c r="D184" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38403,7 +38403,7 @@
       </c>
       <c r="C185" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Delinquent Real Property Tax</v>
+        <v>acfr:RevenueFromDelinquentRealPropertyTax</v>
       </c>
       <c r="D185" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38420,7 +38420,7 @@
       </c>
       <c r="C186" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Dividends</v>
+        <v>acfr:RevenueFromDividends</v>
       </c>
       <c r="D186" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38437,7 +38437,7 @@
       </c>
       <c r="C187" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Documents Transfer Tax</v>
+        <v>acfr:RevenueFromDocumentsTransferTax</v>
       </c>
       <c r="D187" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38454,7 +38454,7 @@
       </c>
       <c r="C188" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Franchise Income Tax</v>
+        <v>acfr:RevenueFromFranchiseIncomeTax</v>
       </c>
       <c r="D188" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38471,7 +38471,7 @@
       </c>
       <c r="C189" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Hotel and Motel Tax</v>
+        <v>acfr:RevenueFromHotelAndMotelTax</v>
       </c>
       <c r="D189" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38488,7 +38488,7 @@
       </c>
       <c r="C190" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Income Tax</v>
+        <v>acfr:RevenueFromIncomeTax</v>
       </c>
       <c r="D190" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38505,7 +38505,7 @@
       </c>
       <c r="C191" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Industrial Facilities Tax</v>
+        <v>acfr:RevenueFromIndustrialFacilitiesTax</v>
       </c>
       <c r="D191" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38522,7 +38522,7 @@
       </c>
       <c r="C192" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Interest</v>
+        <v>acfr:RevenueFromInterest</v>
       </c>
       <c r="D192" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38539,7 +38539,7 @@
       </c>
       <c r="C193" s="135" t="str">
         <f t="shared" si="7"/>
-        <v>acfr:Revenues from Interest and Dividends</v>
+        <v>acfr:RevenueFromInterestAndDividends</v>
       </c>
       <c r="D193" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38555,8 +38555,8 @@
         <v>2194</v>
       </c>
       <c r="C194" s="135" t="str">
-        <f t="shared" ref="C194:C257" si="10">"acfr:"&amp;A194</f>
-        <v>acfr:Revenues from Interest and Dividends</v>
+        <f t="shared" si="7"/>
+        <v>acfr:RevenueFromInterestAndDividends</v>
       </c>
       <c r="D194" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38572,8 +38572,8 @@
         <v>2129</v>
       </c>
       <c r="C195" s="135" t="str">
-        <f t="shared" si="10"/>
-        <v>acfr:Revenues from Interest and Penalties on Special Assessments</v>
+        <f t="shared" ref="C195:C258" si="10">"acfr:"&amp;B195</f>
+        <v>acfr:RevenuesFromInterestAndPenaltiesOnSpecialAssessments</v>
       </c>
       <c r="D195" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38590,7 +38590,7 @@
       </c>
       <c r="C196" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Interest and Penalties on Taxes</v>
+        <v>acfr:RevenueFromInterestAndPenaltiesOnTaxes</v>
       </c>
       <c r="D196" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38607,7 +38607,7 @@
       </c>
       <c r="C197" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Interest and Penalties on Taxes</v>
+        <v>acfr:RevenueFromInterestAndPenaltiesOnTaxes</v>
       </c>
       <c r="D197" s="120" t="str">
         <f t="shared" si="9"/>
@@ -38624,7 +38624,7 @@
       </c>
       <c r="C198" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Interest, Dividends, Royalties and Rent</v>
+        <v>acfr:RevenueFromInterestAndRent</v>
       </c>
       <c r="D198" s="120" t="str">
         <f t="shared" ref="D198:D229" si="11">IF(RIGHT(B198, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -38641,7 +38641,7 @@
       </c>
       <c r="C199" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Lottery for Education, Lottery Proceeds</v>
+        <v>acfr:RevenueFromLotteryForEducationLotteryProceeds</v>
       </c>
       <c r="D199" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38658,7 +38658,7 @@
       </c>
       <c r="C200" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Marijuana Tax</v>
+        <v>acfr:RevenueFromMarijuanaTax</v>
       </c>
       <c r="D200" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38675,7 +38675,7 @@
       </c>
       <c r="C201" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Meals Tax</v>
+        <v>acfr:RevenueFromMealsTax</v>
       </c>
       <c r="D201" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38692,7 +38692,7 @@
       </c>
       <c r="C202" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Motor Fuel Tax</v>
+        <v>acfr:RevenueFromMotorFuelTax</v>
       </c>
       <c r="D202" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38709,7 +38709,7 @@
       </c>
       <c r="C203" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from National Forest Reserve Taxes</v>
+        <v>acfr:RevenueFromNationalForestReserveTaxes</v>
       </c>
       <c r="D203" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38726,7 +38726,7 @@
       </c>
       <c r="C204" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Nursing Home and Hospital Provider Fees</v>
+        <v>acfr:RevenueFromNursingHomeAndHospitalProviderFees</v>
       </c>
       <c r="D204" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38743,7 +38743,7 @@
       </c>
       <c r="C205" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Other Tax for General Purpose</v>
+        <v>acfr:RevenueFromOtherTaxForGeneralPurpose</v>
       </c>
       <c r="D205" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38760,7 +38760,7 @@
       </c>
       <c r="C206" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Parking Occupancy Tax</v>
+        <v>acfr:RevenueFromParkingOccupancyTax</v>
       </c>
       <c r="D206" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38777,7 +38777,7 @@
       </c>
       <c r="C207" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Parking Occupancy Tax</v>
+        <v>acfr:RevenueFromParkingOccupancyTax</v>
       </c>
       <c r="D207" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38794,7 +38794,7 @@
       </c>
       <c r="C208" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Property Tax</v>
+        <v>acfr:RevenueFromPropertyTax</v>
       </c>
       <c r="D208" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38811,7 +38811,7 @@
       </c>
       <c r="C209" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Property Tax Administration Fee</v>
+        <v>acfr:RevenueFromPropertyTaxAdministrationFee</v>
       </c>
       <c r="D209" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38828,7 +38828,7 @@
       </c>
       <c r="C210" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Property Transfer Tax</v>
+        <v>acfr:RevenueFromPropertyTransferTax</v>
       </c>
       <c r="D210" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38845,7 +38845,7 @@
       </c>
       <c r="C211" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Rent</v>
+        <v>acfr:RevenueFromRent</v>
       </c>
       <c r="D211" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38862,7 +38862,7 @@
       </c>
       <c r="C212" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Rents and Royalties</v>
+        <v>acfr:RevenueFromRentsAndRoyalties</v>
       </c>
       <c r="D212" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38879,7 +38879,7 @@
       </c>
       <c r="C213" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Royalties</v>
+        <v>acfr:RevenueFromRoyalties</v>
       </c>
       <c r="D213" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38896,7 +38896,7 @@
       </c>
       <c r="C214" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Sales and Use Tax</v>
+        <v>acfr:RevenueFromSalesAndUseTax</v>
       </c>
       <c r="D214" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38913,7 +38913,7 @@
       </c>
       <c r="C215" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Sales Tax</v>
+        <v>acfr:RevenueFromSalesTax</v>
       </c>
       <c r="D215" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38930,7 +38930,7 @@
       </c>
       <c r="C216" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Special Assessments</v>
+        <v>acfr:RevenueFromSpecialAssessments</v>
       </c>
       <c r="D216" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38947,7 +38947,7 @@
       </c>
       <c r="C217" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Sub Marginal Land Act</v>
+        <v>acfr:RevenueFromSubMarginalLandAct</v>
       </c>
       <c r="D217" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38964,7 +38964,7 @@
       </c>
       <c r="C218" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Subsidies</v>
+        <v>acfr:RevenueFromSubsidies</v>
       </c>
       <c r="D218" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38981,7 +38981,7 @@
       </c>
       <c r="C219" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Tax Reverted Property</v>
+        <v>acfr:RevenueFromTaxRevertedProperty</v>
       </c>
       <c r="D219" s="120" t="str">
         <f t="shared" si="11"/>
@@ -38998,7 +38998,7 @@
       </c>
       <c r="C220" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Taxes</v>
+        <v>acfr:RevenueFromTaxes</v>
       </c>
       <c r="D220" s="120" t="str">
         <f t="shared" si="11"/>
@@ -39015,7 +39015,7 @@
       </c>
       <c r="C221" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Trailer Tax</v>
+        <v>acfr:RevenueFromTrailerTax</v>
       </c>
       <c r="D221" s="120" t="str">
         <f t="shared" si="11"/>
@@ -39032,7 +39032,7 @@
       </c>
       <c r="C222" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Transaction Privilege Tax</v>
+        <v>acfr:RevenueFromTransactionPrivilegeTax</v>
       </c>
       <c r="D222" s="120" t="str">
         <f t="shared" si="11"/>
@@ -39049,7 +39049,7 @@
       </c>
       <c r="C223" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Transfer Stamps Tax</v>
+        <v>acfr:RevenueFromTransferStampsTax</v>
       </c>
       <c r="D223" s="120" t="str">
         <f t="shared" si="11"/>
@@ -39066,7 +39066,7 @@
       </c>
       <c r="C224" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Unclaimed Property</v>
+        <v>acfr:RevenueFromUnclaimedProperty</v>
       </c>
       <c r="D224" s="120" t="str">
         <f t="shared" si="11"/>
@@ -39083,7 +39083,7 @@
       </c>
       <c r="C225" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Usage of Utilities Tax</v>
+        <v>acfr:RevenueFromUsageOfUtilitiesTax</v>
       </c>
       <c r="D225" s="120" t="str">
         <f t="shared" si="11"/>
@@ -39100,7 +39100,7 @@
       </c>
       <c r="C226" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Revenues from Vehicles Tax</v>
+        <v>acfr:RevenueFromVehiclesTax</v>
       </c>
       <c r="D226" s="120" t="str">
         <f t="shared" si="11"/>
@@ -39117,7 +39117,7 @@
       </c>
       <c r="C227" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Appropriations</v>
+        <v>acfr:StateAppropriations</v>
       </c>
       <c r="D227" s="120" t="str">
         <f t="shared" si="11"/>
@@ -39134,7 +39134,7 @@
       </c>
       <c r="C228" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Capital Grants</v>
+        <v>acfr:StateCapitalGrants</v>
       </c>
       <c r="D228" s="120" t="str">
         <f t="shared" si="11"/>
@@ -39151,7 +39151,7 @@
       </c>
       <c r="C229" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Grants, Court Equity</v>
+        <v>acfr:StateGrantsCourtEquity</v>
       </c>
       <c r="D229" s="120" t="str">
         <f t="shared" si="11"/>
@@ -39168,7 +39168,7 @@
       </c>
       <c r="C230" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Grants, Crime Victims Rights</v>
+        <v>acfr:StateGrantsCrimeVictimsRights</v>
       </c>
       <c r="D230" s="120" t="str">
         <f t="shared" ref="D230:D246" si="12">IF(RIGHT(B230, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -39185,7 +39185,7 @@
       </c>
       <c r="C231" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Grants, Culture and Recreation</v>
+        <v>acfr:StateGrantsCultureAndRecreation</v>
       </c>
       <c r="D231" s="120" t="str">
         <f t="shared" si="12"/>
@@ -39202,7 +39202,7 @@
       </c>
       <c r="C232" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Grants, Drug Case Information Management Account</v>
+        <v>acfr:StateGrantsDrugCaseInformationManagementAccount</v>
       </c>
       <c r="D232" s="120" t="str">
         <f t="shared" si="12"/>
@@ -39219,7 +39219,7 @@
       </c>
       <c r="C233" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Grants, Drunk Driving Case Flow Assistance</v>
+        <v>acfr:StateGrantsDrunkDrivingCaseFlowAssistance</v>
       </c>
       <c r="D233" s="120" t="str">
         <f t="shared" si="12"/>
@@ -39236,7 +39236,7 @@
       </c>
       <c r="C234" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Grants, Health</v>
+        <v>acfr:StateGrantsHealth</v>
       </c>
       <c r="D234" s="120" t="str">
         <f t="shared" si="12"/>
@@ -39253,7 +39253,7 @@
       </c>
       <c r="C235" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Grants, Highway and Streets</v>
+        <v>acfr:StateGrantsHighwaysAndStreets</v>
       </c>
       <c r="D235" s="120" t="str">
         <f t="shared" si="12"/>
@@ -39270,7 +39270,7 @@
       </c>
       <c r="C236" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Grants, Indigent Defense Grant</v>
+        <v>acfr:StateGrantsIndigentDefenseGrant</v>
       </c>
       <c r="D236" s="120" t="str">
         <f t="shared" si="12"/>
@@ -39287,7 +39287,7 @@
       </c>
       <c r="C237" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Grants, Local Community Stabilization Share</v>
+        <v>acfr:StateGrantsLocalCommunityStabilizationShare</v>
       </c>
       <c r="D237" s="120" t="str">
         <f t="shared" si="12"/>
@@ -39304,7 +39304,7 @@
       </c>
       <c r="C238" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Grants, Public Safety</v>
+        <v>acfr:StateGrantsPublicSafety</v>
       </c>
       <c r="D238" s="120" t="str">
         <f t="shared" si="12"/>
@@ -39321,7 +39321,7 @@
       </c>
       <c r="C239" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Grants, Sanitation</v>
+        <v>acfr:StateGrantsSanitation</v>
       </c>
       <c r="D239" s="120" t="str">
         <f t="shared" si="12"/>
@@ -39338,7 +39338,7 @@
       </c>
       <c r="C240" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Grants, Special Election Reimbursement</v>
+        <v>acfr:StateGrantsSpecialElectionReimbursement</v>
       </c>
       <c r="D240" s="120" t="str">
         <f t="shared" si="12"/>
@@ -39355,7 +39355,7 @@
       </c>
       <c r="C241" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Grants, State Revenue Sharing</v>
+        <v>acfr:StateGrantsStateRevenueSharing</v>
       </c>
       <c r="D241" s="120" t="str">
         <f t="shared" si="12"/>
@@ -39372,7 +39372,7 @@
       </c>
       <c r="C242" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Grants, Survey and Remonumentation</v>
+        <v>acfr:StateGrantsSurveyAndRemonumentation</v>
       </c>
       <c r="D242" s="120" t="str">
         <f t="shared" si="12"/>
@@ -39389,7 +39389,7 @@
       </c>
       <c r="C243" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Grants, Welfare</v>
+        <v>acfr:StateGrantsWelfare</v>
       </c>
       <c r="D243" s="120" t="str">
         <f t="shared" si="12"/>
@@ -39406,7 +39406,7 @@
       </c>
       <c r="C244" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State OPEB Contribution</v>
+        <v>acfr:StateOPEBContribution</v>
       </c>
       <c r="D244" s="120" t="str">
         <f t="shared" si="12"/>
@@ -39423,7 +39423,7 @@
       </c>
       <c r="C245" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:State Retirement Plan Contributions</v>
+        <v>acfr:StateRetirementPlanContributions</v>
       </c>
       <c r="D245" s="120" t="str">
         <f t="shared" si="12"/>
@@ -39440,7 +39440,7 @@
       </c>
       <c r="C246" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Taxes and Tax Related Revenues</v>
+        <v>acfr:TaxesAndTaxRelatedRevenues</v>
       </c>
       <c r="D246" s="120" t="str">
         <f t="shared" si="12"/>
@@ -39457,7 +39457,7 @@
       </c>
       <c r="C247" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Change in Accounting Principle</v>
+        <v>acfr:ChangeInAccountingPrinciple</v>
       </c>
       <c r="D247" s="120" t="str">
         <f>IF(RIGHT(B247, 8)="Abstract", "Abstract", "Net Position")</f>
@@ -39474,7 +39474,7 @@
       </c>
       <c r="C248" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Net Position, Restated</v>
+        <v>acfr:NetPositionRestated</v>
       </c>
       <c r="D248" s="120" t="str">
         <f>IF(RIGHT(B248, 8)="Abstract", "Abstract", "Net Position")</f>
@@ -39491,7 +39491,7 @@
       </c>
       <c r="C249" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Bond or Insurance Recoveries</v>
+        <v>acfr:BondOrInsuranceRecoveries</v>
       </c>
       <c r="D249" s="120" t="str">
         <f t="shared" ref="D249:D261" si="13">IF(RIGHT(B249, 8)="Abstract", "Abstract", "Capital Contributions")</f>
@@ -39508,7 +39508,7 @@
       </c>
       <c r="C250" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Capital Contributions and Transfers</v>
+        <v>acfr:TotalCapitalContributionsAndTransfers</v>
       </c>
       <c r="D250" s="120" t="str">
         <f t="shared" si="13"/>
@@ -39542,7 +39542,7 @@
       </c>
       <c r="C252" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Contributions from Citizens and Developers</v>
+        <v>acfr:ContributionsfromCitizensAndDevelopers</v>
       </c>
       <c r="D252" s="120" t="str">
         <f t="shared" si="13"/>
@@ -39559,7 +39559,7 @@
       </c>
       <c r="C253" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Contributions, Capital</v>
+        <v>acfr:ContributionsCapital</v>
       </c>
       <c r="D253" s="120" t="str">
         <f t="shared" si="13"/>
@@ -39576,7 +39576,7 @@
       </c>
       <c r="C254" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Contributions, Other</v>
+        <v>acfr:ContributionsOther</v>
       </c>
       <c r="D254" s="120" t="str">
         <f t="shared" si="13"/>
@@ -39593,7 +39593,7 @@
       </c>
       <c r="C255" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Other Financing Sources</v>
+        <v>acfr:OtherFinancingSources</v>
       </c>
       <c r="D255" s="120" t="str">
         <f t="shared" si="13"/>
@@ -39610,7 +39610,7 @@
       </c>
       <c r="C256" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Other Financing Sources, Lease Financing</v>
+        <v>acfr:OtherFinancingSourcesLeaseFinancing</v>
       </c>
       <c r="D256" s="120" t="str">
         <f t="shared" si="13"/>
@@ -39627,7 +39627,7 @@
       </c>
       <c r="C257" s="135" t="str">
         <f t="shared" si="10"/>
-        <v>acfr:Premium on Bonds or Notes</v>
+        <v>acfr:PremiumOnBondsOrNotes</v>
       </c>
       <c r="D257" s="120" t="str">
         <f t="shared" si="13"/>
@@ -39643,8 +39643,8 @@
         <v>2264</v>
       </c>
       <c r="C258" s="135" t="str">
-        <f t="shared" ref="C258:C296" si="14">"acfr:"&amp;A258</f>
-        <v>acfr:Proceeds from Bond and Note Issuance</v>
+        <f t="shared" si="10"/>
+        <v>acfr:ProceedsFromBondAndNoteIssuance</v>
       </c>
       <c r="D258" s="120" t="str">
         <f t="shared" si="13"/>
@@ -39660,8 +39660,8 @@
         <v>2259</v>
       </c>
       <c r="C259" s="135" t="str">
-        <f t="shared" si="14"/>
-        <v>acfr:Proceeds from Sale of Bonds, Notes</v>
+        <f t="shared" ref="C259:C296" si="14">"acfr:"&amp;B259</f>
+        <v>acfr:ProceedsFromSaleOfBondsNotes</v>
       </c>
       <c r="D259" s="120" t="str">
         <f t="shared" si="13"/>
@@ -39678,7 +39678,7 @@
       </c>
       <c r="C260" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Transfer of Capital Assets In</v>
+        <v>acfr:TransfersIn</v>
       </c>
       <c r="D260" s="120" t="str">
         <f t="shared" si="13"/>
@@ -39695,7 +39695,7 @@
       </c>
       <c r="C261" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Transfers of Capital Assets From (To) Other Funds</v>
+        <v>acfr:TransfersofCapitalAssetsFromToOtherFunds</v>
       </c>
       <c r="D261" s="120" t="str">
         <f t="shared" si="13"/>
@@ -39712,7 +39712,7 @@
       </c>
       <c r="C262" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Transfers of Capital Assets Out</v>
+        <v>acfr:TransfersOut</v>
       </c>
       <c r="D262" s="120" t="str">
         <f>IF(RIGHT(B262, 8)="Abstract", "Abstract", "Capital Contributions")</f>
@@ -39729,7 +39729,7 @@
       </c>
       <c r="C263" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Allowances [Abstract]</v>
+        <v>acfr:RevenueFromAllowanceForTaxesAbstract</v>
       </c>
       <c r="D263" s="120" t="str">
         <f>IF(RIGHT(B263, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -39746,7 +39746,7 @@
       </c>
       <c r="C264" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Benefits Expense, Pension and OPEB [Abstract]</v>
+        <v>acfr:BenefitsExpensePensionAndOPEBAbstract</v>
       </c>
       <c r="D264" s="120" t="str">
         <f>IF(RIGHT(B264, 8)="Abstract", "Abstract", "Operating Expenses")</f>
@@ -39763,7 +39763,7 @@
       </c>
       <c r="C265" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Capital Contributions and Transfers [Abstract]</v>
+        <v>acfr:CapitalContributionsAndTransfersAbstract</v>
       </c>
       <c r="D265" s="120" t="str">
         <f>IF(RIGHT(B265, 8)="Abstract", "Abstract", "Capital Contributions")</f>
@@ -39780,7 +39780,7 @@
       </c>
       <c r="C266" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Charges for Services, Fines and Forfeitures [Abstract]</v>
+        <v>acfr:ChargesForServicesFinesAndForfeituresAbstract</v>
       </c>
       <c r="D266" s="120" t="str">
         <f>IF(RIGHT(B266, 8)="Abstract", "Abstract", "Operating Revenues")</f>
@@ -39797,7 +39797,7 @@
       </c>
       <c r="C267" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Charges for Services, General [Abstract]</v>
+        <v>acfr:ChargesForServicesAbstract</v>
       </c>
       <c r="D267" s="120" t="str">
         <f>IF(RIGHT(B267, 8)="Abstract", "Abstract", "Operating Revenues")</f>
@@ -39814,7 +39814,7 @@
       </c>
       <c r="C268" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Charges for Services, Licenses and Permits Revenues [Abstract]</v>
+        <v>acfr:ChargesForServicesLicensesAndPermitsRevenuesAbstract</v>
       </c>
       <c r="D268" s="120" t="str">
         <f>IF(RIGHT(B268, 8)="Abstract", "Abstract", "Operating Revenues")</f>
@@ -39831,7 +39831,7 @@
       </c>
       <c r="C269" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Contributions [Abstract]</v>
+        <v>acfr:ContributionsAbstract</v>
       </c>
       <c r="D269" s="120" t="str">
         <f>IF(RIGHT(B269, 8)="Abstract", "Abstract", "Capital Contributions")</f>
@@ -39848,7 +39848,7 @@
       </c>
       <c r="C270" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Contributions from Local Units [Abstract]</v>
+        <v>acfr:ContributionsFromLocalUnitsAbstract</v>
       </c>
       <c r="D270" s="120" t="str">
         <f>IF(RIGHT(B270, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -39865,7 +39865,7 @@
       </c>
       <c r="C271" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Expenses for Lottery Activities [Abstract]</v>
+        <v>acfr:ExpensesForLotteryActivitiesAbstract</v>
       </c>
       <c r="D271" s="120" t="str">
         <f>IF(RIGHT(B271, 8)="Abstract", "Abstract", "Operating Expenses")</f>
@@ -39882,7 +39882,7 @@
       </c>
       <c r="C272" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Grants, Contributions and Donations [Abstract]</v>
+        <v>acfr:GrantsContributionsAndDonationsAbstract</v>
       </c>
       <c r="D272" s="120" t="str">
         <f>IF(RIGHT(B272, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -39899,7 +39899,7 @@
       </c>
       <c r="C273" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Health Operating Expenses [Abstract]</v>
+        <v>acfr:HealthOperatingExpensesAbstract</v>
       </c>
       <c r="D273" s="120" t="str">
         <f>IF(RIGHT(B273, 8)="Abstract", "Abstract", "Operating Expenses")</f>
@@ -39916,7 +39916,7 @@
       </c>
       <c r="C274" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Intergovernmental Revenue [Abstract]</v>
+        <v>acfr:IntergovernmentalRevenueAbstract</v>
       </c>
       <c r="D274" s="120" t="str">
         <f>IF(RIGHT(B274, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -39933,7 +39933,7 @@
       </c>
       <c r="C275" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Intergovernmental Revenues from Federal Government [Abstract]</v>
+        <v>acfr:IntergovernmentalRevenueFromFederalGovernmentAbstract</v>
       </c>
       <c r="D275" s="120" t="str">
         <f>IF(RIGHT(B275, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -39950,7 +39950,7 @@
       </c>
       <c r="C276" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Intergovernmental Revenues from State Government [Abstract]</v>
+        <v>acfr:IntergovernmentalRevenueFromStateGovernmentAbstract</v>
       </c>
       <c r="D276" s="120" t="str">
         <f>IF(RIGHT(B276, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -39967,7 +39967,7 @@
       </c>
       <c r="C277" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Investment Income [Abstract]</v>
+        <v>acfr:InvestmentIncomeAbstract</v>
       </c>
       <c r="D277" s="120" t="str">
         <f>IF(RIGHT(B277, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -39984,7 +39984,7 @@
       </c>
       <c r="C278" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Investment Income and Rentals [Abstract]</v>
+        <v>acfr:InterestAndRentsRevenuesAbstract</v>
       </c>
       <c r="D278" s="120" t="str">
         <f>IF(RIGHT(B278, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -40001,7 +40001,7 @@
       </c>
       <c r="C279" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Lottery Revenues [Abstract]</v>
+        <v>acfr:LotteryRevenuesAbstract</v>
       </c>
       <c r="D279" s="120" t="str">
         <f>IF(RIGHT(B279, 8)="Abstract", "Abstract", "Operating Revenues")</f>
@@ -40018,7 +40018,7 @@
       </c>
       <c r="C280" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Net Position [Abstract]</v>
+        <v>acfr:NetPositionAbstract</v>
       </c>
       <c r="D280" s="120" t="str">
         <f>IF(RIGHT(B280, 8)="Abstract", "Abstract", "Net Position")</f>
@@ -40035,7 +40035,7 @@
       </c>
       <c r="C281" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Nonoperating Expenses [Abstract]</v>
+        <v>acfr:NonoperatingExpensesAbstract</v>
       </c>
       <c r="D281" s="120" t="str">
         <f>IF(RIGHT(B281, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -40052,7 +40052,7 @@
       </c>
       <c r="C282" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Nonoperating Revenues [Abstract]</v>
+        <v>acfr:NonoperatingRevenuesAbstract</v>
       </c>
       <c r="D282" s="120" t="str">
         <f>IF(RIGHT(B282, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -40069,7 +40069,7 @@
       </c>
       <c r="C283" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Nonoperating Revenues Expenses [Abstract]</v>
+        <v>acfr:NonoperatingRevenuesExpensesAbstract</v>
       </c>
       <c r="D283" s="120" t="str">
         <f>IF(RIGHT(B283, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -40086,7 +40086,7 @@
       </c>
       <c r="C284" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Operating Expenses [Abstract]</v>
+        <v>acfr:OperatingExpensesAbstract</v>
       </c>
       <c r="D284" s="120" t="str">
         <f>IF(RIGHT(B284, 8)="Abstract", "Abstract", "Operating Expenses")</f>
@@ -40103,7 +40103,7 @@
       </c>
       <c r="C285" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Operating Revenues [Abstract]</v>
+        <v>acfr:OperatingRevenuesAbstract</v>
       </c>
       <c r="D285" s="120" t="str">
         <f>IF(RIGHT(B285, 8)="Abstract", "Abstract", "Operating Revenues")</f>
@@ -40120,7 +40120,7 @@
       </c>
       <c r="C286" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Other Financing Sources [Abstract]</v>
+        <v>acfr:OtherFinancingSourcesAbstract</v>
       </c>
       <c r="D286" s="120" t="str">
         <f>IF(RIGHT(B286, 8)="Abstract", "Abstract", "Capital Contributions")</f>
@@ -40137,7 +40137,7 @@
       </c>
       <c r="C287" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Property Tax [Abstract]</v>
+        <v>acfr:PropertyTaxAbstract</v>
       </c>
       <c r="D287" s="120" t="str">
         <f>IF(RIGHT(B287, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -40154,7 +40154,7 @@
       </c>
       <c r="C288" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Proprietary Funds, Revenues, Expenses and Changes in Fund Net Position [Abstract]</v>
+        <v>acfr:ProprietaryFundsRevenuesExpensesAbstract</v>
       </c>
       <c r="D288" s="120" t="str">
         <f>IF(RIGHT(B288, 8)="Abstract", "Abstract", "Operating Revenues")</f>
@@ -40171,7 +40171,7 @@
       </c>
       <c r="C289" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Public Works Operating Expenses [Abstract]</v>
+        <v>acfr:PublicWorksOperatingExpensesAbstract</v>
       </c>
       <c r="D289" s="120" t="str">
         <f>IF(RIGHT(B289, 8)="Abstract", "Abstract", "Operating Expenses")</f>
@@ -40188,7 +40188,7 @@
       </c>
       <c r="C290" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Recreation and Culture Operating Expenses [Abstract]</v>
+        <v>acfr:RecreationAndCultureOperatingExpensesAbstract</v>
       </c>
       <c r="D290" s="120" t="str">
         <f>IF(RIGHT(B290, 8)="Abstract", "Abstract", "Operating Expenses")</f>
@@ -40205,7 +40205,7 @@
       </c>
       <c r="C291" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Revenue from Interest and Dividends [Abstract]</v>
+        <v>acfr:RevenueFromInterestAndDividendsAbstract</v>
       </c>
       <c r="D291" s="120" t="str">
         <f>IF(RIGHT(B291, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -40222,7 +40222,7 @@
       </c>
       <c r="C292" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Revenues from Rents and Royalties [Abstract]</v>
+        <v>acfr:RevenuesFromRentsAndRoyaltiesAbstract</v>
       </c>
       <c r="D292" s="120" t="str">
         <f>IF(RIGHT(B292, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -40239,7 +40239,7 @@
       </c>
       <c r="C293" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Special Assessments [Abstract]</v>
+        <v>acfr:SpecialAssessmentsAbstract</v>
       </c>
       <c r="D293" s="120" t="str">
         <f>IF(RIGHT(B293, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -40256,7 +40256,7 @@
       </c>
       <c r="C294" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Tax and Tax Related Revenues and Allowances [Abstract]</v>
+        <v>acfr:TaxAndTaxRelatedRevenuesAbstract</v>
       </c>
       <c r="D294" s="120" t="str">
         <f>IF(RIGHT(B294, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -40273,7 +40273,7 @@
       </c>
       <c r="C295" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Tax Revenues [Abstract]</v>
+        <v>acfr:TaxRevenuesAbstract</v>
       </c>
       <c r="D295" s="120" t="str">
         <f>IF(RIGHT(B295, 8)="Abstract", "Abstract", "Nonoperating Revenues Expenses")</f>
@@ -40290,7 +40290,7 @@
       </c>
       <c r="C296" s="135" t="str">
         <f t="shared" si="14"/>
-        <v>acfr:Transfers [Abstract]</v>
+        <v>acfr:TransfersAbstract</v>
       </c>
       <c r="D296" s="120" t="str">
         <f>IF(RIGHT(B296, 8)="Abstract", "Abstract", "Capital Contributions")</f>
@@ -41608,7 +41608,7 @@
   </sheetPr>
   <dimension ref="A1:E442"/>
   <sheetViews>
-    <sheetView topLeftCell="A146" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -48029,7 +48029,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -48215,8 +48215,8 @@
   </sheetPr>
   <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScale="88" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView zoomScale="88" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -49877,7 +49877,7 @@
   <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O51" sqref="O51"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
#199 updated template to fix header formulas
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B27A18F-843F-EA4D-98EC-F116869F71BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729E39D0-104E-B14B-8FFE-E49576C28EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32680" yWindow="-9880" windowWidth="28800" windowHeight="17500" tabRatio="834" firstSheet="4" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="834" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup Net Position" sheetId="8" state="hidden" r:id="rId1"/>
@@ -12273,10 +12273,9 @@
   </cellStyles>
   <dxfs count="112">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
-          <bgColor theme="0"/>
+          <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12296,13 +12295,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
@@ -12318,12 +12310,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="1" tint="0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12338,9 +12327,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12529,6 +12521,14 @@
       <fill>
         <patternFill>
           <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12925,25 +12925,9 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color theme="0"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill>
           <bgColor theme="0"/>
@@ -12964,6 +12948,22 @@
       <font>
         <color theme="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -19300,8 +19300,8 @@
   </sheetPr>
   <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView zoomScale="119" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:J59"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -19317,13 +19317,13 @@
     <col min="11" max="16384" width="10.83203125" style="120"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17">
+    <row r="1" spans="1:10" ht="16">
       <c r="A1" s="80" t="s">
         <v>1061</v>
       </c>
       <c r="B1" s="181" t="str">
-        <f>_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3)</f>
-        <v xml:space="preserve">, </v>
+        <f>IF('Master Info'!C2&lt;&gt;"",_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3),"Add location in master info tab")</f>
+        <v>Add location in master info tab</v>
       </c>
       <c r="C1" s="178"/>
       <c r="D1" s="178"/>
@@ -19355,9 +19355,9 @@
       <c r="A4" s="87" t="s">
         <v>1063</v>
       </c>
-      <c r="B4" s="204">
-        <f>'Master Info'!C4</f>
-        <v>0</v>
+      <c r="B4" s="204" t="str">
+        <f>IF('Master Info'!C4, 'Master Info'!C4, "Add date in Master Info tab")</f>
+        <v>Add date in Master Info tab</v>
       </c>
       <c r="C4" s="178"/>
       <c r="D4" s="178"/>
@@ -20747,8 +20747,8 @@
   </sheetPr>
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -20787,9 +20787,9 @@
       <c r="A4" s="87" t="s">
         <v>1063</v>
       </c>
-      <c r="B4" s="219">
-        <f>'Master Info'!C4</f>
-        <v>0</v>
+      <c r="B4" s="219" t="str">
+        <f>IF('Master Info'!C4, 'Master Info'!C4, "Add date in Master Info tab")</f>
+        <v>Add date in Master Info tab</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16">
@@ -20991,8 +20991,8 @@
   </sheetPr>
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M59" sqref="M59"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -21009,13 +21009,13 @@
     <col min="11" max="16384" width="9" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17">
+    <row r="1" spans="1:10" ht="16">
       <c r="A1" s="28" t="s">
         <v>1061</v>
       </c>
       <c r="B1" s="156" t="str">
-        <f>_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3)</f>
-        <v xml:space="preserve">, </v>
+        <f>IF('Master Info'!C2&lt;&gt;"",_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3),"Add location in master info tab")</f>
+        <v>Add location in master info tab</v>
       </c>
       <c r="C1" s="38"/>
       <c r="D1" s="32"/>
@@ -21060,8 +21060,8 @@
         <v>1063</v>
       </c>
       <c r="B4" s="197" t="str">
-        <f>_xlfn.CONCAT("For the year ended ", TEXT('Master Info'!C4, "mmmm dd, yyyy"))</f>
-        <v>For the year ended January 00, 1900</v>
+        <f>IF('Master Info'!C4, 'Master Info'!C4, "Add date in Master Info tab")</f>
+        <v>Add date in Master Info tab</v>
       </c>
       <c r="C4" s="38"/>
       <c r="D4" s="32"/>
@@ -22474,8 +22474,8 @@
   </sheetPr>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -22485,13 +22485,13 @@
     <col min="3" max="16384" width="10.83203125" style="120"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17">
+    <row r="1" spans="1:2" ht="16">
       <c r="A1" s="80" t="s">
         <v>1061</v>
       </c>
       <c r="B1" s="156" t="str">
-        <f>_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3)</f>
-        <v xml:space="preserve">, </v>
+        <f>IF('Master Info'!C2&lt;&gt;"",_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3),"Add location in master info tab")</f>
+        <v>Add location in master info tab</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17">
@@ -22510,13 +22510,13 @@
         <v>2847</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18" thickBot="1">
+    <row r="4" spans="1:2" ht="17" thickBot="1">
       <c r="A4" s="87" t="s">
         <v>1063</v>
       </c>
       <c r="B4" s="226" t="str">
-        <f>_xlfn.CONCAT("For the year ended ", TEXT('Master Info'!C4, "mmmm dd, yyyy"))</f>
-        <v>For the year ended January 00, 1900</v>
+        <f>IF('Master Info'!C4, 'Master Info'!C4, "Add date in Master Info tab")</f>
+        <v>Add date in Master Info tab</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="32">
@@ -22686,14 +22686,14 @@
   </sheetPr>
   <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="33.83203125" style="84" customWidth="1"/>
-    <col min="2" max="2" width="41.5" style="84" customWidth="1"/>
+    <col min="2" max="2" width="35" style="84" customWidth="1"/>
     <col min="3" max="10" width="18.6640625" style="84" customWidth="1"/>
     <col min="11" max="16384" width="9" style="84"/>
   </cols>
@@ -22703,8 +22703,8 @@
         <v>1061</v>
       </c>
       <c r="B1" s="81" t="str">
-        <f>_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3)</f>
-        <v xml:space="preserve">, </v>
+        <f>IF('Master Info'!C2&lt;&gt;"",_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3),"Add location in master info tab")</f>
+        <v>Add location in master info tab</v>
       </c>
       <c r="C1" s="82"/>
       <c r="D1" s="82"/>
@@ -22751,9 +22751,9 @@
       <c r="A4" s="87" t="s">
         <v>1063</v>
       </c>
-      <c r="B4" s="227">
-        <f>'Master Info'!C4</f>
-        <v>0</v>
+      <c r="B4" s="227" t="str">
+        <f>IF('Master Info'!C4, 'Master Info'!C4, "Add date in Master Info tab")</f>
+        <v>Add date in Master Info tab</v>
       </c>
       <c r="C4" s="82"/>
       <c r="D4" s="82"/>
@@ -25027,8 +25027,8 @@
   </sheetPr>
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -25044,8 +25044,8 @@
         <v>1061</v>
       </c>
       <c r="B1" s="81" t="str">
-        <f>_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3)</f>
-        <v xml:space="preserve">, </v>
+        <f>IF('Master Info'!C2&lt;&gt;"",_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3),"Add location in master info tab")</f>
+        <v>Add location in master info tab</v>
       </c>
       <c r="C1" s="82"/>
       <c r="D1" s="82"/>
@@ -25093,8 +25093,8 @@
         <v>1063</v>
       </c>
       <c r="B4" s="227" t="str">
-        <f>_xlfn.CONCAT("For the year ended ", TEXT('Master Info'!C4, "mmmm dd, yyyy"))</f>
-        <v>For the year ended January 00, 1900</v>
+        <f>IF('Master Info'!C4, 'Master Info'!C4, "Add date in Master Info tab")</f>
+        <v>Add date in Master Info tab</v>
       </c>
       <c r="C4" s="82"/>
       <c r="D4" s="82"/>
@@ -25724,27 +25724,27 @@
         <v>0</v>
       </c>
       <c r="D38" s="228" t="str">
-        <f>IF(D$7="Type fund name","",SUM(D26:D37))</f>
+        <f t="shared" ref="D38:I38" si="3">IF(D$7="Type fund name","",SUM(D26:D37))</f>
         <v/>
       </c>
       <c r="E38" s="228" t="str">
-        <f>IF(E$7="Type fund name","",SUM(E26:E37))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F38" s="228" t="str">
-        <f>IF(F$7="Type fund name","",SUM(F26:F37))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="G38" s="228" t="str">
-        <f>IF(G$7="Type fund name","",SUM(G26:G37))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H38" s="228" t="str">
-        <f>IF(H$7="Type fund name","",SUM(H26:H37))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I38" s="228" t="str">
-        <f>IF(I$7="Type fund name","",SUM(I26:I37))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J38" s="228">
@@ -25768,27 +25768,27 @@
         <v/>
       </c>
       <c r="E39" s="229" t="str">
-        <f t="shared" ref="E39:I39" si="3">IF(E$7="Type fund name","",E23-E38)</f>
+        <f t="shared" ref="E39:I39" si="4">IF(E$7="Type fund name","",E23-E38)</f>
         <v/>
       </c>
       <c r="F39" s="229" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="G39" s="229" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="H39" s="229" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I39" s="229" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="J39" s="229">
-        <f t="shared" ref="J39" si="4">IF(J$7="","",SUM(D39:I39))</f>
+        <f t="shared" ref="J39" si="5">IF(J$7="","",SUM(D39:I39))</f>
         <v>0</v>
       </c>
     </row>
@@ -25847,7 +25847,7 @@
       <c r="H43" s="206"/>
       <c r="I43" s="206"/>
       <c r="J43" s="228">
-        <f t="shared" ref="J43:J54" si="5">IF(J$7="","",SUM(D43:I43))</f>
+        <f t="shared" ref="J43:J54" si="6">IF(J$7="","",SUM(D43:I43))</f>
         <v>0</v>
       </c>
     </row>
@@ -25865,7 +25865,7 @@
       <c r="H44" s="205"/>
       <c r="I44" s="205"/>
       <c r="J44" s="228">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -25883,7 +25883,7 @@
       <c r="H45" s="205"/>
       <c r="I45" s="205"/>
       <c r="J45" s="228">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K45" s="194"/>
@@ -25902,7 +25902,7 @@
       <c r="H46" s="205"/>
       <c r="I46" s="205"/>
       <c r="J46" s="228">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -25920,7 +25920,7 @@
       <c r="H47" s="205"/>
       <c r="I47" s="205"/>
       <c r="J47" s="228">
-        <f t="shared" ref="J47:J52" si="6">IF(J$7="","",SUM(D47:I47))</f>
+        <f t="shared" ref="J47:J52" si="7">IF(J$7="","",SUM(D47:I47))</f>
         <v>0</v>
       </c>
     </row>
@@ -25938,7 +25938,7 @@
       <c r="H48" s="205"/>
       <c r="I48" s="205"/>
       <c r="J48" s="228">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -25956,7 +25956,7 @@
       <c r="H49" s="205"/>
       <c r="I49" s="205"/>
       <c r="J49" s="228">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -25974,7 +25974,7 @@
       <c r="H50" s="205"/>
       <c r="I50" s="205"/>
       <c r="J50" s="228">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -25992,7 +25992,7 @@
       <c r="H51" s="205"/>
       <c r="I51" s="205"/>
       <c r="J51" s="228">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -26010,7 +26010,7 @@
       <c r="H52" s="205"/>
       <c r="I52" s="205"/>
       <c r="J52" s="228">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -26026,31 +26026,31 @@
         <v>0</v>
       </c>
       <c r="D53" s="228" t="str">
-        <f t="shared" ref="D53:I53" si="7">IF(D$7="Type fund name","",SUM(D42:D52))</f>
+        <f t="shared" ref="D53:I53" si="8">IF(D$7="Type fund name","",SUM(D42:D52))</f>
         <v/>
       </c>
       <c r="E53" s="228" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F53" s="228" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="G53" s="228" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="H53" s="228" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="I53" s="228" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="J53" s="228">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -26062,35 +26062,35 @@
         <v>2285</v>
       </c>
       <c r="C54" s="229">
-        <f>IF(C$7="Type fund name","",C23-C38+C53)</f>
+        <f t="shared" ref="C54:I54" si="9">IF(C$7="Type fund name","",C23-C38+C53)</f>
         <v>0</v>
       </c>
       <c r="D54" s="229" t="str">
-        <f>IF(D$7="Type fund name","",D23-D38+D53)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="E54" s="229" t="str">
-        <f>IF(E$7="Type fund name","",E23-E38+E53)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="F54" s="229" t="str">
-        <f>IF(F$7="Type fund name","",F23-F38+F53)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G54" s="229" t="str">
-        <f>IF(G$7="Type fund name","",G23-G38+G53)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="H54" s="229" t="str">
-        <f>IF(H$7="Type fund name","",H23-H38+H53)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I54" s="229" t="str">
-        <f>IF(I$7="Type fund name","",I23-I38+I53)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="J54" s="229">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -26134,7 +26134,7 @@
       <c r="H57" s="205"/>
       <c r="I57" s="205"/>
       <c r="J57" s="228">
-        <f t="shared" ref="J57:J67" si="8">IF(J$7="","",SUM(D57:I57))</f>
+        <f t="shared" ref="J57:J67" si="10">IF(J$7="","",SUM(D57:I57))</f>
         <v>0</v>
       </c>
     </row>
@@ -26152,7 +26152,7 @@
       <c r="H58" s="205"/>
       <c r="I58" s="205"/>
       <c r="J58" s="228">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -26170,7 +26170,7 @@
       <c r="H59" s="205"/>
       <c r="I59" s="205"/>
       <c r="J59" s="228">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -26188,7 +26188,7 @@
       <c r="H60" s="205"/>
       <c r="I60" s="205"/>
       <c r="J60" s="228">
-        <f t="shared" ref="J60:J65" si="9">IF(J$7="","",SUM(D60:I60))</f>
+        <f t="shared" ref="J60:J65" si="11">IF(J$7="","",SUM(D60:I60))</f>
         <v>0</v>
       </c>
     </row>
@@ -26206,7 +26206,7 @@
       <c r="H61" s="205"/>
       <c r="I61" s="205"/>
       <c r="J61" s="228">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -26224,7 +26224,7 @@
       <c r="H62" s="205"/>
       <c r="I62" s="205"/>
       <c r="J62" s="228">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -26242,7 +26242,7 @@
       <c r="H63" s="205"/>
       <c r="I63" s="205"/>
       <c r="J63" s="228">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -26260,7 +26260,7 @@
       <c r="H64" s="205"/>
       <c r="I64" s="205"/>
       <c r="J64" s="228">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -26278,7 +26278,7 @@
       <c r="H65" s="205"/>
       <c r="I65" s="205"/>
       <c r="J65" s="228">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -26294,31 +26294,31 @@
         <v>0</v>
       </c>
       <c r="D66" s="228" t="str">
-        <f t="shared" ref="D66:I66" si="10">IF(D$7="Type fund name","",SUM(D57:D65))</f>
+        <f t="shared" ref="D66:I66" si="12">IF(D$7="Type fund name","",SUM(D57:D65))</f>
         <v/>
       </c>
       <c r="E66" s="228" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="F66" s="228" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="G66" s="228" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="H66" s="228" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="I66" s="228" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="J66" s="228">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="F66" s="228" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G66" s="228" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H66" s="228" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="I66" s="228" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="J66" s="228">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -26334,28 +26334,28 @@
         <v>0</v>
       </c>
       <c r="D67" s="230" t="str">
-        <f t="shared" ref="D67:I67" si="11">IF(D$7="Type fund name","",D54+D66)</f>
+        <f t="shared" ref="D67:I67" si="13">IF(D$7="Type fund name","",D54+D66)</f>
         <v/>
       </c>
       <c r="E67" s="230"/>
       <c r="F67" s="230" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="G67" s="230" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="H67" s="230" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I67" s="230" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="J67" s="230">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -26400,7 +26400,7 @@
       <c r="H70" s="200"/>
       <c r="I70" s="200"/>
       <c r="J70" s="228">
-        <f t="shared" ref="J70" si="12">IF(J$7="","",SUM(D70:I70))</f>
+        <f t="shared" ref="J70" si="14">IF(J$7="","",SUM(D70:I70))</f>
         <v>0</v>
       </c>
     </row>
@@ -26416,27 +26416,27 @@
         <v>0</v>
       </c>
       <c r="D71" s="216" t="str">
-        <f>IF(D7="Type fund name","",D67+D70)</f>
+        <f t="shared" ref="D71:I71" si="15">IF(D7="Type fund name","",D67+D70)</f>
         <v/>
       </c>
       <c r="E71" s="216" t="str">
-        <f>IF(E7="Type fund name","",E67+E70)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="F71" s="216" t="str">
-        <f>IF(F7="Type fund name","",F67+F70)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="G71" s="216" t="str">
-        <f>IF(G7="Type fund name","",G67+G70)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H71" s="216" t="str">
-        <f>IF(H7="Type fund name","",H67+H70)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="I71" s="216" t="str">
-        <f>IF(I7="Type fund name","",I67+I70)</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="J71" s="216">
@@ -26566,7 +26566,7 @@
       <formula>NOT(ISERROR(SEARCH("custom",A57)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23:C24 C38 C71:J71 C40">
+  <conditionalFormatting sqref="C23:C24 C38 C40 C71:J71">
     <cfRule type="expression" dxfId="33" priority="17" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
@@ -26576,35 +26576,35 @@
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C39:I39">
+    <cfRule type="expression" dxfId="31" priority="1" stopIfTrue="1">
+      <formula>C$7=""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C53:I55">
-    <cfRule type="expression" dxfId="31" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="8" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66:I67">
-    <cfRule type="expression" dxfId="30" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="7" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:J71">
-    <cfRule type="cellIs" dxfId="29" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="18" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="19" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="20" operator="notEqual">
+    <cfRule type="cellIs" dxfId="26" priority="20" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D71:I71">
-    <cfRule type="expression" dxfId="26" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="21" stopIfTrue="1">
       <formula>#REF!=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C39:I39">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26686,8 +26686,8 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="74" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -26703,8 +26703,8 @@
         <v>1061</v>
       </c>
       <c r="B1" s="81" t="str">
-        <f>_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3)</f>
-        <v xml:space="preserve">, </v>
+        <f>IF('Master Info'!C2&lt;&gt;"",_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3),"Add location in master info tab")</f>
+        <v>Add location in master info tab</v>
       </c>
       <c r="C1" s="82"/>
       <c r="D1" s="82"/>
@@ -26752,8 +26752,8 @@
         <v>1063</v>
       </c>
       <c r="B4" s="227" t="str">
-        <f>_xlfn.CONCAT("For the year ended ", TEXT('Master Info'!C4, "mmmm dd, yyyy"))</f>
-        <v>For the year ended January 00, 1900</v>
+        <f>IF('Master Info'!C4, 'Master Info'!C4, "Add date in Master Info tab")</f>
+        <v>Add date in Master Info tab</v>
       </c>
       <c r="C4" s="82"/>
       <c r="D4" s="82"/>
@@ -28169,106 +28169,106 @@
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
   <conditionalFormatting sqref="A9:A22">
-    <cfRule type="containsText" dxfId="25" priority="5" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="24" priority="5" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:A37">
-    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:A51">
-    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55:A63">
-    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="custom">
+    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="custom">
       <formula>NOT(ISERROR(SEARCH("custom",A55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="20" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="23" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="19" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="22" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:I24 C53:I53">
-    <cfRule type="expression" dxfId="18" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="29" stopIfTrue="1">
       <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:I52">
-    <cfRule type="expression" dxfId="17" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="20" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:I64">
-    <cfRule type="expression" dxfId="16" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D69:I69">
-    <cfRule type="expression" dxfId="15" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
       <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:J65">
-    <cfRule type="expression" dxfId="14" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="8" stopIfTrue="1">
       <formula>D$7=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="notEqual">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
       <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D69:J69">
-    <cfRule type="expression" dxfId="9" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="13" stopIfTrue="1">
       <formula>D$7=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="14" stopIfTrue="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="16" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="16" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="15" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="14" stopIfTrue="1" operator="equal">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J4 J8:J22 J24:J64 J70:J1048574">
-    <cfRule type="expression" dxfId="5" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="24" stopIfTrue="1">
       <formula>COUNTA(D2:I2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:J22 J24:J64 J70:J78">
-    <cfRule type="expression" dxfId="4" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="85" stopIfTrue="1">
       <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J68">
-    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
-      <formula>COUNTA(D69:I69)=1</formula>
-    </cfRule>
     <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">
       <formula>#REF!=""</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="1" priority="6" stopIfTrue="1">
+      <formula>COUNTA(D69:I69)=1</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1048575:J1048576">
-    <cfRule type="expression" dxfId="1" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="87" stopIfTrue="1">
       <formula>COUNTA(D1:I3)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -48124,8 +48124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8474313-8EAC-0141-BA8E-861AF31ED060}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView zoomScale="92" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -48295,7 +48295,7 @@
       <c r="B44" s="252"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C7" xr:uid="{146644EA-53C7-1642-84D4-FDA957F35368}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
@@ -48311,8 +48311,8 @@
   </sheetPr>
   <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView zoomScale="88" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B11" sqref="B9:B11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -48329,7 +48329,7 @@
         <v>1061</v>
       </c>
       <c r="B1" s="42" t="str">
-        <f>IF('Master Info'!C2, _xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3), "Add location in master info tab")</f>
+        <f>IF('Master Info'!C2&lt;&gt;"",_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3),"Add location in master info tab")</f>
         <v>Add location in master info tab</v>
       </c>
       <c r="C1" s="38"/>
@@ -49800,7 +49800,7 @@
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23:F23 C37:F37 C50 C65:F65 C76:C77 C89 C101 D6:F37 D39:F101">
+  <conditionalFormatting sqref="D6:F37 C23:F23 C37:F37 D39:F101 C50 C65:F65 C76:C77 C89 C101">
     <cfRule type="expression" dxfId="97" priority="25" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
@@ -49990,8 +49990,8 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScale="84" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -50012,8 +50012,8 @@
         <v>1061</v>
       </c>
       <c r="B1" s="42" t="str">
-        <f>_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3)</f>
-        <v xml:space="preserve">, </v>
+        <f>IF('Master Info'!C2&lt;&gt;"",_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3),"Add location in master info tab")</f>
+        <v>Add location in master info tab</v>
       </c>
       <c r="C1" s="38"/>
       <c r="D1" s="32"/>
@@ -50043,8 +50043,8 @@
         <v>1063</v>
       </c>
       <c r="B4" s="197" t="str">
-        <f>_xlfn.CONCAT("For the year ended ", TEXT('Master Info'!C4, "mmmm dd, yyyy"))</f>
-        <v>For the year ended January 00, 1900</v>
+        <f>IF('Master Info'!C4, 'Master Info'!C4, "Add date in Master Info tab")</f>
+        <v>Add date in Master Info tab</v>
       </c>
       <c r="C4" s="38"/>
       <c r="D4" s="32"/>
@@ -51688,62 +51688,62 @@
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C71:G71 I71:J71 C72:J72">
-    <cfRule type="expression" dxfId="84" priority="24" stopIfTrue="1">
+  <conditionalFormatting sqref="C71:J71">
+    <cfRule type="expression" dxfId="84" priority="1" stopIfTrue="1">
+      <formula>C$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C72:J72">
+    <cfRule type="expression" dxfId="83" priority="24" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:F6 D52:F52">
-    <cfRule type="expression" dxfId="83" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="60" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39:G51">
-    <cfRule type="expression" dxfId="82" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="20" stopIfTrue="1">
+      <formula>D$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7:J37 J39:J50">
+    <cfRule type="expression" dxfId="80" priority="18" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:J70">
-    <cfRule type="expression" dxfId="81" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="16" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I78:I99 D74:J77">
-    <cfRule type="expression" dxfId="80" priority="15" stopIfTrue="1">
+  <conditionalFormatting sqref="D74:J77 I78:I99">
+    <cfRule type="expression" dxfId="78" priority="15" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39:H50">
-    <cfRule type="expression" dxfId="79" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="19" stopIfTrue="1">
+      <formula>H$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:J6 I39:I51">
+    <cfRule type="expression" dxfId="76" priority="53" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38:J38">
-    <cfRule type="expression" dxfId="78" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="57" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:J6 I39:I51 J23 D7:I37 J37">
-    <cfRule type="expression" dxfId="77" priority="53" stopIfTrue="1">
-      <formula>D$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H52:J63">
-    <cfRule type="expression" dxfId="76" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="17" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J7:J22 J24:J36 J39:J50">
-    <cfRule type="expression" dxfId="73" priority="18" stopIfTrue="1">
-      <formula>J$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H71">
-    <cfRule type="expression" dxfId="71" priority="1" stopIfTrue="1">
-      <formula>H$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B41:B49 B9:B22 B25:B36" xr:uid="{F3C11D5E-2141-5546-AF1F-2279D6DA74D8}">
       <formula1>program_revenues</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
#203 add license disclaimer to Excel template
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729E39D0-104E-B14B-8FFE-E49576C28EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C35B7A-DA6E-3849-A4D5-5BBBD3B99592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="834" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5400" uniqueCount="3654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5403" uniqueCount="3657">
   <si>
     <t>Statement of Net Position</t>
   </si>
@@ -11055,6 +11055,15 @@
   </si>
   <si>
     <t>acfr:OperatingIncomeLoss</t>
+  </si>
+  <si>
+    <t>License information and dislaimer:</t>
+  </si>
+  <si>
+    <t>Read full license</t>
+  </si>
+  <si>
+    <t>By using this tool, you acknowledge that you have read and agreed to the terms of use. This is a research tool that is available for demonstration and educational purposes only and may contain errors. You are expressly prohibited from using the tool for production of official financial reports or regulatory filings. Data uploaded as part of using the tool will not be stored on a server and will be deleted at the end of the session. iXBRL output and downloadable html files will also not be stored on a server, and will be deleted once the browser window has been closed.</t>
   </si>
 </sst>
 </file>
@@ -11724,7 +11733,7 @@
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="270">
+  <cellXfs count="272">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -12218,7 +12227,6 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="44" fontId="23" fillId="13" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -12262,6 +12270,13 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -19317,7 +19332,7 @@
     <col min="11" max="16384" width="10.83203125" style="120"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16">
+    <row r="1" spans="1:10" ht="17">
       <c r="A1" s="80" t="s">
         <v>1061</v>
       </c>
@@ -19351,7 +19366,7 @@
       <c r="D3" s="178"/>
       <c r="E3" s="178"/>
     </row>
-    <row r="4" spans="1:10" ht="17" thickBot="1">
+    <row r="4" spans="1:10" ht="18" thickBot="1">
       <c r="A4" s="87" t="s">
         <v>1063</v>
       </c>
@@ -20372,18 +20387,18 @@
       </c>
     </row>
     <row r="59" spans="1:10" ht="15">
-      <c r="A59" s="265" t="s">
+      <c r="A59" s="264" t="s">
         <v>3611</v>
       </c>
-      <c r="B59" s="266"/>
-      <c r="C59" s="266"/>
-      <c r="D59" s="266"/>
-      <c r="E59" s="266"/>
-      <c r="F59" s="266"/>
-      <c r="G59" s="266"/>
-      <c r="H59" s="266"/>
-      <c r="I59" s="266"/>
-      <c r="J59" s="267"/>
+      <c r="B59" s="265"/>
+      <c r="C59" s="265"/>
+      <c r="D59" s="265"/>
+      <c r="E59" s="265"/>
+      <c r="F59" s="265"/>
+      <c r="G59" s="265"/>
+      <c r="H59" s="265"/>
+      <c r="I59" s="265"/>
+      <c r="J59" s="266"/>
     </row>
     <row r="60" spans="1:10" ht="15">
       <c r="A60" s="108" t="str">
@@ -20420,18 +20435,18 @@
       </c>
     </row>
     <row r="62" spans="1:10" ht="15">
-      <c r="A62" s="265" t="s">
+      <c r="A62" s="264" t="s">
         <v>3612</v>
       </c>
-      <c r="B62" s="266"/>
-      <c r="C62" s="266"/>
-      <c r="D62" s="266"/>
-      <c r="E62" s="266"/>
-      <c r="F62" s="266"/>
-      <c r="G62" s="266"/>
-      <c r="H62" s="266"/>
-      <c r="I62" s="266"/>
-      <c r="J62" s="267"/>
+      <c r="B62" s="265"/>
+      <c r="C62" s="265"/>
+      <c r="D62" s="265"/>
+      <c r="E62" s="265"/>
+      <c r="F62" s="265"/>
+      <c r="G62" s="265"/>
+      <c r="H62" s="265"/>
+      <c r="I62" s="265"/>
+      <c r="J62" s="266"/>
     </row>
     <row r="63" spans="1:10" ht="15">
       <c r="A63" s="108" t="str">
@@ -20468,18 +20483,18 @@
       </c>
     </row>
     <row r="65" spans="1:10" ht="15">
-      <c r="A65" s="265" t="s">
+      <c r="A65" s="264" t="s">
         <v>3613</v>
       </c>
-      <c r="B65" s="266"/>
-      <c r="C65" s="266"/>
-      <c r="D65" s="266"/>
-      <c r="E65" s="266"/>
-      <c r="F65" s="266"/>
-      <c r="G65" s="266"/>
-      <c r="H65" s="266"/>
-      <c r="I65" s="266"/>
-      <c r="J65" s="267"/>
+      <c r="B65" s="265"/>
+      <c r="C65" s="265"/>
+      <c r="D65" s="265"/>
+      <c r="E65" s="265"/>
+      <c r="F65" s="265"/>
+      <c r="G65" s="265"/>
+      <c r="H65" s="265"/>
+      <c r="I65" s="265"/>
+      <c r="J65" s="266"/>
     </row>
     <row r="66" spans="1:10" ht="16">
       <c r="A66" s="131" t="str">
@@ -20783,7 +20798,7 @@
         <v>2460</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17" thickBot="1">
+    <row r="4" spans="1:2" ht="18" thickBot="1">
       <c r="A4" s="87" t="s">
         <v>1063</v>
       </c>
@@ -20829,7 +20844,7 @@
       <c r="B13" s="207"/>
     </row>
     <row r="14" spans="1:2" ht="15">
-      <c r="A14" s="254" t="s">
+      <c r="A14" s="253" t="s">
         <v>3629</v>
       </c>
       <c r="B14" s="207">
@@ -20860,7 +20875,7 @@
       <c r="B19" s="207"/>
     </row>
     <row r="20" spans="1:2" ht="15">
-      <c r="A20" s="254" t="s">
+      <c r="A20" s="253" t="s">
         <v>3630</v>
       </c>
       <c r="B20" s="207">
@@ -20891,7 +20906,7 @@
       <c r="B25" s="207"/>
     </row>
     <row r="26" spans="1:2" ht="15">
-      <c r="A26" s="255" t="s">
+      <c r="A26" s="254" t="s">
         <v>3631</v>
       </c>
       <c r="B26" s="207">
@@ -20922,7 +20937,7 @@
       <c r="B31" s="207"/>
     </row>
     <row r="32" spans="1:2" ht="15">
-      <c r="A32" s="254" t="s">
+      <c r="A32" s="253" t="s">
         <v>3632</v>
       </c>
       <c r="B32" s="221">
@@ -20940,7 +20955,7 @@
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="257" t="s">
+      <c r="A36" s="256" t="s">
         <v>3627</v>
       </c>
       <c r="B36" s="250"/>
@@ -21009,7 +21024,7 @@
     <col min="11" max="16384" width="9" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16">
+    <row r="1" spans="1:10" ht="17">
       <c r="A1" s="28" t="s">
         <v>1061</v>
       </c>
@@ -22358,12 +22373,12 @@
       </c>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" s="261"/>
+      <c r="A73" s="260"/>
       <c r="B73" s="247"/>
       <c r="C73" s="248"/>
     </row>
     <row r="74" spans="1:10">
-      <c r="B74" s="262"/>
+      <c r="B74" s="261"/>
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
@@ -22485,7 +22500,7 @@
     <col min="3" max="16384" width="10.83203125" style="120"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16">
+    <row r="1" spans="1:2" ht="17">
       <c r="A1" s="80" t="s">
         <v>1061</v>
       </c>
@@ -22510,7 +22525,7 @@
         <v>2847</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17" thickBot="1">
+    <row r="4" spans="1:2" ht="18" thickBot="1">
       <c r="A4" s="87" t="s">
         <v>1063</v>
       </c>
@@ -22555,7 +22570,7 @@
       <c r="B12" s="207"/>
     </row>
     <row r="13" spans="1:2" ht="15">
-      <c r="A13" s="254" t="s">
+      <c r="A13" s="253" t="s">
         <v>3633</v>
       </c>
       <c r="B13" s="207">
@@ -22586,7 +22601,7 @@
       <c r="B18" s="207"/>
     </row>
     <row r="19" spans="1:2" ht="15">
-      <c r="A19" s="254" t="s">
+      <c r="A19" s="253" t="s">
         <v>3634</v>
       </c>
       <c r="B19" s="207">
@@ -22617,7 +22632,7 @@
       <c r="B24" s="207"/>
     </row>
     <row r="25" spans="1:2" ht="15">
-      <c r="A25" s="254" t="s">
+      <c r="A25" s="253" t="s">
         <v>3635</v>
       </c>
       <c r="B25" s="207">
@@ -22635,14 +22650,14 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="263" t="s">
+      <c r="A29" s="262" t="s">
         <v>3627</v>
       </c>
-      <c r="B29" s="264"/>
+      <c r="B29" s="263"/>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="264"/>
-      <c r="B30" s="264"/>
+      <c r="A30" s="263"/>
+      <c r="B30" s="263"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24815,7 +24830,7 @@
     </row>
     <row r="112" spans="1:10" s="33" customFormat="1" ht="15">
       <c r="A112" s="249"/>
-      <c r="B112" s="268" t="s">
+      <c r="B112" s="267" t="s">
         <v>3627</v>
       </c>
       <c r="C112" s="84"/>
@@ -24829,7 +24844,7 @@
     </row>
     <row r="113" spans="1:10" s="33" customFormat="1" ht="15">
       <c r="A113" s="249"/>
-      <c r="B113" s="269"/>
+      <c r="B113" s="268"/>
       <c r="C113" s="84"/>
       <c r="D113" s="84"/>
       <c r="E113" s="84"/>
@@ -26459,7 +26474,7 @@
     </row>
     <row r="74" spans="1:10" ht="15">
       <c r="A74" s="251"/>
-      <c r="B74" s="258" t="s">
+      <c r="B74" s="257" t="s">
         <v>3627</v>
       </c>
       <c r="J74" s="112"/>
@@ -28132,7 +28147,7 @@
     </row>
     <row r="77" spans="1:10" ht="15">
       <c r="A77" s="249"/>
-      <c r="B77" s="256" t="s">
+      <c r="B77" s="255" t="s">
         <v>3627</v>
       </c>
       <c r="C77" s="155"/>
@@ -48122,10 +48137,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8474313-8EAC-0141-BA8E-861AF31ED060}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -48164,8 +48179,8 @@
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="260"/>
-      <c r="B6" s="259" t="s">
+      <c r="A6" s="259"/>
+      <c r="B6" s="258" t="s">
         <v>1088</v>
       </c>
       <c r="C6" s="25" t="s">
@@ -48174,7 +48189,7 @@
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="14" thickBot="1">
-      <c r="A7" s="260"/>
+      <c r="A7" s="259"/>
       <c r="B7" s="24" t="s">
         <v>3636</v>
       </c>
@@ -48271,35 +48286,65 @@
         <v>3622</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="253" t="s">
+    <row r="33" spans="2:6" ht="67" customHeight="1">
+      <c r="B33" s="271" t="s">
         <v>3628</v>
       </c>
-    </row>
-    <row r="35" spans="2:2">
+      <c r="C33" s="271"/>
+      <c r="D33" s="271"/>
+      <c r="E33" s="271"/>
+      <c r="F33" s="271"/>
+    </row>
+    <row r="35" spans="2:6">
       <c r="B35" s="60" t="s">
         <v>3643</v>
       </c>
     </row>
-    <row r="36" spans="2:2">
+    <row r="36" spans="2:6">
       <c r="B36" t="s">
         <v>3623</v>
       </c>
     </row>
-    <row r="37" spans="2:2">
+    <row r="37" spans="2:6">
       <c r="B37" t="s">
         <v>3624</v>
       </c>
     </row>
-    <row r="44" spans="2:2">
+    <row r="39" spans="2:6">
+      <c r="B39" s="60" t="s">
+        <v>3654</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="69" customHeight="1">
+      <c r="B40" s="269" t="s">
+        <v>3656</v>
+      </c>
+      <c r="C40" s="269"/>
+      <c r="D40" s="269"/>
+      <c r="E40" s="269"/>
+      <c r="F40" s="269"/>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41" s="270" t="s">
+        <v>3655</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
       <c r="B44" s="252"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B33:F33"/>
+  </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C7" xr:uid="{146644EA-53C7-1642-84D4-FDA957F35368}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B41" r:id="rId1" xr:uid="{4D17274D-0E43-2B45-863C-8156A99400E7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -49733,7 +49778,7 @@
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="249"/>
-      <c r="B104" s="256" t="s">
+      <c r="B104" s="255" t="s">
         <v>3627</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#203 adjust disclaimer language and hyperlinks in Excel template
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C35B7A-DA6E-3849-A4D5-5BBBD3B99592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE508349-6D4A-6247-8B75-E9F9B003616F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="834" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5403" uniqueCount="3657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5402" uniqueCount="3656">
   <si>
     <t>Statement of Net Position</t>
   </si>
@@ -10937,9 +10937,6 @@
     <t>Custom Restricted Fund Balance</t>
   </si>
   <si>
-    <t>This template is designed to help you prepare your financial statements for submission and convert them into XBRL format.</t>
-  </si>
-  <si>
     <t>Steps</t>
   </si>
   <si>
@@ -11060,10 +11057,42 @@
     <t>License information and dislaimer:</t>
   </si>
   <si>
-    <t>Read full license</t>
-  </si>
-  <si>
-    <t>By using this tool, you acknowledge that you have read and agreed to the terms of use. This is a research tool that is available for demonstration and educational purposes only and may contain errors. You are expressly prohibited from using the tool for production of official financial reports or regulatory filings. Data uploaded as part of using the tool will not be stored on a server and will be deleted at the end of the session. iXBRL output and downloadable html files will also not be stored on a server, and will be deleted once the browser window has been closed.</t>
+    <r>
+      <t>This template is designed to convert your financial statements into XBRL format as part of the excel to IXBRL conversion tool:</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> https://closup.umich.edu/acfr-tool.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">By using this tool, you acknowledge that you have read and agreed to the </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>terms of use</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. This is a research tool that is available for demonstration and educational purposes only and may contain errors. You are expressly prohibited from using the tool for production of official financial reports or regulatory filings. Data uploaded as part of using the tool will not be stored on a server and will be deleted at the end of the session. iXBRL output and downloadable html files will also not be stored on a server, and will be deleted once the browser window has been closed.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -11075,7 +11104,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="35">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -11281,6 +11310,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -11733,7 +11769,7 @@
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="272">
+  <cellXfs count="274">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -12256,6 +12292,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -12271,12 +12314,11 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -13341,6 +13383,141 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1866900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1168400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54E475B9-1CDF-97C4-155B-B0E76AA4FD90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2171700" y="2159000"/>
+          <a:ext cx="2070100" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>317500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA202146-2FB5-2485-3A6D-C00C24FB9D17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4724400" y="7696200"/>
+          <a:ext cx="774700" cy="139700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -20387,18 +20564,18 @@
       </c>
     </row>
     <row r="59" spans="1:10" ht="15">
-      <c r="A59" s="264" t="s">
+      <c r="A59" s="267" t="s">
         <v>3611</v>
       </c>
-      <c r="B59" s="265"/>
-      <c r="C59" s="265"/>
-      <c r="D59" s="265"/>
-      <c r="E59" s="265"/>
-      <c r="F59" s="265"/>
-      <c r="G59" s="265"/>
-      <c r="H59" s="265"/>
-      <c r="I59" s="265"/>
-      <c r="J59" s="266"/>
+      <c r="B59" s="268"/>
+      <c r="C59" s="268"/>
+      <c r="D59" s="268"/>
+      <c r="E59" s="268"/>
+      <c r="F59" s="268"/>
+      <c r="G59" s="268"/>
+      <c r="H59" s="268"/>
+      <c r="I59" s="268"/>
+      <c r="J59" s="269"/>
     </row>
     <row r="60" spans="1:10" ht="15">
       <c r="A60" s="108" t="str">
@@ -20435,18 +20612,18 @@
       </c>
     </row>
     <row r="62" spans="1:10" ht="15">
-      <c r="A62" s="264" t="s">
+      <c r="A62" s="267" t="s">
         <v>3612</v>
       </c>
-      <c r="B62" s="265"/>
-      <c r="C62" s="265"/>
-      <c r="D62" s="265"/>
-      <c r="E62" s="265"/>
-      <c r="F62" s="265"/>
-      <c r="G62" s="265"/>
-      <c r="H62" s="265"/>
-      <c r="I62" s="265"/>
-      <c r="J62" s="266"/>
+      <c r="B62" s="268"/>
+      <c r="C62" s="268"/>
+      <c r="D62" s="268"/>
+      <c r="E62" s="268"/>
+      <c r="F62" s="268"/>
+      <c r="G62" s="268"/>
+      <c r="H62" s="268"/>
+      <c r="I62" s="268"/>
+      <c r="J62" s="269"/>
     </row>
     <row r="63" spans="1:10" ht="15">
       <c r="A63" s="108" t="str">
@@ -20483,18 +20660,18 @@
       </c>
     </row>
     <row r="65" spans="1:10" ht="15">
-      <c r="A65" s="264" t="s">
+      <c r="A65" s="267" t="s">
         <v>3613</v>
       </c>
-      <c r="B65" s="265"/>
-      <c r="C65" s="265"/>
-      <c r="D65" s="265"/>
-      <c r="E65" s="265"/>
-      <c r="F65" s="265"/>
-      <c r="G65" s="265"/>
-      <c r="H65" s="265"/>
-      <c r="I65" s="265"/>
-      <c r="J65" s="266"/>
+      <c r="B65" s="268"/>
+      <c r="C65" s="268"/>
+      <c r="D65" s="268"/>
+      <c r="E65" s="268"/>
+      <c r="F65" s="268"/>
+      <c r="G65" s="268"/>
+      <c r="H65" s="268"/>
+      <c r="I65" s="268"/>
+      <c r="J65" s="269"/>
     </row>
     <row r="66" spans="1:10" ht="16">
       <c r="A66" s="131" t="str">
@@ -20610,7 +20787,7 @@
     <row r="72" spans="1:10">
       <c r="A72" s="250"/>
       <c r="B72" s="246" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -20845,7 +21022,7 @@
     </row>
     <row r="14" spans="1:2" ht="15">
       <c r="A14" s="253" t="s">
-        <v>3629</v>
+        <v>3628</v>
       </c>
       <c r="B14" s="207">
         <f>SUM(B9:B13)</f>
@@ -20876,7 +21053,7 @@
     </row>
     <row r="20" spans="1:2" ht="15">
       <c r="A20" s="253" t="s">
-        <v>3630</v>
+        <v>3629</v>
       </c>
       <c r="B20" s="207">
         <f>SUM(B16:B19)</f>
@@ -20907,7 +21084,7 @@
     </row>
     <row r="26" spans="1:2" ht="15">
       <c r="A26" s="254" t="s">
-        <v>3631</v>
+        <v>3630</v>
       </c>
       <c r="B26" s="207">
         <f>SUM(B22:B25)</f>
@@ -20938,7 +21115,7 @@
     </row>
     <row r="32" spans="1:2" ht="15">
       <c r="A32" s="253" t="s">
-        <v>3632</v>
+        <v>3631</v>
       </c>
       <c r="B32" s="221">
         <f>SUM(B28:B31)</f>
@@ -20956,7 +21133,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="256" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
       <c r="B36" s="250"/>
     </row>
@@ -22210,7 +22387,7 @@
         <v>1083</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>3651</v>
+        <v>3650</v>
       </c>
       <c r="C63" s="200"/>
       <c r="D63" s="201"/>
@@ -22369,7 +22546,7 @@
     <row r="72" spans="1:10">
       <c r="A72" s="247"/>
       <c r="B72" s="246" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -22571,7 +22748,7 @@
     </row>
     <row r="13" spans="1:2" ht="15">
       <c r="A13" s="253" t="s">
-        <v>3633</v>
+        <v>3632</v>
       </c>
       <c r="B13" s="207">
         <f>SUM(B9:B12)</f>
@@ -22602,7 +22779,7 @@
     </row>
     <row r="19" spans="1:2" ht="15">
       <c r="A19" s="253" t="s">
-        <v>3634</v>
+        <v>3633</v>
       </c>
       <c r="B19" s="207">
         <f>SUM(B15:B18)</f>
@@ -22633,7 +22810,7 @@
     </row>
     <row r="25" spans="1:2" ht="15">
       <c r="A25" s="253" t="s">
-        <v>3635</v>
+        <v>3634</v>
       </c>
       <c r="B25" s="207">
         <f>SUM(B21:B24)</f>
@@ -22651,7 +22828,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="262" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
       <c r="B29" s="263"/>
     </row>
@@ -24830,8 +25007,8 @@
     </row>
     <row r="112" spans="1:10" s="33" customFormat="1" ht="15">
       <c r="A112" s="249"/>
-      <c r="B112" s="267" t="s">
-        <v>3627</v>
+      <c r="B112" s="270" t="s">
+        <v>3626</v>
       </c>
       <c r="C112" s="84"/>
       <c r="D112" s="84"/>
@@ -24844,7 +25021,7 @@
     </row>
     <row r="113" spans="1:10" s="33" customFormat="1" ht="15">
       <c r="A113" s="249"/>
-      <c r="B113" s="268"/>
+      <c r="B113" s="271"/>
       <c r="C113" s="84"/>
       <c r="D113" s="84"/>
       <c r="E113" s="84"/>
@@ -24871,7 +25048,7 @@
     </row>
     <row r="116" spans="1:10" ht="15">
       <c r="B116" s="246" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
       <c r="J116" s="112"/>
     </row>
@@ -25769,10 +25946,10 @@
     </row>
     <row r="39" spans="1:11" ht="18" customHeight="1">
       <c r="A39" s="139" t="s">
-        <v>3653</v>
+        <v>3652</v>
       </c>
       <c r="B39" s="140" t="s">
-        <v>3652</v>
+        <v>3651</v>
       </c>
       <c r="C39" s="229">
         <f>C23-C38</f>
@@ -26475,7 +26652,7 @@
     <row r="74" spans="1:10" ht="15">
       <c r="A74" s="251"/>
       <c r="B74" s="257" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
       <c r="J74" s="112"/>
     </row>
@@ -28148,7 +28325,7 @@
     <row r="77" spans="1:10" ht="15">
       <c r="A77" s="249"/>
       <c r="B77" s="255" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
       <c r="C77" s="155"/>
       <c r="D77" s="155"/>
@@ -31681,7 +31858,7 @@
         <v>1139</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>3646</v>
+        <v>3645</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15">
@@ -31701,7 +31878,7 @@
         <v>1237</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>3648</v>
+        <v>3647</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15">
@@ -35104,7 +35281,7 @@
         <v>1237</v>
       </c>
       <c r="G202" s="2" t="s">
-        <v>3649</v>
+        <v>3648</v>
       </c>
     </row>
     <row r="203" spans="1:7" ht="15">
@@ -35330,7 +35507,7 @@
     </row>
     <row r="216" spans="1:7" ht="15">
       <c r="A216" s="2" t="s">
-        <v>3650</v>
+        <v>3649</v>
       </c>
       <c r="B216" t="s">
         <v>1237</v>
@@ -35345,7 +35522,7 @@
         <v>1623</v>
       </c>
       <c r="G216" s="2" t="s">
-        <v>3647</v>
+        <v>3646</v>
       </c>
     </row>
     <row r="217" spans="1:7">
@@ -48139,8 +48316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8474313-8EAC-0141-BA8E-861AF31ED060}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -48165,7 +48342,7 @@
     </row>
     <row r="4" spans="1:5" ht="16">
       <c r="B4" s="23" t="s">
-        <v>3645</v>
+        <v>3644</v>
       </c>
       <c r="C4" s="41"/>
     </row>
@@ -48191,36 +48368,39 @@
     <row r="7" spans="1:5" ht="14" thickBot="1">
       <c r="A7" s="259"/>
       <c r="B7" s="24" t="s">
-        <v>3636</v>
+        <v>3635</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>3644</v>
+        <v>3643</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="14">
       <c r="B11" s="245" t="s">
-        <v>3625</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="B12" t="s">
-        <v>3614</v>
-      </c>
+        <v>3624</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="34" customHeight="1">
+      <c r="B12" s="273" t="s">
+        <v>3654</v>
+      </c>
+      <c r="C12" s="272"/>
+      <c r="D12" s="272"/>
+      <c r="E12" s="272"/>
     </row>
     <row r="14" spans="1:5" ht="14" customHeight="1">
       <c r="B14" s="60" t="s">
-        <v>3615</v>
+        <v>3614</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14" customHeight="1">
       <c r="B15" s="60" t="s">
-        <v>3638</v>
+        <v>3637</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14" customHeight="1">
       <c r="B16" s="2" t="s">
-        <v>3637</v>
+        <v>3636</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14" customHeight="1">
@@ -48228,124 +48408,121 @@
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="60" t="s">
-        <v>3639</v>
+        <v>3638</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="2" t="s">
-        <v>3626</v>
+        <v>3625</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>3616</v>
+        <v>3615</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="60" t="s">
-        <v>3640</v>
+        <v>3639</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>3617</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>3618</v>
+        <v>3617</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" s="60" t="s">
-        <v>3641</v>
+        <v>3640</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>3619</v>
+        <v>3618</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" s="60" t="s">
-        <v>3642</v>
+        <v>3641</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" t="s">
-        <v>3620</v>
+        <v>3619</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" t="s">
-        <v>3621</v>
+        <v>3620</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" t="s">
-        <v>3622</v>
+        <v>3621</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="67" customHeight="1">
-      <c r="B33" s="271" t="s">
-        <v>3628</v>
-      </c>
-      <c r="C33" s="271"/>
-      <c r="D33" s="271"/>
-      <c r="E33" s="271"/>
-      <c r="F33" s="271"/>
+      <c r="B33" s="266" t="s">
+        <v>3627</v>
+      </c>
+      <c r="C33" s="266"/>
+      <c r="D33" s="266"/>
+      <c r="E33" s="266"/>
+      <c r="F33" s="266"/>
     </row>
     <row r="35" spans="2:6">
       <c r="B35" s="60" t="s">
-        <v>3643</v>
+        <v>3642</v>
       </c>
     </row>
     <row r="36" spans="2:6">
       <c r="B36" t="s">
-        <v>3623</v>
+        <v>3622</v>
       </c>
     </row>
     <row r="37" spans="2:6">
       <c r="B37" t="s">
-        <v>3624</v>
+        <v>3623</v>
       </c>
     </row>
     <row r="39" spans="2:6">
       <c r="B39" s="60" t="s">
-        <v>3654</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" ht="69" customHeight="1">
-      <c r="B40" s="269" t="s">
-        <v>3656</v>
-      </c>
-      <c r="C40" s="269"/>
-      <c r="D40" s="269"/>
-      <c r="E40" s="269"/>
-      <c r="F40" s="269"/>
+        <v>3653</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="89" customHeight="1">
+      <c r="B40" s="265" t="s">
+        <v>3655</v>
+      </c>
+      <c r="C40" s="265"/>
+      <c r="D40" s="265"/>
+      <c r="E40" s="265"/>
+      <c r="F40" s="265"/>
     </row>
     <row r="41" spans="2:6">
-      <c r="B41" s="270" t="s">
-        <v>3655</v>
-      </c>
+      <c r="B41" s="264"/>
     </row>
     <row r="44" spans="2:6">
       <c r="B44" s="252"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B40:F40"/>
     <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B12:E12"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C7" xr:uid="{146644EA-53C7-1642-84D4-FDA957F35368}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B41" r:id="rId1" xr:uid="{4D17274D-0E43-2B45-863C-8156A99400E7}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -49779,7 +49956,7 @@
     <row r="104" spans="1:6">
       <c r="A104" s="249"/>
       <c r="B104" s="255" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -51633,7 +51810,7 @@
     <row r="80" spans="1:10" ht="15">
       <c r="A80" s="249"/>
       <c r="B80" s="246" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
       <c r="I80" s="54"/>
     </row>

</xml_diff>

<commit_message>
#203 capitalize Excel and merge readme cells
</commit_message>
<xml_diff>
--- a/app/static/input_files/ACFR_template.xlsx
+++ b/app/static/input_files/ACFR_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/app/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE508349-6D4A-6247-8B75-E9F9B003616F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A34D65-6504-0248-9D0C-5C8552F197AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="834" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11058,21 +11058,6 @@
   </si>
   <si>
     <r>
-      <t>This template is designed to convert your financial statements into XBRL format as part of the excel to IXBRL conversion tool:</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> https://closup.umich.edu/acfr-tool.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">By using this tool, you acknowledge that you have read and agreed to the </t>
     </r>
     <r>
@@ -11092,6 +11077,21 @@
         <family val="2"/>
       </rPr>
       <t>. This is a research tool that is available for demonstration and educational purposes only and may contain errors. You are expressly prohibited from using the tool for production of official financial reports or regulatory filings. Data uploaded as part of using the tool will not be stored on a server and will be deleted at the end of the session. iXBRL output and downloadable html files will also not be stored on a server, and will be deleted once the browser window has been closed.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>This template is designed to convert your financial statements into XBRL format as part of the Excel to IXBRL conversion tool:</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> https://closup.umich.edu/acfr-tool.</t>
     </r>
   </si>
 </sst>
@@ -48317,7 +48317,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -48327,26 +48327,26 @@
     <col min="3" max="3" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14" thickBot="1"/>
-    <row r="2" spans="1:5">
+    <row r="1" spans="1:6" ht="14" thickBot="1"/>
+    <row r="2" spans="1:6">
       <c r="B2" s="22" t="s">
         <v>1061</v>
       </c>
       <c r="C2" s="27"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="B3" s="23" t="s">
         <v>1275</v>
       </c>
       <c r="C3" s="72"/>
     </row>
-    <row r="4" spans="1:5" ht="16">
+    <row r="4" spans="1:6" ht="16">
       <c r="B4" s="23" t="s">
         <v>3644</v>
       </c>
       <c r="C4" s="41"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="B5" s="23" t="s">
         <v>1087</v>
       </c>
@@ -48355,7 +48355,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="259"/>
       <c r="B6" s="258" t="s">
         <v>1088</v>
@@ -48365,7 +48365,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" ht="14" thickBot="1">
+    <row r="7" spans="1:6" ht="14" thickBot="1">
       <c r="A7" s="259"/>
       <c r="B7" s="24" t="s">
         <v>3635</v>
@@ -48375,33 +48375,37 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="14">
+    <row r="11" spans="1:6" ht="14">
       <c r="B11" s="245" t="s">
         <v>3624</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="34" customHeight="1">
+    <row r="12" spans="1:6" ht="34" customHeight="1">
       <c r="B12" s="273" t="s">
-        <v>3654</v>
+        <v>3655</v>
       </c>
       <c r="C12" s="272"/>
       <c r="D12" s="272"/>
       <c r="E12" s="272"/>
     </row>
-    <row r="14" spans="1:5" ht="14" customHeight="1">
+    <row r="14" spans="1:6" ht="14" customHeight="1">
       <c r="B14" s="60" t="s">
         <v>3614</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14" customHeight="1">
+    <row r="15" spans="1:6" ht="14" customHeight="1">
       <c r="B15" s="60" t="s">
         <v>3637</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14" customHeight="1">
-      <c r="B16" s="2" t="s">
+    <row r="16" spans="1:6" ht="28" customHeight="1">
+      <c r="B16" s="265" t="s">
         <v>3636</v>
       </c>
+      <c r="C16" s="265"/>
+      <c r="D16" s="265"/>
+      <c r="E16" s="265"/>
+      <c r="F16" s="265"/>
     </row>
     <row r="17" spans="2:2" ht="14" customHeight="1">
       <c r="B17" s="60"/>
@@ -48497,7 +48501,7 @@
     </row>
     <row r="40" spans="2:6" ht="89" customHeight="1">
       <c r="B40" s="265" t="s">
-        <v>3655</v>
+        <v>3654</v>
       </c>
       <c r="C40" s="265"/>
       <c r="D40" s="265"/>
@@ -48511,10 +48515,11 @@
       <c r="B44" s="252"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B40:F40"/>
     <mergeCell ref="B33:F33"/>
     <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B16:F16"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C7" xr:uid="{146644EA-53C7-1642-84D4-FDA957F35368}">

</xml_diff>